<commit_message>
feat: update paper forms
</commit_message>
<xml_diff>
--- a/public/files/bulk-upload-lettings-template-2024-25.xlsx
+++ b/public/files/bulk-upload-lettings-template-2024-25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mhclg.sharepoint.com/sites/HousingandplanningandCOREstatistics/Shared Documents/CORE Lettings/01 Annual log changes/2024-25/03 Materials for providers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="429" documentId="11_77304B1A9BA1AE53F84EE05360D243E6F58DE18B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CF6CFE4-0D5A-4F90-9EA0-403C7BCD8708}"/>
+  <xr:revisionPtr revIDLastSave="445" documentId="11_77304B1A9BA1AE53F84EE05360D243E6F58DE18B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D887E7A-65F3-456B-814B-C04A0C5272FB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="24-25 lettings template" sheetId="1" r:id="rId1"/>
@@ -485,12 +485,6 @@
     <t>General needs housing includes both self-contained and shared housing without support or specific adaptations. Supported housing includes direct access hostels, group homes, residential care and nursing homes.</t>
   </si>
   <si>
-    <t>Scheme code. Include the 'S' at the beginning if it has one.</t>
-  </si>
-  <si>
-    <t>Location code. This is the same as post code.</t>
-  </si>
-  <si>
     <t>If the property was previously being used as temporary accommodation, then answer 'no'.</t>
   </si>
   <si>
@@ -938,6 +932,14 @@
   </si>
   <si>
     <t>Field number</t>
+  </si>
+  <si>
+    <t>Scheme code. Include the 'S' at the beginning if it has one.
+You can find the scheme code on the CORE service under 'Schemes', either by searching for the specific scheme or downloading a csv.</t>
+  </si>
+  <si>
+    <t>Location code.
+You can find the location code on the CORE service under 'Schemes', either by searching for the specific location or downloading a csv.</t>
   </si>
 </sst>
 </file>
@@ -1227,7 +1229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1294,7 +1296,6 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1310,9 +1311,6 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1334,6 +1332,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1343,6 +1371,15 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1352,84 +1389,50 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1652,8 +1655,8 @@
   </sheetPr>
   <dimension ref="A1:EA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="EC5" sqref="EC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1694,150 +1697,150 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="57" t="s">
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="57"/>
-      <c r="V1" s="57"/>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="57"/>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="57"/>
-      <c r="AC1" s="57"/>
-      <c r="AD1" s="57"/>
-      <c r="AE1" s="57"/>
-      <c r="AF1" s="57"/>
-      <c r="AG1" s="57"/>
-      <c r="AH1" s="57"/>
-      <c r="AI1" s="57"/>
-      <c r="AJ1" s="57"/>
-      <c r="AK1" s="58" t="s">
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="59"/>
+      <c r="AA1" s="59"/>
+      <c r="AB1" s="59"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="59"/>
+      <c r="AF1" s="59"/>
+      <c r="AG1" s="59"/>
+      <c r="AH1" s="59"/>
+      <c r="AI1" s="59"/>
+      <c r="AJ1" s="59"/>
+      <c r="AK1" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="58"/>
-      <c r="AM1" s="58"/>
-      <c r="AN1" s="58"/>
-      <c r="AO1" s="58"/>
-      <c r="AP1" s="58"/>
-      <c r="AQ1" s="68" t="s">
+      <c r="AL1" s="60"/>
+      <c r="AM1" s="60"/>
+      <c r="AN1" s="60"/>
+      <c r="AO1" s="60"/>
+      <c r="AP1" s="60"/>
+      <c r="AQ1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="AR1" s="69"/>
-      <c r="AS1" s="69"/>
-      <c r="AT1" s="69"/>
-      <c r="AU1" s="69"/>
-      <c r="AV1" s="69"/>
-      <c r="AW1" s="69"/>
-      <c r="AX1" s="69"/>
-      <c r="AY1" s="69"/>
-      <c r="AZ1" s="69"/>
-      <c r="BA1" s="69"/>
-      <c r="BB1" s="69"/>
-      <c r="BC1" s="69"/>
-      <c r="BD1" s="69"/>
-      <c r="BE1" s="69"/>
-      <c r="BF1" s="69"/>
-      <c r="BG1" s="69"/>
-      <c r="BH1" s="69"/>
-      <c r="BI1" s="69"/>
-      <c r="BJ1" s="69"/>
-      <c r="BK1" s="69"/>
-      <c r="BL1" s="69"/>
-      <c r="BM1" s="69"/>
-      <c r="BN1" s="69"/>
-      <c r="BO1" s="69"/>
-      <c r="BP1" s="69"/>
-      <c r="BQ1" s="69"/>
-      <c r="BR1" s="69"/>
-      <c r="BS1" s="69"/>
-      <c r="BT1" s="69"/>
-      <c r="BU1" s="69"/>
-      <c r="BV1" s="69"/>
-      <c r="BW1" s="70"/>
-      <c r="BX1" s="59" t="s">
+      <c r="AR1" s="44"/>
+      <c r="AS1" s="44"/>
+      <c r="AT1" s="44"/>
+      <c r="AU1" s="44"/>
+      <c r="AV1" s="44"/>
+      <c r="AW1" s="44"/>
+      <c r="AX1" s="44"/>
+      <c r="AY1" s="44"/>
+      <c r="AZ1" s="44"/>
+      <c r="BA1" s="44"/>
+      <c r="BB1" s="44"/>
+      <c r="BC1" s="44"/>
+      <c r="BD1" s="44"/>
+      <c r="BE1" s="44"/>
+      <c r="BF1" s="44"/>
+      <c r="BG1" s="44"/>
+      <c r="BH1" s="44"/>
+      <c r="BI1" s="44"/>
+      <c r="BJ1" s="44"/>
+      <c r="BK1" s="44"/>
+      <c r="BL1" s="44"/>
+      <c r="BM1" s="44"/>
+      <c r="BN1" s="44"/>
+      <c r="BO1" s="44"/>
+      <c r="BP1" s="44"/>
+      <c r="BQ1" s="44"/>
+      <c r="BR1" s="44"/>
+      <c r="BS1" s="44"/>
+      <c r="BT1" s="44"/>
+      <c r="BU1" s="44"/>
+      <c r="BV1" s="44"/>
+      <c r="BW1" s="45"/>
+      <c r="BX1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="BY1" s="60"/>
-      <c r="BZ1" s="60"/>
-      <c r="CA1" s="60"/>
-      <c r="CB1" s="60"/>
-      <c r="CC1" s="60"/>
-      <c r="CD1" s="60"/>
-      <c r="CE1" s="60"/>
-      <c r="CF1" s="60"/>
-      <c r="CG1" s="60"/>
-      <c r="CH1" s="60"/>
-      <c r="CI1" s="60"/>
-      <c r="CJ1" s="60"/>
-      <c r="CK1" s="60"/>
-      <c r="CL1" s="60"/>
-      <c r="CM1" s="60"/>
-      <c r="CN1" s="60"/>
-      <c r="CO1" s="60"/>
-      <c r="CP1" s="60"/>
-      <c r="CQ1" s="60"/>
-      <c r="CR1" s="61"/>
-      <c r="CS1" s="62" t="s">
+      <c r="BY1" s="50"/>
+      <c r="BZ1" s="50"/>
+      <c r="CA1" s="50"/>
+      <c r="CB1" s="50"/>
+      <c r="CC1" s="50"/>
+      <c r="CD1" s="50"/>
+      <c r="CE1" s="50"/>
+      <c r="CF1" s="50"/>
+      <c r="CG1" s="50"/>
+      <c r="CH1" s="50"/>
+      <c r="CI1" s="50"/>
+      <c r="CJ1" s="50"/>
+      <c r="CK1" s="50"/>
+      <c r="CL1" s="50"/>
+      <c r="CM1" s="50"/>
+      <c r="CN1" s="50"/>
+      <c r="CO1" s="50"/>
+      <c r="CP1" s="50"/>
+      <c r="CQ1" s="50"/>
+      <c r="CR1" s="51"/>
+      <c r="CS1" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="CT1" s="63"/>
-      <c r="CU1" s="63"/>
-      <c r="CV1" s="63"/>
-      <c r="CW1" s="63"/>
-      <c r="CX1" s="63"/>
-      <c r="CY1" s="63"/>
-      <c r="CZ1" s="63"/>
-      <c r="DA1" s="63"/>
-      <c r="DB1" s="63"/>
-      <c r="DC1" s="63"/>
-      <c r="DD1" s="63"/>
-      <c r="DE1" s="63"/>
-      <c r="DF1" s="63"/>
-      <c r="DG1" s="63"/>
-      <c r="DH1" s="63"/>
-      <c r="DI1" s="63"/>
-      <c r="DJ1" s="63"/>
-      <c r="DK1" s="63"/>
-      <c r="DL1" s="63"/>
-      <c r="DM1" s="64"/>
-      <c r="DN1" s="65" t="s">
+      <c r="CT1" s="56"/>
+      <c r="CU1" s="56"/>
+      <c r="CV1" s="56"/>
+      <c r="CW1" s="56"/>
+      <c r="CX1" s="56"/>
+      <c r="CY1" s="56"/>
+      <c r="CZ1" s="56"/>
+      <c r="DA1" s="56"/>
+      <c r="DB1" s="56"/>
+      <c r="DC1" s="56"/>
+      <c r="DD1" s="56"/>
+      <c r="DE1" s="56"/>
+      <c r="DF1" s="56"/>
+      <c r="DG1" s="56"/>
+      <c r="DH1" s="56"/>
+      <c r="DI1" s="56"/>
+      <c r="DJ1" s="56"/>
+      <c r="DK1" s="56"/>
+      <c r="DL1" s="56"/>
+      <c r="DM1" s="57"/>
+      <c r="DN1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="DO1" s="66"/>
-      <c r="DP1" s="66"/>
-      <c r="DQ1" s="66"/>
-      <c r="DR1" s="66"/>
-      <c r="DS1" s="66"/>
-      <c r="DT1" s="66"/>
-      <c r="DU1" s="66"/>
-      <c r="DV1" s="66"/>
-      <c r="DW1" s="66"/>
-      <c r="DX1" s="66"/>
-      <c r="DY1" s="66"/>
-      <c r="DZ1" s="66"/>
-      <c r="EA1" s="67"/>
+      <c r="DO1" s="38"/>
+      <c r="DP1" s="38"/>
+      <c r="DQ1" s="38"/>
+      <c r="DR1" s="38"/>
+      <c r="DS1" s="38"/>
+      <c r="DT1" s="38"/>
+      <c r="DU1" s="38"/>
+      <c r="DV1" s="38"/>
+      <c r="DW1" s="38"/>
+      <c r="DX1" s="38"/>
+      <c r="DY1" s="38"/>
+      <c r="DZ1" s="38"/>
+      <c r="EA1" s="39"/>
     </row>
     <row r="2" spans="1:131" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2251,169 +2254,169 @@
         <v>143</v>
       </c>
       <c r="F3" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>144</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>146</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
       <c r="L3" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="M3" s="11"/>
       <c r="N3" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="P3" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="Q3" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="P3" s="31" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q3" s="11" t="s">
-        <v>151</v>
       </c>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
       <c r="V3" s="23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="W3" s="23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="X3" s="11"/>
       <c r="Y3" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Z3" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="AA3" s="11"/>
       <c r="AB3" s="11"/>
       <c r="AC3" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD3" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="AE3" s="63" t="s">
+        <v>155</v>
+      </c>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="AD3" s="11" t="s">
-        <v>279</v>
-      </c>
-      <c r="AE3" s="53" t="s">
+      <c r="AI3" s="64"/>
+      <c r="AJ3" s="64"/>
+      <c r="AK3" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="AF3" s="54"/>
-      <c r="AG3" s="54"/>
-      <c r="AH3" s="53" t="s">
+      <c r="AL3" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="AI3" s="54"/>
-      <c r="AJ3" s="54"/>
-      <c r="AK3" s="11" t="s">
+      <c r="AM3" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="AL3" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="AM3" s="11" t="s">
-        <v>161</v>
       </c>
       <c r="AN3" s="11"/>
       <c r="AO3" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP3" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="AQ3" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AP3" s="11" t="s">
+      <c r="AR3" s="27" t="s">
         <v>163</v>
       </c>
-      <c r="AQ3" s="11" t="s">
+      <c r="AS3" s="28"/>
+      <c r="AT3" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="AR3" s="28" t="s">
+      <c r="AU3" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="AV3" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="AS3" s="29"/>
-      <c r="AT3" s="28" t="s">
+      <c r="AW3" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="AU3" s="28" t="s">
-        <v>164</v>
-      </c>
-      <c r="AV3" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="AW3" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="AX3" s="28" t="s">
-        <v>165</v>
+      <c r="AX3" s="27" t="s">
+        <v>163</v>
       </c>
       <c r="AY3" s="11"/>
       <c r="AZ3" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BA3" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="BB3" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="BB3" s="27" t="s">
+        <v>163</v>
       </c>
       <c r="BC3" s="11"/>
       <c r="BD3" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BE3" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="BF3" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="BF3" s="27" t="s">
+        <v>163</v>
       </c>
       <c r="BG3" s="11"/>
       <c r="BH3" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BI3" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="BJ3" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="BJ3" s="27" t="s">
+        <v>163</v>
       </c>
       <c r="BK3" s="11"/>
       <c r="BL3" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BM3" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="BN3" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="BN3" s="27" t="s">
+        <v>163</v>
       </c>
       <c r="BO3" s="11"/>
       <c r="BP3" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BQ3" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="BR3" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="BR3" s="27" t="s">
+        <v>163</v>
       </c>
       <c r="BS3" s="11"/>
       <c r="BT3" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BU3" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="BV3" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="BV3" s="27" t="s">
+        <v>163</v>
       </c>
       <c r="BW3" s="11"/>
       <c r="BX3" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="BY3" s="11"/>
       <c r="BZ3" s="11"/>
@@ -2426,49 +2429,49 @@
       <c r="CG3" s="11"/>
       <c r="CH3" s="11"/>
       <c r="CI3" s="11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="CJ3" s="11"/>
       <c r="CK3" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="CL3" s="11"/>
       <c r="CM3" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="CN3" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="CO3" s="11" t="s">
         <v>172</v>
-      </c>
-      <c r="CN3" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="CO3" s="11" t="s">
-        <v>174</v>
       </c>
       <c r="CP3" s="11"/>
       <c r="CQ3" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="CR3" s="11"/>
       <c r="CS3" s="11"/>
       <c r="CT3" s="11"/>
       <c r="CU3" s="11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="CV3" s="11"/>
       <c r="CW3" s="11"/>
       <c r="CX3" s="11"/>
       <c r="CY3" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="CZ3" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="DA3" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="CZ3" s="25" t="s">
+      <c r="DB3" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="DC3" s="11" t="s">
         <v>178</v>
-      </c>
-      <c r="DA3" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="DB3" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="DC3" s="11" t="s">
-        <v>180</v>
       </c>
       <c r="DD3" s="11"/>
       <c r="DE3" s="11"/>
@@ -2476,950 +2479,950 @@
       <c r="DG3" s="11"/>
       <c r="DH3" s="11"/>
       <c r="DI3" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="DJ3" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="DK3" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="DJ3" s="11" t="s">
+      <c r="DL3" s="14" t="s">
         <v>182</v>
-      </c>
-      <c r="DK3" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="DL3" s="14" t="s">
-        <v>184</v>
       </c>
       <c r="DM3" s="11"/>
       <c r="DN3" s="11"/>
       <c r="DO3" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="DP3" s="11"/>
       <c r="DQ3" s="11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="DR3" s="11"/>
       <c r="DS3" s="11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="DT3" s="11"/>
       <c r="DU3" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="DV3" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="DW3" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="DV3" s="23" t="s">
+      <c r="DX3" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="DW3" s="23" t="s">
+      <c r="DY3" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="DX3" s="23" t="s">
+      <c r="DZ3" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="DY3" s="23" t="s">
+      <c r="EA3" s="11" t="s">
         <v>192</v>
-      </c>
-      <c r="DZ3" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="EA3" s="11" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:131" ht="115" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B4" s="69" t="s">
+        <v>194</v>
+      </c>
+      <c r="C4" s="70"/>
+      <c r="D4" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="E4" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="15" t="s">
+      <c r="F4" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="I4" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="J4" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="K4" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="P4" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="R4" s="65" t="s">
+        <v>194</v>
+      </c>
+      <c r="S4" s="67"/>
+      <c r="T4" s="65" t="s">
+        <v>201</v>
+      </c>
+      <c r="U4" s="67"/>
+      <c r="V4" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="W4" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="X4" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="Y4" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="Z4" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="AA4" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="AB4" s="65" t="s">
         <v>196</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="AC4" s="67"/>
+      <c r="AD4" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="AE4" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF4" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="AG4" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="AH4" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="AI4" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="AJ4" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="AK4" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="AL4" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="H4" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="J4" s="15" t="s">
+      <c r="AM4" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="AN4" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="AO4" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="AP4" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="AQ4" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="AR4" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="AS4" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="AT4" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="AU4" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="AV4" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="AW4" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="AX4" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="AY4" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="AZ4" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="BA4" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="BB4" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="BC4" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="BD4" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="BE4" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="BF4" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="BG4" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="BH4" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="BI4" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="BJ4" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="BK4" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="BL4" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="BM4" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="BN4" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="BO4" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="BP4" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="BQ4" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="BR4" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="BS4" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="BT4" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="BU4" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="BV4" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="BW4" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="BX4" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="BY4" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="BZ4" s="46" t="s">
+        <v>214</v>
+      </c>
+      <c r="CA4" s="48"/>
+      <c r="CB4" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="CC4" s="47"/>
+      <c r="CD4" s="47"/>
+      <c r="CE4" s="47"/>
+      <c r="CF4" s="47"/>
+      <c r="CG4" s="48"/>
+      <c r="CH4" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="CI4" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="CJ4" s="47"/>
+      <c r="CK4" s="47"/>
+      <c r="CL4" s="47"/>
+      <c r="CM4" s="47"/>
+      <c r="CN4" s="47"/>
+      <c r="CO4" s="47"/>
+      <c r="CP4" s="47"/>
+      <c r="CQ4" s="47"/>
+      <c r="CR4" s="48"/>
+      <c r="CS4" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="CT4" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="CU4" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="CV4" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="L4" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="N4" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="O4" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="P4" s="32">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="R4" s="46" t="s">
+      <c r="CW4" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="CX4" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="CY4" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="S4" s="49"/>
-      <c r="T4" s="46" t="s">
-        <v>203</v>
-      </c>
-      <c r="U4" s="49"/>
-      <c r="V4" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="W4" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="X4" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="Y4" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="Z4" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="AA4" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="AB4" s="46" t="s">
-        <v>198</v>
-      </c>
-      <c r="AC4" s="49"/>
-      <c r="AD4" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="AE4" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="AF4" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="AG4" s="17" t="s">
+      <c r="CZ4" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="DA4" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="DB4" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="DC4" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="AH4" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="AI4" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="AJ4" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="AK4" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="AL4" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="AM4" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="AN4" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="AO4" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="AP4" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="AQ4" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="AR4" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="AS4" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="AT4" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="AU4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="AV4" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="AW4" s="15" t="s">
+      <c r="DD4" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="AX4" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="AY4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="AZ4" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="BA4" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="BB4" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="BC4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="BD4" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="BE4" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="BF4" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="BG4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="BH4" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="BI4" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="BJ4" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="BK4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="BL4" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="BM4" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="BN4" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="BO4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="BP4" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="BQ4" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="BR4" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="BS4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="BT4" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="BU4" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="BV4" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="BW4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="BX4" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="BY4" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="BZ4" s="38" t="s">
-        <v>216</v>
-      </c>
-      <c r="CA4" s="40"/>
-      <c r="CB4" s="38" t="s">
-        <v>227</v>
-      </c>
-      <c r="CC4" s="39"/>
-      <c r="CD4" s="39"/>
-      <c r="CE4" s="39"/>
-      <c r="CF4" s="39"/>
-      <c r="CG4" s="40"/>
-      <c r="CH4" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="CI4" s="38" t="s">
-        <v>227</v>
-      </c>
-      <c r="CJ4" s="39"/>
-      <c r="CK4" s="39"/>
-      <c r="CL4" s="39"/>
-      <c r="CM4" s="39"/>
-      <c r="CN4" s="39"/>
-      <c r="CO4" s="39"/>
-      <c r="CP4" s="39"/>
-      <c r="CQ4" s="39"/>
-      <c r="CR4" s="40"/>
-      <c r="CS4" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="CT4" s="17" t="s">
-        <v>229</v>
-      </c>
-      <c r="CU4" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="CV4" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="CW4" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="CX4" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="CY4" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="CZ4" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="DA4" s="15" t="s">
+      <c r="DE4" s="47"/>
+      <c r="DF4" s="47"/>
+      <c r="DG4" s="47"/>
+      <c r="DH4" s="48"/>
+      <c r="DI4" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="DJ4" s="47"/>
+      <c r="DK4" s="47"/>
+      <c r="DL4" s="48"/>
+      <c r="DM4" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="DB4" s="27" t="s">
+      <c r="DN4" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="DO4" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="DC4" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="DD4" s="38" t="s">
-        <v>227</v>
-      </c>
-      <c r="DE4" s="39"/>
-      <c r="DF4" s="39"/>
-      <c r="DG4" s="39"/>
-      <c r="DH4" s="40"/>
-      <c r="DI4" s="38" t="s">
-        <v>198</v>
-      </c>
-      <c r="DJ4" s="39"/>
-      <c r="DK4" s="39"/>
-      <c r="DL4" s="40"/>
-      <c r="DM4" s="17" t="s">
+      <c r="DP4" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="DQ4" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="DN4" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="DO4" s="15" t="s">
+      <c r="DR4" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="DP4" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="DQ4" s="15" t="s">
+      <c r="DS4" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="DR4" s="15" t="s">
+      <c r="DT4" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="DS4" s="15" t="s">
+      <c r="DU4" s="46" t="s">
         <v>240</v>
       </c>
-      <c r="DT4" s="15" t="s">
+      <c r="DV4" s="47"/>
+      <c r="DW4" s="47"/>
+      <c r="DX4" s="47"/>
+      <c r="DY4" s="48"/>
+      <c r="DZ4" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="EA4" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:131" s="34" customFormat="1" ht="137.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="DU4" s="30" t="s">
+      <c r="B5" s="65" t="s">
         <v>242</v>
       </c>
-      <c r="DV4" s="24"/>
-      <c r="DW4" s="24"/>
-      <c r="DX4" s="24"/>
-      <c r="DY4" s="24"/>
-      <c r="DZ4" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="EA4" s="15" t="s">
+      <c r="C5" s="68"/>
+      <c r="D5" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>242</v>
       </c>
+      <c r="F5" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="H5" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="N5" s="65" t="s">
+        <v>243</v>
+      </c>
+      <c r="O5" s="68"/>
+      <c r="P5" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q5" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="R5" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="S5" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="T5" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="U5" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="V5" s="65" t="s">
+        <v>247</v>
+      </c>
+      <c r="W5" s="68"/>
+      <c r="X5" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="Y5" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z5" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="AA5" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AB5" s="68"/>
+      <c r="AC5" s="68"/>
+      <c r="AD5" s="68"/>
+      <c r="AE5" s="65" t="s">
+        <v>249</v>
+      </c>
+      <c r="AF5" s="68"/>
+      <c r="AG5" s="68"/>
+      <c r="AH5" s="65" t="s">
+        <v>243</v>
+      </c>
+      <c r="AI5" s="68"/>
+      <c r="AJ5" s="68"/>
+      <c r="AK5" s="65" t="s">
+        <v>242</v>
+      </c>
+      <c r="AL5" s="68"/>
+      <c r="AM5" s="68"/>
+      <c r="AN5" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="AO5" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AP5" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="AQ5" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="AR5" s="47"/>
+      <c r="AS5" s="47"/>
+      <c r="AT5" s="47"/>
+      <c r="AU5" s="48"/>
+      <c r="AV5" s="40" t="s">
+        <v>253</v>
+      </c>
+      <c r="AW5" s="41"/>
+      <c r="AX5" s="41"/>
+      <c r="AY5" s="42"/>
+      <c r="AZ5" s="40" t="s">
+        <v>278</v>
+      </c>
+      <c r="BA5" s="41"/>
+      <c r="BB5" s="41"/>
+      <c r="BC5" s="42"/>
+      <c r="BD5" s="40" t="s">
+        <v>254</v>
+      </c>
+      <c r="BE5" s="41"/>
+      <c r="BF5" s="41"/>
+      <c r="BG5" s="42"/>
+      <c r="BH5" s="40" t="s">
+        <v>255</v>
+      </c>
+      <c r="BI5" s="41"/>
+      <c r="BJ5" s="41"/>
+      <c r="BK5" s="42"/>
+      <c r="BL5" s="40" t="s">
+        <v>256</v>
+      </c>
+      <c r="BM5" s="41"/>
+      <c r="BN5" s="41"/>
+      <c r="BO5" s="42"/>
+      <c r="BP5" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="BQ5" s="41"/>
+      <c r="BR5" s="41"/>
+      <c r="BS5" s="42"/>
+      <c r="BT5" s="40" t="s">
+        <v>258</v>
+      </c>
+      <c r="BU5" s="41"/>
+      <c r="BV5" s="41"/>
+      <c r="BW5" s="42"/>
+      <c r="BX5" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="BY5" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="BZ5" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="CA5" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="CB5" s="46" t="s">
+        <v>261</v>
+      </c>
+      <c r="CC5" s="47"/>
+      <c r="CD5" s="47"/>
+      <c r="CE5" s="48"/>
+      <c r="CF5" s="46" t="s">
+        <v>262</v>
+      </c>
+      <c r="CG5" s="48"/>
+      <c r="CH5" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="CI5" s="46" t="s">
+        <v>263</v>
+      </c>
+      <c r="CJ5" s="47"/>
+      <c r="CK5" s="47"/>
+      <c r="CL5" s="47"/>
+      <c r="CM5" s="47"/>
+      <c r="CN5" s="47"/>
+      <c r="CO5" s="47"/>
+      <c r="CP5" s="47"/>
+      <c r="CQ5" s="47"/>
+      <c r="CR5" s="48"/>
+      <c r="CS5" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="CT5" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="CU5" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="CV5" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="CW5" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="CX5" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="CY5" s="48"/>
+      <c r="CZ5" s="46" t="s">
+        <v>265</v>
+      </c>
+      <c r="DA5" s="48"/>
+      <c r="DB5" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="DC5" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="DD5" s="52" t="s">
+        <v>266</v>
+      </c>
+      <c r="DE5" s="53"/>
+      <c r="DF5" s="53"/>
+      <c r="DG5" s="53"/>
+      <c r="DH5" s="54"/>
+      <c r="DI5" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="DJ5" s="47"/>
+      <c r="DK5" s="47"/>
+      <c r="DL5" s="48"/>
+      <c r="DM5" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="DN5" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="DO5" s="46" t="s">
+        <v>267</v>
+      </c>
+      <c r="DP5" s="48"/>
+      <c r="DQ5" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="DR5" s="48"/>
+      <c r="DS5" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="DT5" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="DU5" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="DV5" s="46" t="s">
+        <v>269</v>
+      </c>
+      <c r="DW5" s="47"/>
+      <c r="DX5" s="47"/>
+      <c r="DY5" s="48"/>
+      <c r="DZ5" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="EA5" s="15" t="s">
+        <v>271</v>
+      </c>
     </row>
-    <row r="5" spans="1:131" s="36" customFormat="1" ht="137.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="B5" s="46" t="s">
-        <v>244</v>
-      </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="15" t="s">
-        <v>245</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="H5" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="33" t="s">
-        <v>247</v>
-      </c>
-      <c r="N5" s="46" t="s">
-        <v>245</v>
-      </c>
-      <c r="O5" s="45"/>
-      <c r="P5" s="32" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q5" s="34" t="s">
-        <v>248</v>
-      </c>
-      <c r="R5" s="35" t="s">
-        <v>249</v>
-      </c>
-      <c r="S5" s="34" t="s">
-        <v>245</v>
-      </c>
-      <c r="T5" s="35" t="s">
-        <v>249</v>
-      </c>
-      <c r="U5" s="34" t="s">
-        <v>245</v>
-      </c>
-      <c r="V5" s="46" t="s">
-        <v>249</v>
-      </c>
-      <c r="W5" s="45"/>
-      <c r="X5" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="Y5" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="Z5" s="15" t="s">
-        <v>252</v>
-      </c>
-      <c r="AA5" s="46" t="s">
-        <v>250</v>
-      </c>
-      <c r="AB5" s="45"/>
-      <c r="AC5" s="45"/>
-      <c r="AD5" s="45"/>
-      <c r="AE5" s="46" t="s">
-        <v>251</v>
-      </c>
-      <c r="AF5" s="45"/>
-      <c r="AG5" s="45"/>
-      <c r="AH5" s="46" t="s">
-        <v>245</v>
-      </c>
-      <c r="AI5" s="45"/>
-      <c r="AJ5" s="45"/>
-      <c r="AK5" s="46" t="s">
-        <v>244</v>
-      </c>
-      <c r="AL5" s="45"/>
-      <c r="AM5" s="45"/>
-      <c r="AN5" s="15" t="s">
-        <v>253</v>
-      </c>
-      <c r="AO5" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="AP5" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="AQ5" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="AR5" s="39"/>
-      <c r="AS5" s="39"/>
-      <c r="AT5" s="39"/>
-      <c r="AU5" s="40"/>
-      <c r="AV5" s="50" t="s">
-        <v>255</v>
-      </c>
-      <c r="AW5" s="51"/>
-      <c r="AX5" s="51"/>
-      <c r="AY5" s="52"/>
-      <c r="AZ5" s="50" t="s">
-        <v>280</v>
-      </c>
-      <c r="BA5" s="51"/>
-      <c r="BB5" s="51"/>
-      <c r="BC5" s="52"/>
-      <c r="BD5" s="50" t="s">
-        <v>256</v>
-      </c>
-      <c r="BE5" s="51"/>
-      <c r="BF5" s="51"/>
-      <c r="BG5" s="52"/>
-      <c r="BH5" s="50" t="s">
-        <v>257</v>
-      </c>
-      <c r="BI5" s="51"/>
-      <c r="BJ5" s="51"/>
-      <c r="BK5" s="52"/>
-      <c r="BL5" s="50" t="s">
-        <v>258</v>
-      </c>
-      <c r="BM5" s="51"/>
-      <c r="BN5" s="51"/>
-      <c r="BO5" s="52"/>
-      <c r="BP5" s="50" t="s">
-        <v>259</v>
-      </c>
-      <c r="BQ5" s="51"/>
-      <c r="BR5" s="51"/>
-      <c r="BS5" s="52"/>
-      <c r="BT5" s="50" t="s">
-        <v>260</v>
-      </c>
-      <c r="BU5" s="51"/>
-      <c r="BV5" s="51"/>
-      <c r="BW5" s="52"/>
-      <c r="BX5" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="BY5" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="BZ5" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="CA5" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="CB5" s="38" t="s">
-        <v>263</v>
-      </c>
-      <c r="CC5" s="39"/>
-      <c r="CD5" s="39"/>
-      <c r="CE5" s="40"/>
-      <c r="CF5" s="38" t="s">
-        <v>264</v>
-      </c>
-      <c r="CG5" s="40"/>
-      <c r="CH5" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="CI5" s="38" t="s">
-        <v>265</v>
-      </c>
-      <c r="CJ5" s="39"/>
-      <c r="CK5" s="39"/>
-      <c r="CL5" s="39"/>
-      <c r="CM5" s="39"/>
-      <c r="CN5" s="39"/>
-      <c r="CO5" s="39"/>
-      <c r="CP5" s="39"/>
-      <c r="CQ5" s="39"/>
-      <c r="CR5" s="40"/>
-      <c r="CS5" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="CT5" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="CU5" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="CV5" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="CW5" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="CX5" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="CY5" s="40"/>
-      <c r="CZ5" s="38" t="s">
-        <v>267</v>
-      </c>
-      <c r="DA5" s="40"/>
-      <c r="DB5" s="15" t="s">
-        <v>245</v>
-      </c>
-      <c r="DC5" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="DD5" s="41" t="s">
-        <v>268</v>
-      </c>
-      <c r="DE5" s="42"/>
-      <c r="DF5" s="42"/>
-      <c r="DG5" s="42"/>
-      <c r="DH5" s="43"/>
-      <c r="DI5" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="DJ5" s="39"/>
-      <c r="DK5" s="39"/>
-      <c r="DL5" s="40"/>
-      <c r="DM5" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="DN5" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="DO5" s="38" t="s">
-        <v>269</v>
-      </c>
-      <c r="DP5" s="40"/>
-      <c r="DQ5" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="DR5" s="40"/>
-      <c r="DS5" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="DT5" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="DU5" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="DV5" s="38" t="s">
-        <v>271</v>
-      </c>
-      <c r="DW5" s="39"/>
-      <c r="DX5" s="39"/>
-      <c r="DY5" s="40"/>
-      <c r="DZ5" s="15" t="s">
+    <row r="6" spans="1:131" s="35" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="EA5" s="15" t="s">
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="61" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="6" spans="1:131" s="37" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="G6" s="61"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="44" t="s">
+      <c r="N6" s="65"/>
+      <c r="O6" s="65"/>
+      <c r="P6" s="65"/>
+      <c r="Q6" s="65" t="s">
         <v>275</v>
       </c>
-      <c r="G6" s="44"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="15" t="s">
-        <v>276</v>
-      </c>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46" t="s">
-        <v>277</v>
-      </c>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
-      <c r="U6" s="45"/>
-      <c r="V6" s="45"/>
-      <c r="W6" s="45"/>
-      <c r="X6" s="45"/>
-      <c r="Y6" s="46"/>
-      <c r="Z6" s="46"/>
-      <c r="AA6" s="46" t="s">
-        <v>277</v>
-      </c>
-      <c r="AB6" s="45"/>
-      <c r="AC6" s="45"/>
-      <c r="AD6" s="45"/>
-      <c r="AE6" s="46"/>
-      <c r="AF6" s="46"/>
-      <c r="AG6" s="46"/>
-      <c r="AH6" s="46"/>
-      <c r="AI6" s="46"/>
-      <c r="AJ6" s="46"/>
-      <c r="AK6" s="46"/>
-      <c r="AL6" s="46"/>
-      <c r="AM6" s="46"/>
-      <c r="AN6" s="46"/>
-      <c r="AO6" s="46"/>
+      <c r="R6" s="68"/>
+      <c r="S6" s="68"/>
+      <c r="T6" s="68"/>
+      <c r="U6" s="68"/>
+      <c r="V6" s="68"/>
+      <c r="W6" s="68"/>
+      <c r="X6" s="68"/>
+      <c r="Y6" s="65"/>
+      <c r="Z6" s="65"/>
+      <c r="AA6" s="65" t="s">
+        <v>275</v>
+      </c>
+      <c r="AB6" s="68"/>
+      <c r="AC6" s="68"/>
+      <c r="AD6" s="68"/>
+      <c r="AE6" s="65"/>
+      <c r="AF6" s="65"/>
+      <c r="AG6" s="65"/>
+      <c r="AH6" s="65"/>
+      <c r="AI6" s="65"/>
+      <c r="AJ6" s="65"/>
+      <c r="AK6" s="65"/>
+      <c r="AL6" s="65"/>
+      <c r="AM6" s="65"/>
+      <c r="AN6" s="65"/>
+      <c r="AO6" s="65"/>
       <c r="AP6" s="15" t="s">
-        <v>275</v>
-      </c>
-      <c r="AQ6" s="38"/>
-      <c r="AR6" s="39"/>
-      <c r="AS6" s="39"/>
-      <c r="AT6" s="39"/>
-      <c r="AU6" s="39"/>
-      <c r="AV6" s="39"/>
-      <c r="AW6" s="39"/>
-      <c r="AX6" s="39"/>
-      <c r="AY6" s="39"/>
-      <c r="AZ6" s="39"/>
-      <c r="BA6" s="39"/>
-      <c r="BB6" s="39"/>
-      <c r="BC6" s="39"/>
-      <c r="BD6" s="39"/>
-      <c r="BE6" s="39"/>
-      <c r="BF6" s="39"/>
-      <c r="BG6" s="39"/>
-      <c r="BH6" s="39"/>
-      <c r="BI6" s="39"/>
-      <c r="BJ6" s="39"/>
-      <c r="BK6" s="39"/>
-      <c r="BL6" s="39"/>
-      <c r="BM6" s="39"/>
-      <c r="BN6" s="39"/>
-      <c r="BO6" s="39"/>
-      <c r="BP6" s="39"/>
-      <c r="BQ6" s="39"/>
-      <c r="BR6" s="39"/>
-      <c r="BS6" s="39"/>
-      <c r="BT6" s="39"/>
-      <c r="BU6" s="39"/>
-      <c r="BV6" s="39"/>
-      <c r="BW6" s="40"/>
-      <c r="BX6" s="38"/>
-      <c r="BY6" s="39"/>
-      <c r="BZ6" s="39"/>
-      <c r="CA6" s="39"/>
-      <c r="CB6" s="39"/>
-      <c r="CC6" s="39"/>
-      <c r="CD6" s="39"/>
-      <c r="CE6" s="39"/>
-      <c r="CF6" s="39"/>
-      <c r="CG6" s="39"/>
-      <c r="CH6" s="39"/>
-      <c r="CI6" s="39"/>
-      <c r="CJ6" s="39"/>
-      <c r="CK6" s="39"/>
-      <c r="CL6" s="39"/>
-      <c r="CM6" s="39"/>
-      <c r="CN6" s="39"/>
-      <c r="CO6" s="39"/>
-      <c r="CP6" s="39"/>
-      <c r="CQ6" s="39"/>
-      <c r="CR6" s="40"/>
-      <c r="CS6" s="38"/>
-      <c r="CT6" s="39"/>
-      <c r="CU6" s="39"/>
-      <c r="CV6" s="39"/>
-      <c r="CW6" s="39"/>
-      <c r="CX6" s="39"/>
-      <c r="CY6" s="39"/>
-      <c r="CZ6" s="39"/>
-      <c r="DA6" s="39"/>
-      <c r="DB6" s="39"/>
-      <c r="DC6" s="39"/>
-      <c r="DD6" s="39"/>
-      <c r="DE6" s="39"/>
-      <c r="DF6" s="39"/>
-      <c r="DG6" s="39"/>
-      <c r="DH6" s="39"/>
-      <c r="DI6" s="39"/>
-      <c r="DJ6" s="39"/>
-      <c r="DK6" s="39"/>
-      <c r="DL6" s="39"/>
-      <c r="DM6" s="40"/>
-      <c r="DN6" s="38"/>
-      <c r="DO6" s="39"/>
-      <c r="DP6" s="39"/>
-      <c r="DQ6" s="39"/>
-      <c r="DR6" s="40"/>
+        <v>273</v>
+      </c>
+      <c r="AQ6" s="46"/>
+      <c r="AR6" s="47"/>
+      <c r="AS6" s="47"/>
+      <c r="AT6" s="47"/>
+      <c r="AU6" s="47"/>
+      <c r="AV6" s="47"/>
+      <c r="AW6" s="47"/>
+      <c r="AX6" s="47"/>
+      <c r="AY6" s="47"/>
+      <c r="AZ6" s="47"/>
+      <c r="BA6" s="47"/>
+      <c r="BB6" s="47"/>
+      <c r="BC6" s="47"/>
+      <c r="BD6" s="47"/>
+      <c r="BE6" s="47"/>
+      <c r="BF6" s="47"/>
+      <c r="BG6" s="47"/>
+      <c r="BH6" s="47"/>
+      <c r="BI6" s="47"/>
+      <c r="BJ6" s="47"/>
+      <c r="BK6" s="47"/>
+      <c r="BL6" s="47"/>
+      <c r="BM6" s="47"/>
+      <c r="BN6" s="47"/>
+      <c r="BO6" s="47"/>
+      <c r="BP6" s="47"/>
+      <c r="BQ6" s="47"/>
+      <c r="BR6" s="47"/>
+      <c r="BS6" s="47"/>
+      <c r="BT6" s="47"/>
+      <c r="BU6" s="47"/>
+      <c r="BV6" s="47"/>
+      <c r="BW6" s="48"/>
+      <c r="BX6" s="46"/>
+      <c r="BY6" s="47"/>
+      <c r="BZ6" s="47"/>
+      <c r="CA6" s="47"/>
+      <c r="CB6" s="47"/>
+      <c r="CC6" s="47"/>
+      <c r="CD6" s="47"/>
+      <c r="CE6" s="47"/>
+      <c r="CF6" s="47"/>
+      <c r="CG6" s="47"/>
+      <c r="CH6" s="47"/>
+      <c r="CI6" s="47"/>
+      <c r="CJ6" s="47"/>
+      <c r="CK6" s="47"/>
+      <c r="CL6" s="47"/>
+      <c r="CM6" s="47"/>
+      <c r="CN6" s="47"/>
+      <c r="CO6" s="47"/>
+      <c r="CP6" s="47"/>
+      <c r="CQ6" s="47"/>
+      <c r="CR6" s="48"/>
+      <c r="CS6" s="46"/>
+      <c r="CT6" s="47"/>
+      <c r="CU6" s="47"/>
+      <c r="CV6" s="47"/>
+      <c r="CW6" s="47"/>
+      <c r="CX6" s="47"/>
+      <c r="CY6" s="47"/>
+      <c r="CZ6" s="47"/>
+      <c r="DA6" s="47"/>
+      <c r="DB6" s="47"/>
+      <c r="DC6" s="47"/>
+      <c r="DD6" s="47"/>
+      <c r="DE6" s="47"/>
+      <c r="DF6" s="47"/>
+      <c r="DG6" s="47"/>
+      <c r="DH6" s="47"/>
+      <c r="DI6" s="47"/>
+      <c r="DJ6" s="47"/>
+      <c r="DK6" s="47"/>
+      <c r="DL6" s="47"/>
+      <c r="DM6" s="48"/>
+      <c r="DN6" s="46"/>
+      <c r="DO6" s="47"/>
+      <c r="DP6" s="47"/>
+      <c r="DQ6" s="47"/>
+      <c r="DR6" s="48"/>
       <c r="DS6" s="20" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="DT6" s="20"/>
       <c r="DU6" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="DV6" s="41"/>
-      <c r="DW6" s="42"/>
-      <c r="DX6" s="42"/>
-      <c r="DY6" s="42"/>
-      <c r="DZ6" s="42"/>
-      <c r="EA6" s="43"/>
+        <v>273</v>
+      </c>
+      <c r="DV6" s="52"/>
+      <c r="DW6" s="53"/>
+      <c r="DX6" s="53"/>
+      <c r="DY6" s="53"/>
+      <c r="DZ6" s="53"/>
+      <c r="EA6" s="54"/>
     </row>
-    <row r="7" spans="1:131" s="37" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:131" s="35" customFormat="1" ht="23" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44" t="s">
-        <v>245</v>
-      </c>
-      <c r="G7" s="44"/>
+        <v>243</v>
+      </c>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61" t="s">
+        <v>243</v>
+      </c>
+      <c r="G7" s="61"/>
       <c r="H7" s="21"/>
-      <c r="I7" s="44" t="s">
-        <v>245</v>
-      </c>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
+      <c r="I7" s="61" t="s">
+        <v>243</v>
+      </c>
+      <c r="J7" s="68"/>
+      <c r="K7" s="68"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
       <c r="N7" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="O7" s="41"/>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="42"/>
-      <c r="S7" s="42"/>
-      <c r="T7" s="42"/>
-      <c r="U7" s="43"/>
-      <c r="V7" s="44" t="s">
-        <v>245</v>
-      </c>
-      <c r="W7" s="44"/>
-      <c r="X7" s="41"/>
-      <c r="Y7" s="42"/>
-      <c r="Z7" s="42"/>
-      <c r="AA7" s="42"/>
-      <c r="AB7" s="42"/>
-      <c r="AC7" s="42"/>
-      <c r="AD7" s="42"/>
-      <c r="AE7" s="42"/>
-      <c r="AF7" s="42"/>
-      <c r="AG7" s="42"/>
-      <c r="AH7" s="42"/>
-      <c r="AI7" s="42"/>
-      <c r="AJ7" s="43"/>
-      <c r="AK7" s="41"/>
-      <c r="AL7" s="42"/>
-      <c r="AM7" s="42"/>
-      <c r="AN7" s="42"/>
-      <c r="AO7" s="42"/>
-      <c r="AP7" s="43"/>
-      <c r="AQ7" s="41" t="s">
-        <v>245</v>
-      </c>
-      <c r="AR7" s="43"/>
-      <c r="AS7" s="41"/>
-      <c r="AT7" s="43"/>
+        <v>243</v>
+      </c>
+      <c r="O7" s="52"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="53"/>
+      <c r="S7" s="53"/>
+      <c r="T7" s="53"/>
+      <c r="U7" s="54"/>
+      <c r="V7" s="61" t="s">
+        <v>243</v>
+      </c>
+      <c r="W7" s="61"/>
+      <c r="X7" s="52"/>
+      <c r="Y7" s="53"/>
+      <c r="Z7" s="53"/>
+      <c r="AA7" s="53"/>
+      <c r="AB7" s="53"/>
+      <c r="AC7" s="53"/>
+      <c r="AD7" s="53"/>
+      <c r="AE7" s="53"/>
+      <c r="AF7" s="53"/>
+      <c r="AG7" s="53"/>
+      <c r="AH7" s="53"/>
+      <c r="AI7" s="53"/>
+      <c r="AJ7" s="54"/>
+      <c r="AK7" s="52"/>
+      <c r="AL7" s="53"/>
+      <c r="AM7" s="53"/>
+      <c r="AN7" s="53"/>
+      <c r="AO7" s="53"/>
+      <c r="AP7" s="54"/>
+      <c r="AQ7" s="52" t="s">
+        <v>243</v>
+      </c>
+      <c r="AR7" s="54"/>
+      <c r="AS7" s="52"/>
+      <c r="AT7" s="54"/>
       <c r="AU7" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="AV7" s="41"/>
-      <c r="AW7" s="42"/>
-      <c r="AX7" s="42"/>
-      <c r="AY7" s="42"/>
-      <c r="AZ7" s="42"/>
-      <c r="BA7" s="42"/>
-      <c r="BB7" s="42"/>
-      <c r="BC7" s="42"/>
-      <c r="BD7" s="42"/>
-      <c r="BE7" s="42"/>
-      <c r="BF7" s="42"/>
-      <c r="BG7" s="42"/>
-      <c r="BH7" s="42"/>
-      <c r="BI7" s="42"/>
-      <c r="BJ7" s="42"/>
-      <c r="BK7" s="42"/>
-      <c r="BL7" s="42"/>
-      <c r="BM7" s="42"/>
-      <c r="BN7" s="42"/>
-      <c r="BO7" s="42"/>
-      <c r="BP7" s="42"/>
-      <c r="BQ7" s="42"/>
-      <c r="BR7" s="42"/>
-      <c r="BS7" s="42"/>
-      <c r="BT7" s="42"/>
-      <c r="BU7" s="42"/>
-      <c r="BV7" s="42"/>
-      <c r="BW7" s="43"/>
-      <c r="BX7" s="41"/>
-      <c r="BY7" s="42"/>
-      <c r="BZ7" s="42"/>
-      <c r="CA7" s="42"/>
-      <c r="CB7" s="42"/>
-      <c r="CC7" s="42"/>
-      <c r="CD7" s="42"/>
-      <c r="CE7" s="42"/>
-      <c r="CF7" s="42"/>
-      <c r="CG7" s="42"/>
-      <c r="CH7" s="42"/>
-      <c r="CI7" s="42"/>
-      <c r="CJ7" s="42"/>
-      <c r="CK7" s="42"/>
-      <c r="CL7" s="42"/>
-      <c r="CM7" s="42"/>
-      <c r="CN7" s="42"/>
-      <c r="CO7" s="42"/>
-      <c r="CP7" s="42"/>
-      <c r="CQ7" s="42"/>
-      <c r="CR7" s="43"/>
-      <c r="CS7" s="41"/>
-      <c r="CT7" s="42"/>
-      <c r="CU7" s="42"/>
-      <c r="CV7" s="42"/>
-      <c r="CW7" s="42"/>
-      <c r="CX7" s="42"/>
-      <c r="CY7" s="42"/>
-      <c r="CZ7" s="42"/>
-      <c r="DA7" s="42"/>
-      <c r="DB7" s="42"/>
-      <c r="DC7" s="42"/>
-      <c r="DD7" s="42"/>
-      <c r="DE7" s="42"/>
-      <c r="DF7" s="42"/>
-      <c r="DG7" s="42"/>
-      <c r="DH7" s="42"/>
-      <c r="DI7" s="42"/>
-      <c r="DJ7" s="42"/>
-      <c r="DK7" s="42"/>
-      <c r="DL7" s="42"/>
-      <c r="DM7" s="43"/>
-      <c r="DN7" s="41"/>
-      <c r="DO7" s="42"/>
-      <c r="DP7" s="42"/>
-      <c r="DQ7" s="42"/>
-      <c r="DR7" s="42"/>
-      <c r="DS7" s="43"/>
-      <c r="DT7" s="41" t="s">
-        <v>245</v>
-      </c>
-      <c r="DU7" s="42"/>
-      <c r="DV7" s="43"/>
-      <c r="DW7" s="41"/>
-      <c r="DX7" s="42"/>
-      <c r="DY7" s="42"/>
-      <c r="DZ7" s="42"/>
-      <c r="EA7" s="43"/>
+        <v>243</v>
+      </c>
+      <c r="AV7" s="52"/>
+      <c r="AW7" s="53"/>
+      <c r="AX7" s="53"/>
+      <c r="AY7" s="53"/>
+      <c r="AZ7" s="53"/>
+      <c r="BA7" s="53"/>
+      <c r="BB7" s="53"/>
+      <c r="BC7" s="53"/>
+      <c r="BD7" s="53"/>
+      <c r="BE7" s="53"/>
+      <c r="BF7" s="53"/>
+      <c r="BG7" s="53"/>
+      <c r="BH7" s="53"/>
+      <c r="BI7" s="53"/>
+      <c r="BJ7" s="53"/>
+      <c r="BK7" s="53"/>
+      <c r="BL7" s="53"/>
+      <c r="BM7" s="53"/>
+      <c r="BN7" s="53"/>
+      <c r="BO7" s="53"/>
+      <c r="BP7" s="53"/>
+      <c r="BQ7" s="53"/>
+      <c r="BR7" s="53"/>
+      <c r="BS7" s="53"/>
+      <c r="BT7" s="53"/>
+      <c r="BU7" s="53"/>
+      <c r="BV7" s="53"/>
+      <c r="BW7" s="54"/>
+      <c r="BX7" s="52"/>
+      <c r="BY7" s="53"/>
+      <c r="BZ7" s="53"/>
+      <c r="CA7" s="53"/>
+      <c r="CB7" s="53"/>
+      <c r="CC7" s="53"/>
+      <c r="CD7" s="53"/>
+      <c r="CE7" s="53"/>
+      <c r="CF7" s="53"/>
+      <c r="CG7" s="53"/>
+      <c r="CH7" s="53"/>
+      <c r="CI7" s="53"/>
+      <c r="CJ7" s="53"/>
+      <c r="CK7" s="53"/>
+      <c r="CL7" s="53"/>
+      <c r="CM7" s="53"/>
+      <c r="CN7" s="53"/>
+      <c r="CO7" s="53"/>
+      <c r="CP7" s="53"/>
+      <c r="CQ7" s="53"/>
+      <c r="CR7" s="54"/>
+      <c r="CS7" s="52"/>
+      <c r="CT7" s="53"/>
+      <c r="CU7" s="53"/>
+      <c r="CV7" s="53"/>
+      <c r="CW7" s="53"/>
+      <c r="CX7" s="53"/>
+      <c r="CY7" s="53"/>
+      <c r="CZ7" s="53"/>
+      <c r="DA7" s="53"/>
+      <c r="DB7" s="53"/>
+      <c r="DC7" s="53"/>
+      <c r="DD7" s="53"/>
+      <c r="DE7" s="53"/>
+      <c r="DF7" s="53"/>
+      <c r="DG7" s="53"/>
+      <c r="DH7" s="53"/>
+      <c r="DI7" s="53"/>
+      <c r="DJ7" s="53"/>
+      <c r="DK7" s="53"/>
+      <c r="DL7" s="53"/>
+      <c r="DM7" s="54"/>
+      <c r="DN7" s="52"/>
+      <c r="DO7" s="53"/>
+      <c r="DP7" s="53"/>
+      <c r="DQ7" s="53"/>
+      <c r="DR7" s="53"/>
+      <c r="DS7" s="54"/>
+      <c r="DT7" s="52" t="s">
+        <v>243</v>
+      </c>
+      <c r="DU7" s="53"/>
+      <c r="DV7" s="53"/>
+      <c r="DW7" s="53"/>
+      <c r="DX7" s="53"/>
+      <c r="DY7" s="53"/>
+      <c r="DZ7" s="61"/>
+      <c r="EA7" s="61"/>
     </row>
     <row r="8" spans="1:131" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="71" t="s">
-        <v>281</v>
+      <c r="A8" s="36" t="s">
+        <v>279</v>
       </c>
       <c r="B8" s="17">
         <v>1</v>
@@ -3813,60 +3816,18 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="74">
-    <mergeCell ref="DN1:EA1"/>
-    <mergeCell ref="BL5:BO5"/>
-    <mergeCell ref="BP5:BS5"/>
-    <mergeCell ref="BT5:BW5"/>
-    <mergeCell ref="AQ1:BW1"/>
-    <mergeCell ref="CB4:CG4"/>
-    <mergeCell ref="BX1:CR1"/>
-    <mergeCell ref="BX6:CR6"/>
-    <mergeCell ref="BX7:CR7"/>
-    <mergeCell ref="DI5:DL5"/>
-    <mergeCell ref="CS6:DM6"/>
-    <mergeCell ref="CS7:DM7"/>
-    <mergeCell ref="CS1:DM1"/>
-    <mergeCell ref="B1:P1"/>
-    <mergeCell ref="Q1:AJ1"/>
-    <mergeCell ref="AK1:AP1"/>
-    <mergeCell ref="DV6:EA6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="DT7:DV7"/>
-    <mergeCell ref="DW7:EA7"/>
-    <mergeCell ref="AS7:AT7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="X7:AJ7"/>
-    <mergeCell ref="AK7:AP7"/>
-    <mergeCell ref="AQ7:AR7"/>
-    <mergeCell ref="AV7:BW7"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="AE6:AO6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="DV5:DY5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="BZ4:CA4"/>
-    <mergeCell ref="AV5:AY5"/>
-    <mergeCell ref="AZ5:BC5"/>
-    <mergeCell ref="BD5:BG5"/>
-    <mergeCell ref="BH5:BK5"/>
-    <mergeCell ref="CI4:CR4"/>
-    <mergeCell ref="DQ5:DR5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AK5:AM5"/>
-    <mergeCell ref="AQ5:AU5"/>
+  <mergeCells count="75">
+    <mergeCell ref="DU4:DY4"/>
+    <mergeCell ref="DT7:DY7"/>
+    <mergeCell ref="DZ7:EA7"/>
+    <mergeCell ref="DD4:DH4"/>
+    <mergeCell ref="DI4:DL4"/>
+    <mergeCell ref="DD5:DH5"/>
+    <mergeCell ref="DO5:DP5"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="CZ5:DA5"/>
+    <mergeCell ref="DN6:DR6"/>
+    <mergeCell ref="DN7:DS7"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="CB5:CE5"/>
     <mergeCell ref="CF5:CG5"/>
@@ -3880,14 +3841,57 @@
     <mergeCell ref="Q6:X6"/>
     <mergeCell ref="AA6:AD6"/>
     <mergeCell ref="B6:E6"/>
-    <mergeCell ref="DD4:DH4"/>
-    <mergeCell ref="DI4:DL4"/>
-    <mergeCell ref="DD5:DH5"/>
-    <mergeCell ref="DO5:DP5"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="CZ5:DA5"/>
-    <mergeCell ref="DN6:DR6"/>
-    <mergeCell ref="DN7:DS7"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="BZ4:CA4"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="AE6:AO6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="Q1:AJ1"/>
+    <mergeCell ref="AK1:AP1"/>
+    <mergeCell ref="DV6:EA6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="AS7:AT7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="X7:AJ7"/>
+    <mergeCell ref="AK7:AP7"/>
+    <mergeCell ref="AQ7:AR7"/>
+    <mergeCell ref="AV7:BW7"/>
+    <mergeCell ref="BX6:CR6"/>
+    <mergeCell ref="BX7:CR7"/>
+    <mergeCell ref="DI5:DL5"/>
+    <mergeCell ref="CS6:DM6"/>
+    <mergeCell ref="CS7:DM7"/>
+    <mergeCell ref="DN1:EA1"/>
+    <mergeCell ref="BL5:BO5"/>
+    <mergeCell ref="BP5:BS5"/>
+    <mergeCell ref="BT5:BW5"/>
+    <mergeCell ref="AQ1:BW1"/>
+    <mergeCell ref="CB4:CG4"/>
+    <mergeCell ref="BX1:CR1"/>
+    <mergeCell ref="CS1:DM1"/>
+    <mergeCell ref="DV5:DY5"/>
+    <mergeCell ref="AV5:AY5"/>
+    <mergeCell ref="AZ5:BC5"/>
+    <mergeCell ref="BD5:BG5"/>
+    <mergeCell ref="BH5:BK5"/>
+    <mergeCell ref="CI4:CR4"/>
+    <mergeCell ref="DQ5:DR5"/>
+    <mergeCell ref="AQ5:AU5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="X4" r:id="rId1" xr:uid="{33A4BD0C-7A19-4C88-AF60-902623A24589}"/>
@@ -3898,6 +3902,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000BCF930048F2A84190E342D576E507E9" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a5f7dcad46bf03cd06b92fe3a65eb3e5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ede1785e-3bac-4a90-a48c-62cc0231644e" xmlns:ns3="6c5f9a5a-0dad-4595-a39a-6416e9fb7054" xmlns:ns4="83a87e31-bf32-46ab-8e70-9fa18461fa4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="627fd199b21a7508d85a0883525fd0b8" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
@@ -4157,15 +4170,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4178,10 +4182,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5871B92-FF15-4BFB-BF9C-5F0764F5BD73}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D2572BD-7EE7-4817-BEE4-BB014A85EDEE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -4189,20 +4189,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{844596B9-62AA-44A2-8AEF-70908D01A276}"/>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3234EB82-E598-4D46-AACB-BAE493D677A7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="6c5f9a5a-0dad-4595-a39a-6416e9fb7054"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
refactor: reorder field_118 and 119 in 2024 row parser
</commit_message>
<xml_diff>
--- a/public/files/bulk-upload-lettings-template-2024-25.xlsx
+++ b/public/files/bulk-upload-lettings-template-2024-25.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mhclg.sharepoint.com/sites/HousingandplanningandCOREstatistics/Shared Documents/CORE Lettings/01 Annual log changes/2024-25/03 Materials for providers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamuelIvko\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="445" documentId="11_77304B1A9BA1AE53F84EE05360D243E6F58DE18B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D887E7A-65F3-456B-814B-C04A0C5272FB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF79DF4-BB38-4E64-BFB6-0CF3D9A5A4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="24-25 lettings template" sheetId="1" r:id="rId1"/>
@@ -1335,33 +1335,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1371,68 +1344,95 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1655,9 +1655,7 @@
   </sheetPr>
   <dimension ref="A1:EA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="EC5" sqref="EC5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1688,7 +1686,7 @@
     <col min="93" max="93" width="12.81640625" customWidth="1"/>
     <col min="99" max="99" width="13.453125" customWidth="1"/>
     <col min="116" max="116" width="12.54296875" style="1"/>
-    <col min="119" max="119" width="16.453125" customWidth="1"/>
+    <col min="120" max="120" width="16.453125" customWidth="1"/>
     <col min="123" max="123" width="13.453125" customWidth="1"/>
     <col min="126" max="126" width="12.81640625" customWidth="1"/>
   </cols>
@@ -1697,150 +1695,150 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="59" t="s">
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="59"/>
-      <c r="Z1" s="59"/>
-      <c r="AA1" s="59"/>
-      <c r="AB1" s="59"/>
-      <c r="AC1" s="59"/>
-      <c r="AD1" s="59"/>
-      <c r="AE1" s="59"/>
-      <c r="AF1" s="59"/>
-      <c r="AG1" s="59"/>
-      <c r="AH1" s="59"/>
-      <c r="AI1" s="59"/>
-      <c r="AJ1" s="59"/>
-      <c r="AK1" s="60" t="s">
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="53"/>
+      <c r="AB1" s="53"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="53"/>
+      <c r="AF1" s="53"/>
+      <c r="AG1" s="53"/>
+      <c r="AH1" s="53"/>
+      <c r="AI1" s="53"/>
+      <c r="AJ1" s="53"/>
+      <c r="AK1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="60"/>
-      <c r="AM1" s="60"/>
-      <c r="AN1" s="60"/>
-      <c r="AO1" s="60"/>
-      <c r="AP1" s="60"/>
-      <c r="AQ1" s="43" t="s">
+      <c r="AL1" s="54"/>
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="AR1" s="44"/>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="44"/>
-      <c r="AV1" s="44"/>
-      <c r="AW1" s="44"/>
-      <c r="AX1" s="44"/>
-      <c r="AY1" s="44"/>
-      <c r="AZ1" s="44"/>
-      <c r="BA1" s="44"/>
-      <c r="BB1" s="44"/>
-      <c r="BC1" s="44"/>
-      <c r="BD1" s="44"/>
-      <c r="BE1" s="44"/>
-      <c r="BF1" s="44"/>
-      <c r="BG1" s="44"/>
-      <c r="BH1" s="44"/>
-      <c r="BI1" s="44"/>
-      <c r="BJ1" s="44"/>
-      <c r="BK1" s="44"/>
-      <c r="BL1" s="44"/>
-      <c r="BM1" s="44"/>
-      <c r="BN1" s="44"/>
-      <c r="BO1" s="44"/>
-      <c r="BP1" s="44"/>
-      <c r="BQ1" s="44"/>
-      <c r="BR1" s="44"/>
-      <c r="BS1" s="44"/>
-      <c r="BT1" s="44"/>
-      <c r="BU1" s="44"/>
-      <c r="BV1" s="44"/>
-      <c r="BW1" s="45"/>
-      <c r="BX1" s="49" t="s">
+      <c r="AR1" s="63"/>
+      <c r="AS1" s="63"/>
+      <c r="AT1" s="63"/>
+      <c r="AU1" s="63"/>
+      <c r="AV1" s="63"/>
+      <c r="AW1" s="63"/>
+      <c r="AX1" s="63"/>
+      <c r="AY1" s="63"/>
+      <c r="AZ1" s="63"/>
+      <c r="BA1" s="63"/>
+      <c r="BB1" s="63"/>
+      <c r="BC1" s="63"/>
+      <c r="BD1" s="63"/>
+      <c r="BE1" s="63"/>
+      <c r="BF1" s="63"/>
+      <c r="BG1" s="63"/>
+      <c r="BH1" s="63"/>
+      <c r="BI1" s="63"/>
+      <c r="BJ1" s="63"/>
+      <c r="BK1" s="63"/>
+      <c r="BL1" s="63"/>
+      <c r="BM1" s="63"/>
+      <c r="BN1" s="63"/>
+      <c r="BO1" s="63"/>
+      <c r="BP1" s="63"/>
+      <c r="BQ1" s="63"/>
+      <c r="BR1" s="63"/>
+      <c r="BS1" s="63"/>
+      <c r="BT1" s="63"/>
+      <c r="BU1" s="63"/>
+      <c r="BV1" s="63"/>
+      <c r="BW1" s="64"/>
+      <c r="BX1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="BY1" s="50"/>
-      <c r="BZ1" s="50"/>
-      <c r="CA1" s="50"/>
-      <c r="CB1" s="50"/>
-      <c r="CC1" s="50"/>
-      <c r="CD1" s="50"/>
-      <c r="CE1" s="50"/>
-      <c r="CF1" s="50"/>
-      <c r="CG1" s="50"/>
-      <c r="CH1" s="50"/>
-      <c r="CI1" s="50"/>
-      <c r="CJ1" s="50"/>
-      <c r="CK1" s="50"/>
-      <c r="CL1" s="50"/>
-      <c r="CM1" s="50"/>
-      <c r="CN1" s="50"/>
-      <c r="CO1" s="50"/>
-      <c r="CP1" s="50"/>
-      <c r="CQ1" s="50"/>
-      <c r="CR1" s="51"/>
-      <c r="CS1" s="55" t="s">
+      <c r="BY1" s="66"/>
+      <c r="BZ1" s="66"/>
+      <c r="CA1" s="66"/>
+      <c r="CB1" s="66"/>
+      <c r="CC1" s="66"/>
+      <c r="CD1" s="66"/>
+      <c r="CE1" s="66"/>
+      <c r="CF1" s="66"/>
+      <c r="CG1" s="66"/>
+      <c r="CH1" s="66"/>
+      <c r="CI1" s="66"/>
+      <c r="CJ1" s="66"/>
+      <c r="CK1" s="66"/>
+      <c r="CL1" s="66"/>
+      <c r="CM1" s="66"/>
+      <c r="CN1" s="66"/>
+      <c r="CO1" s="66"/>
+      <c r="CP1" s="66"/>
+      <c r="CQ1" s="66"/>
+      <c r="CR1" s="67"/>
+      <c r="CS1" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="CT1" s="56"/>
-      <c r="CU1" s="56"/>
-      <c r="CV1" s="56"/>
-      <c r="CW1" s="56"/>
-      <c r="CX1" s="56"/>
-      <c r="CY1" s="56"/>
-      <c r="CZ1" s="56"/>
-      <c r="DA1" s="56"/>
-      <c r="DB1" s="56"/>
-      <c r="DC1" s="56"/>
-      <c r="DD1" s="56"/>
-      <c r="DE1" s="56"/>
-      <c r="DF1" s="56"/>
-      <c r="DG1" s="56"/>
-      <c r="DH1" s="56"/>
-      <c r="DI1" s="56"/>
-      <c r="DJ1" s="56"/>
-      <c r="DK1" s="56"/>
-      <c r="DL1" s="56"/>
-      <c r="DM1" s="57"/>
-      <c r="DN1" s="37" t="s">
+      <c r="CT1" s="69"/>
+      <c r="CU1" s="69"/>
+      <c r="CV1" s="69"/>
+      <c r="CW1" s="69"/>
+      <c r="CX1" s="69"/>
+      <c r="CY1" s="69"/>
+      <c r="CZ1" s="69"/>
+      <c r="DA1" s="69"/>
+      <c r="DB1" s="69"/>
+      <c r="DC1" s="69"/>
+      <c r="DD1" s="69"/>
+      <c r="DE1" s="69"/>
+      <c r="DF1" s="69"/>
+      <c r="DG1" s="69"/>
+      <c r="DH1" s="69"/>
+      <c r="DI1" s="69"/>
+      <c r="DJ1" s="69"/>
+      <c r="DK1" s="69"/>
+      <c r="DL1" s="69"/>
+      <c r="DM1" s="70"/>
+      <c r="DN1" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="DO1" s="38"/>
-      <c r="DP1" s="38"/>
-      <c r="DQ1" s="38"/>
-      <c r="DR1" s="38"/>
-      <c r="DS1" s="38"/>
-      <c r="DT1" s="38"/>
-      <c r="DU1" s="38"/>
-      <c r="DV1" s="38"/>
-      <c r="DW1" s="38"/>
-      <c r="DX1" s="38"/>
-      <c r="DY1" s="38"/>
-      <c r="DZ1" s="38"/>
-      <c r="EA1" s="39"/>
+      <c r="DO1" s="57"/>
+      <c r="DP1" s="57"/>
+      <c r="DQ1" s="57"/>
+      <c r="DR1" s="57"/>
+      <c r="DS1" s="57"/>
+      <c r="DT1" s="57"/>
+      <c r="DU1" s="57"/>
+      <c r="DV1" s="57"/>
+      <c r="DW1" s="57"/>
+      <c r="DX1" s="57"/>
+      <c r="DY1" s="57"/>
+      <c r="DZ1" s="57"/>
+      <c r="EA1" s="58"/>
     </row>
     <row r="2" spans="1:131" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2198,10 +2196,10 @@
         <v>125</v>
       </c>
       <c r="DO2" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="DP2" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="DP2" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="DQ2" s="4" t="s">
         <v>128</v>
@@ -2306,16 +2304,16 @@
       <c r="AD3" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="AE3" s="63" t="s">
+      <c r="AE3" s="49" t="s">
         <v>155</v>
       </c>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="63" t="s">
+      <c r="AF3" s="50"/>
+      <c r="AG3" s="50"/>
+      <c r="AH3" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="AI3" s="64"/>
-      <c r="AJ3" s="64"/>
+      <c r="AI3" s="50"/>
+      <c r="AJ3" s="50"/>
       <c r="AK3" s="11" t="s">
         <v>157</v>
       </c>
@@ -2492,10 +2490,10 @@
       </c>
       <c r="DM3" s="11"/>
       <c r="DN3" s="11"/>
-      <c r="DO3" s="11" t="s">
+      <c r="DO3" s="11"/>
+      <c r="DP3" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="DP3" s="11"/>
       <c r="DQ3" s="11" t="s">
         <v>184</v>
       </c>
@@ -2530,10 +2528,10 @@
       <c r="A4" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="46" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="70"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="15" t="s">
         <v>195</v>
       </c>
@@ -2576,14 +2574,14 @@
       <c r="Q4" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="R4" s="65" t="s">
+      <c r="R4" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="S4" s="67"/>
-      <c r="T4" s="65" t="s">
+      <c r="S4" s="48"/>
+      <c r="T4" s="45" t="s">
         <v>201</v>
       </c>
-      <c r="U4" s="67"/>
+      <c r="U4" s="48"/>
       <c r="V4" s="15" t="s">
         <v>205</v>
       </c>
@@ -2602,10 +2600,10 @@
       <c r="AA4" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="AB4" s="65" t="s">
+      <c r="AB4" s="45" t="s">
         <v>196</v>
       </c>
-      <c r="AC4" s="67"/>
+      <c r="AC4" s="48"/>
       <c r="AD4" s="15" t="s">
         <v>211</v>
       </c>
@@ -2750,33 +2748,33 @@
       <c r="BY4" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="BZ4" s="46" t="s">
+      <c r="BZ4" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="CA4" s="48"/>
-      <c r="CB4" s="46" t="s">
+      <c r="CA4" s="39"/>
+      <c r="CB4" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="CC4" s="47"/>
-      <c r="CD4" s="47"/>
-      <c r="CE4" s="47"/>
-      <c r="CF4" s="47"/>
-      <c r="CG4" s="48"/>
+      <c r="CC4" s="38"/>
+      <c r="CD4" s="38"/>
+      <c r="CE4" s="38"/>
+      <c r="CF4" s="38"/>
+      <c r="CG4" s="39"/>
       <c r="CH4" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="CI4" s="46" t="s">
+      <c r="CI4" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="CJ4" s="47"/>
-      <c r="CK4" s="47"/>
-      <c r="CL4" s="47"/>
-      <c r="CM4" s="47"/>
-      <c r="CN4" s="47"/>
-      <c r="CO4" s="47"/>
-      <c r="CP4" s="47"/>
-      <c r="CQ4" s="47"/>
-      <c r="CR4" s="48"/>
+      <c r="CJ4" s="38"/>
+      <c r="CK4" s="38"/>
+      <c r="CL4" s="38"/>
+      <c r="CM4" s="38"/>
+      <c r="CN4" s="38"/>
+      <c r="CO4" s="38"/>
+      <c r="CP4" s="38"/>
+      <c r="CQ4" s="38"/>
+      <c r="CR4" s="39"/>
       <c r="CS4" s="17" t="s">
         <v>226</v>
       </c>
@@ -2810,19 +2808,19 @@
       <c r="DC4" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="DD4" s="46" t="s">
+      <c r="DD4" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="DE4" s="47"/>
-      <c r="DF4" s="47"/>
-      <c r="DG4" s="47"/>
-      <c r="DH4" s="48"/>
-      <c r="DI4" s="46" t="s">
+      <c r="DE4" s="38"/>
+      <c r="DF4" s="38"/>
+      <c r="DG4" s="38"/>
+      <c r="DH4" s="39"/>
+      <c r="DI4" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="DJ4" s="47"/>
-      <c r="DK4" s="47"/>
-      <c r="DL4" s="48"/>
+      <c r="DJ4" s="38"/>
+      <c r="DK4" s="38"/>
+      <c r="DL4" s="39"/>
       <c r="DM4" s="17" t="s">
         <v>234</v>
       </c>
@@ -2830,10 +2828,10 @@
         <v>214</v>
       </c>
       <c r="DO4" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="DP4" s="15" t="s">
         <v>235</v>
-      </c>
-      <c r="DP4" s="15" t="s">
-        <v>214</v>
       </c>
       <c r="DQ4" s="15" t="s">
         <v>236</v>
@@ -2847,13 +2845,13 @@
       <c r="DT4" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="DU4" s="46" t="s">
+      <c r="DU4" s="37" t="s">
         <v>240</v>
       </c>
-      <c r="DV4" s="47"/>
-      <c r="DW4" s="47"/>
-      <c r="DX4" s="47"/>
-      <c r="DY4" s="48"/>
+      <c r="DV4" s="38"/>
+      <c r="DW4" s="38"/>
+      <c r="DX4" s="38"/>
+      <c r="DY4" s="39"/>
       <c r="DZ4" s="15" t="s">
         <v>214</v>
       </c>
@@ -2865,10 +2863,10 @@
       <c r="A5" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="45" t="s">
         <v>242</v>
       </c>
-      <c r="C5" s="68"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="15" t="s">
         <v>243</v>
       </c>
@@ -2881,20 +2879,20 @@
       <c r="G5" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="48"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="39"/>
       <c r="M5" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="N5" s="65" t="s">
+      <c r="N5" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="O5" s="68"/>
+      <c r="O5" s="44"/>
       <c r="P5" s="30" t="s">
         <v>242</v>
       </c>
@@ -2913,10 +2911,10 @@
       <c r="U5" s="32" t="s">
         <v>243</v>
       </c>
-      <c r="V5" s="65" t="s">
+      <c r="V5" s="45" t="s">
         <v>247</v>
       </c>
-      <c r="W5" s="68"/>
+      <c r="W5" s="44"/>
       <c r="X5" s="15" t="s">
         <v>248</v>
       </c>
@@ -2926,27 +2924,27 @@
       <c r="Z5" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="AA5" s="65" t="s">
+      <c r="AA5" s="45" t="s">
         <v>248</v>
       </c>
-      <c r="AB5" s="68"/>
-      <c r="AC5" s="68"/>
-      <c r="AD5" s="68"/>
-      <c r="AE5" s="65" t="s">
+      <c r="AB5" s="44"/>
+      <c r="AC5" s="44"/>
+      <c r="AD5" s="44"/>
+      <c r="AE5" s="45" t="s">
         <v>249</v>
       </c>
-      <c r="AF5" s="68"/>
-      <c r="AG5" s="68"/>
-      <c r="AH5" s="65" t="s">
+      <c r="AF5" s="44"/>
+      <c r="AG5" s="44"/>
+      <c r="AH5" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="AI5" s="68"/>
-      <c r="AJ5" s="68"/>
-      <c r="AK5" s="65" t="s">
+      <c r="AI5" s="44"/>
+      <c r="AJ5" s="44"/>
+      <c r="AK5" s="45" t="s">
         <v>242</v>
       </c>
-      <c r="AL5" s="68"/>
-      <c r="AM5" s="68"/>
+      <c r="AL5" s="44"/>
+      <c r="AM5" s="44"/>
       <c r="AN5" s="15" t="s">
         <v>251</v>
       </c>
@@ -2956,55 +2954,55 @@
       <c r="AP5" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="AQ5" s="46" t="s">
+      <c r="AQ5" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="AR5" s="47"/>
-      <c r="AS5" s="47"/>
-      <c r="AT5" s="47"/>
-      <c r="AU5" s="48"/>
-      <c r="AV5" s="40" t="s">
+      <c r="AR5" s="38"/>
+      <c r="AS5" s="38"/>
+      <c r="AT5" s="38"/>
+      <c r="AU5" s="39"/>
+      <c r="AV5" s="59" t="s">
         <v>253</v>
       </c>
-      <c r="AW5" s="41"/>
-      <c r="AX5" s="41"/>
-      <c r="AY5" s="42"/>
-      <c r="AZ5" s="40" t="s">
+      <c r="AW5" s="60"/>
+      <c r="AX5" s="60"/>
+      <c r="AY5" s="61"/>
+      <c r="AZ5" s="59" t="s">
         <v>278</v>
       </c>
-      <c r="BA5" s="41"/>
-      <c r="BB5" s="41"/>
-      <c r="BC5" s="42"/>
-      <c r="BD5" s="40" t="s">
+      <c r="BA5" s="60"/>
+      <c r="BB5" s="60"/>
+      <c r="BC5" s="61"/>
+      <c r="BD5" s="59" t="s">
         <v>254</v>
       </c>
-      <c r="BE5" s="41"/>
-      <c r="BF5" s="41"/>
-      <c r="BG5" s="42"/>
-      <c r="BH5" s="40" t="s">
+      <c r="BE5" s="60"/>
+      <c r="BF5" s="60"/>
+      <c r="BG5" s="61"/>
+      <c r="BH5" s="59" t="s">
         <v>255</v>
       </c>
-      <c r="BI5" s="41"/>
-      <c r="BJ5" s="41"/>
-      <c r="BK5" s="42"/>
-      <c r="BL5" s="40" t="s">
+      <c r="BI5" s="60"/>
+      <c r="BJ5" s="60"/>
+      <c r="BK5" s="61"/>
+      <c r="BL5" s="59" t="s">
         <v>256</v>
       </c>
-      <c r="BM5" s="41"/>
-      <c r="BN5" s="41"/>
-      <c r="BO5" s="42"/>
-      <c r="BP5" s="40" t="s">
+      <c r="BM5" s="60"/>
+      <c r="BN5" s="60"/>
+      <c r="BO5" s="61"/>
+      <c r="BP5" s="59" t="s">
         <v>257</v>
       </c>
-      <c r="BQ5" s="41"/>
-      <c r="BR5" s="41"/>
-      <c r="BS5" s="42"/>
-      <c r="BT5" s="40" t="s">
+      <c r="BQ5" s="60"/>
+      <c r="BR5" s="60"/>
+      <c r="BS5" s="61"/>
+      <c r="BT5" s="59" t="s">
         <v>258</v>
       </c>
-      <c r="BU5" s="41"/>
-      <c r="BV5" s="41"/>
-      <c r="BW5" s="42"/>
+      <c r="BU5" s="60"/>
+      <c r="BV5" s="60"/>
+      <c r="BW5" s="61"/>
       <c r="BX5" s="15" t="s">
         <v>242</v>
       </c>
@@ -3017,31 +3015,31 @@
       <c r="CA5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="CB5" s="46" t="s">
+      <c r="CB5" s="37" t="s">
         <v>261</v>
       </c>
-      <c r="CC5" s="47"/>
-      <c r="CD5" s="47"/>
-      <c r="CE5" s="48"/>
-      <c r="CF5" s="46" t="s">
+      <c r="CC5" s="38"/>
+      <c r="CD5" s="38"/>
+      <c r="CE5" s="39"/>
+      <c r="CF5" s="37" t="s">
         <v>262</v>
       </c>
-      <c r="CG5" s="48"/>
+      <c r="CG5" s="39"/>
       <c r="CH5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="CI5" s="46" t="s">
+      <c r="CI5" s="37" t="s">
         <v>263</v>
       </c>
-      <c r="CJ5" s="47"/>
-      <c r="CK5" s="47"/>
-      <c r="CL5" s="47"/>
-      <c r="CM5" s="47"/>
-      <c r="CN5" s="47"/>
-      <c r="CO5" s="47"/>
-      <c r="CP5" s="47"/>
-      <c r="CQ5" s="47"/>
-      <c r="CR5" s="48"/>
+      <c r="CJ5" s="38"/>
+      <c r="CK5" s="38"/>
+      <c r="CL5" s="38"/>
+      <c r="CM5" s="38"/>
+      <c r="CN5" s="38"/>
+      <c r="CO5" s="38"/>
+      <c r="CP5" s="38"/>
+      <c r="CQ5" s="38"/>
+      <c r="CR5" s="39"/>
       <c r="CS5" s="15" t="s">
         <v>242</v>
       </c>
@@ -3057,47 +3055,47 @@
       <c r="CW5" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="CX5" s="46" t="s">
+      <c r="CX5" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="CY5" s="48"/>
-      <c r="CZ5" s="46" t="s">
+      <c r="CY5" s="39"/>
+      <c r="CZ5" s="37" t="s">
         <v>265</v>
       </c>
-      <c r="DA5" s="48"/>
+      <c r="DA5" s="39"/>
       <c r="DB5" s="15" t="s">
         <v>243</v>
       </c>
       <c r="DC5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="DD5" s="52" t="s">
+      <c r="DD5" s="40" t="s">
         <v>266</v>
       </c>
-      <c r="DE5" s="53"/>
-      <c r="DF5" s="53"/>
-      <c r="DG5" s="53"/>
-      <c r="DH5" s="54"/>
-      <c r="DI5" s="46" t="s">
+      <c r="DE5" s="41"/>
+      <c r="DF5" s="41"/>
+      <c r="DG5" s="41"/>
+      <c r="DH5" s="43"/>
+      <c r="DI5" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="DJ5" s="47"/>
-      <c r="DK5" s="47"/>
-      <c r="DL5" s="48"/>
+      <c r="DJ5" s="38"/>
+      <c r="DK5" s="38"/>
+      <c r="DL5" s="39"/>
       <c r="DM5" s="15" t="s">
         <v>249</v>
       </c>
       <c r="DN5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="DO5" s="46" t="s">
+      <c r="DO5" s="37" t="s">
         <v>267</v>
       </c>
-      <c r="DP5" s="48"/>
-      <c r="DQ5" s="46" t="s">
+      <c r="DP5" s="39"/>
+      <c r="DQ5" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="DR5" s="48"/>
+      <c r="DR5" s="39"/>
       <c r="DS5" s="15" t="s">
         <v>242</v>
       </c>
@@ -3107,12 +3105,12 @@
       <c r="DU5" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="DV5" s="46" t="s">
+      <c r="DV5" s="37" t="s">
         <v>269</v>
       </c>
-      <c r="DW5" s="47"/>
-      <c r="DX5" s="47"/>
-      <c r="DY5" s="48"/>
+      <c r="DW5" s="38"/>
+      <c r="DX5" s="38"/>
+      <c r="DY5" s="39"/>
       <c r="DZ5" s="15" t="s">
         <v>270</v>
       </c>
@@ -3124,137 +3122,137 @@
       <c r="A6" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="61" t="s">
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="42" t="s">
         <v>273</v>
       </c>
-      <c r="G6" s="61"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
       <c r="M6" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="N6" s="65"/>
-      <c r="O6" s="65"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="65" t="s">
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45" t="s">
         <v>275</v>
       </c>
-      <c r="R6" s="68"/>
-      <c r="S6" s="68"/>
-      <c r="T6" s="68"/>
-      <c r="U6" s="68"/>
-      <c r="V6" s="68"/>
-      <c r="W6" s="68"/>
-      <c r="X6" s="68"/>
-      <c r="Y6" s="65"/>
-      <c r="Z6" s="65"/>
-      <c r="AA6" s="65" t="s">
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
+      <c r="U6" s="44"/>
+      <c r="V6" s="44"/>
+      <c r="W6" s="44"/>
+      <c r="X6" s="44"/>
+      <c r="Y6" s="45"/>
+      <c r="Z6" s="45"/>
+      <c r="AA6" s="45" t="s">
         <v>275</v>
       </c>
-      <c r="AB6" s="68"/>
-      <c r="AC6" s="68"/>
-      <c r="AD6" s="68"/>
-      <c r="AE6" s="65"/>
-      <c r="AF6" s="65"/>
-      <c r="AG6" s="65"/>
-      <c r="AH6" s="65"/>
-      <c r="AI6" s="65"/>
-      <c r="AJ6" s="65"/>
-      <c r="AK6" s="65"/>
-      <c r="AL6" s="65"/>
-      <c r="AM6" s="65"/>
-      <c r="AN6" s="65"/>
-      <c r="AO6" s="65"/>
+      <c r="AB6" s="44"/>
+      <c r="AC6" s="44"/>
+      <c r="AD6" s="44"/>
+      <c r="AE6" s="45"/>
+      <c r="AF6" s="45"/>
+      <c r="AG6" s="45"/>
+      <c r="AH6" s="45"/>
+      <c r="AI6" s="45"/>
+      <c r="AJ6" s="45"/>
+      <c r="AK6" s="45"/>
+      <c r="AL6" s="45"/>
+      <c r="AM6" s="45"/>
+      <c r="AN6" s="45"/>
+      <c r="AO6" s="45"/>
       <c r="AP6" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="AQ6" s="46"/>
-      <c r="AR6" s="47"/>
-      <c r="AS6" s="47"/>
-      <c r="AT6" s="47"/>
-      <c r="AU6" s="47"/>
-      <c r="AV6" s="47"/>
-      <c r="AW6" s="47"/>
-      <c r="AX6" s="47"/>
-      <c r="AY6" s="47"/>
-      <c r="AZ6" s="47"/>
-      <c r="BA6" s="47"/>
-      <c r="BB6" s="47"/>
-      <c r="BC6" s="47"/>
-      <c r="BD6" s="47"/>
-      <c r="BE6" s="47"/>
-      <c r="BF6" s="47"/>
-      <c r="BG6" s="47"/>
-      <c r="BH6" s="47"/>
-      <c r="BI6" s="47"/>
-      <c r="BJ6" s="47"/>
-      <c r="BK6" s="47"/>
-      <c r="BL6" s="47"/>
-      <c r="BM6" s="47"/>
-      <c r="BN6" s="47"/>
-      <c r="BO6" s="47"/>
-      <c r="BP6" s="47"/>
-      <c r="BQ6" s="47"/>
-      <c r="BR6" s="47"/>
-      <c r="BS6" s="47"/>
-      <c r="BT6" s="47"/>
-      <c r="BU6" s="47"/>
-      <c r="BV6" s="47"/>
-      <c r="BW6" s="48"/>
-      <c r="BX6" s="46"/>
-      <c r="BY6" s="47"/>
-      <c r="BZ6" s="47"/>
-      <c r="CA6" s="47"/>
-      <c r="CB6" s="47"/>
-      <c r="CC6" s="47"/>
-      <c r="CD6" s="47"/>
-      <c r="CE6" s="47"/>
-      <c r="CF6" s="47"/>
-      <c r="CG6" s="47"/>
-      <c r="CH6" s="47"/>
-      <c r="CI6" s="47"/>
-      <c r="CJ6" s="47"/>
-      <c r="CK6" s="47"/>
-      <c r="CL6" s="47"/>
-      <c r="CM6" s="47"/>
-      <c r="CN6" s="47"/>
-      <c r="CO6" s="47"/>
-      <c r="CP6" s="47"/>
-      <c r="CQ6" s="47"/>
-      <c r="CR6" s="48"/>
-      <c r="CS6" s="46"/>
-      <c r="CT6" s="47"/>
-      <c r="CU6" s="47"/>
-      <c r="CV6" s="47"/>
-      <c r="CW6" s="47"/>
-      <c r="CX6" s="47"/>
-      <c r="CY6" s="47"/>
-      <c r="CZ6" s="47"/>
-      <c r="DA6" s="47"/>
-      <c r="DB6" s="47"/>
-      <c r="DC6" s="47"/>
-      <c r="DD6" s="47"/>
-      <c r="DE6" s="47"/>
-      <c r="DF6" s="47"/>
-      <c r="DG6" s="47"/>
-      <c r="DH6" s="47"/>
-      <c r="DI6" s="47"/>
-      <c r="DJ6" s="47"/>
-      <c r="DK6" s="47"/>
-      <c r="DL6" s="47"/>
-      <c r="DM6" s="48"/>
-      <c r="DN6" s="46"/>
-      <c r="DO6" s="47"/>
-      <c r="DP6" s="47"/>
-      <c r="DQ6" s="47"/>
-      <c r="DR6" s="48"/>
+      <c r="AQ6" s="37"/>
+      <c r="AR6" s="38"/>
+      <c r="AS6" s="38"/>
+      <c r="AT6" s="38"/>
+      <c r="AU6" s="38"/>
+      <c r="AV6" s="38"/>
+      <c r="AW6" s="38"/>
+      <c r="AX6" s="38"/>
+      <c r="AY6" s="38"/>
+      <c r="AZ6" s="38"/>
+      <c r="BA6" s="38"/>
+      <c r="BB6" s="38"/>
+      <c r="BC6" s="38"/>
+      <c r="BD6" s="38"/>
+      <c r="BE6" s="38"/>
+      <c r="BF6" s="38"/>
+      <c r="BG6" s="38"/>
+      <c r="BH6" s="38"/>
+      <c r="BI6" s="38"/>
+      <c r="BJ6" s="38"/>
+      <c r="BK6" s="38"/>
+      <c r="BL6" s="38"/>
+      <c r="BM6" s="38"/>
+      <c r="BN6" s="38"/>
+      <c r="BO6" s="38"/>
+      <c r="BP6" s="38"/>
+      <c r="BQ6" s="38"/>
+      <c r="BR6" s="38"/>
+      <c r="BS6" s="38"/>
+      <c r="BT6" s="38"/>
+      <c r="BU6" s="38"/>
+      <c r="BV6" s="38"/>
+      <c r="BW6" s="39"/>
+      <c r="BX6" s="37"/>
+      <c r="BY6" s="38"/>
+      <c r="BZ6" s="38"/>
+      <c r="CA6" s="38"/>
+      <c r="CB6" s="38"/>
+      <c r="CC6" s="38"/>
+      <c r="CD6" s="38"/>
+      <c r="CE6" s="38"/>
+      <c r="CF6" s="38"/>
+      <c r="CG6" s="38"/>
+      <c r="CH6" s="38"/>
+      <c r="CI6" s="38"/>
+      <c r="CJ6" s="38"/>
+      <c r="CK6" s="38"/>
+      <c r="CL6" s="38"/>
+      <c r="CM6" s="38"/>
+      <c r="CN6" s="38"/>
+      <c r="CO6" s="38"/>
+      <c r="CP6" s="38"/>
+      <c r="CQ6" s="38"/>
+      <c r="CR6" s="39"/>
+      <c r="CS6" s="37"/>
+      <c r="CT6" s="38"/>
+      <c r="CU6" s="38"/>
+      <c r="CV6" s="38"/>
+      <c r="CW6" s="38"/>
+      <c r="CX6" s="38"/>
+      <c r="CY6" s="38"/>
+      <c r="CZ6" s="38"/>
+      <c r="DA6" s="38"/>
+      <c r="DB6" s="38"/>
+      <c r="DC6" s="38"/>
+      <c r="DD6" s="38"/>
+      <c r="DE6" s="38"/>
+      <c r="DF6" s="38"/>
+      <c r="DG6" s="38"/>
+      <c r="DH6" s="38"/>
+      <c r="DI6" s="38"/>
+      <c r="DJ6" s="38"/>
+      <c r="DK6" s="38"/>
+      <c r="DL6" s="38"/>
+      <c r="DM6" s="39"/>
+      <c r="DN6" s="37"/>
+      <c r="DO6" s="38"/>
+      <c r="DP6" s="38"/>
+      <c r="DQ6" s="38"/>
+      <c r="DR6" s="39"/>
       <c r="DS6" s="20" t="s">
         <v>273</v>
       </c>
@@ -3262,12 +3260,12 @@
       <c r="DU6" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="DV6" s="52"/>
-      <c r="DW6" s="53"/>
-      <c r="DX6" s="53"/>
-      <c r="DY6" s="53"/>
-      <c r="DZ6" s="53"/>
-      <c r="EA6" s="54"/>
+      <c r="DV6" s="40"/>
+      <c r="DW6" s="41"/>
+      <c r="DX6" s="41"/>
+      <c r="DY6" s="41"/>
+      <c r="DZ6" s="41"/>
+      <c r="EA6" s="43"/>
     </row>
     <row r="7" spans="1:131" s="35" customFormat="1" ht="23" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -3276,151 +3274,151 @@
       <c r="B7" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61" t="s">
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42" t="s">
         <v>243</v>
       </c>
-      <c r="G7" s="61"/>
+      <c r="G7" s="42"/>
       <c r="H7" s="21"/>
-      <c r="I7" s="61" t="s">
+      <c r="I7" s="42" t="s">
         <v>243</v>
       </c>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="55"/>
       <c r="N7" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="O7" s="52"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="53"/>
-      <c r="T7" s="53"/>
-      <c r="U7" s="54"/>
-      <c r="V7" s="61" t="s">
+      <c r="O7" s="40"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="41"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="43"/>
+      <c r="V7" s="42" t="s">
         <v>243</v>
       </c>
-      <c r="W7" s="61"/>
-      <c r="X7" s="52"/>
-      <c r="Y7" s="53"/>
-      <c r="Z7" s="53"/>
-      <c r="AA7" s="53"/>
-      <c r="AB7" s="53"/>
-      <c r="AC7" s="53"/>
-      <c r="AD7" s="53"/>
-      <c r="AE7" s="53"/>
-      <c r="AF7" s="53"/>
-      <c r="AG7" s="53"/>
-      <c r="AH7" s="53"/>
-      <c r="AI7" s="53"/>
-      <c r="AJ7" s="54"/>
-      <c r="AK7" s="52"/>
-      <c r="AL7" s="53"/>
-      <c r="AM7" s="53"/>
-      <c r="AN7" s="53"/>
-      <c r="AO7" s="53"/>
-      <c r="AP7" s="54"/>
-      <c r="AQ7" s="52" t="s">
+      <c r="W7" s="42"/>
+      <c r="X7" s="40"/>
+      <c r="Y7" s="41"/>
+      <c r="Z7" s="41"/>
+      <c r="AA7" s="41"/>
+      <c r="AB7" s="41"/>
+      <c r="AC7" s="41"/>
+      <c r="AD7" s="41"/>
+      <c r="AE7" s="41"/>
+      <c r="AF7" s="41"/>
+      <c r="AG7" s="41"/>
+      <c r="AH7" s="41"/>
+      <c r="AI7" s="41"/>
+      <c r="AJ7" s="43"/>
+      <c r="AK7" s="40"/>
+      <c r="AL7" s="41"/>
+      <c r="AM7" s="41"/>
+      <c r="AN7" s="41"/>
+      <c r="AO7" s="41"/>
+      <c r="AP7" s="43"/>
+      <c r="AQ7" s="40" t="s">
         <v>243</v>
       </c>
-      <c r="AR7" s="54"/>
-      <c r="AS7" s="52"/>
-      <c r="AT7" s="54"/>
+      <c r="AR7" s="43"/>
+      <c r="AS7" s="40"/>
+      <c r="AT7" s="43"/>
       <c r="AU7" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="AV7" s="52"/>
-      <c r="AW7" s="53"/>
-      <c r="AX7" s="53"/>
-      <c r="AY7" s="53"/>
-      <c r="AZ7" s="53"/>
-      <c r="BA7" s="53"/>
-      <c r="BB7" s="53"/>
-      <c r="BC7" s="53"/>
-      <c r="BD7" s="53"/>
-      <c r="BE7" s="53"/>
-      <c r="BF7" s="53"/>
-      <c r="BG7" s="53"/>
-      <c r="BH7" s="53"/>
-      <c r="BI7" s="53"/>
-      <c r="BJ7" s="53"/>
-      <c r="BK7" s="53"/>
-      <c r="BL7" s="53"/>
-      <c r="BM7" s="53"/>
-      <c r="BN7" s="53"/>
-      <c r="BO7" s="53"/>
-      <c r="BP7" s="53"/>
-      <c r="BQ7" s="53"/>
-      <c r="BR7" s="53"/>
-      <c r="BS7" s="53"/>
-      <c r="BT7" s="53"/>
-      <c r="BU7" s="53"/>
-      <c r="BV7" s="53"/>
-      <c r="BW7" s="54"/>
-      <c r="BX7" s="52"/>
-      <c r="BY7" s="53"/>
-      <c r="BZ7" s="53"/>
-      <c r="CA7" s="53"/>
-      <c r="CB7" s="53"/>
-      <c r="CC7" s="53"/>
-      <c r="CD7" s="53"/>
-      <c r="CE7" s="53"/>
-      <c r="CF7" s="53"/>
-      <c r="CG7" s="53"/>
-      <c r="CH7" s="53"/>
-      <c r="CI7" s="53"/>
-      <c r="CJ7" s="53"/>
-      <c r="CK7" s="53"/>
-      <c r="CL7" s="53"/>
-      <c r="CM7" s="53"/>
-      <c r="CN7" s="53"/>
-      <c r="CO7" s="53"/>
-      <c r="CP7" s="53"/>
-      <c r="CQ7" s="53"/>
-      <c r="CR7" s="54"/>
-      <c r="CS7" s="52"/>
-      <c r="CT7" s="53"/>
-      <c r="CU7" s="53"/>
-      <c r="CV7" s="53"/>
-      <c r="CW7" s="53"/>
-      <c r="CX7" s="53"/>
-      <c r="CY7" s="53"/>
-      <c r="CZ7" s="53"/>
-      <c r="DA7" s="53"/>
-      <c r="DB7" s="53"/>
-      <c r="DC7" s="53"/>
-      <c r="DD7" s="53"/>
-      <c r="DE7" s="53"/>
-      <c r="DF7" s="53"/>
-      <c r="DG7" s="53"/>
-      <c r="DH7" s="53"/>
-      <c r="DI7" s="53"/>
-      <c r="DJ7" s="53"/>
-      <c r="DK7" s="53"/>
-      <c r="DL7" s="53"/>
-      <c r="DM7" s="54"/>
-      <c r="DN7" s="52"/>
-      <c r="DO7" s="53"/>
-      <c r="DP7" s="53"/>
-      <c r="DQ7" s="53"/>
-      <c r="DR7" s="53"/>
-      <c r="DS7" s="54"/>
-      <c r="DT7" s="52" t="s">
+      <c r="AV7" s="40"/>
+      <c r="AW7" s="41"/>
+      <c r="AX7" s="41"/>
+      <c r="AY7" s="41"/>
+      <c r="AZ7" s="41"/>
+      <c r="BA7" s="41"/>
+      <c r="BB7" s="41"/>
+      <c r="BC7" s="41"/>
+      <c r="BD7" s="41"/>
+      <c r="BE7" s="41"/>
+      <c r="BF7" s="41"/>
+      <c r="BG7" s="41"/>
+      <c r="BH7" s="41"/>
+      <c r="BI7" s="41"/>
+      <c r="BJ7" s="41"/>
+      <c r="BK7" s="41"/>
+      <c r="BL7" s="41"/>
+      <c r="BM7" s="41"/>
+      <c r="BN7" s="41"/>
+      <c r="BO7" s="41"/>
+      <c r="BP7" s="41"/>
+      <c r="BQ7" s="41"/>
+      <c r="BR7" s="41"/>
+      <c r="BS7" s="41"/>
+      <c r="BT7" s="41"/>
+      <c r="BU7" s="41"/>
+      <c r="BV7" s="41"/>
+      <c r="BW7" s="43"/>
+      <c r="BX7" s="40"/>
+      <c r="BY7" s="41"/>
+      <c r="BZ7" s="41"/>
+      <c r="CA7" s="41"/>
+      <c r="CB7" s="41"/>
+      <c r="CC7" s="41"/>
+      <c r="CD7" s="41"/>
+      <c r="CE7" s="41"/>
+      <c r="CF7" s="41"/>
+      <c r="CG7" s="41"/>
+      <c r="CH7" s="41"/>
+      <c r="CI7" s="41"/>
+      <c r="CJ7" s="41"/>
+      <c r="CK7" s="41"/>
+      <c r="CL7" s="41"/>
+      <c r="CM7" s="41"/>
+      <c r="CN7" s="41"/>
+      <c r="CO7" s="41"/>
+      <c r="CP7" s="41"/>
+      <c r="CQ7" s="41"/>
+      <c r="CR7" s="43"/>
+      <c r="CS7" s="40"/>
+      <c r="CT7" s="41"/>
+      <c r="CU7" s="41"/>
+      <c r="CV7" s="41"/>
+      <c r="CW7" s="41"/>
+      <c r="CX7" s="41"/>
+      <c r="CY7" s="41"/>
+      <c r="CZ7" s="41"/>
+      <c r="DA7" s="41"/>
+      <c r="DB7" s="41"/>
+      <c r="DC7" s="41"/>
+      <c r="DD7" s="41"/>
+      <c r="DE7" s="41"/>
+      <c r="DF7" s="41"/>
+      <c r="DG7" s="41"/>
+      <c r="DH7" s="41"/>
+      <c r="DI7" s="41"/>
+      <c r="DJ7" s="41"/>
+      <c r="DK7" s="41"/>
+      <c r="DL7" s="41"/>
+      <c r="DM7" s="43"/>
+      <c r="DN7" s="40"/>
+      <c r="DO7" s="41"/>
+      <c r="DP7" s="41"/>
+      <c r="DQ7" s="41"/>
+      <c r="DR7" s="41"/>
+      <c r="DS7" s="43"/>
+      <c r="DT7" s="40" t="s">
         <v>243</v>
       </c>
-      <c r="DU7" s="53"/>
-      <c r="DV7" s="53"/>
-      <c r="DW7" s="53"/>
-      <c r="DX7" s="53"/>
-      <c r="DY7" s="53"/>
-      <c r="DZ7" s="61"/>
-      <c r="EA7" s="61"/>
+      <c r="DU7" s="41"/>
+      <c r="DV7" s="41"/>
+      <c r="DW7" s="41"/>
+      <c r="DX7" s="41"/>
+      <c r="DY7" s="41"/>
+      <c r="DZ7" s="42"/>
+      <c r="EA7" s="42"/>
     </row>
-    <row r="8" spans="1:131" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:131" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>279</v>
       </c>
@@ -3776,10 +3774,10 @@
         <v>117</v>
       </c>
       <c r="DO8" s="17">
+        <v>118</v>
+      </c>
+      <c r="DP8" s="17">
         <v>119</v>
-      </c>
-      <c r="DP8" s="17">
-        <v>118</v>
       </c>
       <c r="DQ8" s="22">
         <v>120</v>
@@ -3817,46 +3815,22 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="DU4:DY4"/>
-    <mergeCell ref="DT7:DY7"/>
-    <mergeCell ref="DZ7:EA7"/>
-    <mergeCell ref="DD4:DH4"/>
-    <mergeCell ref="DI4:DL4"/>
-    <mergeCell ref="DD5:DH5"/>
-    <mergeCell ref="DO5:DP5"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="CZ5:DA5"/>
-    <mergeCell ref="DN6:DR6"/>
-    <mergeCell ref="DN7:DS7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="CB5:CE5"/>
-    <mergeCell ref="CF5:CG5"/>
-    <mergeCell ref="CI5:CR5"/>
-    <mergeCell ref="CX5:CY5"/>
-    <mergeCell ref="AQ6:BW6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="AA5:AD5"/>
-    <mergeCell ref="Q6:X6"/>
-    <mergeCell ref="AA6:AD6"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="BZ4:CA4"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="AE6:AO6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="DN1:EA1"/>
+    <mergeCell ref="BL5:BO5"/>
+    <mergeCell ref="BP5:BS5"/>
+    <mergeCell ref="BT5:BW5"/>
+    <mergeCell ref="AQ1:BW1"/>
+    <mergeCell ref="CB4:CG4"/>
+    <mergeCell ref="BX1:CR1"/>
+    <mergeCell ref="CS1:DM1"/>
+    <mergeCell ref="DV5:DY5"/>
+    <mergeCell ref="AV5:AY5"/>
+    <mergeCell ref="AZ5:BC5"/>
+    <mergeCell ref="BD5:BG5"/>
+    <mergeCell ref="BH5:BK5"/>
+    <mergeCell ref="CI4:CR4"/>
+    <mergeCell ref="DQ5:DR5"/>
+    <mergeCell ref="AQ5:AU5"/>
     <mergeCell ref="B1:P1"/>
     <mergeCell ref="Q1:AJ1"/>
     <mergeCell ref="AK1:AP1"/>
@@ -3873,25 +3847,49 @@
     <mergeCell ref="AV7:BW7"/>
     <mergeCell ref="BX6:CR6"/>
     <mergeCell ref="BX7:CR7"/>
+    <mergeCell ref="BZ4:CA4"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="AE6:AO6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="CZ5:DA5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="CB5:CE5"/>
+    <mergeCell ref="CF5:CG5"/>
+    <mergeCell ref="CI5:CR5"/>
+    <mergeCell ref="CX5:CY5"/>
+    <mergeCell ref="AQ6:BW6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="AA5:AD5"/>
+    <mergeCell ref="Q6:X6"/>
+    <mergeCell ref="AA6:AD6"/>
+    <mergeCell ref="DU4:DY4"/>
+    <mergeCell ref="DT7:DY7"/>
+    <mergeCell ref="DZ7:EA7"/>
+    <mergeCell ref="DD4:DH4"/>
+    <mergeCell ref="DI4:DL4"/>
+    <mergeCell ref="DD5:DH5"/>
+    <mergeCell ref="DO5:DP5"/>
     <mergeCell ref="DI5:DL5"/>
     <mergeCell ref="CS6:DM6"/>
     <mergeCell ref="CS7:DM7"/>
-    <mergeCell ref="DN1:EA1"/>
-    <mergeCell ref="BL5:BO5"/>
-    <mergeCell ref="BP5:BS5"/>
-    <mergeCell ref="BT5:BW5"/>
-    <mergeCell ref="AQ1:BW1"/>
-    <mergeCell ref="CB4:CG4"/>
-    <mergeCell ref="BX1:CR1"/>
-    <mergeCell ref="CS1:DM1"/>
-    <mergeCell ref="DV5:DY5"/>
-    <mergeCell ref="AV5:AY5"/>
-    <mergeCell ref="AZ5:BC5"/>
-    <mergeCell ref="BD5:BG5"/>
-    <mergeCell ref="BH5:BK5"/>
-    <mergeCell ref="CI4:CR4"/>
-    <mergeCell ref="DQ5:DR5"/>
-    <mergeCell ref="AQ5:AU5"/>
+    <mergeCell ref="DN6:DR6"/>
+    <mergeCell ref="DN7:DS7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="X4" r:id="rId1" xr:uid="{33A4BD0C-7A19-4C88-AF60-902623A24589}"/>
@@ -3902,15 +3900,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000BCF930048F2A84190E342D576E507E9" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a5f7dcad46bf03cd06b92fe3a65eb3e5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ede1785e-3bac-4a90-a48c-62cc0231644e" xmlns:ns3="6c5f9a5a-0dad-4595-a39a-6416e9fb7054" xmlns:ns4="83a87e31-bf32-46ab-8e70-9fa18461fa4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="627fd199b21a7508d85a0883525fd0b8" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
@@ -4170,6 +4159,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4182,15 +4180,31 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{844596B9-62AA-44A2-8AEF-70908D01A276}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
+    <ds:schemaRef ds:uri="6c5f9a5a-0dad-4595-a39a-6416e9fb7054"/>
+    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D2572BD-7EE7-4817-BEE4-BB014A85EDEE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{844596B9-62AA-44A2-8AEF-70908D01A276}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
feat: update 24/25 lettings paper form (#2275)
* feat: update 24/25 lettings paper form

* feat: update renewal answer options accordingly

* refactor: remove extra spaces from other

* refactor: reorder field_118 and 119 in 2024 row parser
</commit_message>
<xml_diff>
--- a/public/files/bulk-upload-lettings-template-2024-25.xlsx
+++ b/public/files/bulk-upload-lettings-template-2024-25.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mhclg.sharepoint.com/sites/HousingandplanningandCOREstatistics/Shared Documents/CORE Lettings/01 Annual log changes/2024-25/03 Materials for providers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamuelIvko\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="445" documentId="11_77304B1A9BA1AE53F84EE05360D243E6F58DE18B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D887E7A-65F3-456B-814B-C04A0C5272FB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF79DF4-BB38-4E64-BFB6-0CF3D9A5A4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="24-25 lettings template" sheetId="1" r:id="rId1"/>
@@ -1335,33 +1335,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1371,68 +1344,95 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1655,9 +1655,7 @@
   </sheetPr>
   <dimension ref="A1:EA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="EC5" sqref="EC5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1688,7 +1686,7 @@
     <col min="93" max="93" width="12.81640625" customWidth="1"/>
     <col min="99" max="99" width="13.453125" customWidth="1"/>
     <col min="116" max="116" width="12.54296875" style="1"/>
-    <col min="119" max="119" width="16.453125" customWidth="1"/>
+    <col min="120" max="120" width="16.453125" customWidth="1"/>
     <col min="123" max="123" width="13.453125" customWidth="1"/>
     <col min="126" max="126" width="12.81640625" customWidth="1"/>
   </cols>
@@ -1697,150 +1695,150 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="59" t="s">
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="59"/>
-      <c r="Z1" s="59"/>
-      <c r="AA1" s="59"/>
-      <c r="AB1" s="59"/>
-      <c r="AC1" s="59"/>
-      <c r="AD1" s="59"/>
-      <c r="AE1" s="59"/>
-      <c r="AF1" s="59"/>
-      <c r="AG1" s="59"/>
-      <c r="AH1" s="59"/>
-      <c r="AI1" s="59"/>
-      <c r="AJ1" s="59"/>
-      <c r="AK1" s="60" t="s">
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="53"/>
+      <c r="AB1" s="53"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="53"/>
+      <c r="AF1" s="53"/>
+      <c r="AG1" s="53"/>
+      <c r="AH1" s="53"/>
+      <c r="AI1" s="53"/>
+      <c r="AJ1" s="53"/>
+      <c r="AK1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="60"/>
-      <c r="AM1" s="60"/>
-      <c r="AN1" s="60"/>
-      <c r="AO1" s="60"/>
-      <c r="AP1" s="60"/>
-      <c r="AQ1" s="43" t="s">
+      <c r="AL1" s="54"/>
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="AR1" s="44"/>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="44"/>
-      <c r="AV1" s="44"/>
-      <c r="AW1" s="44"/>
-      <c r="AX1" s="44"/>
-      <c r="AY1" s="44"/>
-      <c r="AZ1" s="44"/>
-      <c r="BA1" s="44"/>
-      <c r="BB1" s="44"/>
-      <c r="BC1" s="44"/>
-      <c r="BD1" s="44"/>
-      <c r="BE1" s="44"/>
-      <c r="BF1" s="44"/>
-      <c r="BG1" s="44"/>
-      <c r="BH1" s="44"/>
-      <c r="BI1" s="44"/>
-      <c r="BJ1" s="44"/>
-      <c r="BK1" s="44"/>
-      <c r="BL1" s="44"/>
-      <c r="BM1" s="44"/>
-      <c r="BN1" s="44"/>
-      <c r="BO1" s="44"/>
-      <c r="BP1" s="44"/>
-      <c r="BQ1" s="44"/>
-      <c r="BR1" s="44"/>
-      <c r="BS1" s="44"/>
-      <c r="BT1" s="44"/>
-      <c r="BU1" s="44"/>
-      <c r="BV1" s="44"/>
-      <c r="BW1" s="45"/>
-      <c r="BX1" s="49" t="s">
+      <c r="AR1" s="63"/>
+      <c r="AS1" s="63"/>
+      <c r="AT1" s="63"/>
+      <c r="AU1" s="63"/>
+      <c r="AV1" s="63"/>
+      <c r="AW1" s="63"/>
+      <c r="AX1" s="63"/>
+      <c r="AY1" s="63"/>
+      <c r="AZ1" s="63"/>
+      <c r="BA1" s="63"/>
+      <c r="BB1" s="63"/>
+      <c r="BC1" s="63"/>
+      <c r="BD1" s="63"/>
+      <c r="BE1" s="63"/>
+      <c r="BF1" s="63"/>
+      <c r="BG1" s="63"/>
+      <c r="BH1" s="63"/>
+      <c r="BI1" s="63"/>
+      <c r="BJ1" s="63"/>
+      <c r="BK1" s="63"/>
+      <c r="BL1" s="63"/>
+      <c r="BM1" s="63"/>
+      <c r="BN1" s="63"/>
+      <c r="BO1" s="63"/>
+      <c r="BP1" s="63"/>
+      <c r="BQ1" s="63"/>
+      <c r="BR1" s="63"/>
+      <c r="BS1" s="63"/>
+      <c r="BT1" s="63"/>
+      <c r="BU1" s="63"/>
+      <c r="BV1" s="63"/>
+      <c r="BW1" s="64"/>
+      <c r="BX1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="BY1" s="50"/>
-      <c r="BZ1" s="50"/>
-      <c r="CA1" s="50"/>
-      <c r="CB1" s="50"/>
-      <c r="CC1" s="50"/>
-      <c r="CD1" s="50"/>
-      <c r="CE1" s="50"/>
-      <c r="CF1" s="50"/>
-      <c r="CG1" s="50"/>
-      <c r="CH1" s="50"/>
-      <c r="CI1" s="50"/>
-      <c r="CJ1" s="50"/>
-      <c r="CK1" s="50"/>
-      <c r="CL1" s="50"/>
-      <c r="CM1" s="50"/>
-      <c r="CN1" s="50"/>
-      <c r="CO1" s="50"/>
-      <c r="CP1" s="50"/>
-      <c r="CQ1" s="50"/>
-      <c r="CR1" s="51"/>
-      <c r="CS1" s="55" t="s">
+      <c r="BY1" s="66"/>
+      <c r="BZ1" s="66"/>
+      <c r="CA1" s="66"/>
+      <c r="CB1" s="66"/>
+      <c r="CC1" s="66"/>
+      <c r="CD1" s="66"/>
+      <c r="CE1" s="66"/>
+      <c r="CF1" s="66"/>
+      <c r="CG1" s="66"/>
+      <c r="CH1" s="66"/>
+      <c r="CI1" s="66"/>
+      <c r="CJ1" s="66"/>
+      <c r="CK1" s="66"/>
+      <c r="CL1" s="66"/>
+      <c r="CM1" s="66"/>
+      <c r="CN1" s="66"/>
+      <c r="CO1" s="66"/>
+      <c r="CP1" s="66"/>
+      <c r="CQ1" s="66"/>
+      <c r="CR1" s="67"/>
+      <c r="CS1" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="CT1" s="56"/>
-      <c r="CU1" s="56"/>
-      <c r="CV1" s="56"/>
-      <c r="CW1" s="56"/>
-      <c r="CX1" s="56"/>
-      <c r="CY1" s="56"/>
-      <c r="CZ1" s="56"/>
-      <c r="DA1" s="56"/>
-      <c r="DB1" s="56"/>
-      <c r="DC1" s="56"/>
-      <c r="DD1" s="56"/>
-      <c r="DE1" s="56"/>
-      <c r="DF1" s="56"/>
-      <c r="DG1" s="56"/>
-      <c r="DH1" s="56"/>
-      <c r="DI1" s="56"/>
-      <c r="DJ1" s="56"/>
-      <c r="DK1" s="56"/>
-      <c r="DL1" s="56"/>
-      <c r="DM1" s="57"/>
-      <c r="DN1" s="37" t="s">
+      <c r="CT1" s="69"/>
+      <c r="CU1" s="69"/>
+      <c r="CV1" s="69"/>
+      <c r="CW1" s="69"/>
+      <c r="CX1" s="69"/>
+      <c r="CY1" s="69"/>
+      <c r="CZ1" s="69"/>
+      <c r="DA1" s="69"/>
+      <c r="DB1" s="69"/>
+      <c r="DC1" s="69"/>
+      <c r="DD1" s="69"/>
+      <c r="DE1" s="69"/>
+      <c r="DF1" s="69"/>
+      <c r="DG1" s="69"/>
+      <c r="DH1" s="69"/>
+      <c r="DI1" s="69"/>
+      <c r="DJ1" s="69"/>
+      <c r="DK1" s="69"/>
+      <c r="DL1" s="69"/>
+      <c r="DM1" s="70"/>
+      <c r="DN1" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="DO1" s="38"/>
-      <c r="DP1" s="38"/>
-      <c r="DQ1" s="38"/>
-      <c r="DR1" s="38"/>
-      <c r="DS1" s="38"/>
-      <c r="DT1" s="38"/>
-      <c r="DU1" s="38"/>
-      <c r="DV1" s="38"/>
-      <c r="DW1" s="38"/>
-      <c r="DX1" s="38"/>
-      <c r="DY1" s="38"/>
-      <c r="DZ1" s="38"/>
-      <c r="EA1" s="39"/>
+      <c r="DO1" s="57"/>
+      <c r="DP1" s="57"/>
+      <c r="DQ1" s="57"/>
+      <c r="DR1" s="57"/>
+      <c r="DS1" s="57"/>
+      <c r="DT1" s="57"/>
+      <c r="DU1" s="57"/>
+      <c r="DV1" s="57"/>
+      <c r="DW1" s="57"/>
+      <c r="DX1" s="57"/>
+      <c r="DY1" s="57"/>
+      <c r="DZ1" s="57"/>
+      <c r="EA1" s="58"/>
     </row>
     <row r="2" spans="1:131" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2198,10 +2196,10 @@
         <v>125</v>
       </c>
       <c r="DO2" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="DP2" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="DP2" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="DQ2" s="4" t="s">
         <v>128</v>
@@ -2306,16 +2304,16 @@
       <c r="AD3" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="AE3" s="63" t="s">
+      <c r="AE3" s="49" t="s">
         <v>155</v>
       </c>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="63" t="s">
+      <c r="AF3" s="50"/>
+      <c r="AG3" s="50"/>
+      <c r="AH3" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="AI3" s="64"/>
-      <c r="AJ3" s="64"/>
+      <c r="AI3" s="50"/>
+      <c r="AJ3" s="50"/>
       <c r="AK3" s="11" t="s">
         <v>157</v>
       </c>
@@ -2492,10 +2490,10 @@
       </c>
       <c r="DM3" s="11"/>
       <c r="DN3" s="11"/>
-      <c r="DO3" s="11" t="s">
+      <c r="DO3" s="11"/>
+      <c r="DP3" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="DP3" s="11"/>
       <c r="DQ3" s="11" t="s">
         <v>184</v>
       </c>
@@ -2530,10 +2528,10 @@
       <c r="A4" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="46" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="70"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="15" t="s">
         <v>195</v>
       </c>
@@ -2576,14 +2574,14 @@
       <c r="Q4" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="R4" s="65" t="s">
+      <c r="R4" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="S4" s="67"/>
-      <c r="T4" s="65" t="s">
+      <c r="S4" s="48"/>
+      <c r="T4" s="45" t="s">
         <v>201</v>
       </c>
-      <c r="U4" s="67"/>
+      <c r="U4" s="48"/>
       <c r="V4" s="15" t="s">
         <v>205</v>
       </c>
@@ -2602,10 +2600,10 @@
       <c r="AA4" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="AB4" s="65" t="s">
+      <c r="AB4" s="45" t="s">
         <v>196</v>
       </c>
-      <c r="AC4" s="67"/>
+      <c r="AC4" s="48"/>
       <c r="AD4" s="15" t="s">
         <v>211</v>
       </c>
@@ -2750,33 +2748,33 @@
       <c r="BY4" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="BZ4" s="46" t="s">
+      <c r="BZ4" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="CA4" s="48"/>
-      <c r="CB4" s="46" t="s">
+      <c r="CA4" s="39"/>
+      <c r="CB4" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="CC4" s="47"/>
-      <c r="CD4" s="47"/>
-      <c r="CE4" s="47"/>
-      <c r="CF4" s="47"/>
-      <c r="CG4" s="48"/>
+      <c r="CC4" s="38"/>
+      <c r="CD4" s="38"/>
+      <c r="CE4" s="38"/>
+      <c r="CF4" s="38"/>
+      <c r="CG4" s="39"/>
       <c r="CH4" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="CI4" s="46" t="s">
+      <c r="CI4" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="CJ4" s="47"/>
-      <c r="CK4" s="47"/>
-      <c r="CL4" s="47"/>
-      <c r="CM4" s="47"/>
-      <c r="CN4" s="47"/>
-      <c r="CO4" s="47"/>
-      <c r="CP4" s="47"/>
-      <c r="CQ4" s="47"/>
-      <c r="CR4" s="48"/>
+      <c r="CJ4" s="38"/>
+      <c r="CK4" s="38"/>
+      <c r="CL4" s="38"/>
+      <c r="CM4" s="38"/>
+      <c r="CN4" s="38"/>
+      <c r="CO4" s="38"/>
+      <c r="CP4" s="38"/>
+      <c r="CQ4" s="38"/>
+      <c r="CR4" s="39"/>
       <c r="CS4" s="17" t="s">
         <v>226</v>
       </c>
@@ -2810,19 +2808,19 @@
       <c r="DC4" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="DD4" s="46" t="s">
+      <c r="DD4" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="DE4" s="47"/>
-      <c r="DF4" s="47"/>
-      <c r="DG4" s="47"/>
-      <c r="DH4" s="48"/>
-      <c r="DI4" s="46" t="s">
+      <c r="DE4" s="38"/>
+      <c r="DF4" s="38"/>
+      <c r="DG4" s="38"/>
+      <c r="DH4" s="39"/>
+      <c r="DI4" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="DJ4" s="47"/>
-      <c r="DK4" s="47"/>
-      <c r="DL4" s="48"/>
+      <c r="DJ4" s="38"/>
+      <c r="DK4" s="38"/>
+      <c r="DL4" s="39"/>
       <c r="DM4" s="17" t="s">
         <v>234</v>
       </c>
@@ -2830,10 +2828,10 @@
         <v>214</v>
       </c>
       <c r="DO4" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="DP4" s="15" t="s">
         <v>235</v>
-      </c>
-      <c r="DP4" s="15" t="s">
-        <v>214</v>
       </c>
       <c r="DQ4" s="15" t="s">
         <v>236</v>
@@ -2847,13 +2845,13 @@
       <c r="DT4" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="DU4" s="46" t="s">
+      <c r="DU4" s="37" t="s">
         <v>240</v>
       </c>
-      <c r="DV4" s="47"/>
-      <c r="DW4" s="47"/>
-      <c r="DX4" s="47"/>
-      <c r="DY4" s="48"/>
+      <c r="DV4" s="38"/>
+      <c r="DW4" s="38"/>
+      <c r="DX4" s="38"/>
+      <c r="DY4" s="39"/>
       <c r="DZ4" s="15" t="s">
         <v>214</v>
       </c>
@@ -2865,10 +2863,10 @@
       <c r="A5" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="45" t="s">
         <v>242</v>
       </c>
-      <c r="C5" s="68"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="15" t="s">
         <v>243</v>
       </c>
@@ -2881,20 +2879,20 @@
       <c r="G5" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="48"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="39"/>
       <c r="M5" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="N5" s="65" t="s">
+      <c r="N5" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="O5" s="68"/>
+      <c r="O5" s="44"/>
       <c r="P5" s="30" t="s">
         <v>242</v>
       </c>
@@ -2913,10 +2911,10 @@
       <c r="U5" s="32" t="s">
         <v>243</v>
       </c>
-      <c r="V5" s="65" t="s">
+      <c r="V5" s="45" t="s">
         <v>247</v>
       </c>
-      <c r="W5" s="68"/>
+      <c r="W5" s="44"/>
       <c r="X5" s="15" t="s">
         <v>248</v>
       </c>
@@ -2926,27 +2924,27 @@
       <c r="Z5" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="AA5" s="65" t="s">
+      <c r="AA5" s="45" t="s">
         <v>248</v>
       </c>
-      <c r="AB5" s="68"/>
-      <c r="AC5" s="68"/>
-      <c r="AD5" s="68"/>
-      <c r="AE5" s="65" t="s">
+      <c r="AB5" s="44"/>
+      <c r="AC5" s="44"/>
+      <c r="AD5" s="44"/>
+      <c r="AE5" s="45" t="s">
         <v>249</v>
       </c>
-      <c r="AF5" s="68"/>
-      <c r="AG5" s="68"/>
-      <c r="AH5" s="65" t="s">
+      <c r="AF5" s="44"/>
+      <c r="AG5" s="44"/>
+      <c r="AH5" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="AI5" s="68"/>
-      <c r="AJ5" s="68"/>
-      <c r="AK5" s="65" t="s">
+      <c r="AI5" s="44"/>
+      <c r="AJ5" s="44"/>
+      <c r="AK5" s="45" t="s">
         <v>242</v>
       </c>
-      <c r="AL5" s="68"/>
-      <c r="AM5" s="68"/>
+      <c r="AL5" s="44"/>
+      <c r="AM5" s="44"/>
       <c r="AN5" s="15" t="s">
         <v>251</v>
       </c>
@@ -2956,55 +2954,55 @@
       <c r="AP5" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="AQ5" s="46" t="s">
+      <c r="AQ5" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="AR5" s="47"/>
-      <c r="AS5" s="47"/>
-      <c r="AT5" s="47"/>
-      <c r="AU5" s="48"/>
-      <c r="AV5" s="40" t="s">
+      <c r="AR5" s="38"/>
+      <c r="AS5" s="38"/>
+      <c r="AT5" s="38"/>
+      <c r="AU5" s="39"/>
+      <c r="AV5" s="59" t="s">
         <v>253</v>
       </c>
-      <c r="AW5" s="41"/>
-      <c r="AX5" s="41"/>
-      <c r="AY5" s="42"/>
-      <c r="AZ5" s="40" t="s">
+      <c r="AW5" s="60"/>
+      <c r="AX5" s="60"/>
+      <c r="AY5" s="61"/>
+      <c r="AZ5" s="59" t="s">
         <v>278</v>
       </c>
-      <c r="BA5" s="41"/>
-      <c r="BB5" s="41"/>
-      <c r="BC5" s="42"/>
-      <c r="BD5" s="40" t="s">
+      <c r="BA5" s="60"/>
+      <c r="BB5" s="60"/>
+      <c r="BC5" s="61"/>
+      <c r="BD5" s="59" t="s">
         <v>254</v>
       </c>
-      <c r="BE5" s="41"/>
-      <c r="BF5" s="41"/>
-      <c r="BG5" s="42"/>
-      <c r="BH5" s="40" t="s">
+      <c r="BE5" s="60"/>
+      <c r="BF5" s="60"/>
+      <c r="BG5" s="61"/>
+      <c r="BH5" s="59" t="s">
         <v>255</v>
       </c>
-      <c r="BI5" s="41"/>
-      <c r="BJ5" s="41"/>
-      <c r="BK5" s="42"/>
-      <c r="BL5" s="40" t="s">
+      <c r="BI5" s="60"/>
+      <c r="BJ5" s="60"/>
+      <c r="BK5" s="61"/>
+      <c r="BL5" s="59" t="s">
         <v>256</v>
       </c>
-      <c r="BM5" s="41"/>
-      <c r="BN5" s="41"/>
-      <c r="BO5" s="42"/>
-      <c r="BP5" s="40" t="s">
+      <c r="BM5" s="60"/>
+      <c r="BN5" s="60"/>
+      <c r="BO5" s="61"/>
+      <c r="BP5" s="59" t="s">
         <v>257</v>
       </c>
-      <c r="BQ5" s="41"/>
-      <c r="BR5" s="41"/>
-      <c r="BS5" s="42"/>
-      <c r="BT5" s="40" t="s">
+      <c r="BQ5" s="60"/>
+      <c r="BR5" s="60"/>
+      <c r="BS5" s="61"/>
+      <c r="BT5" s="59" t="s">
         <v>258</v>
       </c>
-      <c r="BU5" s="41"/>
-      <c r="BV5" s="41"/>
-      <c r="BW5" s="42"/>
+      <c r="BU5" s="60"/>
+      <c r="BV5" s="60"/>
+      <c r="BW5" s="61"/>
       <c r="BX5" s="15" t="s">
         <v>242</v>
       </c>
@@ -3017,31 +3015,31 @@
       <c r="CA5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="CB5" s="46" t="s">
+      <c r="CB5" s="37" t="s">
         <v>261</v>
       </c>
-      <c r="CC5" s="47"/>
-      <c r="CD5" s="47"/>
-      <c r="CE5" s="48"/>
-      <c r="CF5" s="46" t="s">
+      <c r="CC5" s="38"/>
+      <c r="CD5" s="38"/>
+      <c r="CE5" s="39"/>
+      <c r="CF5" s="37" t="s">
         <v>262</v>
       </c>
-      <c r="CG5" s="48"/>
+      <c r="CG5" s="39"/>
       <c r="CH5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="CI5" s="46" t="s">
+      <c r="CI5" s="37" t="s">
         <v>263</v>
       </c>
-      <c r="CJ5" s="47"/>
-      <c r="CK5" s="47"/>
-      <c r="CL5" s="47"/>
-      <c r="CM5" s="47"/>
-      <c r="CN5" s="47"/>
-      <c r="CO5" s="47"/>
-      <c r="CP5" s="47"/>
-      <c r="CQ5" s="47"/>
-      <c r="CR5" s="48"/>
+      <c r="CJ5" s="38"/>
+      <c r="CK5" s="38"/>
+      <c r="CL5" s="38"/>
+      <c r="CM5" s="38"/>
+      <c r="CN5" s="38"/>
+      <c r="CO5" s="38"/>
+      <c r="CP5" s="38"/>
+      <c r="CQ5" s="38"/>
+      <c r="CR5" s="39"/>
       <c r="CS5" s="15" t="s">
         <v>242</v>
       </c>
@@ -3057,47 +3055,47 @@
       <c r="CW5" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="CX5" s="46" t="s">
+      <c r="CX5" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="CY5" s="48"/>
-      <c r="CZ5" s="46" t="s">
+      <c r="CY5" s="39"/>
+      <c r="CZ5" s="37" t="s">
         <v>265</v>
       </c>
-      <c r="DA5" s="48"/>
+      <c r="DA5" s="39"/>
       <c r="DB5" s="15" t="s">
         <v>243</v>
       </c>
       <c r="DC5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="DD5" s="52" t="s">
+      <c r="DD5" s="40" t="s">
         <v>266</v>
       </c>
-      <c r="DE5" s="53"/>
-      <c r="DF5" s="53"/>
-      <c r="DG5" s="53"/>
-      <c r="DH5" s="54"/>
-      <c r="DI5" s="46" t="s">
+      <c r="DE5" s="41"/>
+      <c r="DF5" s="41"/>
+      <c r="DG5" s="41"/>
+      <c r="DH5" s="43"/>
+      <c r="DI5" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="DJ5" s="47"/>
-      <c r="DK5" s="47"/>
-      <c r="DL5" s="48"/>
+      <c r="DJ5" s="38"/>
+      <c r="DK5" s="38"/>
+      <c r="DL5" s="39"/>
       <c r="DM5" s="15" t="s">
         <v>249</v>
       </c>
       <c r="DN5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="DO5" s="46" t="s">
+      <c r="DO5" s="37" t="s">
         <v>267</v>
       </c>
-      <c r="DP5" s="48"/>
-      <c r="DQ5" s="46" t="s">
+      <c r="DP5" s="39"/>
+      <c r="DQ5" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="DR5" s="48"/>
+      <c r="DR5" s="39"/>
       <c r="DS5" s="15" t="s">
         <v>242</v>
       </c>
@@ -3107,12 +3105,12 @@
       <c r="DU5" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="DV5" s="46" t="s">
+      <c r="DV5" s="37" t="s">
         <v>269</v>
       </c>
-      <c r="DW5" s="47"/>
-      <c r="DX5" s="47"/>
-      <c r="DY5" s="48"/>
+      <c r="DW5" s="38"/>
+      <c r="DX5" s="38"/>
+      <c r="DY5" s="39"/>
       <c r="DZ5" s="15" t="s">
         <v>270</v>
       </c>
@@ -3124,137 +3122,137 @@
       <c r="A6" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="61" t="s">
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="42" t="s">
         <v>273</v>
       </c>
-      <c r="G6" s="61"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
       <c r="M6" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="N6" s="65"/>
-      <c r="O6" s="65"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="65" t="s">
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45" t="s">
         <v>275</v>
       </c>
-      <c r="R6" s="68"/>
-      <c r="S6" s="68"/>
-      <c r="T6" s="68"/>
-      <c r="U6" s="68"/>
-      <c r="V6" s="68"/>
-      <c r="W6" s="68"/>
-      <c r="X6" s="68"/>
-      <c r="Y6" s="65"/>
-      <c r="Z6" s="65"/>
-      <c r="AA6" s="65" t="s">
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
+      <c r="U6" s="44"/>
+      <c r="V6" s="44"/>
+      <c r="W6" s="44"/>
+      <c r="X6" s="44"/>
+      <c r="Y6" s="45"/>
+      <c r="Z6" s="45"/>
+      <c r="AA6" s="45" t="s">
         <v>275</v>
       </c>
-      <c r="AB6" s="68"/>
-      <c r="AC6" s="68"/>
-      <c r="AD6" s="68"/>
-      <c r="AE6" s="65"/>
-      <c r="AF6" s="65"/>
-      <c r="AG6" s="65"/>
-      <c r="AH6" s="65"/>
-      <c r="AI6" s="65"/>
-      <c r="AJ6" s="65"/>
-      <c r="AK6" s="65"/>
-      <c r="AL6" s="65"/>
-      <c r="AM6" s="65"/>
-      <c r="AN6" s="65"/>
-      <c r="AO6" s="65"/>
+      <c r="AB6" s="44"/>
+      <c r="AC6" s="44"/>
+      <c r="AD6" s="44"/>
+      <c r="AE6" s="45"/>
+      <c r="AF6" s="45"/>
+      <c r="AG6" s="45"/>
+      <c r="AH6" s="45"/>
+      <c r="AI6" s="45"/>
+      <c r="AJ6" s="45"/>
+      <c r="AK6" s="45"/>
+      <c r="AL6" s="45"/>
+      <c r="AM6" s="45"/>
+      <c r="AN6" s="45"/>
+      <c r="AO6" s="45"/>
       <c r="AP6" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="AQ6" s="46"/>
-      <c r="AR6" s="47"/>
-      <c r="AS6" s="47"/>
-      <c r="AT6" s="47"/>
-      <c r="AU6" s="47"/>
-      <c r="AV6" s="47"/>
-      <c r="AW6" s="47"/>
-      <c r="AX6" s="47"/>
-      <c r="AY6" s="47"/>
-      <c r="AZ6" s="47"/>
-      <c r="BA6" s="47"/>
-      <c r="BB6" s="47"/>
-      <c r="BC6" s="47"/>
-      <c r="BD6" s="47"/>
-      <c r="BE6" s="47"/>
-      <c r="BF6" s="47"/>
-      <c r="BG6" s="47"/>
-      <c r="BH6" s="47"/>
-      <c r="BI6" s="47"/>
-      <c r="BJ6" s="47"/>
-      <c r="BK6" s="47"/>
-      <c r="BL6" s="47"/>
-      <c r="BM6" s="47"/>
-      <c r="BN6" s="47"/>
-      <c r="BO6" s="47"/>
-      <c r="BP6" s="47"/>
-      <c r="BQ6" s="47"/>
-      <c r="BR6" s="47"/>
-      <c r="BS6" s="47"/>
-      <c r="BT6" s="47"/>
-      <c r="BU6" s="47"/>
-      <c r="BV6" s="47"/>
-      <c r="BW6" s="48"/>
-      <c r="BX6" s="46"/>
-      <c r="BY6" s="47"/>
-      <c r="BZ6" s="47"/>
-      <c r="CA6" s="47"/>
-      <c r="CB6" s="47"/>
-      <c r="CC6" s="47"/>
-      <c r="CD6" s="47"/>
-      <c r="CE6" s="47"/>
-      <c r="CF6" s="47"/>
-      <c r="CG6" s="47"/>
-      <c r="CH6" s="47"/>
-      <c r="CI6" s="47"/>
-      <c r="CJ6" s="47"/>
-      <c r="CK6" s="47"/>
-      <c r="CL6" s="47"/>
-      <c r="CM6" s="47"/>
-      <c r="CN6" s="47"/>
-      <c r="CO6" s="47"/>
-      <c r="CP6" s="47"/>
-      <c r="CQ6" s="47"/>
-      <c r="CR6" s="48"/>
-      <c r="CS6" s="46"/>
-      <c r="CT6" s="47"/>
-      <c r="CU6" s="47"/>
-      <c r="CV6" s="47"/>
-      <c r="CW6" s="47"/>
-      <c r="CX6" s="47"/>
-      <c r="CY6" s="47"/>
-      <c r="CZ6" s="47"/>
-      <c r="DA6" s="47"/>
-      <c r="DB6" s="47"/>
-      <c r="DC6" s="47"/>
-      <c r="DD6" s="47"/>
-      <c r="DE6" s="47"/>
-      <c r="DF6" s="47"/>
-      <c r="DG6" s="47"/>
-      <c r="DH6" s="47"/>
-      <c r="DI6" s="47"/>
-      <c r="DJ6" s="47"/>
-      <c r="DK6" s="47"/>
-      <c r="DL6" s="47"/>
-      <c r="DM6" s="48"/>
-      <c r="DN6" s="46"/>
-      <c r="DO6" s="47"/>
-      <c r="DP6" s="47"/>
-      <c r="DQ6" s="47"/>
-      <c r="DR6" s="48"/>
+      <c r="AQ6" s="37"/>
+      <c r="AR6" s="38"/>
+      <c r="AS6" s="38"/>
+      <c r="AT6" s="38"/>
+      <c r="AU6" s="38"/>
+      <c r="AV6" s="38"/>
+      <c r="AW6" s="38"/>
+      <c r="AX6" s="38"/>
+      <c r="AY6" s="38"/>
+      <c r="AZ6" s="38"/>
+      <c r="BA6" s="38"/>
+      <c r="BB6" s="38"/>
+      <c r="BC6" s="38"/>
+      <c r="BD6" s="38"/>
+      <c r="BE6" s="38"/>
+      <c r="BF6" s="38"/>
+      <c r="BG6" s="38"/>
+      <c r="BH6" s="38"/>
+      <c r="BI6" s="38"/>
+      <c r="BJ6" s="38"/>
+      <c r="BK6" s="38"/>
+      <c r="BL6" s="38"/>
+      <c r="BM6" s="38"/>
+      <c r="BN6" s="38"/>
+      <c r="BO6" s="38"/>
+      <c r="BP6" s="38"/>
+      <c r="BQ6" s="38"/>
+      <c r="BR6" s="38"/>
+      <c r="BS6" s="38"/>
+      <c r="BT6" s="38"/>
+      <c r="BU6" s="38"/>
+      <c r="BV6" s="38"/>
+      <c r="BW6" s="39"/>
+      <c r="BX6" s="37"/>
+      <c r="BY6" s="38"/>
+      <c r="BZ6" s="38"/>
+      <c r="CA6" s="38"/>
+      <c r="CB6" s="38"/>
+      <c r="CC6" s="38"/>
+      <c r="CD6" s="38"/>
+      <c r="CE6" s="38"/>
+      <c r="CF6" s="38"/>
+      <c r="CG6" s="38"/>
+      <c r="CH6" s="38"/>
+      <c r="CI6" s="38"/>
+      <c r="CJ6" s="38"/>
+      <c r="CK6" s="38"/>
+      <c r="CL6" s="38"/>
+      <c r="CM6" s="38"/>
+      <c r="CN6" s="38"/>
+      <c r="CO6" s="38"/>
+      <c r="CP6" s="38"/>
+      <c r="CQ6" s="38"/>
+      <c r="CR6" s="39"/>
+      <c r="CS6" s="37"/>
+      <c r="CT6" s="38"/>
+      <c r="CU6" s="38"/>
+      <c r="CV6" s="38"/>
+      <c r="CW6" s="38"/>
+      <c r="CX6" s="38"/>
+      <c r="CY6" s="38"/>
+      <c r="CZ6" s="38"/>
+      <c r="DA6" s="38"/>
+      <c r="DB6" s="38"/>
+      <c r="DC6" s="38"/>
+      <c r="DD6" s="38"/>
+      <c r="DE6" s="38"/>
+      <c r="DF6" s="38"/>
+      <c r="DG6" s="38"/>
+      <c r="DH6" s="38"/>
+      <c r="DI6" s="38"/>
+      <c r="DJ6" s="38"/>
+      <c r="DK6" s="38"/>
+      <c r="DL6" s="38"/>
+      <c r="DM6" s="39"/>
+      <c r="DN6" s="37"/>
+      <c r="DO6" s="38"/>
+      <c r="DP6" s="38"/>
+      <c r="DQ6" s="38"/>
+      <c r="DR6" s="39"/>
       <c r="DS6" s="20" t="s">
         <v>273</v>
       </c>
@@ -3262,12 +3260,12 @@
       <c r="DU6" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="DV6" s="52"/>
-      <c r="DW6" s="53"/>
-      <c r="DX6" s="53"/>
-      <c r="DY6" s="53"/>
-      <c r="DZ6" s="53"/>
-      <c r="EA6" s="54"/>
+      <c r="DV6" s="40"/>
+      <c r="DW6" s="41"/>
+      <c r="DX6" s="41"/>
+      <c r="DY6" s="41"/>
+      <c r="DZ6" s="41"/>
+      <c r="EA6" s="43"/>
     </row>
     <row r="7" spans="1:131" s="35" customFormat="1" ht="23" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -3276,151 +3274,151 @@
       <c r="B7" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61" t="s">
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42" t="s">
         <v>243</v>
       </c>
-      <c r="G7" s="61"/>
+      <c r="G7" s="42"/>
       <c r="H7" s="21"/>
-      <c r="I7" s="61" t="s">
+      <c r="I7" s="42" t="s">
         <v>243</v>
       </c>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="55"/>
       <c r="N7" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="O7" s="52"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="53"/>
-      <c r="T7" s="53"/>
-      <c r="U7" s="54"/>
-      <c r="V7" s="61" t="s">
+      <c r="O7" s="40"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="41"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="43"/>
+      <c r="V7" s="42" t="s">
         <v>243</v>
       </c>
-      <c r="W7" s="61"/>
-      <c r="X7" s="52"/>
-      <c r="Y7" s="53"/>
-      <c r="Z7" s="53"/>
-      <c r="AA7" s="53"/>
-      <c r="AB7" s="53"/>
-      <c r="AC7" s="53"/>
-      <c r="AD7" s="53"/>
-      <c r="AE7" s="53"/>
-      <c r="AF7" s="53"/>
-      <c r="AG7" s="53"/>
-      <c r="AH7" s="53"/>
-      <c r="AI7" s="53"/>
-      <c r="AJ7" s="54"/>
-      <c r="AK7" s="52"/>
-      <c r="AL7" s="53"/>
-      <c r="AM7" s="53"/>
-      <c r="AN7" s="53"/>
-      <c r="AO7" s="53"/>
-      <c r="AP7" s="54"/>
-      <c r="AQ7" s="52" t="s">
+      <c r="W7" s="42"/>
+      <c r="X7" s="40"/>
+      <c r="Y7" s="41"/>
+      <c r="Z7" s="41"/>
+      <c r="AA7" s="41"/>
+      <c r="AB7" s="41"/>
+      <c r="AC7" s="41"/>
+      <c r="AD7" s="41"/>
+      <c r="AE7" s="41"/>
+      <c r="AF7" s="41"/>
+      <c r="AG7" s="41"/>
+      <c r="AH7" s="41"/>
+      <c r="AI7" s="41"/>
+      <c r="AJ7" s="43"/>
+      <c r="AK7" s="40"/>
+      <c r="AL7" s="41"/>
+      <c r="AM7" s="41"/>
+      <c r="AN7" s="41"/>
+      <c r="AO7" s="41"/>
+      <c r="AP7" s="43"/>
+      <c r="AQ7" s="40" t="s">
         <v>243</v>
       </c>
-      <c r="AR7" s="54"/>
-      <c r="AS7" s="52"/>
-      <c r="AT7" s="54"/>
+      <c r="AR7" s="43"/>
+      <c r="AS7" s="40"/>
+      <c r="AT7" s="43"/>
       <c r="AU7" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="AV7" s="52"/>
-      <c r="AW7" s="53"/>
-      <c r="AX7" s="53"/>
-      <c r="AY7" s="53"/>
-      <c r="AZ7" s="53"/>
-      <c r="BA7" s="53"/>
-      <c r="BB7" s="53"/>
-      <c r="BC7" s="53"/>
-      <c r="BD7" s="53"/>
-      <c r="BE7" s="53"/>
-      <c r="BF7" s="53"/>
-      <c r="BG7" s="53"/>
-      <c r="BH7" s="53"/>
-      <c r="BI7" s="53"/>
-      <c r="BJ7" s="53"/>
-      <c r="BK7" s="53"/>
-      <c r="BL7" s="53"/>
-      <c r="BM7" s="53"/>
-      <c r="BN7" s="53"/>
-      <c r="BO7" s="53"/>
-      <c r="BP7" s="53"/>
-      <c r="BQ7" s="53"/>
-      <c r="BR7" s="53"/>
-      <c r="BS7" s="53"/>
-      <c r="BT7" s="53"/>
-      <c r="BU7" s="53"/>
-      <c r="BV7" s="53"/>
-      <c r="BW7" s="54"/>
-      <c r="BX7" s="52"/>
-      <c r="BY7" s="53"/>
-      <c r="BZ7" s="53"/>
-      <c r="CA7" s="53"/>
-      <c r="CB7" s="53"/>
-      <c r="CC7" s="53"/>
-      <c r="CD7" s="53"/>
-      <c r="CE7" s="53"/>
-      <c r="CF7" s="53"/>
-      <c r="CG7" s="53"/>
-      <c r="CH7" s="53"/>
-      <c r="CI7" s="53"/>
-      <c r="CJ7" s="53"/>
-      <c r="CK7" s="53"/>
-      <c r="CL7" s="53"/>
-      <c r="CM7" s="53"/>
-      <c r="CN7" s="53"/>
-      <c r="CO7" s="53"/>
-      <c r="CP7" s="53"/>
-      <c r="CQ7" s="53"/>
-      <c r="CR7" s="54"/>
-      <c r="CS7" s="52"/>
-      <c r="CT7" s="53"/>
-      <c r="CU7" s="53"/>
-      <c r="CV7" s="53"/>
-      <c r="CW7" s="53"/>
-      <c r="CX7" s="53"/>
-      <c r="CY7" s="53"/>
-      <c r="CZ7" s="53"/>
-      <c r="DA7" s="53"/>
-      <c r="DB7" s="53"/>
-      <c r="DC7" s="53"/>
-      <c r="DD7" s="53"/>
-      <c r="DE7" s="53"/>
-      <c r="DF7" s="53"/>
-      <c r="DG7" s="53"/>
-      <c r="DH7" s="53"/>
-      <c r="DI7" s="53"/>
-      <c r="DJ7" s="53"/>
-      <c r="DK7" s="53"/>
-      <c r="DL7" s="53"/>
-      <c r="DM7" s="54"/>
-      <c r="DN7" s="52"/>
-      <c r="DO7" s="53"/>
-      <c r="DP7" s="53"/>
-      <c r="DQ7" s="53"/>
-      <c r="DR7" s="53"/>
-      <c r="DS7" s="54"/>
-      <c r="DT7" s="52" t="s">
+      <c r="AV7" s="40"/>
+      <c r="AW7" s="41"/>
+      <c r="AX7" s="41"/>
+      <c r="AY7" s="41"/>
+      <c r="AZ7" s="41"/>
+      <c r="BA7" s="41"/>
+      <c r="BB7" s="41"/>
+      <c r="BC7" s="41"/>
+      <c r="BD7" s="41"/>
+      <c r="BE7" s="41"/>
+      <c r="BF7" s="41"/>
+      <c r="BG7" s="41"/>
+      <c r="BH7" s="41"/>
+      <c r="BI7" s="41"/>
+      <c r="BJ7" s="41"/>
+      <c r="BK7" s="41"/>
+      <c r="BL7" s="41"/>
+      <c r="BM7" s="41"/>
+      <c r="BN7" s="41"/>
+      <c r="BO7" s="41"/>
+      <c r="BP7" s="41"/>
+      <c r="BQ7" s="41"/>
+      <c r="BR7" s="41"/>
+      <c r="BS7" s="41"/>
+      <c r="BT7" s="41"/>
+      <c r="BU7" s="41"/>
+      <c r="BV7" s="41"/>
+      <c r="BW7" s="43"/>
+      <c r="BX7" s="40"/>
+      <c r="BY7" s="41"/>
+      <c r="BZ7" s="41"/>
+      <c r="CA7" s="41"/>
+      <c r="CB7" s="41"/>
+      <c r="CC7" s="41"/>
+      <c r="CD7" s="41"/>
+      <c r="CE7" s="41"/>
+      <c r="CF7" s="41"/>
+      <c r="CG7" s="41"/>
+      <c r="CH7" s="41"/>
+      <c r="CI7" s="41"/>
+      <c r="CJ7" s="41"/>
+      <c r="CK7" s="41"/>
+      <c r="CL7" s="41"/>
+      <c r="CM7" s="41"/>
+      <c r="CN7" s="41"/>
+      <c r="CO7" s="41"/>
+      <c r="CP7" s="41"/>
+      <c r="CQ7" s="41"/>
+      <c r="CR7" s="43"/>
+      <c r="CS7" s="40"/>
+      <c r="CT7" s="41"/>
+      <c r="CU7" s="41"/>
+      <c r="CV7" s="41"/>
+      <c r="CW7" s="41"/>
+      <c r="CX7" s="41"/>
+      <c r="CY7" s="41"/>
+      <c r="CZ7" s="41"/>
+      <c r="DA7" s="41"/>
+      <c r="DB7" s="41"/>
+      <c r="DC7" s="41"/>
+      <c r="DD7" s="41"/>
+      <c r="DE7" s="41"/>
+      <c r="DF7" s="41"/>
+      <c r="DG7" s="41"/>
+      <c r="DH7" s="41"/>
+      <c r="DI7" s="41"/>
+      <c r="DJ7" s="41"/>
+      <c r="DK7" s="41"/>
+      <c r="DL7" s="41"/>
+      <c r="DM7" s="43"/>
+      <c r="DN7" s="40"/>
+      <c r="DO7" s="41"/>
+      <c r="DP7" s="41"/>
+      <c r="DQ7" s="41"/>
+      <c r="DR7" s="41"/>
+      <c r="DS7" s="43"/>
+      <c r="DT7" s="40" t="s">
         <v>243</v>
       </c>
-      <c r="DU7" s="53"/>
-      <c r="DV7" s="53"/>
-      <c r="DW7" s="53"/>
-      <c r="DX7" s="53"/>
-      <c r="DY7" s="53"/>
-      <c r="DZ7" s="61"/>
-      <c r="EA7" s="61"/>
+      <c r="DU7" s="41"/>
+      <c r="DV7" s="41"/>
+      <c r="DW7" s="41"/>
+      <c r="DX7" s="41"/>
+      <c r="DY7" s="41"/>
+      <c r="DZ7" s="42"/>
+      <c r="EA7" s="42"/>
     </row>
-    <row r="8" spans="1:131" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:131" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>279</v>
       </c>
@@ -3776,10 +3774,10 @@
         <v>117</v>
       </c>
       <c r="DO8" s="17">
+        <v>118</v>
+      </c>
+      <c r="DP8" s="17">
         <v>119</v>
-      </c>
-      <c r="DP8" s="17">
-        <v>118</v>
       </c>
       <c r="DQ8" s="22">
         <v>120</v>
@@ -3817,46 +3815,22 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="DU4:DY4"/>
-    <mergeCell ref="DT7:DY7"/>
-    <mergeCell ref="DZ7:EA7"/>
-    <mergeCell ref="DD4:DH4"/>
-    <mergeCell ref="DI4:DL4"/>
-    <mergeCell ref="DD5:DH5"/>
-    <mergeCell ref="DO5:DP5"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="CZ5:DA5"/>
-    <mergeCell ref="DN6:DR6"/>
-    <mergeCell ref="DN7:DS7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="CB5:CE5"/>
-    <mergeCell ref="CF5:CG5"/>
-    <mergeCell ref="CI5:CR5"/>
-    <mergeCell ref="CX5:CY5"/>
-    <mergeCell ref="AQ6:BW6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="AA5:AD5"/>
-    <mergeCell ref="Q6:X6"/>
-    <mergeCell ref="AA6:AD6"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="BZ4:CA4"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="AE6:AO6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="DN1:EA1"/>
+    <mergeCell ref="BL5:BO5"/>
+    <mergeCell ref="BP5:BS5"/>
+    <mergeCell ref="BT5:BW5"/>
+    <mergeCell ref="AQ1:BW1"/>
+    <mergeCell ref="CB4:CG4"/>
+    <mergeCell ref="BX1:CR1"/>
+    <mergeCell ref="CS1:DM1"/>
+    <mergeCell ref="DV5:DY5"/>
+    <mergeCell ref="AV5:AY5"/>
+    <mergeCell ref="AZ5:BC5"/>
+    <mergeCell ref="BD5:BG5"/>
+    <mergeCell ref="BH5:BK5"/>
+    <mergeCell ref="CI4:CR4"/>
+    <mergeCell ref="DQ5:DR5"/>
+    <mergeCell ref="AQ5:AU5"/>
     <mergeCell ref="B1:P1"/>
     <mergeCell ref="Q1:AJ1"/>
     <mergeCell ref="AK1:AP1"/>
@@ -3873,25 +3847,49 @@
     <mergeCell ref="AV7:BW7"/>
     <mergeCell ref="BX6:CR6"/>
     <mergeCell ref="BX7:CR7"/>
+    <mergeCell ref="BZ4:CA4"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="AE6:AO6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="CZ5:DA5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="CB5:CE5"/>
+    <mergeCell ref="CF5:CG5"/>
+    <mergeCell ref="CI5:CR5"/>
+    <mergeCell ref="CX5:CY5"/>
+    <mergeCell ref="AQ6:BW6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="AA5:AD5"/>
+    <mergeCell ref="Q6:X6"/>
+    <mergeCell ref="AA6:AD6"/>
+    <mergeCell ref="DU4:DY4"/>
+    <mergeCell ref="DT7:DY7"/>
+    <mergeCell ref="DZ7:EA7"/>
+    <mergeCell ref="DD4:DH4"/>
+    <mergeCell ref="DI4:DL4"/>
+    <mergeCell ref="DD5:DH5"/>
+    <mergeCell ref="DO5:DP5"/>
     <mergeCell ref="DI5:DL5"/>
     <mergeCell ref="CS6:DM6"/>
     <mergeCell ref="CS7:DM7"/>
-    <mergeCell ref="DN1:EA1"/>
-    <mergeCell ref="BL5:BO5"/>
-    <mergeCell ref="BP5:BS5"/>
-    <mergeCell ref="BT5:BW5"/>
-    <mergeCell ref="AQ1:BW1"/>
-    <mergeCell ref="CB4:CG4"/>
-    <mergeCell ref="BX1:CR1"/>
-    <mergeCell ref="CS1:DM1"/>
-    <mergeCell ref="DV5:DY5"/>
-    <mergeCell ref="AV5:AY5"/>
-    <mergeCell ref="AZ5:BC5"/>
-    <mergeCell ref="BD5:BG5"/>
-    <mergeCell ref="BH5:BK5"/>
-    <mergeCell ref="CI4:CR4"/>
-    <mergeCell ref="DQ5:DR5"/>
-    <mergeCell ref="AQ5:AU5"/>
+    <mergeCell ref="DN6:DR6"/>
+    <mergeCell ref="DN7:DS7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="X4" r:id="rId1" xr:uid="{33A4BD0C-7A19-4C88-AF60-902623A24589}"/>
@@ -3902,15 +3900,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000BCF930048F2A84190E342D576E507E9" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a5f7dcad46bf03cd06b92fe3a65eb3e5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ede1785e-3bac-4a90-a48c-62cc0231644e" xmlns:ns3="6c5f9a5a-0dad-4595-a39a-6416e9fb7054" xmlns:ns4="83a87e31-bf32-46ab-8e70-9fa18461fa4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="627fd199b21a7508d85a0883525fd0b8" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
@@ -4170,6 +4159,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4182,15 +4180,31 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{844596B9-62AA-44A2-8AEF-70908D01A276}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
+    <ds:schemaRef ds:uri="6c5f9a5a-0dad-4595-a39a-6416e9fb7054"/>
+    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D2572BD-7EE7-4817-BEE4-BB014A85EDEE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{844596B9-62AA-44A2-8AEF-70908D01A276}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Update lettings 24/25 resources
</commit_message>
<xml_diff>
--- a/public/files/bulk-upload-lettings-template-2024-25.xlsx
+++ b/public/files/bulk-upload-lettings-template-2024-25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamuelIvko\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF79DF4-BB38-4E64-BFB6-0CF3D9A5A4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978CC0EC-F1B6-485C-BCB6-65B9FA874100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="283">
   <si>
     <t>Section</t>
   </si>
@@ -898,13 +898,7 @@
     <t>Yes, if household's income is unknown (if field 118 = 2 or 3)</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes, if rent is charged (if field 125 is not empty) </t>
-  </si>
-  <si>
     <t>Yes, if the household does not pay rent (if field 122 = 1) or if the accommodation is not a care home (if field 124 is empty)</t>
-  </si>
-  <si>
-    <t>Yes, if the household doesn't receive housing benefits, or if it is unknown (if field 120 = 3, 9 or 10)</t>
   </si>
   <si>
     <t>Yes, if the household does not need to pay rent or charges after receiving housing benefits (if field 130 is not 1)</t>
@@ -940,6 +934,15 @@
   <si>
     <t>Location code.
 You can find the location code on the CORE service under 'Schemes', either by searching for the specific location or downloading a csv.</t>
+  </si>
+  <si>
+    <t>Yes, if rent is charged (if field 125 is not empty), or if there is no charge (if field 122 is 1)</t>
+  </si>
+  <si>
+    <t>Yes, if the household doesn't receive housing benefits, or if it is unknown (if field 120 = 3, 9 or 10), or if there are no charges (if field 122 = 1)</t>
+  </si>
+  <si>
+    <t>Yes, if there are no charges (if field 122 = 1)</t>
   </si>
 </sst>
 </file>
@@ -1335,6 +1338,33 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1344,24 +1374,63 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1369,72 +1438,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1695,150 +1698,150 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="53" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="54" t="s">
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
+      <c r="AF1" s="56"/>
+      <c r="AG1" s="56"/>
+      <c r="AH1" s="56"/>
+      <c r="AI1" s="56"/>
+      <c r="AJ1" s="56"/>
+      <c r="AK1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="62" t="s">
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="AR1" s="63"/>
-      <c r="AS1" s="63"/>
-      <c r="AT1" s="63"/>
-      <c r="AU1" s="63"/>
-      <c r="AV1" s="63"/>
-      <c r="AW1" s="63"/>
-      <c r="AX1" s="63"/>
-      <c r="AY1" s="63"/>
-      <c r="AZ1" s="63"/>
-      <c r="BA1" s="63"/>
-      <c r="BB1" s="63"/>
-      <c r="BC1" s="63"/>
-      <c r="BD1" s="63"/>
-      <c r="BE1" s="63"/>
-      <c r="BF1" s="63"/>
-      <c r="BG1" s="63"/>
-      <c r="BH1" s="63"/>
-      <c r="BI1" s="63"/>
-      <c r="BJ1" s="63"/>
-      <c r="BK1" s="63"/>
-      <c r="BL1" s="63"/>
-      <c r="BM1" s="63"/>
-      <c r="BN1" s="63"/>
-      <c r="BO1" s="63"/>
-      <c r="BP1" s="63"/>
-      <c r="BQ1" s="63"/>
-      <c r="BR1" s="63"/>
-      <c r="BS1" s="63"/>
-      <c r="BT1" s="63"/>
-      <c r="BU1" s="63"/>
-      <c r="BV1" s="63"/>
-      <c r="BW1" s="64"/>
-      <c r="BX1" s="65" t="s">
+      <c r="AR1" s="44"/>
+      <c r="AS1" s="44"/>
+      <c r="AT1" s="44"/>
+      <c r="AU1" s="44"/>
+      <c r="AV1" s="44"/>
+      <c r="AW1" s="44"/>
+      <c r="AX1" s="44"/>
+      <c r="AY1" s="44"/>
+      <c r="AZ1" s="44"/>
+      <c r="BA1" s="44"/>
+      <c r="BB1" s="44"/>
+      <c r="BC1" s="44"/>
+      <c r="BD1" s="44"/>
+      <c r="BE1" s="44"/>
+      <c r="BF1" s="44"/>
+      <c r="BG1" s="44"/>
+      <c r="BH1" s="44"/>
+      <c r="BI1" s="44"/>
+      <c r="BJ1" s="44"/>
+      <c r="BK1" s="44"/>
+      <c r="BL1" s="44"/>
+      <c r="BM1" s="44"/>
+      <c r="BN1" s="44"/>
+      <c r="BO1" s="44"/>
+      <c r="BP1" s="44"/>
+      <c r="BQ1" s="44"/>
+      <c r="BR1" s="44"/>
+      <c r="BS1" s="44"/>
+      <c r="BT1" s="44"/>
+      <c r="BU1" s="44"/>
+      <c r="BV1" s="44"/>
+      <c r="BW1" s="45"/>
+      <c r="BX1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="BY1" s="66"/>
-      <c r="BZ1" s="66"/>
-      <c r="CA1" s="66"/>
-      <c r="CB1" s="66"/>
-      <c r="CC1" s="66"/>
-      <c r="CD1" s="66"/>
-      <c r="CE1" s="66"/>
-      <c r="CF1" s="66"/>
-      <c r="CG1" s="66"/>
-      <c r="CH1" s="66"/>
-      <c r="CI1" s="66"/>
-      <c r="CJ1" s="66"/>
-      <c r="CK1" s="66"/>
-      <c r="CL1" s="66"/>
-      <c r="CM1" s="66"/>
-      <c r="CN1" s="66"/>
-      <c r="CO1" s="66"/>
-      <c r="CP1" s="66"/>
-      <c r="CQ1" s="66"/>
-      <c r="CR1" s="67"/>
-      <c r="CS1" s="68" t="s">
+      <c r="BY1" s="50"/>
+      <c r="BZ1" s="50"/>
+      <c r="CA1" s="50"/>
+      <c r="CB1" s="50"/>
+      <c r="CC1" s="50"/>
+      <c r="CD1" s="50"/>
+      <c r="CE1" s="50"/>
+      <c r="CF1" s="50"/>
+      <c r="CG1" s="50"/>
+      <c r="CH1" s="50"/>
+      <c r="CI1" s="50"/>
+      <c r="CJ1" s="50"/>
+      <c r="CK1" s="50"/>
+      <c r="CL1" s="50"/>
+      <c r="CM1" s="50"/>
+      <c r="CN1" s="50"/>
+      <c r="CO1" s="50"/>
+      <c r="CP1" s="50"/>
+      <c r="CQ1" s="50"/>
+      <c r="CR1" s="51"/>
+      <c r="CS1" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="CT1" s="69"/>
-      <c r="CU1" s="69"/>
-      <c r="CV1" s="69"/>
-      <c r="CW1" s="69"/>
-      <c r="CX1" s="69"/>
-      <c r="CY1" s="69"/>
-      <c r="CZ1" s="69"/>
-      <c r="DA1" s="69"/>
-      <c r="DB1" s="69"/>
-      <c r="DC1" s="69"/>
-      <c r="DD1" s="69"/>
-      <c r="DE1" s="69"/>
-      <c r="DF1" s="69"/>
-      <c r="DG1" s="69"/>
-      <c r="DH1" s="69"/>
-      <c r="DI1" s="69"/>
-      <c r="DJ1" s="69"/>
-      <c r="DK1" s="69"/>
-      <c r="DL1" s="69"/>
-      <c r="DM1" s="70"/>
-      <c r="DN1" s="56" t="s">
+      <c r="CT1" s="53"/>
+      <c r="CU1" s="53"/>
+      <c r="CV1" s="53"/>
+      <c r="CW1" s="53"/>
+      <c r="CX1" s="53"/>
+      <c r="CY1" s="53"/>
+      <c r="CZ1" s="53"/>
+      <c r="DA1" s="53"/>
+      <c r="DB1" s="53"/>
+      <c r="DC1" s="53"/>
+      <c r="DD1" s="53"/>
+      <c r="DE1" s="53"/>
+      <c r="DF1" s="53"/>
+      <c r="DG1" s="53"/>
+      <c r="DH1" s="53"/>
+      <c r="DI1" s="53"/>
+      <c r="DJ1" s="53"/>
+      <c r="DK1" s="53"/>
+      <c r="DL1" s="53"/>
+      <c r="DM1" s="54"/>
+      <c r="DN1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="DO1" s="57"/>
-      <c r="DP1" s="57"/>
-      <c r="DQ1" s="57"/>
-      <c r="DR1" s="57"/>
-      <c r="DS1" s="57"/>
-      <c r="DT1" s="57"/>
-      <c r="DU1" s="57"/>
-      <c r="DV1" s="57"/>
-      <c r="DW1" s="57"/>
-      <c r="DX1" s="57"/>
-      <c r="DY1" s="57"/>
-      <c r="DZ1" s="57"/>
-      <c r="EA1" s="58"/>
+      <c r="DO1" s="38"/>
+      <c r="DP1" s="38"/>
+      <c r="DQ1" s="38"/>
+      <c r="DR1" s="38"/>
+      <c r="DS1" s="38"/>
+      <c r="DT1" s="38"/>
+      <c r="DU1" s="38"/>
+      <c r="DV1" s="38"/>
+      <c r="DW1" s="38"/>
+      <c r="DX1" s="38"/>
+      <c r="DY1" s="38"/>
+      <c r="DZ1" s="38"/>
+      <c r="EA1" s="39"/>
     </row>
     <row r="2" spans="1:131" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2252,10 +2255,10 @@
         <v>143</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>144</v>
@@ -2302,18 +2305,18 @@
         <v>154</v>
       </c>
       <c r="AD3" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="AE3" s="49" t="s">
+        <v>275</v>
+      </c>
+      <c r="AE3" s="63" t="s">
         <v>155</v>
       </c>
-      <c r="AF3" s="50"/>
-      <c r="AG3" s="50"/>
-      <c r="AH3" s="49" t="s">
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="AI3" s="50"/>
-      <c r="AJ3" s="50"/>
+      <c r="AI3" s="64"/>
+      <c r="AJ3" s="64"/>
       <c r="AK3" s="11" t="s">
         <v>157</v>
       </c>
@@ -2528,10 +2531,10 @@
       <c r="A4" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="68" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="47"/>
+      <c r="C4" s="69"/>
       <c r="D4" s="15" t="s">
         <v>195</v>
       </c>
@@ -2574,14 +2577,14 @@
       <c r="Q4" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="R4" s="45" t="s">
+      <c r="R4" s="65" t="s">
         <v>194</v>
       </c>
-      <c r="S4" s="48"/>
-      <c r="T4" s="45" t="s">
+      <c r="S4" s="70"/>
+      <c r="T4" s="65" t="s">
         <v>201</v>
       </c>
-      <c r="U4" s="48"/>
+      <c r="U4" s="70"/>
       <c r="V4" s="15" t="s">
         <v>205</v>
       </c>
@@ -2600,10 +2603,10 @@
       <c r="AA4" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="AB4" s="45" t="s">
+      <c r="AB4" s="65" t="s">
         <v>196</v>
       </c>
-      <c r="AC4" s="48"/>
+      <c r="AC4" s="70"/>
       <c r="AD4" s="15" t="s">
         <v>211</v>
       </c>
@@ -2748,33 +2751,33 @@
       <c r="BY4" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="BZ4" s="37" t="s">
+      <c r="BZ4" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="CA4" s="39"/>
-      <c r="CB4" s="37" t="s">
+      <c r="CA4" s="48"/>
+      <c r="CB4" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="CC4" s="38"/>
-      <c r="CD4" s="38"/>
-      <c r="CE4" s="38"/>
-      <c r="CF4" s="38"/>
-      <c r="CG4" s="39"/>
+      <c r="CC4" s="47"/>
+      <c r="CD4" s="47"/>
+      <c r="CE4" s="47"/>
+      <c r="CF4" s="47"/>
+      <c r="CG4" s="48"/>
       <c r="CH4" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="CI4" s="37" t="s">
+      <c r="CI4" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="CJ4" s="38"/>
-      <c r="CK4" s="38"/>
-      <c r="CL4" s="38"/>
-      <c r="CM4" s="38"/>
-      <c r="CN4" s="38"/>
-      <c r="CO4" s="38"/>
-      <c r="CP4" s="38"/>
-      <c r="CQ4" s="38"/>
-      <c r="CR4" s="39"/>
+      <c r="CJ4" s="47"/>
+      <c r="CK4" s="47"/>
+      <c r="CL4" s="47"/>
+      <c r="CM4" s="47"/>
+      <c r="CN4" s="47"/>
+      <c r="CO4" s="47"/>
+      <c r="CP4" s="47"/>
+      <c r="CQ4" s="47"/>
+      <c r="CR4" s="48"/>
       <c r="CS4" s="17" t="s">
         <v>226</v>
       </c>
@@ -2808,19 +2811,19 @@
       <c r="DC4" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="DD4" s="37" t="s">
+      <c r="DD4" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="DE4" s="38"/>
-      <c r="DF4" s="38"/>
-      <c r="DG4" s="38"/>
-      <c r="DH4" s="39"/>
-      <c r="DI4" s="37" t="s">
+      <c r="DE4" s="47"/>
+      <c r="DF4" s="47"/>
+      <c r="DG4" s="47"/>
+      <c r="DH4" s="48"/>
+      <c r="DI4" s="46" t="s">
         <v>196</v>
       </c>
-      <c r="DJ4" s="38"/>
-      <c r="DK4" s="38"/>
-      <c r="DL4" s="39"/>
+      <c r="DJ4" s="47"/>
+      <c r="DK4" s="47"/>
+      <c r="DL4" s="48"/>
       <c r="DM4" s="17" t="s">
         <v>234</v>
       </c>
@@ -2845,13 +2848,13 @@
       <c r="DT4" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="DU4" s="37" t="s">
+      <c r="DU4" s="46" t="s">
         <v>240</v>
       </c>
-      <c r="DV4" s="38"/>
-      <c r="DW4" s="38"/>
-      <c r="DX4" s="38"/>
-      <c r="DY4" s="39"/>
+      <c r="DV4" s="47"/>
+      <c r="DW4" s="47"/>
+      <c r="DX4" s="47"/>
+      <c r="DY4" s="48"/>
       <c r="DZ4" s="15" t="s">
         <v>214</v>
       </c>
@@ -2863,10 +2866,10 @@
       <c r="A5" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="65" t="s">
         <v>242</v>
       </c>
-      <c r="C5" s="44"/>
+      <c r="C5" s="67"/>
       <c r="D5" s="15" t="s">
         <v>243</v>
       </c>
@@ -2879,20 +2882,20 @@
       <c r="G5" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="H5" s="37" t="s">
+      <c r="H5" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="39"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="48"/>
       <c r="M5" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="N5" s="45" t="s">
+      <c r="N5" s="65" t="s">
         <v>243</v>
       </c>
-      <c r="O5" s="44"/>
+      <c r="O5" s="67"/>
       <c r="P5" s="30" t="s">
         <v>242</v>
       </c>
@@ -2911,10 +2914,10 @@
       <c r="U5" s="32" t="s">
         <v>243</v>
       </c>
-      <c r="V5" s="45" t="s">
+      <c r="V5" s="65" t="s">
         <v>247</v>
       </c>
-      <c r="W5" s="44"/>
+      <c r="W5" s="67"/>
       <c r="X5" s="15" t="s">
         <v>248</v>
       </c>
@@ -2924,27 +2927,27 @@
       <c r="Z5" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="AA5" s="45" t="s">
+      <c r="AA5" s="65" t="s">
         <v>248</v>
       </c>
-      <c r="AB5" s="44"/>
-      <c r="AC5" s="44"/>
-      <c r="AD5" s="44"/>
-      <c r="AE5" s="45" t="s">
+      <c r="AB5" s="67"/>
+      <c r="AC5" s="67"/>
+      <c r="AD5" s="67"/>
+      <c r="AE5" s="65" t="s">
         <v>249</v>
       </c>
-      <c r="AF5" s="44"/>
-      <c r="AG5" s="44"/>
-      <c r="AH5" s="45" t="s">
+      <c r="AF5" s="67"/>
+      <c r="AG5" s="67"/>
+      <c r="AH5" s="65" t="s">
         <v>243</v>
       </c>
-      <c r="AI5" s="44"/>
-      <c r="AJ5" s="44"/>
-      <c r="AK5" s="45" t="s">
+      <c r="AI5" s="67"/>
+      <c r="AJ5" s="67"/>
+      <c r="AK5" s="65" t="s">
         <v>242</v>
       </c>
-      <c r="AL5" s="44"/>
-      <c r="AM5" s="44"/>
+      <c r="AL5" s="67"/>
+      <c r="AM5" s="67"/>
       <c r="AN5" s="15" t="s">
         <v>251</v>
       </c>
@@ -2954,55 +2957,55 @@
       <c r="AP5" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="AQ5" s="37" t="s">
+      <c r="AQ5" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="AR5" s="38"/>
-      <c r="AS5" s="38"/>
-      <c r="AT5" s="38"/>
-      <c r="AU5" s="39"/>
-      <c r="AV5" s="59" t="s">
+      <c r="AR5" s="47"/>
+      <c r="AS5" s="47"/>
+      <c r="AT5" s="47"/>
+      <c r="AU5" s="48"/>
+      <c r="AV5" s="40" t="s">
         <v>253</v>
       </c>
-      <c r="AW5" s="60"/>
-      <c r="AX5" s="60"/>
-      <c r="AY5" s="61"/>
-      <c r="AZ5" s="59" t="s">
-        <v>278</v>
-      </c>
-      <c r="BA5" s="60"/>
-      <c r="BB5" s="60"/>
-      <c r="BC5" s="61"/>
-      <c r="BD5" s="59" t="s">
+      <c r="AW5" s="41"/>
+      <c r="AX5" s="41"/>
+      <c r="AY5" s="42"/>
+      <c r="AZ5" s="40" t="s">
+        <v>276</v>
+      </c>
+      <c r="BA5" s="41"/>
+      <c r="BB5" s="41"/>
+      <c r="BC5" s="42"/>
+      <c r="BD5" s="40" t="s">
         <v>254</v>
       </c>
-      <c r="BE5" s="60"/>
-      <c r="BF5" s="60"/>
-      <c r="BG5" s="61"/>
-      <c r="BH5" s="59" t="s">
+      <c r="BE5" s="41"/>
+      <c r="BF5" s="41"/>
+      <c r="BG5" s="42"/>
+      <c r="BH5" s="40" t="s">
         <v>255</v>
       </c>
-      <c r="BI5" s="60"/>
-      <c r="BJ5" s="60"/>
-      <c r="BK5" s="61"/>
-      <c r="BL5" s="59" t="s">
+      <c r="BI5" s="41"/>
+      <c r="BJ5" s="41"/>
+      <c r="BK5" s="42"/>
+      <c r="BL5" s="40" t="s">
         <v>256</v>
       </c>
-      <c r="BM5" s="60"/>
-      <c r="BN5" s="60"/>
-      <c r="BO5" s="61"/>
-      <c r="BP5" s="59" t="s">
+      <c r="BM5" s="41"/>
+      <c r="BN5" s="41"/>
+      <c r="BO5" s="42"/>
+      <c r="BP5" s="40" t="s">
         <v>257</v>
       </c>
-      <c r="BQ5" s="60"/>
-      <c r="BR5" s="60"/>
-      <c r="BS5" s="61"/>
-      <c r="BT5" s="59" t="s">
+      <c r="BQ5" s="41"/>
+      <c r="BR5" s="41"/>
+      <c r="BS5" s="42"/>
+      <c r="BT5" s="40" t="s">
         <v>258</v>
       </c>
-      <c r="BU5" s="60"/>
-      <c r="BV5" s="60"/>
-      <c r="BW5" s="61"/>
+      <c r="BU5" s="41"/>
+      <c r="BV5" s="41"/>
+      <c r="BW5" s="42"/>
       <c r="BX5" s="15" t="s">
         <v>242</v>
       </c>
@@ -3015,31 +3018,31 @@
       <c r="CA5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="CB5" s="37" t="s">
+      <c r="CB5" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="CC5" s="38"/>
-      <c r="CD5" s="38"/>
-      <c r="CE5" s="39"/>
-      <c r="CF5" s="37" t="s">
+      <c r="CC5" s="47"/>
+      <c r="CD5" s="47"/>
+      <c r="CE5" s="48"/>
+      <c r="CF5" s="46" t="s">
         <v>262</v>
       </c>
-      <c r="CG5" s="39"/>
+      <c r="CG5" s="48"/>
       <c r="CH5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="CI5" s="37" t="s">
+      <c r="CI5" s="46" t="s">
         <v>263</v>
       </c>
-      <c r="CJ5" s="38"/>
-      <c r="CK5" s="38"/>
-      <c r="CL5" s="38"/>
-      <c r="CM5" s="38"/>
-      <c r="CN5" s="38"/>
-      <c r="CO5" s="38"/>
-      <c r="CP5" s="38"/>
-      <c r="CQ5" s="38"/>
-      <c r="CR5" s="39"/>
+      <c r="CJ5" s="47"/>
+      <c r="CK5" s="47"/>
+      <c r="CL5" s="47"/>
+      <c r="CM5" s="47"/>
+      <c r="CN5" s="47"/>
+      <c r="CO5" s="47"/>
+      <c r="CP5" s="47"/>
+      <c r="CQ5" s="47"/>
+      <c r="CR5" s="48"/>
       <c r="CS5" s="15" t="s">
         <v>242</v>
       </c>
@@ -3055,372 +3058,372 @@
       <c r="CW5" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="CX5" s="37" t="s">
+      <c r="CX5" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="CY5" s="39"/>
-      <c r="CZ5" s="37" t="s">
+      <c r="CY5" s="48"/>
+      <c r="CZ5" s="46" t="s">
         <v>265</v>
       </c>
-      <c r="DA5" s="39"/>
+      <c r="DA5" s="48"/>
       <c r="DB5" s="15" t="s">
         <v>243</v>
       </c>
       <c r="DC5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="DD5" s="40" t="s">
+      <c r="DD5" s="58" t="s">
         <v>266</v>
       </c>
-      <c r="DE5" s="41"/>
-      <c r="DF5" s="41"/>
-      <c r="DG5" s="41"/>
-      <c r="DH5" s="43"/>
-      <c r="DI5" s="37" t="s">
+      <c r="DE5" s="59"/>
+      <c r="DF5" s="59"/>
+      <c r="DG5" s="59"/>
+      <c r="DH5" s="60"/>
+      <c r="DI5" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="DJ5" s="38"/>
-      <c r="DK5" s="38"/>
-      <c r="DL5" s="39"/>
+      <c r="DJ5" s="47"/>
+      <c r="DK5" s="47"/>
+      <c r="DL5" s="48"/>
       <c r="DM5" s="15" t="s">
         <v>249</v>
       </c>
       <c r="DN5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="DO5" s="37" t="s">
+      <c r="DO5" s="46" t="s">
         <v>267</v>
       </c>
-      <c r="DP5" s="39"/>
-      <c r="DQ5" s="37" t="s">
+      <c r="DP5" s="48"/>
+      <c r="DQ5" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="DR5" s="39"/>
+      <c r="DR5" s="48"/>
       <c r="DS5" s="15" t="s">
         <v>242</v>
       </c>
       <c r="DT5" s="15" t="s">
-        <v>242</v>
+        <v>282</v>
       </c>
       <c r="DU5" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="DV5" s="46" t="s">
         <v>268</v>
       </c>
-      <c r="DV5" s="37" t="s">
+      <c r="DW5" s="47"/>
+      <c r="DX5" s="47"/>
+      <c r="DY5" s="48"/>
+      <c r="DZ5" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="EA5" s="15" t="s">
         <v>269</v>
-      </c>
-      <c r="DW5" s="38"/>
-      <c r="DX5" s="38"/>
-      <c r="DY5" s="39"/>
-      <c r="DZ5" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="EA5" s="15" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:131" s="35" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="61" t="s">
+        <v>271</v>
+      </c>
+      <c r="G6" s="61"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="42" t="s">
+      <c r="N6" s="65"/>
+      <c r="O6" s="65"/>
+      <c r="P6" s="65"/>
+      <c r="Q6" s="65" t="s">
         <v>273</v>
       </c>
-      <c r="G6" s="42"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="15" t="s">
-        <v>274</v>
-      </c>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45" t="s">
-        <v>275</v>
-      </c>
-      <c r="R6" s="44"/>
-      <c r="S6" s="44"/>
-      <c r="T6" s="44"/>
-      <c r="U6" s="44"/>
-      <c r="V6" s="44"/>
-      <c r="W6" s="44"/>
-      <c r="X6" s="44"/>
-      <c r="Y6" s="45"/>
-      <c r="Z6" s="45"/>
-      <c r="AA6" s="45" t="s">
-        <v>275</v>
-      </c>
-      <c r="AB6" s="44"/>
-      <c r="AC6" s="44"/>
-      <c r="AD6" s="44"/>
-      <c r="AE6" s="45"/>
-      <c r="AF6" s="45"/>
-      <c r="AG6" s="45"/>
-      <c r="AH6" s="45"/>
-      <c r="AI6" s="45"/>
-      <c r="AJ6" s="45"/>
-      <c r="AK6" s="45"/>
-      <c r="AL6" s="45"/>
-      <c r="AM6" s="45"/>
-      <c r="AN6" s="45"/>
-      <c r="AO6" s="45"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="67"/>
+      <c r="V6" s="67"/>
+      <c r="W6" s="67"/>
+      <c r="X6" s="67"/>
+      <c r="Y6" s="65"/>
+      <c r="Z6" s="65"/>
+      <c r="AA6" s="65" t="s">
+        <v>273</v>
+      </c>
+      <c r="AB6" s="67"/>
+      <c r="AC6" s="67"/>
+      <c r="AD6" s="67"/>
+      <c r="AE6" s="65"/>
+      <c r="AF6" s="65"/>
+      <c r="AG6" s="65"/>
+      <c r="AH6" s="65"/>
+      <c r="AI6" s="65"/>
+      <c r="AJ6" s="65"/>
+      <c r="AK6" s="65"/>
+      <c r="AL6" s="65"/>
+      <c r="AM6" s="65"/>
+      <c r="AN6" s="65"/>
+      <c r="AO6" s="65"/>
       <c r="AP6" s="15" t="s">
-        <v>273</v>
-      </c>
-      <c r="AQ6" s="37"/>
-      <c r="AR6" s="38"/>
-      <c r="AS6" s="38"/>
-      <c r="AT6" s="38"/>
-      <c r="AU6" s="38"/>
-      <c r="AV6" s="38"/>
-      <c r="AW6" s="38"/>
-      <c r="AX6" s="38"/>
-      <c r="AY6" s="38"/>
-      <c r="AZ6" s="38"/>
-      <c r="BA6" s="38"/>
-      <c r="BB6" s="38"/>
-      <c r="BC6" s="38"/>
-      <c r="BD6" s="38"/>
-      <c r="BE6" s="38"/>
-      <c r="BF6" s="38"/>
-      <c r="BG6" s="38"/>
-      <c r="BH6" s="38"/>
-      <c r="BI6" s="38"/>
-      <c r="BJ6" s="38"/>
-      <c r="BK6" s="38"/>
-      <c r="BL6" s="38"/>
-      <c r="BM6" s="38"/>
-      <c r="BN6" s="38"/>
-      <c r="BO6" s="38"/>
-      <c r="BP6" s="38"/>
-      <c r="BQ6" s="38"/>
-      <c r="BR6" s="38"/>
-      <c r="BS6" s="38"/>
-      <c r="BT6" s="38"/>
-      <c r="BU6" s="38"/>
-      <c r="BV6" s="38"/>
-      <c r="BW6" s="39"/>
-      <c r="BX6" s="37"/>
-      <c r="BY6" s="38"/>
-      <c r="BZ6" s="38"/>
-      <c r="CA6" s="38"/>
-      <c r="CB6" s="38"/>
-      <c r="CC6" s="38"/>
-      <c r="CD6" s="38"/>
-      <c r="CE6" s="38"/>
-      <c r="CF6" s="38"/>
-      <c r="CG6" s="38"/>
-      <c r="CH6" s="38"/>
-      <c r="CI6" s="38"/>
-      <c r="CJ6" s="38"/>
-      <c r="CK6" s="38"/>
-      <c r="CL6" s="38"/>
-      <c r="CM6" s="38"/>
-      <c r="CN6" s="38"/>
-      <c r="CO6" s="38"/>
-      <c r="CP6" s="38"/>
-      <c r="CQ6" s="38"/>
-      <c r="CR6" s="39"/>
-      <c r="CS6" s="37"/>
-      <c r="CT6" s="38"/>
-      <c r="CU6" s="38"/>
-      <c r="CV6" s="38"/>
-      <c r="CW6" s="38"/>
-      <c r="CX6" s="38"/>
-      <c r="CY6" s="38"/>
-      <c r="CZ6" s="38"/>
-      <c r="DA6" s="38"/>
-      <c r="DB6" s="38"/>
-      <c r="DC6" s="38"/>
-      <c r="DD6" s="38"/>
-      <c r="DE6" s="38"/>
-      <c r="DF6" s="38"/>
-      <c r="DG6" s="38"/>
-      <c r="DH6" s="38"/>
-      <c r="DI6" s="38"/>
-      <c r="DJ6" s="38"/>
-      <c r="DK6" s="38"/>
-      <c r="DL6" s="38"/>
-      <c r="DM6" s="39"/>
-      <c r="DN6" s="37"/>
-      <c r="DO6" s="38"/>
-      <c r="DP6" s="38"/>
-      <c r="DQ6" s="38"/>
-      <c r="DR6" s="39"/>
+        <v>271</v>
+      </c>
+      <c r="AQ6" s="46"/>
+      <c r="AR6" s="47"/>
+      <c r="AS6" s="47"/>
+      <c r="AT6" s="47"/>
+      <c r="AU6" s="47"/>
+      <c r="AV6" s="47"/>
+      <c r="AW6" s="47"/>
+      <c r="AX6" s="47"/>
+      <c r="AY6" s="47"/>
+      <c r="AZ6" s="47"/>
+      <c r="BA6" s="47"/>
+      <c r="BB6" s="47"/>
+      <c r="BC6" s="47"/>
+      <c r="BD6" s="47"/>
+      <c r="BE6" s="47"/>
+      <c r="BF6" s="47"/>
+      <c r="BG6" s="47"/>
+      <c r="BH6" s="47"/>
+      <c r="BI6" s="47"/>
+      <c r="BJ6" s="47"/>
+      <c r="BK6" s="47"/>
+      <c r="BL6" s="47"/>
+      <c r="BM6" s="47"/>
+      <c r="BN6" s="47"/>
+      <c r="BO6" s="47"/>
+      <c r="BP6" s="47"/>
+      <c r="BQ6" s="47"/>
+      <c r="BR6" s="47"/>
+      <c r="BS6" s="47"/>
+      <c r="BT6" s="47"/>
+      <c r="BU6" s="47"/>
+      <c r="BV6" s="47"/>
+      <c r="BW6" s="48"/>
+      <c r="BX6" s="46"/>
+      <c r="BY6" s="47"/>
+      <c r="BZ6" s="47"/>
+      <c r="CA6" s="47"/>
+      <c r="CB6" s="47"/>
+      <c r="CC6" s="47"/>
+      <c r="CD6" s="47"/>
+      <c r="CE6" s="47"/>
+      <c r="CF6" s="47"/>
+      <c r="CG6" s="47"/>
+      <c r="CH6" s="47"/>
+      <c r="CI6" s="47"/>
+      <c r="CJ6" s="47"/>
+      <c r="CK6" s="47"/>
+      <c r="CL6" s="47"/>
+      <c r="CM6" s="47"/>
+      <c r="CN6" s="47"/>
+      <c r="CO6" s="47"/>
+      <c r="CP6" s="47"/>
+      <c r="CQ6" s="47"/>
+      <c r="CR6" s="48"/>
+      <c r="CS6" s="46"/>
+      <c r="CT6" s="47"/>
+      <c r="CU6" s="47"/>
+      <c r="CV6" s="47"/>
+      <c r="CW6" s="47"/>
+      <c r="CX6" s="47"/>
+      <c r="CY6" s="47"/>
+      <c r="CZ6" s="47"/>
+      <c r="DA6" s="47"/>
+      <c r="DB6" s="47"/>
+      <c r="DC6" s="47"/>
+      <c r="DD6" s="47"/>
+      <c r="DE6" s="47"/>
+      <c r="DF6" s="47"/>
+      <c r="DG6" s="47"/>
+      <c r="DH6" s="47"/>
+      <c r="DI6" s="47"/>
+      <c r="DJ6" s="47"/>
+      <c r="DK6" s="47"/>
+      <c r="DL6" s="47"/>
+      <c r="DM6" s="48"/>
+      <c r="DN6" s="46"/>
+      <c r="DO6" s="47"/>
+      <c r="DP6" s="47"/>
+      <c r="DQ6" s="47"/>
+      <c r="DR6" s="48"/>
       <c r="DS6" s="20" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="DT6" s="20"/>
       <c r="DU6" s="20" t="s">
-        <v>273</v>
-      </c>
-      <c r="DV6" s="40"/>
-      <c r="DW6" s="41"/>
-      <c r="DX6" s="41"/>
-      <c r="DY6" s="41"/>
-      <c r="DZ6" s="41"/>
-      <c r="EA6" s="43"/>
+        <v>271</v>
+      </c>
+      <c r="DV6" s="58"/>
+      <c r="DW6" s="59"/>
+      <c r="DX6" s="59"/>
+      <c r="DY6" s="59"/>
+      <c r="DZ6" s="59"/>
+      <c r="EA6" s="60"/>
     </row>
     <row r="7" spans="1:131" s="35" customFormat="1" ht="23" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42" t="s">
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61" t="s">
         <v>243</v>
       </c>
-      <c r="G7" s="42"/>
+      <c r="G7" s="61"/>
       <c r="H7" s="21"/>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="61" t="s">
         <v>243</v>
       </c>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="55"/>
-      <c r="M7" s="55"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
       <c r="N7" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="O7" s="40"/>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="41"/>
-      <c r="S7" s="41"/>
-      <c r="T7" s="41"/>
-      <c r="U7" s="43"/>
-      <c r="V7" s="42" t="s">
+      <c r="O7" s="58"/>
+      <c r="P7" s="60"/>
+      <c r="Q7" s="58"/>
+      <c r="R7" s="59"/>
+      <c r="S7" s="59"/>
+      <c r="T7" s="59"/>
+      <c r="U7" s="60"/>
+      <c r="V7" s="61" t="s">
         <v>243</v>
       </c>
-      <c r="W7" s="42"/>
-      <c r="X7" s="40"/>
-      <c r="Y7" s="41"/>
-      <c r="Z7" s="41"/>
-      <c r="AA7" s="41"/>
-      <c r="AB7" s="41"/>
-      <c r="AC7" s="41"/>
-      <c r="AD7" s="41"/>
-      <c r="AE7" s="41"/>
-      <c r="AF7" s="41"/>
-      <c r="AG7" s="41"/>
-      <c r="AH7" s="41"/>
-      <c r="AI7" s="41"/>
-      <c r="AJ7" s="43"/>
-      <c r="AK7" s="40"/>
-      <c r="AL7" s="41"/>
-      <c r="AM7" s="41"/>
-      <c r="AN7" s="41"/>
-      <c r="AO7" s="41"/>
-      <c r="AP7" s="43"/>
-      <c r="AQ7" s="40" t="s">
+      <c r="W7" s="61"/>
+      <c r="X7" s="58"/>
+      <c r="Y7" s="59"/>
+      <c r="Z7" s="59"/>
+      <c r="AA7" s="59"/>
+      <c r="AB7" s="59"/>
+      <c r="AC7" s="59"/>
+      <c r="AD7" s="59"/>
+      <c r="AE7" s="59"/>
+      <c r="AF7" s="59"/>
+      <c r="AG7" s="59"/>
+      <c r="AH7" s="59"/>
+      <c r="AI7" s="59"/>
+      <c r="AJ7" s="60"/>
+      <c r="AK7" s="58"/>
+      <c r="AL7" s="59"/>
+      <c r="AM7" s="59"/>
+      <c r="AN7" s="59"/>
+      <c r="AO7" s="59"/>
+      <c r="AP7" s="60"/>
+      <c r="AQ7" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="AR7" s="43"/>
-      <c r="AS7" s="40"/>
-      <c r="AT7" s="43"/>
+      <c r="AR7" s="60"/>
+      <c r="AS7" s="58"/>
+      <c r="AT7" s="60"/>
       <c r="AU7" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="AV7" s="40"/>
-      <c r="AW7" s="41"/>
-      <c r="AX7" s="41"/>
-      <c r="AY7" s="41"/>
-      <c r="AZ7" s="41"/>
-      <c r="BA7" s="41"/>
-      <c r="BB7" s="41"/>
-      <c r="BC7" s="41"/>
-      <c r="BD7" s="41"/>
-      <c r="BE7" s="41"/>
-      <c r="BF7" s="41"/>
-      <c r="BG7" s="41"/>
-      <c r="BH7" s="41"/>
-      <c r="BI7" s="41"/>
-      <c r="BJ7" s="41"/>
-      <c r="BK7" s="41"/>
-      <c r="BL7" s="41"/>
-      <c r="BM7" s="41"/>
-      <c r="BN7" s="41"/>
-      <c r="BO7" s="41"/>
-      <c r="BP7" s="41"/>
-      <c r="BQ7" s="41"/>
-      <c r="BR7" s="41"/>
-      <c r="BS7" s="41"/>
-      <c r="BT7" s="41"/>
-      <c r="BU7" s="41"/>
-      <c r="BV7" s="41"/>
-      <c r="BW7" s="43"/>
-      <c r="BX7" s="40"/>
-      <c r="BY7" s="41"/>
-      <c r="BZ7" s="41"/>
-      <c r="CA7" s="41"/>
-      <c r="CB7" s="41"/>
-      <c r="CC7" s="41"/>
-      <c r="CD7" s="41"/>
-      <c r="CE7" s="41"/>
-      <c r="CF7" s="41"/>
-      <c r="CG7" s="41"/>
-      <c r="CH7" s="41"/>
-      <c r="CI7" s="41"/>
-      <c r="CJ7" s="41"/>
-      <c r="CK7" s="41"/>
-      <c r="CL7" s="41"/>
-      <c r="CM7" s="41"/>
-      <c r="CN7" s="41"/>
-      <c r="CO7" s="41"/>
-      <c r="CP7" s="41"/>
-      <c r="CQ7" s="41"/>
-      <c r="CR7" s="43"/>
-      <c r="CS7" s="40"/>
-      <c r="CT7" s="41"/>
-      <c r="CU7" s="41"/>
-      <c r="CV7" s="41"/>
-      <c r="CW7" s="41"/>
-      <c r="CX7" s="41"/>
-      <c r="CY7" s="41"/>
-      <c r="CZ7" s="41"/>
-      <c r="DA7" s="41"/>
-      <c r="DB7" s="41"/>
-      <c r="DC7" s="41"/>
-      <c r="DD7" s="41"/>
-      <c r="DE7" s="41"/>
-      <c r="DF7" s="41"/>
-      <c r="DG7" s="41"/>
-      <c r="DH7" s="41"/>
-      <c r="DI7" s="41"/>
-      <c r="DJ7" s="41"/>
-      <c r="DK7" s="41"/>
-      <c r="DL7" s="41"/>
-      <c r="DM7" s="43"/>
-      <c r="DN7" s="40"/>
-      <c r="DO7" s="41"/>
-      <c r="DP7" s="41"/>
-      <c r="DQ7" s="41"/>
-      <c r="DR7" s="41"/>
-      <c r="DS7" s="43"/>
-      <c r="DT7" s="40" t="s">
+      <c r="AV7" s="58"/>
+      <c r="AW7" s="59"/>
+      <c r="AX7" s="59"/>
+      <c r="AY7" s="59"/>
+      <c r="AZ7" s="59"/>
+      <c r="BA7" s="59"/>
+      <c r="BB7" s="59"/>
+      <c r="BC7" s="59"/>
+      <c r="BD7" s="59"/>
+      <c r="BE7" s="59"/>
+      <c r="BF7" s="59"/>
+      <c r="BG7" s="59"/>
+      <c r="BH7" s="59"/>
+      <c r="BI7" s="59"/>
+      <c r="BJ7" s="59"/>
+      <c r="BK7" s="59"/>
+      <c r="BL7" s="59"/>
+      <c r="BM7" s="59"/>
+      <c r="BN7" s="59"/>
+      <c r="BO7" s="59"/>
+      <c r="BP7" s="59"/>
+      <c r="BQ7" s="59"/>
+      <c r="BR7" s="59"/>
+      <c r="BS7" s="59"/>
+      <c r="BT7" s="59"/>
+      <c r="BU7" s="59"/>
+      <c r="BV7" s="59"/>
+      <c r="BW7" s="60"/>
+      <c r="BX7" s="58"/>
+      <c r="BY7" s="59"/>
+      <c r="BZ7" s="59"/>
+      <c r="CA7" s="59"/>
+      <c r="CB7" s="59"/>
+      <c r="CC7" s="59"/>
+      <c r="CD7" s="59"/>
+      <c r="CE7" s="59"/>
+      <c r="CF7" s="59"/>
+      <c r="CG7" s="59"/>
+      <c r="CH7" s="59"/>
+      <c r="CI7" s="59"/>
+      <c r="CJ7" s="59"/>
+      <c r="CK7" s="59"/>
+      <c r="CL7" s="59"/>
+      <c r="CM7" s="59"/>
+      <c r="CN7" s="59"/>
+      <c r="CO7" s="59"/>
+      <c r="CP7" s="59"/>
+      <c r="CQ7" s="59"/>
+      <c r="CR7" s="60"/>
+      <c r="CS7" s="58"/>
+      <c r="CT7" s="59"/>
+      <c r="CU7" s="59"/>
+      <c r="CV7" s="59"/>
+      <c r="CW7" s="59"/>
+      <c r="CX7" s="59"/>
+      <c r="CY7" s="59"/>
+      <c r="CZ7" s="59"/>
+      <c r="DA7" s="59"/>
+      <c r="DB7" s="59"/>
+      <c r="DC7" s="59"/>
+      <c r="DD7" s="59"/>
+      <c r="DE7" s="59"/>
+      <c r="DF7" s="59"/>
+      <c r="DG7" s="59"/>
+      <c r="DH7" s="59"/>
+      <c r="DI7" s="59"/>
+      <c r="DJ7" s="59"/>
+      <c r="DK7" s="59"/>
+      <c r="DL7" s="59"/>
+      <c r="DM7" s="60"/>
+      <c r="DN7" s="58"/>
+      <c r="DO7" s="59"/>
+      <c r="DP7" s="59"/>
+      <c r="DQ7" s="59"/>
+      <c r="DR7" s="59"/>
+      <c r="DS7" s="60"/>
+      <c r="DT7" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="DU7" s="41"/>
-      <c r="DV7" s="41"/>
-      <c r="DW7" s="41"/>
-      <c r="DX7" s="41"/>
-      <c r="DY7" s="41"/>
-      <c r="DZ7" s="42"/>
-      <c r="EA7" s="42"/>
+      <c r="DU7" s="59"/>
+      <c r="DV7" s="59"/>
+      <c r="DW7" s="59"/>
+      <c r="DX7" s="59"/>
+      <c r="DY7" s="59"/>
+      <c r="DZ7" s="61"/>
+      <c r="EA7" s="61"/>
     </row>
     <row r="8" spans="1:131" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B8" s="17">
         <v>1</v>
@@ -3815,6 +3818,65 @@
     </row>
   </sheetData>
   <mergeCells count="75">
+    <mergeCell ref="DU4:DY4"/>
+    <mergeCell ref="DT7:DY7"/>
+    <mergeCell ref="DZ7:EA7"/>
+    <mergeCell ref="DD4:DH4"/>
+    <mergeCell ref="DI4:DL4"/>
+    <mergeCell ref="DD5:DH5"/>
+    <mergeCell ref="DO5:DP5"/>
+    <mergeCell ref="DI5:DL5"/>
+    <mergeCell ref="CS6:DM6"/>
+    <mergeCell ref="CS7:DM7"/>
+    <mergeCell ref="DN6:DR6"/>
+    <mergeCell ref="DN7:DS7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="CZ5:DA5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="CB5:CE5"/>
+    <mergeCell ref="CF5:CG5"/>
+    <mergeCell ref="CI5:CR5"/>
+    <mergeCell ref="CX5:CY5"/>
+    <mergeCell ref="AQ6:BW6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="AA5:AD5"/>
+    <mergeCell ref="Q6:X6"/>
+    <mergeCell ref="AA6:AD6"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="BZ4:CA4"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="AE6:AO6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="Q1:AJ1"/>
+    <mergeCell ref="AK1:AP1"/>
+    <mergeCell ref="DV6:EA6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="AS7:AT7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="X7:AJ7"/>
+    <mergeCell ref="AK7:AP7"/>
+    <mergeCell ref="AQ7:AR7"/>
+    <mergeCell ref="AV7:BW7"/>
+    <mergeCell ref="BX6:CR6"/>
+    <mergeCell ref="BX7:CR7"/>
     <mergeCell ref="DN1:EA1"/>
     <mergeCell ref="BL5:BO5"/>
     <mergeCell ref="BP5:BS5"/>
@@ -3831,65 +3893,6 @@
     <mergeCell ref="CI4:CR4"/>
     <mergeCell ref="DQ5:DR5"/>
     <mergeCell ref="AQ5:AU5"/>
-    <mergeCell ref="B1:P1"/>
-    <mergeCell ref="Q1:AJ1"/>
-    <mergeCell ref="AK1:AP1"/>
-    <mergeCell ref="DV6:EA6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="AS7:AT7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="X7:AJ7"/>
-    <mergeCell ref="AK7:AP7"/>
-    <mergeCell ref="AQ7:AR7"/>
-    <mergeCell ref="AV7:BW7"/>
-    <mergeCell ref="BX6:CR6"/>
-    <mergeCell ref="BX7:CR7"/>
-    <mergeCell ref="BZ4:CA4"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="AE6:AO6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AK5:AM5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="CZ5:DA5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="CB5:CE5"/>
-    <mergeCell ref="CF5:CG5"/>
-    <mergeCell ref="CI5:CR5"/>
-    <mergeCell ref="CX5:CY5"/>
-    <mergeCell ref="AQ6:BW6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="AA5:AD5"/>
-    <mergeCell ref="Q6:X6"/>
-    <mergeCell ref="AA6:AD6"/>
-    <mergeCell ref="DU4:DY4"/>
-    <mergeCell ref="DT7:DY7"/>
-    <mergeCell ref="DZ7:EA7"/>
-    <mergeCell ref="DD4:DH4"/>
-    <mergeCell ref="DI4:DL4"/>
-    <mergeCell ref="DD5:DH5"/>
-    <mergeCell ref="DO5:DP5"/>
-    <mergeCell ref="DI5:DL5"/>
-    <mergeCell ref="CS6:DM6"/>
-    <mergeCell ref="CS7:DM7"/>
-    <mergeCell ref="DN6:DR6"/>
-    <mergeCell ref="DN7:DS7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="X4" r:id="rId1" xr:uid="{33A4BD0C-7A19-4C88-AF60-902623A24589}"/>
@@ -4160,15 +4163,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
@@ -4177,6 +4171,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4200,14 +4203,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D2572BD-7EE7-4817-BEE4-BB014A85EDEE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3234EB82-E598-4D46-AACB-BAE493D677A7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
@@ -4223,4 +4218,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D2572BD-7EE7-4817-BEE4-BB014A85EDEE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update lettings 24/25 resources (#2303)
</commit_message>
<xml_diff>
--- a/public/files/bulk-upload-lettings-template-2024-25.xlsx
+++ b/public/files/bulk-upload-lettings-template-2024-25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamuelIvko\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF79DF4-BB38-4E64-BFB6-0CF3D9A5A4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978CC0EC-F1B6-485C-BCB6-65B9FA874100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="283">
   <si>
     <t>Section</t>
   </si>
@@ -898,13 +898,7 @@
     <t>Yes, if household's income is unknown (if field 118 = 2 or 3)</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes, if rent is charged (if field 125 is not empty) </t>
-  </si>
-  <si>
     <t>Yes, if the household does not pay rent (if field 122 = 1) or if the accommodation is not a care home (if field 124 is empty)</t>
-  </si>
-  <si>
-    <t>Yes, if the household doesn't receive housing benefits, or if it is unknown (if field 120 = 3, 9 or 10)</t>
   </si>
   <si>
     <t>Yes, if the household does not need to pay rent or charges after receiving housing benefits (if field 130 is not 1)</t>
@@ -940,6 +934,15 @@
   <si>
     <t>Location code.
 You can find the location code on the CORE service under 'Schemes', either by searching for the specific location or downloading a csv.</t>
+  </si>
+  <si>
+    <t>Yes, if rent is charged (if field 125 is not empty), or if there is no charge (if field 122 is 1)</t>
+  </si>
+  <si>
+    <t>Yes, if the household doesn't receive housing benefits, or if it is unknown (if field 120 = 3, 9 or 10), or if there are no charges (if field 122 = 1)</t>
+  </si>
+  <si>
+    <t>Yes, if there are no charges (if field 122 = 1)</t>
   </si>
 </sst>
 </file>
@@ -1335,6 +1338,33 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1344,24 +1374,63 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1369,72 +1438,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1695,150 +1698,150 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="53" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="54" t="s">
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
+      <c r="AF1" s="56"/>
+      <c r="AG1" s="56"/>
+      <c r="AH1" s="56"/>
+      <c r="AI1" s="56"/>
+      <c r="AJ1" s="56"/>
+      <c r="AK1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="62" t="s">
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="AR1" s="63"/>
-      <c r="AS1" s="63"/>
-      <c r="AT1" s="63"/>
-      <c r="AU1" s="63"/>
-      <c r="AV1" s="63"/>
-      <c r="AW1" s="63"/>
-      <c r="AX1" s="63"/>
-      <c r="AY1" s="63"/>
-      <c r="AZ1" s="63"/>
-      <c r="BA1" s="63"/>
-      <c r="BB1" s="63"/>
-      <c r="BC1" s="63"/>
-      <c r="BD1" s="63"/>
-      <c r="BE1" s="63"/>
-      <c r="BF1" s="63"/>
-      <c r="BG1" s="63"/>
-      <c r="BH1" s="63"/>
-      <c r="BI1" s="63"/>
-      <c r="BJ1" s="63"/>
-      <c r="BK1" s="63"/>
-      <c r="BL1" s="63"/>
-      <c r="BM1" s="63"/>
-      <c r="BN1" s="63"/>
-      <c r="BO1" s="63"/>
-      <c r="BP1" s="63"/>
-      <c r="BQ1" s="63"/>
-      <c r="BR1" s="63"/>
-      <c r="BS1" s="63"/>
-      <c r="BT1" s="63"/>
-      <c r="BU1" s="63"/>
-      <c r="BV1" s="63"/>
-      <c r="BW1" s="64"/>
-      <c r="BX1" s="65" t="s">
+      <c r="AR1" s="44"/>
+      <c r="AS1" s="44"/>
+      <c r="AT1" s="44"/>
+      <c r="AU1" s="44"/>
+      <c r="AV1" s="44"/>
+      <c r="AW1" s="44"/>
+      <c r="AX1" s="44"/>
+      <c r="AY1" s="44"/>
+      <c r="AZ1" s="44"/>
+      <c r="BA1" s="44"/>
+      <c r="BB1" s="44"/>
+      <c r="BC1" s="44"/>
+      <c r="BD1" s="44"/>
+      <c r="BE1" s="44"/>
+      <c r="BF1" s="44"/>
+      <c r="BG1" s="44"/>
+      <c r="BH1" s="44"/>
+      <c r="BI1" s="44"/>
+      <c r="BJ1" s="44"/>
+      <c r="BK1" s="44"/>
+      <c r="BL1" s="44"/>
+      <c r="BM1" s="44"/>
+      <c r="BN1" s="44"/>
+      <c r="BO1" s="44"/>
+      <c r="BP1" s="44"/>
+      <c r="BQ1" s="44"/>
+      <c r="BR1" s="44"/>
+      <c r="BS1" s="44"/>
+      <c r="BT1" s="44"/>
+      <c r="BU1" s="44"/>
+      <c r="BV1" s="44"/>
+      <c r="BW1" s="45"/>
+      <c r="BX1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="BY1" s="66"/>
-      <c r="BZ1" s="66"/>
-      <c r="CA1" s="66"/>
-      <c r="CB1" s="66"/>
-      <c r="CC1" s="66"/>
-      <c r="CD1" s="66"/>
-      <c r="CE1" s="66"/>
-      <c r="CF1" s="66"/>
-      <c r="CG1" s="66"/>
-      <c r="CH1" s="66"/>
-      <c r="CI1" s="66"/>
-      <c r="CJ1" s="66"/>
-      <c r="CK1" s="66"/>
-      <c r="CL1" s="66"/>
-      <c r="CM1" s="66"/>
-      <c r="CN1" s="66"/>
-      <c r="CO1" s="66"/>
-      <c r="CP1" s="66"/>
-      <c r="CQ1" s="66"/>
-      <c r="CR1" s="67"/>
-      <c r="CS1" s="68" t="s">
+      <c r="BY1" s="50"/>
+      <c r="BZ1" s="50"/>
+      <c r="CA1" s="50"/>
+      <c r="CB1" s="50"/>
+      <c r="CC1" s="50"/>
+      <c r="CD1" s="50"/>
+      <c r="CE1" s="50"/>
+      <c r="CF1" s="50"/>
+      <c r="CG1" s="50"/>
+      <c r="CH1" s="50"/>
+      <c r="CI1" s="50"/>
+      <c r="CJ1" s="50"/>
+      <c r="CK1" s="50"/>
+      <c r="CL1" s="50"/>
+      <c r="CM1" s="50"/>
+      <c r="CN1" s="50"/>
+      <c r="CO1" s="50"/>
+      <c r="CP1" s="50"/>
+      <c r="CQ1" s="50"/>
+      <c r="CR1" s="51"/>
+      <c r="CS1" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="CT1" s="69"/>
-      <c r="CU1" s="69"/>
-      <c r="CV1" s="69"/>
-      <c r="CW1" s="69"/>
-      <c r="CX1" s="69"/>
-      <c r="CY1" s="69"/>
-      <c r="CZ1" s="69"/>
-      <c r="DA1" s="69"/>
-      <c r="DB1" s="69"/>
-      <c r="DC1" s="69"/>
-      <c r="DD1" s="69"/>
-      <c r="DE1" s="69"/>
-      <c r="DF1" s="69"/>
-      <c r="DG1" s="69"/>
-      <c r="DH1" s="69"/>
-      <c r="DI1" s="69"/>
-      <c r="DJ1" s="69"/>
-      <c r="DK1" s="69"/>
-      <c r="DL1" s="69"/>
-      <c r="DM1" s="70"/>
-      <c r="DN1" s="56" t="s">
+      <c r="CT1" s="53"/>
+      <c r="CU1" s="53"/>
+      <c r="CV1" s="53"/>
+      <c r="CW1" s="53"/>
+      <c r="CX1" s="53"/>
+      <c r="CY1" s="53"/>
+      <c r="CZ1" s="53"/>
+      <c r="DA1" s="53"/>
+      <c r="DB1" s="53"/>
+      <c r="DC1" s="53"/>
+      <c r="DD1" s="53"/>
+      <c r="DE1" s="53"/>
+      <c r="DF1" s="53"/>
+      <c r="DG1" s="53"/>
+      <c r="DH1" s="53"/>
+      <c r="DI1" s="53"/>
+      <c r="DJ1" s="53"/>
+      <c r="DK1" s="53"/>
+      <c r="DL1" s="53"/>
+      <c r="DM1" s="54"/>
+      <c r="DN1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="DO1" s="57"/>
-      <c r="DP1" s="57"/>
-      <c r="DQ1" s="57"/>
-      <c r="DR1" s="57"/>
-      <c r="DS1" s="57"/>
-      <c r="DT1" s="57"/>
-      <c r="DU1" s="57"/>
-      <c r="DV1" s="57"/>
-      <c r="DW1" s="57"/>
-      <c r="DX1" s="57"/>
-      <c r="DY1" s="57"/>
-      <c r="DZ1" s="57"/>
-      <c r="EA1" s="58"/>
+      <c r="DO1" s="38"/>
+      <c r="DP1" s="38"/>
+      <c r="DQ1" s="38"/>
+      <c r="DR1" s="38"/>
+      <c r="DS1" s="38"/>
+      <c r="DT1" s="38"/>
+      <c r="DU1" s="38"/>
+      <c r="DV1" s="38"/>
+      <c r="DW1" s="38"/>
+      <c r="DX1" s="38"/>
+      <c r="DY1" s="38"/>
+      <c r="DZ1" s="38"/>
+      <c r="EA1" s="39"/>
     </row>
     <row r="2" spans="1:131" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2252,10 +2255,10 @@
         <v>143</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>144</v>
@@ -2302,18 +2305,18 @@
         <v>154</v>
       </c>
       <c r="AD3" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="AE3" s="49" t="s">
+        <v>275</v>
+      </c>
+      <c r="AE3" s="63" t="s">
         <v>155</v>
       </c>
-      <c r="AF3" s="50"/>
-      <c r="AG3" s="50"/>
-      <c r="AH3" s="49" t="s">
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="AI3" s="50"/>
-      <c r="AJ3" s="50"/>
+      <c r="AI3" s="64"/>
+      <c r="AJ3" s="64"/>
       <c r="AK3" s="11" t="s">
         <v>157</v>
       </c>
@@ -2528,10 +2531,10 @@
       <c r="A4" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="68" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="47"/>
+      <c r="C4" s="69"/>
       <c r="D4" s="15" t="s">
         <v>195</v>
       </c>
@@ -2574,14 +2577,14 @@
       <c r="Q4" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="R4" s="45" t="s">
+      <c r="R4" s="65" t="s">
         <v>194</v>
       </c>
-      <c r="S4" s="48"/>
-      <c r="T4" s="45" t="s">
+      <c r="S4" s="70"/>
+      <c r="T4" s="65" t="s">
         <v>201</v>
       </c>
-      <c r="U4" s="48"/>
+      <c r="U4" s="70"/>
       <c r="V4" s="15" t="s">
         <v>205</v>
       </c>
@@ -2600,10 +2603,10 @@
       <c r="AA4" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="AB4" s="45" t="s">
+      <c r="AB4" s="65" t="s">
         <v>196</v>
       </c>
-      <c r="AC4" s="48"/>
+      <c r="AC4" s="70"/>
       <c r="AD4" s="15" t="s">
         <v>211</v>
       </c>
@@ -2748,33 +2751,33 @@
       <c r="BY4" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="BZ4" s="37" t="s">
+      <c r="BZ4" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="CA4" s="39"/>
-      <c r="CB4" s="37" t="s">
+      <c r="CA4" s="48"/>
+      <c r="CB4" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="CC4" s="38"/>
-      <c r="CD4" s="38"/>
-      <c r="CE4" s="38"/>
-      <c r="CF4" s="38"/>
-      <c r="CG4" s="39"/>
+      <c r="CC4" s="47"/>
+      <c r="CD4" s="47"/>
+      <c r="CE4" s="47"/>
+      <c r="CF4" s="47"/>
+      <c r="CG4" s="48"/>
       <c r="CH4" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="CI4" s="37" t="s">
+      <c r="CI4" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="CJ4" s="38"/>
-      <c r="CK4" s="38"/>
-      <c r="CL4" s="38"/>
-      <c r="CM4" s="38"/>
-      <c r="CN4" s="38"/>
-      <c r="CO4" s="38"/>
-      <c r="CP4" s="38"/>
-      <c r="CQ4" s="38"/>
-      <c r="CR4" s="39"/>
+      <c r="CJ4" s="47"/>
+      <c r="CK4" s="47"/>
+      <c r="CL4" s="47"/>
+      <c r="CM4" s="47"/>
+      <c r="CN4" s="47"/>
+      <c r="CO4" s="47"/>
+      <c r="CP4" s="47"/>
+      <c r="CQ4" s="47"/>
+      <c r="CR4" s="48"/>
       <c r="CS4" s="17" t="s">
         <v>226</v>
       </c>
@@ -2808,19 +2811,19 @@
       <c r="DC4" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="DD4" s="37" t="s">
+      <c r="DD4" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="DE4" s="38"/>
-      <c r="DF4" s="38"/>
-      <c r="DG4" s="38"/>
-      <c r="DH4" s="39"/>
-      <c r="DI4" s="37" t="s">
+      <c r="DE4" s="47"/>
+      <c r="DF4" s="47"/>
+      <c r="DG4" s="47"/>
+      <c r="DH4" s="48"/>
+      <c r="DI4" s="46" t="s">
         <v>196</v>
       </c>
-      <c r="DJ4" s="38"/>
-      <c r="DK4" s="38"/>
-      <c r="DL4" s="39"/>
+      <c r="DJ4" s="47"/>
+      <c r="DK4" s="47"/>
+      <c r="DL4" s="48"/>
       <c r="DM4" s="17" t="s">
         <v>234</v>
       </c>
@@ -2845,13 +2848,13 @@
       <c r="DT4" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="DU4" s="37" t="s">
+      <c r="DU4" s="46" t="s">
         <v>240</v>
       </c>
-      <c r="DV4" s="38"/>
-      <c r="DW4" s="38"/>
-      <c r="DX4" s="38"/>
-      <c r="DY4" s="39"/>
+      <c r="DV4" s="47"/>
+      <c r="DW4" s="47"/>
+      <c r="DX4" s="47"/>
+      <c r="DY4" s="48"/>
       <c r="DZ4" s="15" t="s">
         <v>214</v>
       </c>
@@ -2863,10 +2866,10 @@
       <c r="A5" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="65" t="s">
         <v>242</v>
       </c>
-      <c r="C5" s="44"/>
+      <c r="C5" s="67"/>
       <c r="D5" s="15" t="s">
         <v>243</v>
       </c>
@@ -2879,20 +2882,20 @@
       <c r="G5" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="H5" s="37" t="s">
+      <c r="H5" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="39"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="48"/>
       <c r="M5" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="N5" s="45" t="s">
+      <c r="N5" s="65" t="s">
         <v>243</v>
       </c>
-      <c r="O5" s="44"/>
+      <c r="O5" s="67"/>
       <c r="P5" s="30" t="s">
         <v>242</v>
       </c>
@@ -2911,10 +2914,10 @@
       <c r="U5" s="32" t="s">
         <v>243</v>
       </c>
-      <c r="V5" s="45" t="s">
+      <c r="V5" s="65" t="s">
         <v>247</v>
       </c>
-      <c r="W5" s="44"/>
+      <c r="W5" s="67"/>
       <c r="X5" s="15" t="s">
         <v>248</v>
       </c>
@@ -2924,27 +2927,27 @@
       <c r="Z5" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="AA5" s="45" t="s">
+      <c r="AA5" s="65" t="s">
         <v>248</v>
       </c>
-      <c r="AB5" s="44"/>
-      <c r="AC5" s="44"/>
-      <c r="AD5" s="44"/>
-      <c r="AE5" s="45" t="s">
+      <c r="AB5" s="67"/>
+      <c r="AC5" s="67"/>
+      <c r="AD5" s="67"/>
+      <c r="AE5" s="65" t="s">
         <v>249</v>
       </c>
-      <c r="AF5" s="44"/>
-      <c r="AG5" s="44"/>
-      <c r="AH5" s="45" t="s">
+      <c r="AF5" s="67"/>
+      <c r="AG5" s="67"/>
+      <c r="AH5" s="65" t="s">
         <v>243</v>
       </c>
-      <c r="AI5" s="44"/>
-      <c r="AJ5" s="44"/>
-      <c r="AK5" s="45" t="s">
+      <c r="AI5" s="67"/>
+      <c r="AJ5" s="67"/>
+      <c r="AK5" s="65" t="s">
         <v>242</v>
       </c>
-      <c r="AL5" s="44"/>
-      <c r="AM5" s="44"/>
+      <c r="AL5" s="67"/>
+      <c r="AM5" s="67"/>
       <c r="AN5" s="15" t="s">
         <v>251</v>
       </c>
@@ -2954,55 +2957,55 @@
       <c r="AP5" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="AQ5" s="37" t="s">
+      <c r="AQ5" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="AR5" s="38"/>
-      <c r="AS5" s="38"/>
-      <c r="AT5" s="38"/>
-      <c r="AU5" s="39"/>
-      <c r="AV5" s="59" t="s">
+      <c r="AR5" s="47"/>
+      <c r="AS5" s="47"/>
+      <c r="AT5" s="47"/>
+      <c r="AU5" s="48"/>
+      <c r="AV5" s="40" t="s">
         <v>253</v>
       </c>
-      <c r="AW5" s="60"/>
-      <c r="AX5" s="60"/>
-      <c r="AY5" s="61"/>
-      <c r="AZ5" s="59" t="s">
-        <v>278</v>
-      </c>
-      <c r="BA5" s="60"/>
-      <c r="BB5" s="60"/>
-      <c r="BC5" s="61"/>
-      <c r="BD5" s="59" t="s">
+      <c r="AW5" s="41"/>
+      <c r="AX5" s="41"/>
+      <c r="AY5" s="42"/>
+      <c r="AZ5" s="40" t="s">
+        <v>276</v>
+      </c>
+      <c r="BA5" s="41"/>
+      <c r="BB5" s="41"/>
+      <c r="BC5" s="42"/>
+      <c r="BD5" s="40" t="s">
         <v>254</v>
       </c>
-      <c r="BE5" s="60"/>
-      <c r="BF5" s="60"/>
-      <c r="BG5" s="61"/>
-      <c r="BH5" s="59" t="s">
+      <c r="BE5" s="41"/>
+      <c r="BF5" s="41"/>
+      <c r="BG5" s="42"/>
+      <c r="BH5" s="40" t="s">
         <v>255</v>
       </c>
-      <c r="BI5" s="60"/>
-      <c r="BJ5" s="60"/>
-      <c r="BK5" s="61"/>
-      <c r="BL5" s="59" t="s">
+      <c r="BI5" s="41"/>
+      <c r="BJ5" s="41"/>
+      <c r="BK5" s="42"/>
+      <c r="BL5" s="40" t="s">
         <v>256</v>
       </c>
-      <c r="BM5" s="60"/>
-      <c r="BN5" s="60"/>
-      <c r="BO5" s="61"/>
-      <c r="BP5" s="59" t="s">
+      <c r="BM5" s="41"/>
+      <c r="BN5" s="41"/>
+      <c r="BO5" s="42"/>
+      <c r="BP5" s="40" t="s">
         <v>257</v>
       </c>
-      <c r="BQ5" s="60"/>
-      <c r="BR5" s="60"/>
-      <c r="BS5" s="61"/>
-      <c r="BT5" s="59" t="s">
+      <c r="BQ5" s="41"/>
+      <c r="BR5" s="41"/>
+      <c r="BS5" s="42"/>
+      <c r="BT5" s="40" t="s">
         <v>258</v>
       </c>
-      <c r="BU5" s="60"/>
-      <c r="BV5" s="60"/>
-      <c r="BW5" s="61"/>
+      <c r="BU5" s="41"/>
+      <c r="BV5" s="41"/>
+      <c r="BW5" s="42"/>
       <c r="BX5" s="15" t="s">
         <v>242</v>
       </c>
@@ -3015,31 +3018,31 @@
       <c r="CA5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="CB5" s="37" t="s">
+      <c r="CB5" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="CC5" s="38"/>
-      <c r="CD5" s="38"/>
-      <c r="CE5" s="39"/>
-      <c r="CF5" s="37" t="s">
+      <c r="CC5" s="47"/>
+      <c r="CD5" s="47"/>
+      <c r="CE5" s="48"/>
+      <c r="CF5" s="46" t="s">
         <v>262</v>
       </c>
-      <c r="CG5" s="39"/>
+      <c r="CG5" s="48"/>
       <c r="CH5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="CI5" s="37" t="s">
+      <c r="CI5" s="46" t="s">
         <v>263</v>
       </c>
-      <c r="CJ5" s="38"/>
-      <c r="CK5" s="38"/>
-      <c r="CL5" s="38"/>
-      <c r="CM5" s="38"/>
-      <c r="CN5" s="38"/>
-      <c r="CO5" s="38"/>
-      <c r="CP5" s="38"/>
-      <c r="CQ5" s="38"/>
-      <c r="CR5" s="39"/>
+      <c r="CJ5" s="47"/>
+      <c r="CK5" s="47"/>
+      <c r="CL5" s="47"/>
+      <c r="CM5" s="47"/>
+      <c r="CN5" s="47"/>
+      <c r="CO5" s="47"/>
+      <c r="CP5" s="47"/>
+      <c r="CQ5" s="47"/>
+      <c r="CR5" s="48"/>
       <c r="CS5" s="15" t="s">
         <v>242</v>
       </c>
@@ -3055,372 +3058,372 @@
       <c r="CW5" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="CX5" s="37" t="s">
+      <c r="CX5" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="CY5" s="39"/>
-      <c r="CZ5" s="37" t="s">
+      <c r="CY5" s="48"/>
+      <c r="CZ5" s="46" t="s">
         <v>265</v>
       </c>
-      <c r="DA5" s="39"/>
+      <c r="DA5" s="48"/>
       <c r="DB5" s="15" t="s">
         <v>243</v>
       </c>
       <c r="DC5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="DD5" s="40" t="s">
+      <c r="DD5" s="58" t="s">
         <v>266</v>
       </c>
-      <c r="DE5" s="41"/>
-      <c r="DF5" s="41"/>
-      <c r="DG5" s="41"/>
-      <c r="DH5" s="43"/>
-      <c r="DI5" s="37" t="s">
+      <c r="DE5" s="59"/>
+      <c r="DF5" s="59"/>
+      <c r="DG5" s="59"/>
+      <c r="DH5" s="60"/>
+      <c r="DI5" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="DJ5" s="38"/>
-      <c r="DK5" s="38"/>
-      <c r="DL5" s="39"/>
+      <c r="DJ5" s="47"/>
+      <c r="DK5" s="47"/>
+      <c r="DL5" s="48"/>
       <c r="DM5" s="15" t="s">
         <v>249</v>
       </c>
       <c r="DN5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="DO5" s="37" t="s">
+      <c r="DO5" s="46" t="s">
         <v>267</v>
       </c>
-      <c r="DP5" s="39"/>
-      <c r="DQ5" s="37" t="s">
+      <c r="DP5" s="48"/>
+      <c r="DQ5" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="DR5" s="39"/>
+      <c r="DR5" s="48"/>
       <c r="DS5" s="15" t="s">
         <v>242</v>
       </c>
       <c r="DT5" s="15" t="s">
-        <v>242</v>
+        <v>282</v>
       </c>
       <c r="DU5" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="DV5" s="46" t="s">
         <v>268</v>
       </c>
-      <c r="DV5" s="37" t="s">
+      <c r="DW5" s="47"/>
+      <c r="DX5" s="47"/>
+      <c r="DY5" s="48"/>
+      <c r="DZ5" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="EA5" s="15" t="s">
         <v>269</v>
-      </c>
-      <c r="DW5" s="38"/>
-      <c r="DX5" s="38"/>
-      <c r="DY5" s="39"/>
-      <c r="DZ5" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="EA5" s="15" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:131" s="35" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="61" t="s">
+        <v>271</v>
+      </c>
+      <c r="G6" s="61"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="42" t="s">
+      <c r="N6" s="65"/>
+      <c r="O6" s="65"/>
+      <c r="P6" s="65"/>
+      <c r="Q6" s="65" t="s">
         <v>273</v>
       </c>
-      <c r="G6" s="42"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="15" t="s">
-        <v>274</v>
-      </c>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45" t="s">
-        <v>275</v>
-      </c>
-      <c r="R6" s="44"/>
-      <c r="S6" s="44"/>
-      <c r="T6" s="44"/>
-      <c r="U6" s="44"/>
-      <c r="V6" s="44"/>
-      <c r="W6" s="44"/>
-      <c r="X6" s="44"/>
-      <c r="Y6" s="45"/>
-      <c r="Z6" s="45"/>
-      <c r="AA6" s="45" t="s">
-        <v>275</v>
-      </c>
-      <c r="AB6" s="44"/>
-      <c r="AC6" s="44"/>
-      <c r="AD6" s="44"/>
-      <c r="AE6" s="45"/>
-      <c r="AF6" s="45"/>
-      <c r="AG6" s="45"/>
-      <c r="AH6" s="45"/>
-      <c r="AI6" s="45"/>
-      <c r="AJ6" s="45"/>
-      <c r="AK6" s="45"/>
-      <c r="AL6" s="45"/>
-      <c r="AM6" s="45"/>
-      <c r="AN6" s="45"/>
-      <c r="AO6" s="45"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="67"/>
+      <c r="V6" s="67"/>
+      <c r="W6" s="67"/>
+      <c r="X6" s="67"/>
+      <c r="Y6" s="65"/>
+      <c r="Z6" s="65"/>
+      <c r="AA6" s="65" t="s">
+        <v>273</v>
+      </c>
+      <c r="AB6" s="67"/>
+      <c r="AC6" s="67"/>
+      <c r="AD6" s="67"/>
+      <c r="AE6" s="65"/>
+      <c r="AF6" s="65"/>
+      <c r="AG6" s="65"/>
+      <c r="AH6" s="65"/>
+      <c r="AI6" s="65"/>
+      <c r="AJ6" s="65"/>
+      <c r="AK6" s="65"/>
+      <c r="AL6" s="65"/>
+      <c r="AM6" s="65"/>
+      <c r="AN6" s="65"/>
+      <c r="AO6" s="65"/>
       <c r="AP6" s="15" t="s">
-        <v>273</v>
-      </c>
-      <c r="AQ6" s="37"/>
-      <c r="AR6" s="38"/>
-      <c r="AS6" s="38"/>
-      <c r="AT6" s="38"/>
-      <c r="AU6" s="38"/>
-      <c r="AV6" s="38"/>
-      <c r="AW6" s="38"/>
-      <c r="AX6" s="38"/>
-      <c r="AY6" s="38"/>
-      <c r="AZ6" s="38"/>
-      <c r="BA6" s="38"/>
-      <c r="BB6" s="38"/>
-      <c r="BC6" s="38"/>
-      <c r="BD6" s="38"/>
-      <c r="BE6" s="38"/>
-      <c r="BF6" s="38"/>
-      <c r="BG6" s="38"/>
-      <c r="BH6" s="38"/>
-      <c r="BI6" s="38"/>
-      <c r="BJ6" s="38"/>
-      <c r="BK6" s="38"/>
-      <c r="BL6" s="38"/>
-      <c r="BM6" s="38"/>
-      <c r="BN6" s="38"/>
-      <c r="BO6" s="38"/>
-      <c r="BP6" s="38"/>
-      <c r="BQ6" s="38"/>
-      <c r="BR6" s="38"/>
-      <c r="BS6" s="38"/>
-      <c r="BT6" s="38"/>
-      <c r="BU6" s="38"/>
-      <c r="BV6" s="38"/>
-      <c r="BW6" s="39"/>
-      <c r="BX6" s="37"/>
-      <c r="BY6" s="38"/>
-      <c r="BZ6" s="38"/>
-      <c r="CA6" s="38"/>
-      <c r="CB6" s="38"/>
-      <c r="CC6" s="38"/>
-      <c r="CD6" s="38"/>
-      <c r="CE6" s="38"/>
-      <c r="CF6" s="38"/>
-      <c r="CG6" s="38"/>
-      <c r="CH6" s="38"/>
-      <c r="CI6" s="38"/>
-      <c r="CJ6" s="38"/>
-      <c r="CK6" s="38"/>
-      <c r="CL6" s="38"/>
-      <c r="CM6" s="38"/>
-      <c r="CN6" s="38"/>
-      <c r="CO6" s="38"/>
-      <c r="CP6" s="38"/>
-      <c r="CQ6" s="38"/>
-      <c r="CR6" s="39"/>
-      <c r="CS6" s="37"/>
-      <c r="CT6" s="38"/>
-      <c r="CU6" s="38"/>
-      <c r="CV6" s="38"/>
-      <c r="CW6" s="38"/>
-      <c r="CX6" s="38"/>
-      <c r="CY6" s="38"/>
-      <c r="CZ6" s="38"/>
-      <c r="DA6" s="38"/>
-      <c r="DB6" s="38"/>
-      <c r="DC6" s="38"/>
-      <c r="DD6" s="38"/>
-      <c r="DE6" s="38"/>
-      <c r="DF6" s="38"/>
-      <c r="DG6" s="38"/>
-      <c r="DH6" s="38"/>
-      <c r="DI6" s="38"/>
-      <c r="DJ6" s="38"/>
-      <c r="DK6" s="38"/>
-      <c r="DL6" s="38"/>
-      <c r="DM6" s="39"/>
-      <c r="DN6" s="37"/>
-      <c r="DO6" s="38"/>
-      <c r="DP6" s="38"/>
-      <c r="DQ6" s="38"/>
-      <c r="DR6" s="39"/>
+        <v>271</v>
+      </c>
+      <c r="AQ6" s="46"/>
+      <c r="AR6" s="47"/>
+      <c r="AS6" s="47"/>
+      <c r="AT6" s="47"/>
+      <c r="AU6" s="47"/>
+      <c r="AV6" s="47"/>
+      <c r="AW6" s="47"/>
+      <c r="AX6" s="47"/>
+      <c r="AY6" s="47"/>
+      <c r="AZ6" s="47"/>
+      <c r="BA6" s="47"/>
+      <c r="BB6" s="47"/>
+      <c r="BC6" s="47"/>
+      <c r="BD6" s="47"/>
+      <c r="BE6" s="47"/>
+      <c r="BF6" s="47"/>
+      <c r="BG6" s="47"/>
+      <c r="BH6" s="47"/>
+      <c r="BI6" s="47"/>
+      <c r="BJ6" s="47"/>
+      <c r="BK6" s="47"/>
+      <c r="BL6" s="47"/>
+      <c r="BM6" s="47"/>
+      <c r="BN6" s="47"/>
+      <c r="BO6" s="47"/>
+      <c r="BP6" s="47"/>
+      <c r="BQ6" s="47"/>
+      <c r="BR6" s="47"/>
+      <c r="BS6" s="47"/>
+      <c r="BT6" s="47"/>
+      <c r="BU6" s="47"/>
+      <c r="BV6" s="47"/>
+      <c r="BW6" s="48"/>
+      <c r="BX6" s="46"/>
+      <c r="BY6" s="47"/>
+      <c r="BZ6" s="47"/>
+      <c r="CA6" s="47"/>
+      <c r="CB6" s="47"/>
+      <c r="CC6" s="47"/>
+      <c r="CD6" s="47"/>
+      <c r="CE6" s="47"/>
+      <c r="CF6" s="47"/>
+      <c r="CG6" s="47"/>
+      <c r="CH6" s="47"/>
+      <c r="CI6" s="47"/>
+      <c r="CJ6" s="47"/>
+      <c r="CK6" s="47"/>
+      <c r="CL6" s="47"/>
+      <c r="CM6" s="47"/>
+      <c r="CN6" s="47"/>
+      <c r="CO6" s="47"/>
+      <c r="CP6" s="47"/>
+      <c r="CQ6" s="47"/>
+      <c r="CR6" s="48"/>
+      <c r="CS6" s="46"/>
+      <c r="CT6" s="47"/>
+      <c r="CU6" s="47"/>
+      <c r="CV6" s="47"/>
+      <c r="CW6" s="47"/>
+      <c r="CX6" s="47"/>
+      <c r="CY6" s="47"/>
+      <c r="CZ6" s="47"/>
+      <c r="DA6" s="47"/>
+      <c r="DB6" s="47"/>
+      <c r="DC6" s="47"/>
+      <c r="DD6" s="47"/>
+      <c r="DE6" s="47"/>
+      <c r="DF6" s="47"/>
+      <c r="DG6" s="47"/>
+      <c r="DH6" s="47"/>
+      <c r="DI6" s="47"/>
+      <c r="DJ6" s="47"/>
+      <c r="DK6" s="47"/>
+      <c r="DL6" s="47"/>
+      <c r="DM6" s="48"/>
+      <c r="DN6" s="46"/>
+      <c r="DO6" s="47"/>
+      <c r="DP6" s="47"/>
+      <c r="DQ6" s="47"/>
+      <c r="DR6" s="48"/>
       <c r="DS6" s="20" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="DT6" s="20"/>
       <c r="DU6" s="20" t="s">
-        <v>273</v>
-      </c>
-      <c r="DV6" s="40"/>
-      <c r="DW6" s="41"/>
-      <c r="DX6" s="41"/>
-      <c r="DY6" s="41"/>
-      <c r="DZ6" s="41"/>
-      <c r="EA6" s="43"/>
+        <v>271</v>
+      </c>
+      <c r="DV6" s="58"/>
+      <c r="DW6" s="59"/>
+      <c r="DX6" s="59"/>
+      <c r="DY6" s="59"/>
+      <c r="DZ6" s="59"/>
+      <c r="EA6" s="60"/>
     </row>
     <row r="7" spans="1:131" s="35" customFormat="1" ht="23" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42" t="s">
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61" t="s">
         <v>243</v>
       </c>
-      <c r="G7" s="42"/>
+      <c r="G7" s="61"/>
       <c r="H7" s="21"/>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="61" t="s">
         <v>243</v>
       </c>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="55"/>
-      <c r="M7" s="55"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
       <c r="N7" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="O7" s="40"/>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="41"/>
-      <c r="S7" s="41"/>
-      <c r="T7" s="41"/>
-      <c r="U7" s="43"/>
-      <c r="V7" s="42" t="s">
+      <c r="O7" s="58"/>
+      <c r="P7" s="60"/>
+      <c r="Q7" s="58"/>
+      <c r="R7" s="59"/>
+      <c r="S7" s="59"/>
+      <c r="T7" s="59"/>
+      <c r="U7" s="60"/>
+      <c r="V7" s="61" t="s">
         <v>243</v>
       </c>
-      <c r="W7" s="42"/>
-      <c r="X7" s="40"/>
-      <c r="Y7" s="41"/>
-      <c r="Z7" s="41"/>
-      <c r="AA7" s="41"/>
-      <c r="AB7" s="41"/>
-      <c r="AC7" s="41"/>
-      <c r="AD7" s="41"/>
-      <c r="AE7" s="41"/>
-      <c r="AF7" s="41"/>
-      <c r="AG7" s="41"/>
-      <c r="AH7" s="41"/>
-      <c r="AI7" s="41"/>
-      <c r="AJ7" s="43"/>
-      <c r="AK7" s="40"/>
-      <c r="AL7" s="41"/>
-      <c r="AM7" s="41"/>
-      <c r="AN7" s="41"/>
-      <c r="AO7" s="41"/>
-      <c r="AP7" s="43"/>
-      <c r="AQ7" s="40" t="s">
+      <c r="W7" s="61"/>
+      <c r="X7" s="58"/>
+      <c r="Y7" s="59"/>
+      <c r="Z7" s="59"/>
+      <c r="AA7" s="59"/>
+      <c r="AB7" s="59"/>
+      <c r="AC7" s="59"/>
+      <c r="AD7" s="59"/>
+      <c r="AE7" s="59"/>
+      <c r="AF7" s="59"/>
+      <c r="AG7" s="59"/>
+      <c r="AH7" s="59"/>
+      <c r="AI7" s="59"/>
+      <c r="AJ7" s="60"/>
+      <c r="AK7" s="58"/>
+      <c r="AL7" s="59"/>
+      <c r="AM7" s="59"/>
+      <c r="AN7" s="59"/>
+      <c r="AO7" s="59"/>
+      <c r="AP7" s="60"/>
+      <c r="AQ7" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="AR7" s="43"/>
-      <c r="AS7" s="40"/>
-      <c r="AT7" s="43"/>
+      <c r="AR7" s="60"/>
+      <c r="AS7" s="58"/>
+      <c r="AT7" s="60"/>
       <c r="AU7" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="AV7" s="40"/>
-      <c r="AW7" s="41"/>
-      <c r="AX7" s="41"/>
-      <c r="AY7" s="41"/>
-      <c r="AZ7" s="41"/>
-      <c r="BA7" s="41"/>
-      <c r="BB7" s="41"/>
-      <c r="BC7" s="41"/>
-      <c r="BD7" s="41"/>
-      <c r="BE7" s="41"/>
-      <c r="BF7" s="41"/>
-      <c r="BG7" s="41"/>
-      <c r="BH7" s="41"/>
-      <c r="BI7" s="41"/>
-      <c r="BJ7" s="41"/>
-      <c r="BK7" s="41"/>
-      <c r="BL7" s="41"/>
-      <c r="BM7" s="41"/>
-      <c r="BN7" s="41"/>
-      <c r="BO7" s="41"/>
-      <c r="BP7" s="41"/>
-      <c r="BQ7" s="41"/>
-      <c r="BR7" s="41"/>
-      <c r="BS7" s="41"/>
-      <c r="BT7" s="41"/>
-      <c r="BU7" s="41"/>
-      <c r="BV7" s="41"/>
-      <c r="BW7" s="43"/>
-      <c r="BX7" s="40"/>
-      <c r="BY7" s="41"/>
-      <c r="BZ7" s="41"/>
-      <c r="CA7" s="41"/>
-      <c r="CB7" s="41"/>
-      <c r="CC7" s="41"/>
-      <c r="CD7" s="41"/>
-      <c r="CE7" s="41"/>
-      <c r="CF7" s="41"/>
-      <c r="CG7" s="41"/>
-      <c r="CH7" s="41"/>
-      <c r="CI7" s="41"/>
-      <c r="CJ7" s="41"/>
-      <c r="CK7" s="41"/>
-      <c r="CL7" s="41"/>
-      <c r="CM7" s="41"/>
-      <c r="CN7" s="41"/>
-      <c r="CO7" s="41"/>
-      <c r="CP7" s="41"/>
-      <c r="CQ7" s="41"/>
-      <c r="CR7" s="43"/>
-      <c r="CS7" s="40"/>
-      <c r="CT7" s="41"/>
-      <c r="CU7" s="41"/>
-      <c r="CV7" s="41"/>
-      <c r="CW7" s="41"/>
-      <c r="CX7" s="41"/>
-      <c r="CY7" s="41"/>
-      <c r="CZ7" s="41"/>
-      <c r="DA7" s="41"/>
-      <c r="DB7" s="41"/>
-      <c r="DC7" s="41"/>
-      <c r="DD7" s="41"/>
-      <c r="DE7" s="41"/>
-      <c r="DF7" s="41"/>
-      <c r="DG7" s="41"/>
-      <c r="DH7" s="41"/>
-      <c r="DI7" s="41"/>
-      <c r="DJ7" s="41"/>
-      <c r="DK7" s="41"/>
-      <c r="DL7" s="41"/>
-      <c r="DM7" s="43"/>
-      <c r="DN7" s="40"/>
-      <c r="DO7" s="41"/>
-      <c r="DP7" s="41"/>
-      <c r="DQ7" s="41"/>
-      <c r="DR7" s="41"/>
-      <c r="DS7" s="43"/>
-      <c r="DT7" s="40" t="s">
+      <c r="AV7" s="58"/>
+      <c r="AW7" s="59"/>
+      <c r="AX7" s="59"/>
+      <c r="AY7" s="59"/>
+      <c r="AZ7" s="59"/>
+      <c r="BA7" s="59"/>
+      <c r="BB7" s="59"/>
+      <c r="BC7" s="59"/>
+      <c r="BD7" s="59"/>
+      <c r="BE7" s="59"/>
+      <c r="BF7" s="59"/>
+      <c r="BG7" s="59"/>
+      <c r="BH7" s="59"/>
+      <c r="BI7" s="59"/>
+      <c r="BJ7" s="59"/>
+      <c r="BK7" s="59"/>
+      <c r="BL7" s="59"/>
+      <c r="BM7" s="59"/>
+      <c r="BN7" s="59"/>
+      <c r="BO7" s="59"/>
+      <c r="BP7" s="59"/>
+      <c r="BQ7" s="59"/>
+      <c r="BR7" s="59"/>
+      <c r="BS7" s="59"/>
+      <c r="BT7" s="59"/>
+      <c r="BU7" s="59"/>
+      <c r="BV7" s="59"/>
+      <c r="BW7" s="60"/>
+      <c r="BX7" s="58"/>
+      <c r="BY7" s="59"/>
+      <c r="BZ7" s="59"/>
+      <c r="CA7" s="59"/>
+      <c r="CB7" s="59"/>
+      <c r="CC7" s="59"/>
+      <c r="CD7" s="59"/>
+      <c r="CE7" s="59"/>
+      <c r="CF7" s="59"/>
+      <c r="CG7" s="59"/>
+      <c r="CH7" s="59"/>
+      <c r="CI7" s="59"/>
+      <c r="CJ7" s="59"/>
+      <c r="CK7" s="59"/>
+      <c r="CL7" s="59"/>
+      <c r="CM7" s="59"/>
+      <c r="CN7" s="59"/>
+      <c r="CO7" s="59"/>
+      <c r="CP7" s="59"/>
+      <c r="CQ7" s="59"/>
+      <c r="CR7" s="60"/>
+      <c r="CS7" s="58"/>
+      <c r="CT7" s="59"/>
+      <c r="CU7" s="59"/>
+      <c r="CV7" s="59"/>
+      <c r="CW7" s="59"/>
+      <c r="CX7" s="59"/>
+      <c r="CY7" s="59"/>
+      <c r="CZ7" s="59"/>
+      <c r="DA7" s="59"/>
+      <c r="DB7" s="59"/>
+      <c r="DC7" s="59"/>
+      <c r="DD7" s="59"/>
+      <c r="DE7" s="59"/>
+      <c r="DF7" s="59"/>
+      <c r="DG7" s="59"/>
+      <c r="DH7" s="59"/>
+      <c r="DI7" s="59"/>
+      <c r="DJ7" s="59"/>
+      <c r="DK7" s="59"/>
+      <c r="DL7" s="59"/>
+      <c r="DM7" s="60"/>
+      <c r="DN7" s="58"/>
+      <c r="DO7" s="59"/>
+      <c r="DP7" s="59"/>
+      <c r="DQ7" s="59"/>
+      <c r="DR7" s="59"/>
+      <c r="DS7" s="60"/>
+      <c r="DT7" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="DU7" s="41"/>
-      <c r="DV7" s="41"/>
-      <c r="DW7" s="41"/>
-      <c r="DX7" s="41"/>
-      <c r="DY7" s="41"/>
-      <c r="DZ7" s="42"/>
-      <c r="EA7" s="42"/>
+      <c r="DU7" s="59"/>
+      <c r="DV7" s="59"/>
+      <c r="DW7" s="59"/>
+      <c r="DX7" s="59"/>
+      <c r="DY7" s="59"/>
+      <c r="DZ7" s="61"/>
+      <c r="EA7" s="61"/>
     </row>
     <row r="8" spans="1:131" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B8" s="17">
         <v>1</v>
@@ -3815,6 +3818,65 @@
     </row>
   </sheetData>
   <mergeCells count="75">
+    <mergeCell ref="DU4:DY4"/>
+    <mergeCell ref="DT7:DY7"/>
+    <mergeCell ref="DZ7:EA7"/>
+    <mergeCell ref="DD4:DH4"/>
+    <mergeCell ref="DI4:DL4"/>
+    <mergeCell ref="DD5:DH5"/>
+    <mergeCell ref="DO5:DP5"/>
+    <mergeCell ref="DI5:DL5"/>
+    <mergeCell ref="CS6:DM6"/>
+    <mergeCell ref="CS7:DM7"/>
+    <mergeCell ref="DN6:DR6"/>
+    <mergeCell ref="DN7:DS7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="CZ5:DA5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="CB5:CE5"/>
+    <mergeCell ref="CF5:CG5"/>
+    <mergeCell ref="CI5:CR5"/>
+    <mergeCell ref="CX5:CY5"/>
+    <mergeCell ref="AQ6:BW6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="AA5:AD5"/>
+    <mergeCell ref="Q6:X6"/>
+    <mergeCell ref="AA6:AD6"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="BZ4:CA4"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="AE6:AO6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="Q1:AJ1"/>
+    <mergeCell ref="AK1:AP1"/>
+    <mergeCell ref="DV6:EA6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="AS7:AT7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="X7:AJ7"/>
+    <mergeCell ref="AK7:AP7"/>
+    <mergeCell ref="AQ7:AR7"/>
+    <mergeCell ref="AV7:BW7"/>
+    <mergeCell ref="BX6:CR6"/>
+    <mergeCell ref="BX7:CR7"/>
     <mergeCell ref="DN1:EA1"/>
     <mergeCell ref="BL5:BO5"/>
     <mergeCell ref="BP5:BS5"/>
@@ -3831,65 +3893,6 @@
     <mergeCell ref="CI4:CR4"/>
     <mergeCell ref="DQ5:DR5"/>
     <mergeCell ref="AQ5:AU5"/>
-    <mergeCell ref="B1:P1"/>
-    <mergeCell ref="Q1:AJ1"/>
-    <mergeCell ref="AK1:AP1"/>
-    <mergeCell ref="DV6:EA6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="AS7:AT7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="X7:AJ7"/>
-    <mergeCell ref="AK7:AP7"/>
-    <mergeCell ref="AQ7:AR7"/>
-    <mergeCell ref="AV7:BW7"/>
-    <mergeCell ref="BX6:CR6"/>
-    <mergeCell ref="BX7:CR7"/>
-    <mergeCell ref="BZ4:CA4"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="AE6:AO6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AK5:AM5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="CZ5:DA5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="CB5:CE5"/>
-    <mergeCell ref="CF5:CG5"/>
-    <mergeCell ref="CI5:CR5"/>
-    <mergeCell ref="CX5:CY5"/>
-    <mergeCell ref="AQ6:BW6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="AA5:AD5"/>
-    <mergeCell ref="Q6:X6"/>
-    <mergeCell ref="AA6:AD6"/>
-    <mergeCell ref="DU4:DY4"/>
-    <mergeCell ref="DT7:DY7"/>
-    <mergeCell ref="DZ7:EA7"/>
-    <mergeCell ref="DD4:DH4"/>
-    <mergeCell ref="DI4:DL4"/>
-    <mergeCell ref="DD5:DH5"/>
-    <mergeCell ref="DO5:DP5"/>
-    <mergeCell ref="DI5:DL5"/>
-    <mergeCell ref="CS6:DM6"/>
-    <mergeCell ref="CS7:DM7"/>
-    <mergeCell ref="DN6:DR6"/>
-    <mergeCell ref="DN7:DS7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="X4" r:id="rId1" xr:uid="{33A4BD0C-7A19-4C88-AF60-902623A24589}"/>
@@ -4160,15 +4163,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
@@ -4177,6 +4171,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4200,14 +4203,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D2572BD-7EE7-4817-BEE4-BB014A85EDEE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3234EB82-E598-4D46-AACB-BAE493D677A7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
@@ -4223,4 +4218,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D2572BD-7EE7-4817-BEE4-BB014A85EDEE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: update resources (#2319)
</commit_message>
<xml_diff>
--- a/public/files/bulk-upload-lettings-template-2024-25.xlsx
+++ b/public/files/bulk-upload-lettings-template-2024-25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamuelIvko\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978CC0EC-F1B6-485C-BCB6-65B9FA874100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF48AE0-8B3F-45D4-B152-45AFD82D442E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1232,7 +1232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1338,31 +1338,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1374,70 +1350,97 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1698,150 +1701,150 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="56" t="s">
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
-      <c r="AF1" s="56"/>
-      <c r="AG1" s="56"/>
-      <c r="AH1" s="56"/>
-      <c r="AI1" s="56"/>
-      <c r="AJ1" s="56"/>
-      <c r="AK1" s="57" t="s">
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="57"/>
-      <c r="AM1" s="57"/>
-      <c r="AN1" s="57"/>
-      <c r="AO1" s="57"/>
-      <c r="AP1" s="57"/>
-      <c r="AQ1" s="43" t="s">
+      <c r="AL1" s="55"/>
+      <c r="AM1" s="55"/>
+      <c r="AN1" s="55"/>
+      <c r="AO1" s="55"/>
+      <c r="AP1" s="55"/>
+      <c r="AQ1" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="AR1" s="44"/>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="44"/>
-      <c r="AV1" s="44"/>
-      <c r="AW1" s="44"/>
-      <c r="AX1" s="44"/>
-      <c r="AY1" s="44"/>
-      <c r="AZ1" s="44"/>
-      <c r="BA1" s="44"/>
-      <c r="BB1" s="44"/>
-      <c r="BC1" s="44"/>
-      <c r="BD1" s="44"/>
-      <c r="BE1" s="44"/>
-      <c r="BF1" s="44"/>
-      <c r="BG1" s="44"/>
-      <c r="BH1" s="44"/>
-      <c r="BI1" s="44"/>
-      <c r="BJ1" s="44"/>
-      <c r="BK1" s="44"/>
-      <c r="BL1" s="44"/>
-      <c r="BM1" s="44"/>
-      <c r="BN1" s="44"/>
-      <c r="BO1" s="44"/>
-      <c r="BP1" s="44"/>
-      <c r="BQ1" s="44"/>
-      <c r="BR1" s="44"/>
-      <c r="BS1" s="44"/>
-      <c r="BT1" s="44"/>
-      <c r="BU1" s="44"/>
-      <c r="BV1" s="44"/>
-      <c r="BW1" s="45"/>
-      <c r="BX1" s="49" t="s">
+      <c r="AR1" s="64"/>
+      <c r="AS1" s="64"/>
+      <c r="AT1" s="64"/>
+      <c r="AU1" s="64"/>
+      <c r="AV1" s="64"/>
+      <c r="AW1" s="64"/>
+      <c r="AX1" s="64"/>
+      <c r="AY1" s="64"/>
+      <c r="AZ1" s="64"/>
+      <c r="BA1" s="64"/>
+      <c r="BB1" s="64"/>
+      <c r="BC1" s="64"/>
+      <c r="BD1" s="64"/>
+      <c r="BE1" s="64"/>
+      <c r="BF1" s="64"/>
+      <c r="BG1" s="64"/>
+      <c r="BH1" s="64"/>
+      <c r="BI1" s="64"/>
+      <c r="BJ1" s="64"/>
+      <c r="BK1" s="64"/>
+      <c r="BL1" s="64"/>
+      <c r="BM1" s="64"/>
+      <c r="BN1" s="64"/>
+      <c r="BO1" s="64"/>
+      <c r="BP1" s="64"/>
+      <c r="BQ1" s="64"/>
+      <c r="BR1" s="64"/>
+      <c r="BS1" s="64"/>
+      <c r="BT1" s="64"/>
+      <c r="BU1" s="64"/>
+      <c r="BV1" s="64"/>
+      <c r="BW1" s="65"/>
+      <c r="BX1" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="BY1" s="50"/>
-      <c r="BZ1" s="50"/>
-      <c r="CA1" s="50"/>
-      <c r="CB1" s="50"/>
-      <c r="CC1" s="50"/>
-      <c r="CD1" s="50"/>
-      <c r="CE1" s="50"/>
-      <c r="CF1" s="50"/>
-      <c r="CG1" s="50"/>
-      <c r="CH1" s="50"/>
-      <c r="CI1" s="50"/>
-      <c r="CJ1" s="50"/>
-      <c r="CK1" s="50"/>
-      <c r="CL1" s="50"/>
-      <c r="CM1" s="50"/>
-      <c r="CN1" s="50"/>
-      <c r="CO1" s="50"/>
-      <c r="CP1" s="50"/>
-      <c r="CQ1" s="50"/>
-      <c r="CR1" s="51"/>
-      <c r="CS1" s="52" t="s">
+      <c r="BY1" s="67"/>
+      <c r="BZ1" s="67"/>
+      <c r="CA1" s="67"/>
+      <c r="CB1" s="67"/>
+      <c r="CC1" s="67"/>
+      <c r="CD1" s="67"/>
+      <c r="CE1" s="67"/>
+      <c r="CF1" s="67"/>
+      <c r="CG1" s="67"/>
+      <c r="CH1" s="67"/>
+      <c r="CI1" s="67"/>
+      <c r="CJ1" s="67"/>
+      <c r="CK1" s="67"/>
+      <c r="CL1" s="67"/>
+      <c r="CM1" s="67"/>
+      <c r="CN1" s="67"/>
+      <c r="CO1" s="67"/>
+      <c r="CP1" s="67"/>
+      <c r="CQ1" s="67"/>
+      <c r="CR1" s="68"/>
+      <c r="CS1" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="CT1" s="53"/>
-      <c r="CU1" s="53"/>
-      <c r="CV1" s="53"/>
-      <c r="CW1" s="53"/>
-      <c r="CX1" s="53"/>
-      <c r="CY1" s="53"/>
-      <c r="CZ1" s="53"/>
-      <c r="DA1" s="53"/>
-      <c r="DB1" s="53"/>
-      <c r="DC1" s="53"/>
-      <c r="DD1" s="53"/>
-      <c r="DE1" s="53"/>
-      <c r="DF1" s="53"/>
-      <c r="DG1" s="53"/>
-      <c r="DH1" s="53"/>
-      <c r="DI1" s="53"/>
-      <c r="DJ1" s="53"/>
-      <c r="DK1" s="53"/>
-      <c r="DL1" s="53"/>
-      <c r="DM1" s="54"/>
-      <c r="DN1" s="37" t="s">
+      <c r="CT1" s="70"/>
+      <c r="CU1" s="70"/>
+      <c r="CV1" s="70"/>
+      <c r="CW1" s="70"/>
+      <c r="CX1" s="70"/>
+      <c r="CY1" s="70"/>
+      <c r="CZ1" s="70"/>
+      <c r="DA1" s="70"/>
+      <c r="DB1" s="70"/>
+      <c r="DC1" s="70"/>
+      <c r="DD1" s="70"/>
+      <c r="DE1" s="70"/>
+      <c r="DF1" s="70"/>
+      <c r="DG1" s="70"/>
+      <c r="DH1" s="70"/>
+      <c r="DI1" s="70"/>
+      <c r="DJ1" s="70"/>
+      <c r="DK1" s="70"/>
+      <c r="DL1" s="70"/>
+      <c r="DM1" s="71"/>
+      <c r="DN1" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="DO1" s="38"/>
-      <c r="DP1" s="38"/>
-      <c r="DQ1" s="38"/>
-      <c r="DR1" s="38"/>
-      <c r="DS1" s="38"/>
-      <c r="DT1" s="38"/>
-      <c r="DU1" s="38"/>
-      <c r="DV1" s="38"/>
-      <c r="DW1" s="38"/>
-      <c r="DX1" s="38"/>
-      <c r="DY1" s="38"/>
-      <c r="DZ1" s="38"/>
-      <c r="EA1" s="39"/>
+      <c r="DO1" s="58"/>
+      <c r="DP1" s="58"/>
+      <c r="DQ1" s="58"/>
+      <c r="DR1" s="58"/>
+      <c r="DS1" s="58"/>
+      <c r="DT1" s="58"/>
+      <c r="DU1" s="58"/>
+      <c r="DV1" s="58"/>
+      <c r="DW1" s="58"/>
+      <c r="DX1" s="58"/>
+      <c r="DY1" s="58"/>
+      <c r="DZ1" s="58"/>
+      <c r="EA1" s="59"/>
     </row>
     <row r="2" spans="1:131" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2307,16 +2310,16 @@
       <c r="AD3" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="AE3" s="63" t="s">
+      <c r="AE3" s="50" t="s">
         <v>155</v>
       </c>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="63" t="s">
+      <c r="AF3" s="51"/>
+      <c r="AG3" s="51"/>
+      <c r="AH3" s="50" t="s">
         <v>156</v>
       </c>
-      <c r="AI3" s="64"/>
-      <c r="AJ3" s="64"/>
+      <c r="AI3" s="51"/>
+      <c r="AJ3" s="51"/>
       <c r="AK3" s="11" t="s">
         <v>157</v>
       </c>
@@ -2531,10 +2534,10 @@
       <c r="A4" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="47" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="69"/>
+      <c r="C4" s="48"/>
       <c r="D4" s="15" t="s">
         <v>195</v>
       </c>
@@ -2577,14 +2580,14 @@
       <c r="Q4" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="R4" s="65" t="s">
+      <c r="R4" s="46" t="s">
         <v>194</v>
       </c>
-      <c r="S4" s="70"/>
-      <c r="T4" s="65" t="s">
+      <c r="S4" s="49"/>
+      <c r="T4" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="U4" s="70"/>
+      <c r="U4" s="49"/>
       <c r="V4" s="15" t="s">
         <v>205</v>
       </c>
@@ -2603,10 +2606,10 @@
       <c r="AA4" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="AB4" s="65" t="s">
+      <c r="AB4" s="46" t="s">
         <v>196</v>
       </c>
-      <c r="AC4" s="70"/>
+      <c r="AC4" s="49"/>
       <c r="AD4" s="15" t="s">
         <v>211</v>
       </c>
@@ -2751,33 +2754,33 @@
       <c r="BY4" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="BZ4" s="46" t="s">
+      <c r="BZ4" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="CA4" s="48"/>
-      <c r="CB4" s="46" t="s">
+      <c r="CA4" s="40"/>
+      <c r="CB4" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="CC4" s="47"/>
-      <c r="CD4" s="47"/>
-      <c r="CE4" s="47"/>
-      <c r="CF4" s="47"/>
-      <c r="CG4" s="48"/>
+      <c r="CC4" s="39"/>
+      <c r="CD4" s="39"/>
+      <c r="CE4" s="39"/>
+      <c r="CF4" s="39"/>
+      <c r="CG4" s="40"/>
       <c r="CH4" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="CI4" s="46" t="s">
+      <c r="CI4" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="CJ4" s="47"/>
-      <c r="CK4" s="47"/>
-      <c r="CL4" s="47"/>
-      <c r="CM4" s="47"/>
-      <c r="CN4" s="47"/>
-      <c r="CO4" s="47"/>
-      <c r="CP4" s="47"/>
-      <c r="CQ4" s="47"/>
-      <c r="CR4" s="48"/>
+      <c r="CJ4" s="39"/>
+      <c r="CK4" s="39"/>
+      <c r="CL4" s="39"/>
+      <c r="CM4" s="39"/>
+      <c r="CN4" s="39"/>
+      <c r="CO4" s="39"/>
+      <c r="CP4" s="39"/>
+      <c r="CQ4" s="39"/>
+      <c r="CR4" s="40"/>
       <c r="CS4" s="17" t="s">
         <v>226</v>
       </c>
@@ -2811,19 +2814,19 @@
       <c r="DC4" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="DD4" s="46" t="s">
+      <c r="DD4" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="DE4" s="47"/>
-      <c r="DF4" s="47"/>
-      <c r="DG4" s="47"/>
-      <c r="DH4" s="48"/>
-      <c r="DI4" s="46" t="s">
+      <c r="DE4" s="39"/>
+      <c r="DF4" s="39"/>
+      <c r="DG4" s="39"/>
+      <c r="DH4" s="40"/>
+      <c r="DI4" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="DJ4" s="47"/>
-      <c r="DK4" s="47"/>
-      <c r="DL4" s="48"/>
+      <c r="DJ4" s="39"/>
+      <c r="DK4" s="39"/>
+      <c r="DL4" s="40"/>
       <c r="DM4" s="17" t="s">
         <v>234</v>
       </c>
@@ -2848,13 +2851,13 @@
       <c r="DT4" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="DU4" s="46" t="s">
+      <c r="DU4" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="DV4" s="47"/>
-      <c r="DW4" s="47"/>
-      <c r="DX4" s="47"/>
-      <c r="DY4" s="48"/>
+      <c r="DV4" s="39"/>
+      <c r="DW4" s="39"/>
+      <c r="DX4" s="39"/>
+      <c r="DY4" s="40"/>
       <c r="DZ4" s="15" t="s">
         <v>214</v>
       </c>
@@ -2866,10 +2869,10 @@
       <c r="A5" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="C5" s="67"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="15" t="s">
         <v>243</v>
       </c>
@@ -2882,20 +2885,20 @@
       <c r="G5" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="48"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="40"/>
       <c r="M5" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="N5" s="65" t="s">
+      <c r="N5" s="46" t="s">
         <v>243</v>
       </c>
-      <c r="O5" s="67"/>
+      <c r="O5" s="45"/>
       <c r="P5" s="30" t="s">
         <v>242</v>
       </c>
@@ -2914,10 +2917,10 @@
       <c r="U5" s="32" t="s">
         <v>243</v>
       </c>
-      <c r="V5" s="65" t="s">
+      <c r="V5" s="46" t="s">
         <v>247</v>
       </c>
-      <c r="W5" s="67"/>
+      <c r="W5" s="45"/>
       <c r="X5" s="15" t="s">
         <v>248</v>
       </c>
@@ -2927,27 +2930,27 @@
       <c r="Z5" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="AA5" s="65" t="s">
+      <c r="AA5" s="46" t="s">
         <v>248</v>
       </c>
-      <c r="AB5" s="67"/>
-      <c r="AC5" s="67"/>
-      <c r="AD5" s="67"/>
-      <c r="AE5" s="65" t="s">
+      <c r="AB5" s="45"/>
+      <c r="AC5" s="45"/>
+      <c r="AD5" s="45"/>
+      <c r="AE5" s="46" t="s">
         <v>249</v>
       </c>
-      <c r="AF5" s="67"/>
-      <c r="AG5" s="67"/>
-      <c r="AH5" s="65" t="s">
+      <c r="AF5" s="45"/>
+      <c r="AG5" s="45"/>
+      <c r="AH5" s="46" t="s">
         <v>243</v>
       </c>
-      <c r="AI5" s="67"/>
-      <c r="AJ5" s="67"/>
-      <c r="AK5" s="65" t="s">
+      <c r="AI5" s="45"/>
+      <c r="AJ5" s="45"/>
+      <c r="AK5" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="AL5" s="67"/>
-      <c r="AM5" s="67"/>
+      <c r="AL5" s="45"/>
+      <c r="AM5" s="45"/>
       <c r="AN5" s="15" t="s">
         <v>251</v>
       </c>
@@ -2957,55 +2960,55 @@
       <c r="AP5" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="AQ5" s="46" t="s">
+      <c r="AQ5" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="AR5" s="47"/>
-      <c r="AS5" s="47"/>
-      <c r="AT5" s="47"/>
-      <c r="AU5" s="48"/>
-      <c r="AV5" s="40" t="s">
+      <c r="AR5" s="39"/>
+      <c r="AS5" s="39"/>
+      <c r="AT5" s="39"/>
+      <c r="AU5" s="40"/>
+      <c r="AV5" s="60" t="s">
         <v>253</v>
       </c>
-      <c r="AW5" s="41"/>
-      <c r="AX5" s="41"/>
-      <c r="AY5" s="42"/>
-      <c r="AZ5" s="40" t="s">
+      <c r="AW5" s="61"/>
+      <c r="AX5" s="61"/>
+      <c r="AY5" s="62"/>
+      <c r="AZ5" s="60" t="s">
         <v>276</v>
       </c>
-      <c r="BA5" s="41"/>
-      <c r="BB5" s="41"/>
-      <c r="BC5" s="42"/>
-      <c r="BD5" s="40" t="s">
+      <c r="BA5" s="61"/>
+      <c r="BB5" s="61"/>
+      <c r="BC5" s="62"/>
+      <c r="BD5" s="60" t="s">
         <v>254</v>
       </c>
-      <c r="BE5" s="41"/>
-      <c r="BF5" s="41"/>
-      <c r="BG5" s="42"/>
-      <c r="BH5" s="40" t="s">
+      <c r="BE5" s="61"/>
+      <c r="BF5" s="61"/>
+      <c r="BG5" s="62"/>
+      <c r="BH5" s="60" t="s">
         <v>255</v>
       </c>
-      <c r="BI5" s="41"/>
-      <c r="BJ5" s="41"/>
-      <c r="BK5" s="42"/>
-      <c r="BL5" s="40" t="s">
+      <c r="BI5" s="61"/>
+      <c r="BJ5" s="61"/>
+      <c r="BK5" s="62"/>
+      <c r="BL5" s="60" t="s">
         <v>256</v>
       </c>
-      <c r="BM5" s="41"/>
-      <c r="BN5" s="41"/>
-      <c r="BO5" s="42"/>
-      <c r="BP5" s="40" t="s">
+      <c r="BM5" s="61"/>
+      <c r="BN5" s="61"/>
+      <c r="BO5" s="62"/>
+      <c r="BP5" s="60" t="s">
         <v>257</v>
       </c>
-      <c r="BQ5" s="41"/>
-      <c r="BR5" s="41"/>
-      <c r="BS5" s="42"/>
-      <c r="BT5" s="40" t="s">
+      <c r="BQ5" s="61"/>
+      <c r="BR5" s="61"/>
+      <c r="BS5" s="62"/>
+      <c r="BT5" s="60" t="s">
         <v>258</v>
       </c>
-      <c r="BU5" s="41"/>
-      <c r="BV5" s="41"/>
-      <c r="BW5" s="42"/>
+      <c r="BU5" s="61"/>
+      <c r="BV5" s="61"/>
+      <c r="BW5" s="62"/>
       <c r="BX5" s="15" t="s">
         <v>242</v>
       </c>
@@ -3018,31 +3021,31 @@
       <c r="CA5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="CB5" s="46" t="s">
+      <c r="CB5" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="CC5" s="47"/>
-      <c r="CD5" s="47"/>
-      <c r="CE5" s="48"/>
-      <c r="CF5" s="46" t="s">
+      <c r="CC5" s="39"/>
+      <c r="CD5" s="39"/>
+      <c r="CE5" s="40"/>
+      <c r="CF5" s="38" t="s">
         <v>262</v>
       </c>
-      <c r="CG5" s="48"/>
+      <c r="CG5" s="40"/>
       <c r="CH5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="CI5" s="46" t="s">
+      <c r="CI5" s="38" t="s">
         <v>263</v>
       </c>
-      <c r="CJ5" s="47"/>
-      <c r="CK5" s="47"/>
-      <c r="CL5" s="47"/>
-      <c r="CM5" s="47"/>
-      <c r="CN5" s="47"/>
-      <c r="CO5" s="47"/>
-      <c r="CP5" s="47"/>
-      <c r="CQ5" s="47"/>
-      <c r="CR5" s="48"/>
+      <c r="CJ5" s="39"/>
+      <c r="CK5" s="39"/>
+      <c r="CL5" s="39"/>
+      <c r="CM5" s="39"/>
+      <c r="CN5" s="39"/>
+      <c r="CO5" s="39"/>
+      <c r="CP5" s="39"/>
+      <c r="CQ5" s="39"/>
+      <c r="CR5" s="40"/>
       <c r="CS5" s="15" t="s">
         <v>242</v>
       </c>
@@ -3058,49 +3061,49 @@
       <c r="CW5" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="CX5" s="46" t="s">
+      <c r="CX5" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="CY5" s="48"/>
-      <c r="CZ5" s="46" t="s">
+      <c r="CY5" s="40"/>
+      <c r="CZ5" s="38" t="s">
         <v>265</v>
       </c>
-      <c r="DA5" s="48"/>
+      <c r="DA5" s="40"/>
       <c r="DB5" s="15" t="s">
         <v>243</v>
       </c>
       <c r="DC5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="DD5" s="58" t="s">
+      <c r="DD5" s="41" t="s">
         <v>266</v>
       </c>
-      <c r="DE5" s="59"/>
-      <c r="DF5" s="59"/>
-      <c r="DG5" s="59"/>
-      <c r="DH5" s="60"/>
-      <c r="DI5" s="46" t="s">
+      <c r="DE5" s="42"/>
+      <c r="DF5" s="42"/>
+      <c r="DG5" s="42"/>
+      <c r="DH5" s="44"/>
+      <c r="DI5" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="DJ5" s="47"/>
-      <c r="DK5" s="47"/>
-      <c r="DL5" s="48"/>
+      <c r="DJ5" s="39"/>
+      <c r="DK5" s="39"/>
+      <c r="DL5" s="40"/>
       <c r="DM5" s="15" t="s">
         <v>249</v>
       </c>
       <c r="DN5" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="DO5" s="46" t="s">
+      <c r="DO5" s="38" t="s">
         <v>267</v>
       </c>
-      <c r="DP5" s="48"/>
-      <c r="DQ5" s="46" t="s">
+      <c r="DP5" s="40"/>
+      <c r="DQ5" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="DR5" s="48"/>
-      <c r="DS5" s="15" t="s">
-        <v>242</v>
+      <c r="DR5" s="40"/>
+      <c r="DS5" s="37" t="s">
+        <v>244</v>
       </c>
       <c r="DT5" s="15" t="s">
         <v>282</v>
@@ -3108,12 +3111,12 @@
       <c r="DU5" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="DV5" s="46" t="s">
+      <c r="DV5" s="38" t="s">
         <v>268</v>
       </c>
-      <c r="DW5" s="47"/>
-      <c r="DX5" s="47"/>
-      <c r="DY5" s="48"/>
+      <c r="DW5" s="39"/>
+      <c r="DX5" s="39"/>
+      <c r="DY5" s="40"/>
       <c r="DZ5" s="15" t="s">
         <v>281</v>
       </c>
@@ -3125,137 +3128,137 @@
       <c r="A6" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="61" t="s">
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="43" t="s">
         <v>271</v>
       </c>
-      <c r="G6" s="61"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
       <c r="M6" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="N6" s="65"/>
-      <c r="O6" s="65"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="65" t="s">
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46" t="s">
         <v>273</v>
       </c>
-      <c r="R6" s="67"/>
-      <c r="S6" s="67"/>
-      <c r="T6" s="67"/>
-      <c r="U6" s="67"/>
-      <c r="V6" s="67"/>
-      <c r="W6" s="67"/>
-      <c r="X6" s="67"/>
-      <c r="Y6" s="65"/>
-      <c r="Z6" s="65"/>
-      <c r="AA6" s="65" t="s">
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="45"/>
+      <c r="U6" s="45"/>
+      <c r="V6" s="45"/>
+      <c r="W6" s="45"/>
+      <c r="X6" s="45"/>
+      <c r="Y6" s="46"/>
+      <c r="Z6" s="46"/>
+      <c r="AA6" s="46" t="s">
         <v>273</v>
       </c>
-      <c r="AB6" s="67"/>
-      <c r="AC6" s="67"/>
-      <c r="AD6" s="67"/>
-      <c r="AE6" s="65"/>
-      <c r="AF6" s="65"/>
-      <c r="AG6" s="65"/>
-      <c r="AH6" s="65"/>
-      <c r="AI6" s="65"/>
-      <c r="AJ6" s="65"/>
-      <c r="AK6" s="65"/>
-      <c r="AL6" s="65"/>
-      <c r="AM6" s="65"/>
-      <c r="AN6" s="65"/>
-      <c r="AO6" s="65"/>
+      <c r="AB6" s="45"/>
+      <c r="AC6" s="45"/>
+      <c r="AD6" s="45"/>
+      <c r="AE6" s="46"/>
+      <c r="AF6" s="46"/>
+      <c r="AG6" s="46"/>
+      <c r="AH6" s="46"/>
+      <c r="AI6" s="46"/>
+      <c r="AJ6" s="46"/>
+      <c r="AK6" s="46"/>
+      <c r="AL6" s="46"/>
+      <c r="AM6" s="46"/>
+      <c r="AN6" s="46"/>
+      <c r="AO6" s="46"/>
       <c r="AP6" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="AQ6" s="46"/>
-      <c r="AR6" s="47"/>
-      <c r="AS6" s="47"/>
-      <c r="AT6" s="47"/>
-      <c r="AU6" s="47"/>
-      <c r="AV6" s="47"/>
-      <c r="AW6" s="47"/>
-      <c r="AX6" s="47"/>
-      <c r="AY6" s="47"/>
-      <c r="AZ6" s="47"/>
-      <c r="BA6" s="47"/>
-      <c r="BB6" s="47"/>
-      <c r="BC6" s="47"/>
-      <c r="BD6" s="47"/>
-      <c r="BE6" s="47"/>
-      <c r="BF6" s="47"/>
-      <c r="BG6" s="47"/>
-      <c r="BH6" s="47"/>
-      <c r="BI6" s="47"/>
-      <c r="BJ6" s="47"/>
-      <c r="BK6" s="47"/>
-      <c r="BL6" s="47"/>
-      <c r="BM6" s="47"/>
-      <c r="BN6" s="47"/>
-      <c r="BO6" s="47"/>
-      <c r="BP6" s="47"/>
-      <c r="BQ6" s="47"/>
-      <c r="BR6" s="47"/>
-      <c r="BS6" s="47"/>
-      <c r="BT6" s="47"/>
-      <c r="BU6" s="47"/>
-      <c r="BV6" s="47"/>
-      <c r="BW6" s="48"/>
-      <c r="BX6" s="46"/>
-      <c r="BY6" s="47"/>
-      <c r="BZ6" s="47"/>
-      <c r="CA6" s="47"/>
-      <c r="CB6" s="47"/>
-      <c r="CC6" s="47"/>
-      <c r="CD6" s="47"/>
-      <c r="CE6" s="47"/>
-      <c r="CF6" s="47"/>
-      <c r="CG6" s="47"/>
-      <c r="CH6" s="47"/>
-      <c r="CI6" s="47"/>
-      <c r="CJ6" s="47"/>
-      <c r="CK6" s="47"/>
-      <c r="CL6" s="47"/>
-      <c r="CM6" s="47"/>
-      <c r="CN6" s="47"/>
-      <c r="CO6" s="47"/>
-      <c r="CP6" s="47"/>
-      <c r="CQ6" s="47"/>
-      <c r="CR6" s="48"/>
-      <c r="CS6" s="46"/>
-      <c r="CT6" s="47"/>
-      <c r="CU6" s="47"/>
-      <c r="CV6" s="47"/>
-      <c r="CW6" s="47"/>
-      <c r="CX6" s="47"/>
-      <c r="CY6" s="47"/>
-      <c r="CZ6" s="47"/>
-      <c r="DA6" s="47"/>
-      <c r="DB6" s="47"/>
-      <c r="DC6" s="47"/>
-      <c r="DD6" s="47"/>
-      <c r="DE6" s="47"/>
-      <c r="DF6" s="47"/>
-      <c r="DG6" s="47"/>
-      <c r="DH6" s="47"/>
-      <c r="DI6" s="47"/>
-      <c r="DJ6" s="47"/>
-      <c r="DK6" s="47"/>
-      <c r="DL6" s="47"/>
-      <c r="DM6" s="48"/>
-      <c r="DN6" s="46"/>
-      <c r="DO6" s="47"/>
-      <c r="DP6" s="47"/>
-      <c r="DQ6" s="47"/>
-      <c r="DR6" s="48"/>
+      <c r="AQ6" s="38"/>
+      <c r="AR6" s="39"/>
+      <c r="AS6" s="39"/>
+      <c r="AT6" s="39"/>
+      <c r="AU6" s="39"/>
+      <c r="AV6" s="39"/>
+      <c r="AW6" s="39"/>
+      <c r="AX6" s="39"/>
+      <c r="AY6" s="39"/>
+      <c r="AZ6" s="39"/>
+      <c r="BA6" s="39"/>
+      <c r="BB6" s="39"/>
+      <c r="BC6" s="39"/>
+      <c r="BD6" s="39"/>
+      <c r="BE6" s="39"/>
+      <c r="BF6" s="39"/>
+      <c r="BG6" s="39"/>
+      <c r="BH6" s="39"/>
+      <c r="BI6" s="39"/>
+      <c r="BJ6" s="39"/>
+      <c r="BK6" s="39"/>
+      <c r="BL6" s="39"/>
+      <c r="BM6" s="39"/>
+      <c r="BN6" s="39"/>
+      <c r="BO6" s="39"/>
+      <c r="BP6" s="39"/>
+      <c r="BQ6" s="39"/>
+      <c r="BR6" s="39"/>
+      <c r="BS6" s="39"/>
+      <c r="BT6" s="39"/>
+      <c r="BU6" s="39"/>
+      <c r="BV6" s="39"/>
+      <c r="BW6" s="40"/>
+      <c r="BX6" s="38"/>
+      <c r="BY6" s="39"/>
+      <c r="BZ6" s="39"/>
+      <c r="CA6" s="39"/>
+      <c r="CB6" s="39"/>
+      <c r="CC6" s="39"/>
+      <c r="CD6" s="39"/>
+      <c r="CE6" s="39"/>
+      <c r="CF6" s="39"/>
+      <c r="CG6" s="39"/>
+      <c r="CH6" s="39"/>
+      <c r="CI6" s="39"/>
+      <c r="CJ6" s="39"/>
+      <c r="CK6" s="39"/>
+      <c r="CL6" s="39"/>
+      <c r="CM6" s="39"/>
+      <c r="CN6" s="39"/>
+      <c r="CO6" s="39"/>
+      <c r="CP6" s="39"/>
+      <c r="CQ6" s="39"/>
+      <c r="CR6" s="40"/>
+      <c r="CS6" s="38"/>
+      <c r="CT6" s="39"/>
+      <c r="CU6" s="39"/>
+      <c r="CV6" s="39"/>
+      <c r="CW6" s="39"/>
+      <c r="CX6" s="39"/>
+      <c r="CY6" s="39"/>
+      <c r="CZ6" s="39"/>
+      <c r="DA6" s="39"/>
+      <c r="DB6" s="39"/>
+      <c r="DC6" s="39"/>
+      <c r="DD6" s="39"/>
+      <c r="DE6" s="39"/>
+      <c r="DF6" s="39"/>
+      <c r="DG6" s="39"/>
+      <c r="DH6" s="39"/>
+      <c r="DI6" s="39"/>
+      <c r="DJ6" s="39"/>
+      <c r="DK6" s="39"/>
+      <c r="DL6" s="39"/>
+      <c r="DM6" s="40"/>
+      <c r="DN6" s="38"/>
+      <c r="DO6" s="39"/>
+      <c r="DP6" s="39"/>
+      <c r="DQ6" s="39"/>
+      <c r="DR6" s="40"/>
       <c r="DS6" s="20" t="s">
         <v>271</v>
       </c>
@@ -3263,12 +3266,12 @@
       <c r="DU6" s="20" t="s">
         <v>271</v>
       </c>
-      <c r="DV6" s="58"/>
-      <c r="DW6" s="59"/>
-      <c r="DX6" s="59"/>
-      <c r="DY6" s="59"/>
-      <c r="DZ6" s="59"/>
-      <c r="EA6" s="60"/>
+      <c r="DV6" s="41"/>
+      <c r="DW6" s="42"/>
+      <c r="DX6" s="42"/>
+      <c r="DY6" s="42"/>
+      <c r="DZ6" s="42"/>
+      <c r="EA6" s="44"/>
     </row>
     <row r="7" spans="1:131" s="35" customFormat="1" ht="23" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -3277,149 +3280,149 @@
       <c r="B7" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61" t="s">
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43" t="s">
         <v>243</v>
       </c>
-      <c r="G7" s="61"/>
+      <c r="G7" s="43"/>
       <c r="H7" s="21"/>
-      <c r="I7" s="61" t="s">
+      <c r="I7" s="43" t="s">
         <v>243</v>
       </c>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="56"/>
       <c r="N7" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="O7" s="58"/>
-      <c r="P7" s="60"/>
-      <c r="Q7" s="58"/>
-      <c r="R7" s="59"/>
-      <c r="S7" s="59"/>
-      <c r="T7" s="59"/>
-      <c r="U7" s="60"/>
-      <c r="V7" s="61" t="s">
+      <c r="O7" s="41"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="41"/>
+      <c r="R7" s="42"/>
+      <c r="S7" s="42"/>
+      <c r="T7" s="42"/>
+      <c r="U7" s="44"/>
+      <c r="V7" s="43" t="s">
         <v>243</v>
       </c>
-      <c r="W7" s="61"/>
-      <c r="X7" s="58"/>
-      <c r="Y7" s="59"/>
-      <c r="Z7" s="59"/>
-      <c r="AA7" s="59"/>
-      <c r="AB7" s="59"/>
-      <c r="AC7" s="59"/>
-      <c r="AD7" s="59"/>
-      <c r="AE7" s="59"/>
-      <c r="AF7" s="59"/>
-      <c r="AG7" s="59"/>
-      <c r="AH7" s="59"/>
-      <c r="AI7" s="59"/>
-      <c r="AJ7" s="60"/>
-      <c r="AK7" s="58"/>
-      <c r="AL7" s="59"/>
-      <c r="AM7" s="59"/>
-      <c r="AN7" s="59"/>
-      <c r="AO7" s="59"/>
-      <c r="AP7" s="60"/>
-      <c r="AQ7" s="58" t="s">
+      <c r="W7" s="43"/>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="42"/>
+      <c r="Z7" s="42"/>
+      <c r="AA7" s="42"/>
+      <c r="AB7" s="42"/>
+      <c r="AC7" s="42"/>
+      <c r="AD7" s="42"/>
+      <c r="AE7" s="42"/>
+      <c r="AF7" s="42"/>
+      <c r="AG7" s="42"/>
+      <c r="AH7" s="42"/>
+      <c r="AI7" s="42"/>
+      <c r="AJ7" s="44"/>
+      <c r="AK7" s="41"/>
+      <c r="AL7" s="42"/>
+      <c r="AM7" s="42"/>
+      <c r="AN7" s="42"/>
+      <c r="AO7" s="42"/>
+      <c r="AP7" s="44"/>
+      <c r="AQ7" s="41" t="s">
         <v>243</v>
       </c>
-      <c r="AR7" s="60"/>
-      <c r="AS7" s="58"/>
-      <c r="AT7" s="60"/>
+      <c r="AR7" s="44"/>
+      <c r="AS7" s="41"/>
+      <c r="AT7" s="44"/>
       <c r="AU7" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="AV7" s="58"/>
-      <c r="AW7" s="59"/>
-      <c r="AX7" s="59"/>
-      <c r="AY7" s="59"/>
-      <c r="AZ7" s="59"/>
-      <c r="BA7" s="59"/>
-      <c r="BB7" s="59"/>
-      <c r="BC7" s="59"/>
-      <c r="BD7" s="59"/>
-      <c r="BE7" s="59"/>
-      <c r="BF7" s="59"/>
-      <c r="BG7" s="59"/>
-      <c r="BH7" s="59"/>
-      <c r="BI7" s="59"/>
-      <c r="BJ7" s="59"/>
-      <c r="BK7" s="59"/>
-      <c r="BL7" s="59"/>
-      <c r="BM7" s="59"/>
-      <c r="BN7" s="59"/>
-      <c r="BO7" s="59"/>
-      <c r="BP7" s="59"/>
-      <c r="BQ7" s="59"/>
-      <c r="BR7" s="59"/>
-      <c r="BS7" s="59"/>
-      <c r="BT7" s="59"/>
-      <c r="BU7" s="59"/>
-      <c r="BV7" s="59"/>
-      <c r="BW7" s="60"/>
-      <c r="BX7" s="58"/>
-      <c r="BY7" s="59"/>
-      <c r="BZ7" s="59"/>
-      <c r="CA7" s="59"/>
-      <c r="CB7" s="59"/>
-      <c r="CC7" s="59"/>
-      <c r="CD7" s="59"/>
-      <c r="CE7" s="59"/>
-      <c r="CF7" s="59"/>
-      <c r="CG7" s="59"/>
-      <c r="CH7" s="59"/>
-      <c r="CI7" s="59"/>
-      <c r="CJ7" s="59"/>
-      <c r="CK7" s="59"/>
-      <c r="CL7" s="59"/>
-      <c r="CM7" s="59"/>
-      <c r="CN7" s="59"/>
-      <c r="CO7" s="59"/>
-      <c r="CP7" s="59"/>
-      <c r="CQ7" s="59"/>
-      <c r="CR7" s="60"/>
-      <c r="CS7" s="58"/>
-      <c r="CT7" s="59"/>
-      <c r="CU7" s="59"/>
-      <c r="CV7" s="59"/>
-      <c r="CW7" s="59"/>
-      <c r="CX7" s="59"/>
-      <c r="CY7" s="59"/>
-      <c r="CZ7" s="59"/>
-      <c r="DA7" s="59"/>
-      <c r="DB7" s="59"/>
-      <c r="DC7" s="59"/>
-      <c r="DD7" s="59"/>
-      <c r="DE7" s="59"/>
-      <c r="DF7" s="59"/>
-      <c r="DG7" s="59"/>
-      <c r="DH7" s="59"/>
-      <c r="DI7" s="59"/>
-      <c r="DJ7" s="59"/>
-      <c r="DK7" s="59"/>
-      <c r="DL7" s="59"/>
-      <c r="DM7" s="60"/>
-      <c r="DN7" s="58"/>
-      <c r="DO7" s="59"/>
-      <c r="DP7" s="59"/>
-      <c r="DQ7" s="59"/>
-      <c r="DR7" s="59"/>
-      <c r="DS7" s="60"/>
-      <c r="DT7" s="58" t="s">
+      <c r="AV7" s="41"/>
+      <c r="AW7" s="42"/>
+      <c r="AX7" s="42"/>
+      <c r="AY7" s="42"/>
+      <c r="AZ7" s="42"/>
+      <c r="BA7" s="42"/>
+      <c r="BB7" s="42"/>
+      <c r="BC7" s="42"/>
+      <c r="BD7" s="42"/>
+      <c r="BE7" s="42"/>
+      <c r="BF7" s="42"/>
+      <c r="BG7" s="42"/>
+      <c r="BH7" s="42"/>
+      <c r="BI7" s="42"/>
+      <c r="BJ7" s="42"/>
+      <c r="BK7" s="42"/>
+      <c r="BL7" s="42"/>
+      <c r="BM7" s="42"/>
+      <c r="BN7" s="42"/>
+      <c r="BO7" s="42"/>
+      <c r="BP7" s="42"/>
+      <c r="BQ7" s="42"/>
+      <c r="BR7" s="42"/>
+      <c r="BS7" s="42"/>
+      <c r="BT7" s="42"/>
+      <c r="BU7" s="42"/>
+      <c r="BV7" s="42"/>
+      <c r="BW7" s="44"/>
+      <c r="BX7" s="41"/>
+      <c r="BY7" s="42"/>
+      <c r="BZ7" s="42"/>
+      <c r="CA7" s="42"/>
+      <c r="CB7" s="42"/>
+      <c r="CC7" s="42"/>
+      <c r="CD7" s="42"/>
+      <c r="CE7" s="42"/>
+      <c r="CF7" s="42"/>
+      <c r="CG7" s="42"/>
+      <c r="CH7" s="42"/>
+      <c r="CI7" s="42"/>
+      <c r="CJ7" s="42"/>
+      <c r="CK7" s="42"/>
+      <c r="CL7" s="42"/>
+      <c r="CM7" s="42"/>
+      <c r="CN7" s="42"/>
+      <c r="CO7" s="42"/>
+      <c r="CP7" s="42"/>
+      <c r="CQ7" s="42"/>
+      <c r="CR7" s="44"/>
+      <c r="CS7" s="41"/>
+      <c r="CT7" s="42"/>
+      <c r="CU7" s="42"/>
+      <c r="CV7" s="42"/>
+      <c r="CW7" s="42"/>
+      <c r="CX7" s="42"/>
+      <c r="CY7" s="42"/>
+      <c r="CZ7" s="42"/>
+      <c r="DA7" s="42"/>
+      <c r="DB7" s="42"/>
+      <c r="DC7" s="42"/>
+      <c r="DD7" s="42"/>
+      <c r="DE7" s="42"/>
+      <c r="DF7" s="42"/>
+      <c r="DG7" s="42"/>
+      <c r="DH7" s="42"/>
+      <c r="DI7" s="42"/>
+      <c r="DJ7" s="42"/>
+      <c r="DK7" s="42"/>
+      <c r="DL7" s="42"/>
+      <c r="DM7" s="44"/>
+      <c r="DN7" s="41"/>
+      <c r="DO7" s="42"/>
+      <c r="DP7" s="42"/>
+      <c r="DQ7" s="42"/>
+      <c r="DR7" s="42"/>
+      <c r="DS7" s="44"/>
+      <c r="DT7" s="41" t="s">
         <v>243</v>
       </c>
-      <c r="DU7" s="59"/>
-      <c r="DV7" s="59"/>
-      <c r="DW7" s="59"/>
-      <c r="DX7" s="59"/>
-      <c r="DY7" s="59"/>
-      <c r="DZ7" s="61"/>
-      <c r="EA7" s="61"/>
+      <c r="DU7" s="42"/>
+      <c r="DV7" s="42"/>
+      <c r="DW7" s="42"/>
+      <c r="DX7" s="42"/>
+      <c r="DY7" s="42"/>
+      <c r="DZ7" s="43"/>
+      <c r="EA7" s="43"/>
     </row>
     <row r="8" spans="1:131" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
@@ -3818,49 +3821,22 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="DU4:DY4"/>
-    <mergeCell ref="DT7:DY7"/>
-    <mergeCell ref="DZ7:EA7"/>
-    <mergeCell ref="DD4:DH4"/>
-    <mergeCell ref="DI4:DL4"/>
-    <mergeCell ref="DD5:DH5"/>
-    <mergeCell ref="DO5:DP5"/>
-    <mergeCell ref="DI5:DL5"/>
-    <mergeCell ref="CS6:DM6"/>
-    <mergeCell ref="CS7:DM7"/>
-    <mergeCell ref="DN6:DR6"/>
-    <mergeCell ref="DN7:DS7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="CZ5:DA5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="CB5:CE5"/>
-    <mergeCell ref="CF5:CG5"/>
-    <mergeCell ref="CI5:CR5"/>
-    <mergeCell ref="CX5:CY5"/>
-    <mergeCell ref="AQ6:BW6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="AA5:AD5"/>
-    <mergeCell ref="Q6:X6"/>
-    <mergeCell ref="AA6:AD6"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="BZ4:CA4"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="AE6:AO6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="DN1:EA1"/>
+    <mergeCell ref="BL5:BO5"/>
+    <mergeCell ref="BP5:BS5"/>
+    <mergeCell ref="BT5:BW5"/>
+    <mergeCell ref="AQ1:BW1"/>
+    <mergeCell ref="CB4:CG4"/>
+    <mergeCell ref="BX1:CR1"/>
+    <mergeCell ref="CS1:DM1"/>
+    <mergeCell ref="DV5:DY5"/>
+    <mergeCell ref="AV5:AY5"/>
+    <mergeCell ref="AZ5:BC5"/>
+    <mergeCell ref="BD5:BG5"/>
+    <mergeCell ref="BH5:BK5"/>
+    <mergeCell ref="CI4:CR4"/>
+    <mergeCell ref="DQ5:DR5"/>
+    <mergeCell ref="AQ5:AU5"/>
     <mergeCell ref="B1:P1"/>
     <mergeCell ref="Q1:AJ1"/>
     <mergeCell ref="AK1:AP1"/>
@@ -3877,32 +3853,74 @@
     <mergeCell ref="AV7:BW7"/>
     <mergeCell ref="BX6:CR6"/>
     <mergeCell ref="BX7:CR7"/>
-    <mergeCell ref="DN1:EA1"/>
-    <mergeCell ref="BL5:BO5"/>
-    <mergeCell ref="BP5:BS5"/>
-    <mergeCell ref="BT5:BW5"/>
-    <mergeCell ref="AQ1:BW1"/>
-    <mergeCell ref="CB4:CG4"/>
-    <mergeCell ref="BX1:CR1"/>
-    <mergeCell ref="CS1:DM1"/>
-    <mergeCell ref="DV5:DY5"/>
-    <mergeCell ref="AV5:AY5"/>
-    <mergeCell ref="AZ5:BC5"/>
-    <mergeCell ref="BD5:BG5"/>
-    <mergeCell ref="BH5:BK5"/>
-    <mergeCell ref="CI4:CR4"/>
-    <mergeCell ref="DQ5:DR5"/>
-    <mergeCell ref="AQ5:AU5"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="AE6:AO6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="BZ4:CA4"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="CZ5:DA5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="CB5:CE5"/>
+    <mergeCell ref="CF5:CG5"/>
+    <mergeCell ref="CI5:CR5"/>
+    <mergeCell ref="CX5:CY5"/>
+    <mergeCell ref="AQ6:BW6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="AA5:AD5"/>
+    <mergeCell ref="Q6:X6"/>
+    <mergeCell ref="AA6:AD6"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="DU4:DY4"/>
+    <mergeCell ref="DT7:DY7"/>
+    <mergeCell ref="DZ7:EA7"/>
+    <mergeCell ref="DD4:DH4"/>
+    <mergeCell ref="DI4:DL4"/>
+    <mergeCell ref="DD5:DH5"/>
+    <mergeCell ref="DO5:DP5"/>
+    <mergeCell ref="DI5:DL5"/>
+    <mergeCell ref="CS6:DM6"/>
+    <mergeCell ref="CS7:DM7"/>
+    <mergeCell ref="DN6:DR6"/>
+    <mergeCell ref="DN7:DS7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="X4" r:id="rId1" xr:uid="{33A4BD0C-7A19-4C88-AF60-902623A24589}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000 OFFICIAL&amp;1#_x000D_</oddHeader>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 OFFICIAL</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ede1785e-3bac-4a90-a48c-62cc0231644e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000BCF930048F2A84190E342D576E507E9" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a5f7dcad46bf03cd06b92fe3a65eb3e5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ede1785e-3bac-4a90-a48c-62cc0231644e" xmlns:ns3="6c5f9a5a-0dad-4595-a39a-6416e9fb7054" xmlns:ns4="83a87e31-bf32-46ab-8e70-9fa18461fa4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="627fd199b21a7508d85a0883525fd0b8" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
@@ -4162,17 +4180,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ede1785e-3bac-4a90-a48c-62cc0231644e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4183,6 +4190,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3234EB82-E598-4D46-AACB-BAE493D677A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6c5f9a5a-0dad-4595-a39a-6416e9fb7054"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{844596B9-62AA-44A2-8AEF-70908D01A276}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4202,28 +4227,16 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3234EB82-E598-4D46-AACB-BAE493D677A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6c5f9a5a-0dad-4595-a39a-6416e9fb7054"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D2572BD-7EE7-4817-BEE4-BB014A85EDEE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{fbd41ebe-fca6-4f2c-aecb-bf3a17e72416}" enabled="1" method="Privileged" siteId="{bf346810-9c7d-43de-a872-24a2ef3995a8}" contentBits="3" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
feat: update documents with new period
</commit_message>
<xml_diff>
--- a/public/files/bulk-upload-lettings-template-2024-25.xlsx
+++ b/public/files/bulk-upload-lettings-template-2024-25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamuelIvko\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF48AE0-8B3F-45D4-B152-45AFD82D442E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F7A164-145F-401A-B0DA-F89299092402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -809,9 +809,6 @@
     <t>0 - 1</t>
   </si>
   <si>
-    <t>1 - 10</t>
-  </si>
-  <si>
     <t>xxxx.xx</t>
   </si>
   <si>
@@ -943,6 +940,9 @@
   </si>
   <si>
     <t>Yes, if there are no charges (if field 122 = 1)</t>
+  </si>
+  <si>
+    <t>1 - 11</t>
   </si>
 </sst>
 </file>
@@ -2258,10 +2258,10 @@
         <v>143</v>
       </c>
       <c r="F3" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>278</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>279</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>144</v>
@@ -2308,7 +2308,7 @@
         <v>154</v>
       </c>
       <c r="AD3" s="11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AE3" s="50" t="s">
         <v>155</v>
@@ -2848,11 +2848,11 @@
       <c r="DS4" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="DT4" s="15" t="s">
+      <c r="DT4" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="DU4" s="38" t="s">
         <v>239</v>
-      </c>
-      <c r="DU4" s="38" t="s">
-        <v>240</v>
       </c>
       <c r="DV4" s="39"/>
       <c r="DW4" s="39"/>
@@ -2862,180 +2862,180 @@
         <v>214</v>
       </c>
       <c r="EA4" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:131" s="34" customFormat="1" ht="137.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5" s="46" t="s">
         <v>241</v>
-      </c>
-      <c r="B5" s="46" t="s">
-        <v>242</v>
       </c>
       <c r="C5" s="45"/>
       <c r="D5" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="F5" s="15" t="s">
         <v>243</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>244</v>
-      </c>
       <c r="G5" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H5" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I5" s="39"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
       <c r="L5" s="40"/>
       <c r="M5" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N5" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O5" s="45"/>
       <c r="P5" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q5" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="R5" s="33" t="s">
+        <v>246</v>
+      </c>
+      <c r="S5" s="32" t="s">
         <v>242</v>
       </c>
-      <c r="Q5" s="32" t="s">
+      <c r="T5" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="R5" s="33" t="s">
-        <v>247</v>
-      </c>
-      <c r="S5" s="32" t="s">
-        <v>243</v>
-      </c>
-      <c r="T5" s="33" t="s">
-        <v>247</v>
-      </c>
       <c r="U5" s="32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="V5" s="46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="W5" s="45"/>
       <c r="X5" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="Y5" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="Y5" s="15" t="s">
+      <c r="Z5" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="Z5" s="15" t="s">
-        <v>250</v>
-      </c>
       <c r="AA5" s="46" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AB5" s="45"/>
       <c r="AC5" s="45"/>
       <c r="AD5" s="45"/>
       <c r="AE5" s="46" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AF5" s="45"/>
       <c r="AG5" s="45"/>
       <c r="AH5" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AI5" s="45"/>
       <c r="AJ5" s="45"/>
       <c r="AK5" s="46" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AL5" s="45"/>
       <c r="AM5" s="45"/>
       <c r="AN5" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="AO5" s="15" t="s">
         <v>251</v>
       </c>
-      <c r="AO5" s="15" t="s">
-        <v>252</v>
-      </c>
       <c r="AP5" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AQ5" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AR5" s="39"/>
       <c r="AS5" s="39"/>
       <c r="AT5" s="39"/>
       <c r="AU5" s="40"/>
       <c r="AV5" s="60" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AW5" s="61"/>
       <c r="AX5" s="61"/>
       <c r="AY5" s="62"/>
       <c r="AZ5" s="60" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="BA5" s="61"/>
       <c r="BB5" s="61"/>
       <c r="BC5" s="62"/>
       <c r="BD5" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="BE5" s="61"/>
       <c r="BF5" s="61"/>
       <c r="BG5" s="62"/>
       <c r="BH5" s="60" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="BI5" s="61"/>
       <c r="BJ5" s="61"/>
       <c r="BK5" s="62"/>
       <c r="BL5" s="60" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BM5" s="61"/>
       <c r="BN5" s="61"/>
       <c r="BO5" s="62"/>
       <c r="BP5" s="60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="BQ5" s="61"/>
       <c r="BR5" s="61"/>
       <c r="BS5" s="62"/>
       <c r="BT5" s="60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BU5" s="61"/>
       <c r="BV5" s="61"/>
       <c r="BW5" s="62"/>
       <c r="BX5" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="BY5" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="BZ5" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="BZ5" s="15" t="s">
+      <c r="CA5" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="CB5" s="38" t="s">
         <v>260</v>
-      </c>
-      <c r="CA5" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="CB5" s="38" t="s">
-        <v>261</v>
       </c>
       <c r="CC5" s="39"/>
       <c r="CD5" s="39"/>
       <c r="CE5" s="40"/>
       <c r="CF5" s="38" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="CG5" s="40"/>
       <c r="CH5" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="CI5" s="38" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="CJ5" s="39"/>
       <c r="CK5" s="39"/>
@@ -3047,93 +3047,93 @@
       <c r="CQ5" s="39"/>
       <c r="CR5" s="40"/>
       <c r="CS5" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="CT5" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="CU5" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="CV5" s="15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="CW5" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="CX5" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="CY5" s="40"/>
       <c r="CZ5" s="38" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="DA5" s="40"/>
       <c r="DB5" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="DC5" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="DD5" s="41" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="DE5" s="42"/>
       <c r="DF5" s="42"/>
       <c r="DG5" s="42"/>
       <c r="DH5" s="44"/>
       <c r="DI5" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="DJ5" s="39"/>
       <c r="DK5" s="39"/>
       <c r="DL5" s="40"/>
       <c r="DM5" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="DN5" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="DO5" s="38" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="DP5" s="40"/>
       <c r="DQ5" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="DR5" s="40"/>
       <c r="DS5" s="37" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="DT5" s="15" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="DU5" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="DV5" s="38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="DW5" s="39"/>
       <c r="DX5" s="39"/>
       <c r="DY5" s="40"/>
       <c r="DZ5" s="15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="EA5" s="15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:131" s="35" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B6" s="46"/>
       <c r="C6" s="46"/>
       <c r="D6" s="46"/>
       <c r="E6" s="46"/>
       <c r="F6" s="43" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G6" s="43"/>
       <c r="H6" s="52"/>
@@ -3142,13 +3142,13 @@
       <c r="K6" s="52"/>
       <c r="L6" s="52"/>
       <c r="M6" s="15" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N6" s="46"/>
       <c r="O6" s="46"/>
       <c r="P6" s="46"/>
       <c r="Q6" s="46" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="R6" s="45"/>
       <c r="S6" s="45"/>
@@ -3160,7 +3160,7 @@
       <c r="Y6" s="46"/>
       <c r="Z6" s="46"/>
       <c r="AA6" s="46" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AB6" s="45"/>
       <c r="AC6" s="45"/>
@@ -3177,7 +3177,7 @@
       <c r="AN6" s="46"/>
       <c r="AO6" s="46"/>
       <c r="AP6" s="15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AQ6" s="38"/>
       <c r="AR6" s="39"/>
@@ -3260,11 +3260,11 @@
       <c r="DQ6" s="39"/>
       <c r="DR6" s="40"/>
       <c r="DS6" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DT6" s="20"/>
       <c r="DU6" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DV6" s="41"/>
       <c r="DW6" s="42"/>
@@ -3275,28 +3275,28 @@
     </row>
     <row r="7" spans="1:131" s="35" customFormat="1" ht="23" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C7" s="43"/>
       <c r="D7" s="43"/>
       <c r="E7" s="43"/>
       <c r="F7" s="43" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G7" s="43"/>
       <c r="H7" s="21"/>
       <c r="I7" s="43" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J7" s="45"/>
       <c r="K7" s="45"/>
       <c r="L7" s="56"/>
       <c r="M7" s="56"/>
       <c r="N7" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O7" s="41"/>
       <c r="P7" s="44"/>
@@ -3306,7 +3306,7 @@
       <c r="T7" s="42"/>
       <c r="U7" s="44"/>
       <c r="V7" s="43" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W7" s="43"/>
       <c r="X7" s="41"/>
@@ -3329,13 +3329,13 @@
       <c r="AO7" s="42"/>
       <c r="AP7" s="44"/>
       <c r="AQ7" s="41" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AR7" s="44"/>
       <c r="AS7" s="41"/>
       <c r="AT7" s="44"/>
       <c r="AU7" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AV7" s="41"/>
       <c r="AW7" s="42"/>
@@ -3414,7 +3414,7 @@
       <c r="DR7" s="42"/>
       <c r="DS7" s="44"/>
       <c r="DT7" s="41" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="DU7" s="42"/>
       <c r="DV7" s="42"/>
@@ -3426,7 +3426,7 @@
     </row>
     <row r="8" spans="1:131" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B8" s="17">
         <v>1</v>

</xml_diff>

<commit_message>
CLDC-3391 Update resources with new rent period (#2387)
* feat: update documents with new period

* feat: update tests
</commit_message>
<xml_diff>
--- a/public/files/bulk-upload-lettings-template-2024-25.xlsx
+++ b/public/files/bulk-upload-lettings-template-2024-25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamuelIvko\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF48AE0-8B3F-45D4-B152-45AFD82D442E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F7A164-145F-401A-B0DA-F89299092402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -809,9 +809,6 @@
     <t>0 - 1</t>
   </si>
   <si>
-    <t>1 - 10</t>
-  </si>
-  <si>
     <t>xxxx.xx</t>
   </si>
   <si>
@@ -943,6 +940,9 @@
   </si>
   <si>
     <t>Yes, if there are no charges (if field 122 = 1)</t>
+  </si>
+  <si>
+    <t>1 - 11</t>
   </si>
 </sst>
 </file>
@@ -2258,10 +2258,10 @@
         <v>143</v>
       </c>
       <c r="F3" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>278</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>279</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>144</v>
@@ -2308,7 +2308,7 @@
         <v>154</v>
       </c>
       <c r="AD3" s="11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AE3" s="50" t="s">
         <v>155</v>
@@ -2848,11 +2848,11 @@
       <c r="DS4" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="DT4" s="15" t="s">
+      <c r="DT4" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="DU4" s="38" t="s">
         <v>239</v>
-      </c>
-      <c r="DU4" s="38" t="s">
-        <v>240</v>
       </c>
       <c r="DV4" s="39"/>
       <c r="DW4" s="39"/>
@@ -2862,180 +2862,180 @@
         <v>214</v>
       </c>
       <c r="EA4" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:131" s="34" customFormat="1" ht="137.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5" s="46" t="s">
         <v>241</v>
-      </c>
-      <c r="B5" s="46" t="s">
-        <v>242</v>
       </c>
       <c r="C5" s="45"/>
       <c r="D5" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="F5" s="15" t="s">
         <v>243</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>244</v>
-      </c>
       <c r="G5" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H5" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I5" s="39"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
       <c r="L5" s="40"/>
       <c r="M5" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N5" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O5" s="45"/>
       <c r="P5" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q5" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="R5" s="33" t="s">
+        <v>246</v>
+      </c>
+      <c r="S5" s="32" t="s">
         <v>242</v>
       </c>
-      <c r="Q5" s="32" t="s">
+      <c r="T5" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="R5" s="33" t="s">
-        <v>247</v>
-      </c>
-      <c r="S5" s="32" t="s">
-        <v>243</v>
-      </c>
-      <c r="T5" s="33" t="s">
-        <v>247</v>
-      </c>
       <c r="U5" s="32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="V5" s="46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="W5" s="45"/>
       <c r="X5" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="Y5" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="Y5" s="15" t="s">
+      <c r="Z5" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="Z5" s="15" t="s">
-        <v>250</v>
-      </c>
       <c r="AA5" s="46" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AB5" s="45"/>
       <c r="AC5" s="45"/>
       <c r="AD5" s="45"/>
       <c r="AE5" s="46" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AF5" s="45"/>
       <c r="AG5" s="45"/>
       <c r="AH5" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AI5" s="45"/>
       <c r="AJ5" s="45"/>
       <c r="AK5" s="46" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AL5" s="45"/>
       <c r="AM5" s="45"/>
       <c r="AN5" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="AO5" s="15" t="s">
         <v>251</v>
       </c>
-      <c r="AO5" s="15" t="s">
-        <v>252</v>
-      </c>
       <c r="AP5" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AQ5" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AR5" s="39"/>
       <c r="AS5" s="39"/>
       <c r="AT5" s="39"/>
       <c r="AU5" s="40"/>
       <c r="AV5" s="60" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AW5" s="61"/>
       <c r="AX5" s="61"/>
       <c r="AY5" s="62"/>
       <c r="AZ5" s="60" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="BA5" s="61"/>
       <c r="BB5" s="61"/>
       <c r="BC5" s="62"/>
       <c r="BD5" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="BE5" s="61"/>
       <c r="BF5" s="61"/>
       <c r="BG5" s="62"/>
       <c r="BH5" s="60" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="BI5" s="61"/>
       <c r="BJ5" s="61"/>
       <c r="BK5" s="62"/>
       <c r="BL5" s="60" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BM5" s="61"/>
       <c r="BN5" s="61"/>
       <c r="BO5" s="62"/>
       <c r="BP5" s="60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="BQ5" s="61"/>
       <c r="BR5" s="61"/>
       <c r="BS5" s="62"/>
       <c r="BT5" s="60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BU5" s="61"/>
       <c r="BV5" s="61"/>
       <c r="BW5" s="62"/>
       <c r="BX5" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="BY5" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="BZ5" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="BZ5" s="15" t="s">
+      <c r="CA5" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="CB5" s="38" t="s">
         <v>260</v>
-      </c>
-      <c r="CA5" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="CB5" s="38" t="s">
-        <v>261</v>
       </c>
       <c r="CC5" s="39"/>
       <c r="CD5" s="39"/>
       <c r="CE5" s="40"/>
       <c r="CF5" s="38" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="CG5" s="40"/>
       <c r="CH5" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="CI5" s="38" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="CJ5" s="39"/>
       <c r="CK5" s="39"/>
@@ -3047,93 +3047,93 @@
       <c r="CQ5" s="39"/>
       <c r="CR5" s="40"/>
       <c r="CS5" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="CT5" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="CU5" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="CV5" s="15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="CW5" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="CX5" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="CY5" s="40"/>
       <c r="CZ5" s="38" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="DA5" s="40"/>
       <c r="DB5" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="DC5" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="DD5" s="41" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="DE5" s="42"/>
       <c r="DF5" s="42"/>
       <c r="DG5" s="42"/>
       <c r="DH5" s="44"/>
       <c r="DI5" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="DJ5" s="39"/>
       <c r="DK5" s="39"/>
       <c r="DL5" s="40"/>
       <c r="DM5" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="DN5" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="DO5" s="38" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="DP5" s="40"/>
       <c r="DQ5" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="DR5" s="40"/>
       <c r="DS5" s="37" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="DT5" s="15" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="DU5" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="DV5" s="38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="DW5" s="39"/>
       <c r="DX5" s="39"/>
       <c r="DY5" s="40"/>
       <c r="DZ5" s="15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="EA5" s="15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:131" s="35" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B6" s="46"/>
       <c r="C6" s="46"/>
       <c r="D6" s="46"/>
       <c r="E6" s="46"/>
       <c r="F6" s="43" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G6" s="43"/>
       <c r="H6" s="52"/>
@@ -3142,13 +3142,13 @@
       <c r="K6" s="52"/>
       <c r="L6" s="52"/>
       <c r="M6" s="15" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N6" s="46"/>
       <c r="O6" s="46"/>
       <c r="P6" s="46"/>
       <c r="Q6" s="46" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="R6" s="45"/>
       <c r="S6" s="45"/>
@@ -3160,7 +3160,7 @@
       <c r="Y6" s="46"/>
       <c r="Z6" s="46"/>
       <c r="AA6" s="46" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AB6" s="45"/>
       <c r="AC6" s="45"/>
@@ -3177,7 +3177,7 @@
       <c r="AN6" s="46"/>
       <c r="AO6" s="46"/>
       <c r="AP6" s="15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AQ6" s="38"/>
       <c r="AR6" s="39"/>
@@ -3260,11 +3260,11 @@
       <c r="DQ6" s="39"/>
       <c r="DR6" s="40"/>
       <c r="DS6" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DT6" s="20"/>
       <c r="DU6" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DV6" s="41"/>
       <c r="DW6" s="42"/>
@@ -3275,28 +3275,28 @@
     </row>
     <row r="7" spans="1:131" s="35" customFormat="1" ht="23" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C7" s="43"/>
       <c r="D7" s="43"/>
       <c r="E7" s="43"/>
       <c r="F7" s="43" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G7" s="43"/>
       <c r="H7" s="21"/>
       <c r="I7" s="43" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J7" s="45"/>
       <c r="K7" s="45"/>
       <c r="L7" s="56"/>
       <c r="M7" s="56"/>
       <c r="N7" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O7" s="41"/>
       <c r="P7" s="44"/>
@@ -3306,7 +3306,7 @@
       <c r="T7" s="42"/>
       <c r="U7" s="44"/>
       <c r="V7" s="43" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W7" s="43"/>
       <c r="X7" s="41"/>
@@ -3329,13 +3329,13 @@
       <c r="AO7" s="42"/>
       <c r="AP7" s="44"/>
       <c r="AQ7" s="41" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AR7" s="44"/>
       <c r="AS7" s="41"/>
       <c r="AT7" s="44"/>
       <c r="AU7" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AV7" s="41"/>
       <c r="AW7" s="42"/>
@@ -3414,7 +3414,7 @@
       <c r="DR7" s="42"/>
       <c r="DS7" s="44"/>
       <c r="DT7" s="41" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="DU7" s="42"/>
       <c r="DV7" s="42"/>
@@ -3426,7 +3426,7 @@
     </row>
     <row r="8" spans="1:131" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B8" s="17">
         <v>1</v>

</xml_diff>

<commit_message>
CLDC-3568: Update collection resources for MHCLG name change
</commit_message>
<xml_diff>
--- a/public/files/bulk-upload-lettings-template-2024-25.xlsx
+++ b/public/files/bulk-upload-lettings-template-2024-25.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamuelIvko\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mhclg.sharepoint.com/sites/HousingandplanningandCOREstatistics/Shared Documents/CORE Lettings/01 CORE service/04 Annual log reviews/2024-25/03 Materials for providers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F7A164-145F-401A-B0DA-F89299092402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{296AE3D4-73F7-4BC5-957A-5710BD8CDEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79E053AA-7BEE-4F89-A465-E2DA330BC6D4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="282">
   <si>
     <t>Section</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>What is the property reference?</t>
-  </si>
-  <si>
-    <t>Has the tenant seen or been given access to the DLUHC privacy notice?</t>
   </si>
   <si>
     <t>If known, provide this property’s UPRN</t>
@@ -495,9 +492,6 @@
   </si>
   <si>
     <t>This is how you usually refer to this property on your own systems.</t>
-  </si>
-  <si>
-    <t>Make sure the lead tenant has seen or been given access to the Department for Levelling Up, Housing and Communities (DLUHC) privacy notice before completing this log. This is a legal requirement under data protection legislation.</t>
   </si>
   <si>
     <t>The Unique Property Reference Number (UPRN) is a unique number system created by Ordnance Survey and used by housing providers and various industries across the UK. An example UPRN is 10010457355. 
@@ -809,6 +803,9 @@
     <t>0 - 1</t>
   </si>
   <si>
+    <t>1 - 10</t>
+  </si>
+  <si>
     <t>xxxx.xx</t>
   </si>
   <si>
@@ -895,7 +892,13 @@
     <t>Yes, if household's income is unknown (if field 118 = 2 or 3)</t>
   </si>
   <si>
+    <t xml:space="preserve">Yes, if rent is charged (if field 125 is not empty) </t>
+  </si>
+  <si>
     <t>Yes, if the household does not pay rent (if field 122 = 1) or if the accommodation is not a care home (if field 124 is empty)</t>
+  </si>
+  <si>
+    <t>Yes, if the household doesn't receive housing benefits, or if it is unknown (if field 120 = 3, 9 or 10)</t>
   </si>
   <si>
     <t>Yes, if the household does not need to pay rent or charges after receiving housing benefits (if field 130 is not 1)</t>
@@ -933,16 +936,10 @@
 You can find the location code on the CORE service under 'Schemes', either by searching for the specific location or downloading a csv.</t>
   </si>
   <si>
-    <t>Yes, if rent is charged (if field 125 is not empty), or if there is no charge (if field 122 is 1)</t>
-  </si>
-  <si>
-    <t>Yes, if the household doesn't receive housing benefits, or if it is unknown (if field 120 = 3, 9 or 10), or if there are no charges (if field 122 = 1)</t>
-  </si>
-  <si>
-    <t>Yes, if there are no charges (if field 122 = 1)</t>
-  </si>
-  <si>
-    <t>1 - 11</t>
+    <t>Has the tenant seen or been given access to the MHCLG privacy notice?</t>
+  </si>
+  <si>
+    <t>Make sure the lead tenant has seen or been given access to the Ministry of Housing, Communities and Local Government (MHCLG) privacy notice before completing this log. This is a legal requirement under data protection legislation.</t>
   </si>
 </sst>
 </file>
@@ -1248,9 +1245,6 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1315,9 +1309,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1338,36 +1329,108 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1375,72 +1438,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1661,7 +1658,9 @@
   </sheetPr>
   <dimension ref="A1:EA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="DD1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="DN7" sqref="DN7:DS7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1701,150 +1700,150 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="54" t="s">
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="55" t="s">
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="55"/>
-      <c r="AM1" s="55"/>
-      <c r="AN1" s="55"/>
-      <c r="AO1" s="55"/>
-      <c r="AP1" s="55"/>
-      <c r="AQ1" s="63" t="s">
+      <c r="AL1" s="58"/>
+      <c r="AM1" s="58"/>
+      <c r="AN1" s="58"/>
+      <c r="AO1" s="58"/>
+      <c r="AP1" s="58"/>
+      <c r="AQ1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="AR1" s="64"/>
-      <c r="AS1" s="64"/>
-      <c r="AT1" s="64"/>
-      <c r="AU1" s="64"/>
-      <c r="AV1" s="64"/>
-      <c r="AW1" s="64"/>
-      <c r="AX1" s="64"/>
-      <c r="AY1" s="64"/>
-      <c r="AZ1" s="64"/>
-      <c r="BA1" s="64"/>
-      <c r="BB1" s="64"/>
-      <c r="BC1" s="64"/>
-      <c r="BD1" s="64"/>
-      <c r="BE1" s="64"/>
-      <c r="BF1" s="64"/>
-      <c r="BG1" s="64"/>
-      <c r="BH1" s="64"/>
-      <c r="BI1" s="64"/>
-      <c r="BJ1" s="64"/>
-      <c r="BK1" s="64"/>
-      <c r="BL1" s="64"/>
-      <c r="BM1" s="64"/>
-      <c r="BN1" s="64"/>
-      <c r="BO1" s="64"/>
-      <c r="BP1" s="64"/>
-      <c r="BQ1" s="64"/>
-      <c r="BR1" s="64"/>
-      <c r="BS1" s="64"/>
-      <c r="BT1" s="64"/>
-      <c r="BU1" s="64"/>
-      <c r="BV1" s="64"/>
-      <c r="BW1" s="65"/>
-      <c r="BX1" s="66" t="s">
+      <c r="AR1" s="45"/>
+      <c r="AS1" s="45"/>
+      <c r="AT1" s="45"/>
+      <c r="AU1" s="45"/>
+      <c r="AV1" s="45"/>
+      <c r="AW1" s="45"/>
+      <c r="AX1" s="45"/>
+      <c r="AY1" s="45"/>
+      <c r="AZ1" s="45"/>
+      <c r="BA1" s="45"/>
+      <c r="BB1" s="45"/>
+      <c r="BC1" s="45"/>
+      <c r="BD1" s="45"/>
+      <c r="BE1" s="45"/>
+      <c r="BF1" s="45"/>
+      <c r="BG1" s="45"/>
+      <c r="BH1" s="45"/>
+      <c r="BI1" s="45"/>
+      <c r="BJ1" s="45"/>
+      <c r="BK1" s="45"/>
+      <c r="BL1" s="45"/>
+      <c r="BM1" s="45"/>
+      <c r="BN1" s="45"/>
+      <c r="BO1" s="45"/>
+      <c r="BP1" s="45"/>
+      <c r="BQ1" s="45"/>
+      <c r="BR1" s="45"/>
+      <c r="BS1" s="45"/>
+      <c r="BT1" s="45"/>
+      <c r="BU1" s="45"/>
+      <c r="BV1" s="45"/>
+      <c r="BW1" s="46"/>
+      <c r="BX1" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="BY1" s="67"/>
-      <c r="BZ1" s="67"/>
-      <c r="CA1" s="67"/>
-      <c r="CB1" s="67"/>
-      <c r="CC1" s="67"/>
-      <c r="CD1" s="67"/>
-      <c r="CE1" s="67"/>
-      <c r="CF1" s="67"/>
-      <c r="CG1" s="67"/>
-      <c r="CH1" s="67"/>
-      <c r="CI1" s="67"/>
-      <c r="CJ1" s="67"/>
-      <c r="CK1" s="67"/>
-      <c r="CL1" s="67"/>
-      <c r="CM1" s="67"/>
-      <c r="CN1" s="67"/>
-      <c r="CO1" s="67"/>
-      <c r="CP1" s="67"/>
-      <c r="CQ1" s="67"/>
-      <c r="CR1" s="68"/>
-      <c r="CS1" s="69" t="s">
+      <c r="BY1" s="51"/>
+      <c r="BZ1" s="51"/>
+      <c r="CA1" s="51"/>
+      <c r="CB1" s="51"/>
+      <c r="CC1" s="51"/>
+      <c r="CD1" s="51"/>
+      <c r="CE1" s="51"/>
+      <c r="CF1" s="51"/>
+      <c r="CG1" s="51"/>
+      <c r="CH1" s="51"/>
+      <c r="CI1" s="51"/>
+      <c r="CJ1" s="51"/>
+      <c r="CK1" s="51"/>
+      <c r="CL1" s="51"/>
+      <c r="CM1" s="51"/>
+      <c r="CN1" s="51"/>
+      <c r="CO1" s="51"/>
+      <c r="CP1" s="51"/>
+      <c r="CQ1" s="51"/>
+      <c r="CR1" s="52"/>
+      <c r="CS1" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="CT1" s="70"/>
-      <c r="CU1" s="70"/>
-      <c r="CV1" s="70"/>
-      <c r="CW1" s="70"/>
-      <c r="CX1" s="70"/>
-      <c r="CY1" s="70"/>
-      <c r="CZ1" s="70"/>
-      <c r="DA1" s="70"/>
-      <c r="DB1" s="70"/>
-      <c r="DC1" s="70"/>
-      <c r="DD1" s="70"/>
-      <c r="DE1" s="70"/>
-      <c r="DF1" s="70"/>
-      <c r="DG1" s="70"/>
-      <c r="DH1" s="70"/>
-      <c r="DI1" s="70"/>
-      <c r="DJ1" s="70"/>
-      <c r="DK1" s="70"/>
-      <c r="DL1" s="70"/>
-      <c r="DM1" s="71"/>
-      <c r="DN1" s="57" t="s">
+      <c r="CT1" s="54"/>
+      <c r="CU1" s="54"/>
+      <c r="CV1" s="54"/>
+      <c r="CW1" s="54"/>
+      <c r="CX1" s="54"/>
+      <c r="CY1" s="54"/>
+      <c r="CZ1" s="54"/>
+      <c r="DA1" s="54"/>
+      <c r="DB1" s="54"/>
+      <c r="DC1" s="54"/>
+      <c r="DD1" s="54"/>
+      <c r="DE1" s="54"/>
+      <c r="DF1" s="54"/>
+      <c r="DG1" s="54"/>
+      <c r="DH1" s="54"/>
+      <c r="DI1" s="54"/>
+      <c r="DJ1" s="54"/>
+      <c r="DK1" s="54"/>
+      <c r="DL1" s="54"/>
+      <c r="DM1" s="55"/>
+      <c r="DN1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="DO1" s="58"/>
-      <c r="DP1" s="58"/>
-      <c r="DQ1" s="58"/>
-      <c r="DR1" s="58"/>
-      <c r="DS1" s="58"/>
-      <c r="DT1" s="58"/>
-      <c r="DU1" s="58"/>
-      <c r="DV1" s="58"/>
-      <c r="DW1" s="58"/>
-      <c r="DX1" s="58"/>
-      <c r="DY1" s="58"/>
-      <c r="DZ1" s="58"/>
-      <c r="EA1" s="59"/>
+      <c r="DO1" s="39"/>
+      <c r="DP1" s="39"/>
+      <c r="DQ1" s="39"/>
+      <c r="DR1" s="39"/>
+      <c r="DS1" s="39"/>
+      <c r="DT1" s="39"/>
+      <c r="DU1" s="39"/>
+      <c r="DV1" s="39"/>
+      <c r="DW1" s="39"/>
+      <c r="DX1" s="39"/>
+      <c r="DY1" s="39"/>
+      <c r="DZ1" s="39"/>
+      <c r="EA1" s="40"/>
     </row>
     <row r="2" spans="1:131" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1892,1935 +1891,1994 @@
       <c r="O2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="36" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AF2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AK2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AL2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AM2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AN2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AO2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AP2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AS2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AT2" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="AT2" s="8" t="s">
+      <c r="AU2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AV2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AW2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AX2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AY2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="BA2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BA2" s="4" t="s">
+      <c r="BB2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="BB2" s="4" t="s">
+      <c r="BC2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="BC2" s="4" t="s">
+      <c r="BD2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BD2" s="4" t="s">
+      <c r="BE2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="BE2" s="4" t="s">
+      <c r="BF2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BF2" s="4" t="s">
+      <c r="BG2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BG2" s="4" t="s">
+      <c r="BH2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BH2" s="4" t="s">
+      <c r="BI2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="BI2" s="4" t="s">
+      <c r="BJ2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BJ2" s="4" t="s">
+      <c r="BK2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="BK2" s="4" t="s">
+      <c r="BL2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="BL2" s="4" t="s">
+      <c r="BM2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="BM2" s="4" t="s">
+      <c r="BN2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BN2" s="4" t="s">
+      <c r="BO2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="BO2" s="4" t="s">
+      <c r="BP2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="BP2" s="4" t="s">
+      <c r="BQ2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="BQ2" s="4" t="s">
+      <c r="BR2" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="BR2" s="4" t="s">
+      <c r="BS2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="BS2" s="4" t="s">
+      <c r="BT2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="BT2" s="4" t="s">
+      <c r="BU2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="BU2" s="4" t="s">
+      <c r="BV2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BV2" s="4" t="s">
+      <c r="BW2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BW2" s="4" t="s">
+      <c r="BX2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BX2" s="4" t="s">
+      <c r="BY2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BY2" s="4" t="s">
+      <c r="BZ2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="BZ2" s="4" t="s">
+      <c r="CA2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="CA2" s="4" t="s">
+      <c r="CB2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="CB2" s="4" t="s">
+      <c r="CC2" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="CC2" s="4" t="s">
+      <c r="CD2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="CD2" s="4" t="s">
+      <c r="CE2" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="CE2" s="4" t="s">
+      <c r="CF2" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="CF2" s="4" t="s">
+      <c r="CG2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="CG2" s="4" t="s">
+      <c r="CH2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="CH2" s="4" t="s">
+      <c r="CI2" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="CI2" s="4" t="s">
+      <c r="CJ2" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="CJ2" s="4" t="s">
+      <c r="CK2" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="CK2" s="4" t="s">
+      <c r="CL2" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="CL2" s="4" t="s">
+      <c r="CM2" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="CM2" s="4" t="s">
+      <c r="CN2" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="CN2" s="4" t="s">
+      <c r="CO2" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="CO2" s="4" t="s">
+      <c r="CP2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="CP2" s="4" t="s">
+      <c r="CQ2" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="CQ2" s="4" t="s">
+      <c r="CR2" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="CR2" s="4" t="s">
+      <c r="CS2" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="CS2" s="4" t="s">
+      <c r="CT2" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="CT2" s="4" t="s">
+      <c r="CU2" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="CU2" s="4" t="s">
+      <c r="CV2" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="CV2" s="4" t="s">
+      <c r="CW2" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="CW2" s="4" t="s">
+      <c r="CX2" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="CX2" s="4" t="s">
+      <c r="CY2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="CY2" s="4" t="s">
+      <c r="CZ2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="CZ2" s="4" t="s">
+      <c r="DA2" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="DA2" s="4" t="s">
+      <c r="DB2" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="DB2" s="4" t="s">
+      <c r="DC2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="DC2" s="4" t="s">
+      <c r="DD2" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="DD2" s="4" t="s">
+      <c r="DE2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="DE2" s="4" t="s">
+      <c r="DF2" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="DF2" s="4" t="s">
+      <c r="DG2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="DG2" s="4" t="s">
+      <c r="DH2" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="DH2" s="4" t="s">
+      <c r="DI2" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="DI2" s="4" t="s">
+      <c r="DJ2" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="DJ2" s="4" t="s">
+      <c r="DK2" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="DK2" s="4" t="s">
+      <c r="DL2" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="DL2" s="9" t="s">
+      <c r="DM2" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="DM2" s="4" t="s">
+      <c r="DN2" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="DN2" s="4" t="s">
+      <c r="DO2" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="DP2" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="DO2" s="4" t="s">
+      <c r="DQ2" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="DP2" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="DQ2" s="4" t="s">
+      <c r="DR2" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="DR2" s="4" t="s">
+      <c r="DS2" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="DS2" s="4" t="s">
+      <c r="DT2" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="DT2" s="4" t="s">
+      <c r="DU2" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="DU2" s="10" t="s">
+      <c r="DV2" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="DV2" s="4" t="s">
+      <c r="DW2" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="DW2" s="4" t="s">
+      <c r="DX2" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="DX2" s="4" t="s">
+      <c r="DY2" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="DY2" s="4" t="s">
+      <c r="DZ2" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="DZ2" s="4" t="s">
+      <c r="EA2" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="EA2" s="4" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:131" ht="368" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="D3" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="13" t="s">
+      <c r="M3" s="10"/>
+      <c r="N3" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11" t="s">
+      <c r="O3" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="P3" s="37" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q3" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="P3" s="29" t="s">
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="W3" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="23" t="s">
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="W3" s="23" t="s">
+      <c r="Z3" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11" t="s">
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="Z3" s="11" t="s">
+      <c r="AD3" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="AE3" s="64" t="s">
         <v>153</v>
       </c>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="11"/>
-      <c r="AC3" s="11" t="s">
+      <c r="AF3" s="65"/>
+      <c r="AG3" s="65"/>
+      <c r="AH3" s="64" t="s">
         <v>154</v>
       </c>
-      <c r="AD3" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="AE3" s="50" t="s">
+      <c r="AI3" s="65"/>
+      <c r="AJ3" s="65"/>
+      <c r="AK3" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="AF3" s="51"/>
-      <c r="AG3" s="51"/>
-      <c r="AH3" s="50" t="s">
+      <c r="AL3" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="AI3" s="51"/>
-      <c r="AJ3" s="51"/>
-      <c r="AK3" s="11" t="s">
+      <c r="AM3" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="AL3" s="11" t="s">
+      <c r="AN3" s="10"/>
+      <c r="AO3" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="AM3" s="11" t="s">
+      <c r="AP3" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="AN3" s="11"/>
-      <c r="AO3" s="11" t="s">
+      <c r="AQ3" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="AP3" s="11" t="s">
+      <c r="AR3" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="AQ3" s="11" t="s">
+      <c r="AS3" s="27"/>
+      <c r="AT3" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="AR3" s="27" t="s">
+      <c r="AU3" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="AV3" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="AS3" s="28"/>
-      <c r="AT3" s="27" t="s">
+      <c r="AW3" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="AU3" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="AV3" s="11" t="s">
+      <c r="AX3" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="AY3" s="10"/>
+      <c r="AZ3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="BA3" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="BB3" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="BC3" s="10"/>
+      <c r="BD3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="BE3" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="BF3" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="BG3" s="10"/>
+      <c r="BH3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="BI3" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="BJ3" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="BK3" s="10"/>
+      <c r="BL3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="BM3" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="BN3" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="BO3" s="10"/>
+      <c r="BP3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="BQ3" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="BR3" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="BS3" s="10"/>
+      <c r="BT3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="BU3" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="BV3" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="BW3" s="10"/>
+      <c r="BX3" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="AW3" s="11" t="s">
+      <c r="BY3" s="10"/>
+      <c r="BZ3" s="10"/>
+      <c r="CA3" s="10"/>
+      <c r="CB3" s="10"/>
+      <c r="CC3" s="10"/>
+      <c r="CD3" s="10"/>
+      <c r="CE3" s="10"/>
+      <c r="CF3" s="10"/>
+      <c r="CG3" s="10"/>
+      <c r="CH3" s="10"/>
+      <c r="CI3" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="AX3" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="AY3" s="11"/>
-      <c r="AZ3" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="BA3" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="BB3" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="BC3" s="11"/>
-      <c r="BD3" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="BE3" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="BF3" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="BG3" s="11"/>
-      <c r="BH3" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="BI3" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="BJ3" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="BK3" s="11"/>
-      <c r="BL3" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="BM3" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="BN3" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="BO3" s="11"/>
-      <c r="BP3" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="BQ3" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="BR3" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="BS3" s="11"/>
-      <c r="BT3" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="BU3" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="BV3" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="BW3" s="11"/>
-      <c r="BX3" s="11" t="s">
+      <c r="CJ3" s="10"/>
+      <c r="CK3" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="BY3" s="11"/>
-      <c r="BZ3" s="11"/>
-      <c r="CA3" s="11"/>
-      <c r="CB3" s="11"/>
-      <c r="CC3" s="11"/>
-      <c r="CD3" s="11"/>
-      <c r="CE3" s="11"/>
-      <c r="CF3" s="11"/>
-      <c r="CG3" s="11"/>
-      <c r="CH3" s="11"/>
-      <c r="CI3" s="11" t="s">
+      <c r="CL3" s="10"/>
+      <c r="CM3" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="CJ3" s="11"/>
-      <c r="CK3" s="11" t="s">
+      <c r="CN3" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="CL3" s="11"/>
-      <c r="CM3" s="11" t="s">
+      <c r="CO3" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="CN3" s="11" t="s">
+      <c r="CP3" s="10"/>
+      <c r="CQ3" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="CO3" s="11" t="s">
+      <c r="CR3" s="10"/>
+      <c r="CS3" s="10"/>
+      <c r="CT3" s="10"/>
+      <c r="CU3" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="CP3" s="11"/>
-      <c r="CQ3" s="11" t="s">
+      <c r="CV3" s="10"/>
+      <c r="CW3" s="10"/>
+      <c r="CX3" s="10"/>
+      <c r="CY3" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="CR3" s="11"/>
-      <c r="CS3" s="11"/>
-      <c r="CT3" s="11"/>
-      <c r="CU3" s="11" t="s">
+      <c r="CZ3" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="CV3" s="11"/>
-      <c r="CW3" s="11"/>
-      <c r="CX3" s="11"/>
-      <c r="CY3" s="11" t="s">
+      <c r="DA3" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="CZ3" s="24" t="s">
+      <c r="DB3" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="DC3" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="DA3" s="24" t="s">
+      <c r="DD3" s="10"/>
+      <c r="DE3" s="10"/>
+      <c r="DF3" s="10"/>
+      <c r="DG3" s="10"/>
+      <c r="DH3" s="10"/>
+      <c r="DI3" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="DB3" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="DC3" s="11" t="s">
+      <c r="DJ3" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="DD3" s="11"/>
-      <c r="DE3" s="11"/>
-      <c r="DF3" s="11"/>
-      <c r="DG3" s="11"/>
-      <c r="DH3" s="11"/>
-      <c r="DI3" s="11" t="s">
+      <c r="DK3" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="DJ3" s="11" t="s">
+      <c r="DL3" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="DK3" s="11" t="s">
+      <c r="DM3" s="10"/>
+      <c r="DN3" s="10"/>
+      <c r="DO3" s="10"/>
+      <c r="DP3" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="DL3" s="14" t="s">
+      <c r="DQ3" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="DM3" s="11"/>
-      <c r="DN3" s="11"/>
-      <c r="DO3" s="11"/>
-      <c r="DP3" s="11" t="s">
+      <c r="DR3" s="10"/>
+      <c r="DS3" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="DQ3" s="11" t="s">
+      <c r="DT3" s="10"/>
+      <c r="DU3" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="DR3" s="11"/>
-      <c r="DS3" s="11" t="s">
+      <c r="DV3" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="DT3" s="11"/>
-      <c r="DU3" s="11" t="s">
+      <c r="DW3" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="DV3" s="23" t="s">
+      <c r="DX3" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="DW3" s="23" t="s">
+      <c r="DY3" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="DX3" s="23" t="s">
+      <c r="DZ3" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="DY3" s="23" t="s">
+      <c r="EA3" s="10" t="s">
         <v>190</v>
-      </c>
-      <c r="DZ3" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="EA3" s="11" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:131" ht="115" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="69" t="s">
+        <v>192</v>
+      </c>
+      <c r="C4" s="70"/>
+      <c r="D4" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="E4" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="15" t="s">
+      <c r="F4" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="I4" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="J4" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="K4" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="P4" s="28">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="R4" s="66" t="s">
+        <v>192</v>
+      </c>
+      <c r="S4" s="71"/>
+      <c r="T4" s="66" t="s">
+        <v>199</v>
+      </c>
+      <c r="U4" s="71"/>
+      <c r="V4" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="W4" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="X4" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="Y4" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="Z4" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="AA4" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB4" s="66" t="s">
         <v>194</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="H4" s="16" t="s">
+      <c r="AC4" s="71"/>
+      <c r="AD4" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="AE4" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="AF4" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="I4" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="J4" s="15" t="s">
+      <c r="AG4" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="AH4" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="AI4" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="AJ4" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="AK4" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="AL4" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="AM4" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="AN4" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO4" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="AP4" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="AQ4" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="AR4" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="AS4" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="AT4" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="AU4" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="AV4" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="AW4" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="AX4" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="AY4" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="AZ4" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="BA4" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="BB4" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="BC4" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="BD4" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="BE4" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="BF4" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="BG4" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="BH4" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="BI4" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="BJ4" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="BK4" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="BL4" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="BM4" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="BN4" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="BO4" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="BP4" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="BQ4" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="BR4" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="BS4" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="BT4" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="BU4" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="BV4" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="BW4" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="BX4" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="BY4" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="BZ4" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="CA4" s="49"/>
+      <c r="CB4" s="47" t="s">
+        <v>223</v>
+      </c>
+      <c r="CC4" s="48"/>
+      <c r="CD4" s="48"/>
+      <c r="CE4" s="48"/>
+      <c r="CF4" s="48"/>
+      <c r="CG4" s="49"/>
+      <c r="CH4" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="CI4" s="47" t="s">
+        <v>223</v>
+      </c>
+      <c r="CJ4" s="48"/>
+      <c r="CK4" s="48"/>
+      <c r="CL4" s="48"/>
+      <c r="CM4" s="48"/>
+      <c r="CN4" s="48"/>
+      <c r="CO4" s="48"/>
+      <c r="CP4" s="48"/>
+      <c r="CQ4" s="48"/>
+      <c r="CR4" s="49"/>
+      <c r="CS4" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="CT4" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="CU4" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="CV4" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="L4" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="N4" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="O4" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="P4" s="30">
+      <c r="CW4" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="CX4" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="CY4" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="CZ4" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="DA4" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="DB4" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="DC4" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="DD4" s="47" t="s">
+        <v>223</v>
+      </c>
+      <c r="DE4" s="48"/>
+      <c r="DF4" s="48"/>
+      <c r="DG4" s="48"/>
+      <c r="DH4" s="49"/>
+      <c r="DI4" s="47" t="s">
+        <v>194</v>
+      </c>
+      <c r="DJ4" s="48"/>
+      <c r="DK4" s="48"/>
+      <c r="DL4" s="49"/>
+      <c r="DM4" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="DN4" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="DO4" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="DP4" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="DQ4" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="DR4" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="DS4" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="DT4" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="DU4" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="DV4" s="48"/>
+      <c r="DW4" s="48"/>
+      <c r="DX4" s="48"/>
+      <c r="DY4" s="49"/>
+      <c r="DZ4" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="EA4" s="14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:131" s="32" customFormat="1" ht="137.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="66" t="s">
+        <v>240</v>
+      </c>
+      <c r="C5" s="68"/>
+      <c r="D5" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="H5" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="N5" s="66" t="s">
+        <v>241</v>
+      </c>
+      <c r="O5" s="68"/>
+      <c r="P5" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q5" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="R5" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="S5" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="T5" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="U5" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="V5" s="66" t="s">
+        <v>245</v>
+      </c>
+      <c r="W5" s="68"/>
+      <c r="X5" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="Y5" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="Z5" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA5" s="66" t="s">
+        <v>246</v>
+      </c>
+      <c r="AB5" s="68"/>
+      <c r="AC5" s="68"/>
+      <c r="AD5" s="68"/>
+      <c r="AE5" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="AF5" s="68"/>
+      <c r="AG5" s="68"/>
+      <c r="AH5" s="66" t="s">
+        <v>241</v>
+      </c>
+      <c r="AI5" s="68"/>
+      <c r="AJ5" s="68"/>
+      <c r="AK5" s="66" t="s">
+        <v>240</v>
+      </c>
+      <c r="AL5" s="68"/>
+      <c r="AM5" s="68"/>
+      <c r="AN5" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="AO5" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="AP5" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="AQ5" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="AR5" s="48"/>
+      <c r="AS5" s="48"/>
+      <c r="AT5" s="48"/>
+      <c r="AU5" s="49"/>
+      <c r="AV5" s="41" t="s">
+        <v>251</v>
+      </c>
+      <c r="AW5" s="42"/>
+      <c r="AX5" s="42"/>
+      <c r="AY5" s="43"/>
+      <c r="AZ5" s="41" t="s">
+        <v>276</v>
+      </c>
+      <c r="BA5" s="42"/>
+      <c r="BB5" s="42"/>
+      <c r="BC5" s="43"/>
+      <c r="BD5" s="41" t="s">
+        <v>252</v>
+      </c>
+      <c r="BE5" s="42"/>
+      <c r="BF5" s="42"/>
+      <c r="BG5" s="43"/>
+      <c r="BH5" s="41" t="s">
+        <v>253</v>
+      </c>
+      <c r="BI5" s="42"/>
+      <c r="BJ5" s="42"/>
+      <c r="BK5" s="43"/>
+      <c r="BL5" s="41" t="s">
+        <v>254</v>
+      </c>
+      <c r="BM5" s="42"/>
+      <c r="BN5" s="42"/>
+      <c r="BO5" s="43"/>
+      <c r="BP5" s="41" t="s">
+        <v>255</v>
+      </c>
+      <c r="BQ5" s="42"/>
+      <c r="BR5" s="42"/>
+      <c r="BS5" s="43"/>
+      <c r="BT5" s="41" t="s">
+        <v>256</v>
+      </c>
+      <c r="BU5" s="42"/>
+      <c r="BV5" s="42"/>
+      <c r="BW5" s="43"/>
+      <c r="BX5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="BY5" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="BZ5" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="CA5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="CB5" s="47" t="s">
+        <v>259</v>
+      </c>
+      <c r="CC5" s="48"/>
+      <c r="CD5" s="48"/>
+      <c r="CE5" s="49"/>
+      <c r="CF5" s="47" t="s">
+        <v>260</v>
+      </c>
+      <c r="CG5" s="49"/>
+      <c r="CH5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="CI5" s="47" t="s">
+        <v>261</v>
+      </c>
+      <c r="CJ5" s="48"/>
+      <c r="CK5" s="48"/>
+      <c r="CL5" s="48"/>
+      <c r="CM5" s="48"/>
+      <c r="CN5" s="48"/>
+      <c r="CO5" s="48"/>
+      <c r="CP5" s="48"/>
+      <c r="CQ5" s="48"/>
+      <c r="CR5" s="49"/>
+      <c r="CS5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="CT5" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="CU5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="CV5" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="CW5" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="CX5" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="CY5" s="49"/>
+      <c r="CZ5" s="47" t="s">
+        <v>263</v>
+      </c>
+      <c r="DA5" s="49"/>
+      <c r="DB5" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="DC5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="DD5" s="59" t="s">
+        <v>264</v>
+      </c>
+      <c r="DE5" s="60"/>
+      <c r="DF5" s="60"/>
+      <c r="DG5" s="60"/>
+      <c r="DH5" s="61"/>
+      <c r="DI5" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="DJ5" s="48"/>
+      <c r="DK5" s="48"/>
+      <c r="DL5" s="49"/>
+      <c r="DM5" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="DN5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="DO5" s="47" t="s">
+        <v>265</v>
+      </c>
+      <c r="DP5" s="49"/>
+      <c r="DQ5" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="DR5" s="49"/>
+      <c r="DS5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="DT5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="DU5" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="DV5" s="47" t="s">
+        <v>267</v>
+      </c>
+      <c r="DW5" s="48"/>
+      <c r="DX5" s="48"/>
+      <c r="DY5" s="49"/>
+      <c r="DZ5" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="EA5" s="14" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:131" s="33" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="62" t="s">
+        <v>271</v>
+      </c>
+      <c r="G6" s="62"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="66" t="s">
+        <v>273</v>
+      </c>
+      <c r="R6" s="68"/>
+      <c r="S6" s="68"/>
+      <c r="T6" s="68"/>
+      <c r="U6" s="68"/>
+      <c r="V6" s="68"/>
+      <c r="W6" s="68"/>
+      <c r="X6" s="68"/>
+      <c r="Y6" s="66"/>
+      <c r="Z6" s="66"/>
+      <c r="AA6" s="66" t="s">
+        <v>273</v>
+      </c>
+      <c r="AB6" s="68"/>
+      <c r="AC6" s="68"/>
+      <c r="AD6" s="68"/>
+      <c r="AE6" s="66"/>
+      <c r="AF6" s="66"/>
+      <c r="AG6" s="66"/>
+      <c r="AH6" s="66"/>
+      <c r="AI6" s="66"/>
+      <c r="AJ6" s="66"/>
+      <c r="AK6" s="66"/>
+      <c r="AL6" s="66"/>
+      <c r="AM6" s="66"/>
+      <c r="AN6" s="66"/>
+      <c r="AO6" s="66"/>
+      <c r="AP6" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="AQ6" s="47"/>
+      <c r="AR6" s="48"/>
+      <c r="AS6" s="48"/>
+      <c r="AT6" s="48"/>
+      <c r="AU6" s="48"/>
+      <c r="AV6" s="48"/>
+      <c r="AW6" s="48"/>
+      <c r="AX6" s="48"/>
+      <c r="AY6" s="48"/>
+      <c r="AZ6" s="48"/>
+      <c r="BA6" s="48"/>
+      <c r="BB6" s="48"/>
+      <c r="BC6" s="48"/>
+      <c r="BD6" s="48"/>
+      <c r="BE6" s="48"/>
+      <c r="BF6" s="48"/>
+      <c r="BG6" s="48"/>
+      <c r="BH6" s="48"/>
+      <c r="BI6" s="48"/>
+      <c r="BJ6" s="48"/>
+      <c r="BK6" s="48"/>
+      <c r="BL6" s="48"/>
+      <c r="BM6" s="48"/>
+      <c r="BN6" s="48"/>
+      <c r="BO6" s="48"/>
+      <c r="BP6" s="48"/>
+      <c r="BQ6" s="48"/>
+      <c r="BR6" s="48"/>
+      <c r="BS6" s="48"/>
+      <c r="BT6" s="48"/>
+      <c r="BU6" s="48"/>
+      <c r="BV6" s="48"/>
+      <c r="BW6" s="49"/>
+      <c r="BX6" s="47"/>
+      <c r="BY6" s="48"/>
+      <c r="BZ6" s="48"/>
+      <c r="CA6" s="48"/>
+      <c r="CB6" s="48"/>
+      <c r="CC6" s="48"/>
+      <c r="CD6" s="48"/>
+      <c r="CE6" s="48"/>
+      <c r="CF6" s="48"/>
+      <c r="CG6" s="48"/>
+      <c r="CH6" s="48"/>
+      <c r="CI6" s="48"/>
+      <c r="CJ6" s="48"/>
+      <c r="CK6" s="48"/>
+      <c r="CL6" s="48"/>
+      <c r="CM6" s="48"/>
+      <c r="CN6" s="48"/>
+      <c r="CO6" s="48"/>
+      <c r="CP6" s="48"/>
+      <c r="CQ6" s="48"/>
+      <c r="CR6" s="49"/>
+      <c r="CS6" s="47"/>
+      <c r="CT6" s="48"/>
+      <c r="CU6" s="48"/>
+      <c r="CV6" s="48"/>
+      <c r="CW6" s="48"/>
+      <c r="CX6" s="48"/>
+      <c r="CY6" s="48"/>
+      <c r="CZ6" s="48"/>
+      <c r="DA6" s="48"/>
+      <c r="DB6" s="48"/>
+      <c r="DC6" s="48"/>
+      <c r="DD6" s="48"/>
+      <c r="DE6" s="48"/>
+      <c r="DF6" s="48"/>
+      <c r="DG6" s="48"/>
+      <c r="DH6" s="48"/>
+      <c r="DI6" s="48"/>
+      <c r="DJ6" s="48"/>
+      <c r="DK6" s="48"/>
+      <c r="DL6" s="48"/>
+      <c r="DM6" s="49"/>
+      <c r="DN6" s="47"/>
+      <c r="DO6" s="48"/>
+      <c r="DP6" s="48"/>
+      <c r="DQ6" s="48"/>
+      <c r="DR6" s="49"/>
+      <c r="DS6" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="DT6" s="19"/>
+      <c r="DU6" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="DV6" s="59"/>
+      <c r="DW6" s="60"/>
+      <c r="DX6" s="60"/>
+      <c r="DY6" s="60"/>
+      <c r="DZ6" s="60"/>
+      <c r="EA6" s="61"/>
+    </row>
+    <row r="7" spans="1:131" s="33" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62" t="s">
+        <v>241</v>
+      </c>
+      <c r="G7" s="62"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="62" t="s">
+        <v>241</v>
+      </c>
+      <c r="J7" s="68"/>
+      <c r="K7" s="68"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
+      <c r="N7" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="O7" s="59"/>
+      <c r="P7" s="61"/>
+      <c r="Q7" s="59"/>
+      <c r="R7" s="60"/>
+      <c r="S7" s="60"/>
+      <c r="T7" s="60"/>
+      <c r="U7" s="61"/>
+      <c r="V7" s="62" t="s">
+        <v>241</v>
+      </c>
+      <c r="W7" s="62"/>
+      <c r="X7" s="59"/>
+      <c r="Y7" s="60"/>
+      <c r="Z7" s="60"/>
+      <c r="AA7" s="60"/>
+      <c r="AB7" s="60"/>
+      <c r="AC7" s="60"/>
+      <c r="AD7" s="60"/>
+      <c r="AE7" s="60"/>
+      <c r="AF7" s="60"/>
+      <c r="AG7" s="60"/>
+      <c r="AH7" s="60"/>
+      <c r="AI7" s="60"/>
+      <c r="AJ7" s="61"/>
+      <c r="AK7" s="59"/>
+      <c r="AL7" s="60"/>
+      <c r="AM7" s="60"/>
+      <c r="AN7" s="60"/>
+      <c r="AO7" s="60"/>
+      <c r="AP7" s="61"/>
+      <c r="AQ7" s="59" t="s">
+        <v>241</v>
+      </c>
+      <c r="AR7" s="61"/>
+      <c r="AS7" s="59"/>
+      <c r="AT7" s="61"/>
+      <c r="AU7" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="AV7" s="59"/>
+      <c r="AW7" s="60"/>
+      <c r="AX7" s="60"/>
+      <c r="AY7" s="60"/>
+      <c r="AZ7" s="60"/>
+      <c r="BA7" s="60"/>
+      <c r="BB7" s="60"/>
+      <c r="BC7" s="60"/>
+      <c r="BD7" s="60"/>
+      <c r="BE7" s="60"/>
+      <c r="BF7" s="60"/>
+      <c r="BG7" s="60"/>
+      <c r="BH7" s="60"/>
+      <c r="BI7" s="60"/>
+      <c r="BJ7" s="60"/>
+      <c r="BK7" s="60"/>
+      <c r="BL7" s="60"/>
+      <c r="BM7" s="60"/>
+      <c r="BN7" s="60"/>
+      <c r="BO7" s="60"/>
+      <c r="BP7" s="60"/>
+      <c r="BQ7" s="60"/>
+      <c r="BR7" s="60"/>
+      <c r="BS7" s="60"/>
+      <c r="BT7" s="60"/>
+      <c r="BU7" s="60"/>
+      <c r="BV7" s="60"/>
+      <c r="BW7" s="61"/>
+      <c r="BX7" s="59"/>
+      <c r="BY7" s="60"/>
+      <c r="BZ7" s="60"/>
+      <c r="CA7" s="60"/>
+      <c r="CB7" s="60"/>
+      <c r="CC7" s="60"/>
+      <c r="CD7" s="60"/>
+      <c r="CE7" s="60"/>
+      <c r="CF7" s="60"/>
+      <c r="CG7" s="60"/>
+      <c r="CH7" s="60"/>
+      <c r="CI7" s="60"/>
+      <c r="CJ7" s="60"/>
+      <c r="CK7" s="60"/>
+      <c r="CL7" s="60"/>
+      <c r="CM7" s="60"/>
+      <c r="CN7" s="60"/>
+      <c r="CO7" s="60"/>
+      <c r="CP7" s="60"/>
+      <c r="CQ7" s="60"/>
+      <c r="CR7" s="61"/>
+      <c r="CS7" s="59"/>
+      <c r="CT7" s="60"/>
+      <c r="CU7" s="60"/>
+      <c r="CV7" s="60"/>
+      <c r="CW7" s="60"/>
+      <c r="CX7" s="60"/>
+      <c r="CY7" s="60"/>
+      <c r="CZ7" s="60"/>
+      <c r="DA7" s="60"/>
+      <c r="DB7" s="60"/>
+      <c r="DC7" s="60"/>
+      <c r="DD7" s="60"/>
+      <c r="DE7" s="60"/>
+      <c r="DF7" s="60"/>
+      <c r="DG7" s="60"/>
+      <c r="DH7" s="60"/>
+      <c r="DI7" s="60"/>
+      <c r="DJ7" s="60"/>
+      <c r="DK7" s="60"/>
+      <c r="DL7" s="60"/>
+      <c r="DM7" s="61"/>
+      <c r="DN7" s="59"/>
+      <c r="DO7" s="60"/>
+      <c r="DP7" s="60"/>
+      <c r="DQ7" s="60"/>
+      <c r="DR7" s="60"/>
+      <c r="DS7" s="61"/>
+      <c r="DT7" s="59" t="s">
+        <v>241</v>
+      </c>
+      <c r="DU7" s="60"/>
+      <c r="DV7" s="60"/>
+      <c r="DW7" s="60"/>
+      <c r="DX7" s="60"/>
+      <c r="DY7" s="60"/>
+      <c r="DZ7" s="62"/>
+      <c r="EA7" s="62"/>
+    </row>
+    <row r="8" spans="1:131" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="B8" s="16">
         <v>1</v>
       </c>
-      <c r="Q4" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="R4" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="S4" s="49"/>
-      <c r="T4" s="46" t="s">
-        <v>201</v>
-      </c>
-      <c r="U4" s="49"/>
-      <c r="V4" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="W4" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="X4" s="25" t="s">
-        <v>207</v>
-      </c>
-      <c r="Y4" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="Z4" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="AA4" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="AB4" s="46" t="s">
-        <v>196</v>
-      </c>
-      <c r="AC4" s="49"/>
-      <c r="AD4" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="AE4" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="AF4" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="AG4" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="AH4" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="AI4" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="AJ4" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="AK4" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="AL4" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="AM4" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="AN4" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="AO4" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="AP4" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="AQ4" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="AR4" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="AS4" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="AT4" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="AU4" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="AV4" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="AW4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="AX4" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="AY4" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="AZ4" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="BA4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="BB4" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="BC4" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="BD4" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="BE4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="BF4" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="BG4" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="BH4" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="BI4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="BJ4" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="BK4" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="BL4" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="BM4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="BN4" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="BO4" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="BP4" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="BQ4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="BR4" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="BS4" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="BT4" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="BU4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="BV4" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="BW4" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="BX4" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="BY4" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="BZ4" s="38" t="s">
-        <v>214</v>
-      </c>
-      <c r="CA4" s="40"/>
-      <c r="CB4" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="CC4" s="39"/>
-      <c r="CD4" s="39"/>
-      <c r="CE4" s="39"/>
-      <c r="CF4" s="39"/>
-      <c r="CG4" s="40"/>
-      <c r="CH4" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="CI4" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="CJ4" s="39"/>
-      <c r="CK4" s="39"/>
-      <c r="CL4" s="39"/>
-      <c r="CM4" s="39"/>
-      <c r="CN4" s="39"/>
-      <c r="CO4" s="39"/>
-      <c r="CP4" s="39"/>
-      <c r="CQ4" s="39"/>
-      <c r="CR4" s="40"/>
-      <c r="CS4" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="CT4" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="CU4" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="CV4" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="CW4" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="CX4" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="CY4" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="CZ4" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="DA4" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="DB4" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="DC4" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="DD4" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="DE4" s="39"/>
-      <c r="DF4" s="39"/>
-      <c r="DG4" s="39"/>
-      <c r="DH4" s="40"/>
-      <c r="DI4" s="38" t="s">
-        <v>196</v>
-      </c>
-      <c r="DJ4" s="39"/>
-      <c r="DK4" s="39"/>
-      <c r="DL4" s="40"/>
-      <c r="DM4" s="17" t="s">
-        <v>234</v>
-      </c>
-      <c r="DN4" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="DO4" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="DP4" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="DQ4" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="DR4" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="DS4" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="DT4" s="18" t="s">
-        <v>282</v>
-      </c>
-      <c r="DU4" s="38" t="s">
-        <v>239</v>
-      </c>
-      <c r="DV4" s="39"/>
-      <c r="DW4" s="39"/>
-      <c r="DX4" s="39"/>
-      <c r="DY4" s="40"/>
-      <c r="DZ4" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="EA4" s="15" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="5" spans="1:131" s="34" customFormat="1" ht="137.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="B5" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="H5" s="38" t="s">
-        <v>241</v>
-      </c>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="31" t="s">
-        <v>244</v>
-      </c>
-      <c r="N5" s="46" t="s">
-        <v>242</v>
-      </c>
-      <c r="O5" s="45"/>
-      <c r="P5" s="30" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q5" s="32" t="s">
-        <v>245</v>
-      </c>
-      <c r="R5" s="33" t="s">
-        <v>246</v>
-      </c>
-      <c r="S5" s="32" t="s">
-        <v>242</v>
-      </c>
-      <c r="T5" s="33" t="s">
-        <v>246</v>
-      </c>
-      <c r="U5" s="32" t="s">
-        <v>242</v>
-      </c>
-      <c r="V5" s="46" t="s">
-        <v>246</v>
-      </c>
-      <c r="W5" s="45"/>
-      <c r="X5" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="Y5" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="Z5" s="15" t="s">
-        <v>249</v>
-      </c>
-      <c r="AA5" s="46" t="s">
-        <v>247</v>
-      </c>
-      <c r="AB5" s="45"/>
-      <c r="AC5" s="45"/>
-      <c r="AD5" s="45"/>
-      <c r="AE5" s="46" t="s">
-        <v>248</v>
-      </c>
-      <c r="AF5" s="45"/>
-      <c r="AG5" s="45"/>
-      <c r="AH5" s="46" t="s">
-        <v>242</v>
-      </c>
-      <c r="AI5" s="45"/>
-      <c r="AJ5" s="45"/>
-      <c r="AK5" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="AL5" s="45"/>
-      <c r="AM5" s="45"/>
-      <c r="AN5" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="AO5" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="AP5" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="AQ5" s="38" t="s">
-        <v>241</v>
-      </c>
-      <c r="AR5" s="39"/>
-      <c r="AS5" s="39"/>
-      <c r="AT5" s="39"/>
-      <c r="AU5" s="40"/>
-      <c r="AV5" s="60" t="s">
-        <v>252</v>
-      </c>
-      <c r="AW5" s="61"/>
-      <c r="AX5" s="61"/>
-      <c r="AY5" s="62"/>
-      <c r="AZ5" s="60" t="s">
-        <v>275</v>
-      </c>
-      <c r="BA5" s="61"/>
-      <c r="BB5" s="61"/>
-      <c r="BC5" s="62"/>
-      <c r="BD5" s="60" t="s">
-        <v>253</v>
-      </c>
-      <c r="BE5" s="61"/>
-      <c r="BF5" s="61"/>
-      <c r="BG5" s="62"/>
-      <c r="BH5" s="60" t="s">
-        <v>254</v>
-      </c>
-      <c r="BI5" s="61"/>
-      <c r="BJ5" s="61"/>
-      <c r="BK5" s="62"/>
-      <c r="BL5" s="60" t="s">
-        <v>255</v>
-      </c>
-      <c r="BM5" s="61"/>
-      <c r="BN5" s="61"/>
-      <c r="BO5" s="62"/>
-      <c r="BP5" s="60" t="s">
-        <v>256</v>
-      </c>
-      <c r="BQ5" s="61"/>
-      <c r="BR5" s="61"/>
-      <c r="BS5" s="62"/>
-      <c r="BT5" s="60" t="s">
-        <v>257</v>
-      </c>
-      <c r="BU5" s="61"/>
-      <c r="BV5" s="61"/>
-      <c r="BW5" s="62"/>
-      <c r="BX5" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="BY5" s="15" t="s">
-        <v>258</v>
-      </c>
-      <c r="BZ5" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="CA5" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="CB5" s="38" t="s">
-        <v>260</v>
-      </c>
-      <c r="CC5" s="39"/>
-      <c r="CD5" s="39"/>
-      <c r="CE5" s="40"/>
-      <c r="CF5" s="38" t="s">
-        <v>261</v>
-      </c>
-      <c r="CG5" s="40"/>
-      <c r="CH5" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="CI5" s="38" t="s">
-        <v>262</v>
-      </c>
-      <c r="CJ5" s="39"/>
-      <c r="CK5" s="39"/>
-      <c r="CL5" s="39"/>
-      <c r="CM5" s="39"/>
-      <c r="CN5" s="39"/>
-      <c r="CO5" s="39"/>
-      <c r="CP5" s="39"/>
-      <c r="CQ5" s="39"/>
-      <c r="CR5" s="40"/>
-      <c r="CS5" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="CT5" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="CU5" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="CV5" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="CW5" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="CX5" s="38" t="s">
-        <v>241</v>
-      </c>
-      <c r="CY5" s="40"/>
-      <c r="CZ5" s="38" t="s">
-        <v>264</v>
-      </c>
-      <c r="DA5" s="40"/>
-      <c r="DB5" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="DC5" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="DD5" s="41" t="s">
-        <v>265</v>
-      </c>
-      <c r="DE5" s="42"/>
-      <c r="DF5" s="42"/>
-      <c r="DG5" s="42"/>
-      <c r="DH5" s="44"/>
-      <c r="DI5" s="38" t="s">
-        <v>241</v>
-      </c>
-      <c r="DJ5" s="39"/>
-      <c r="DK5" s="39"/>
-      <c r="DL5" s="40"/>
-      <c r="DM5" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="DN5" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="DO5" s="38" t="s">
-        <v>266</v>
-      </c>
-      <c r="DP5" s="40"/>
-      <c r="DQ5" s="38" t="s">
-        <v>241</v>
-      </c>
-      <c r="DR5" s="40"/>
-      <c r="DS5" s="37" t="s">
-        <v>243</v>
-      </c>
-      <c r="DT5" s="15" t="s">
-        <v>281</v>
-      </c>
-      <c r="DU5" s="15" t="s">
-        <v>279</v>
-      </c>
-      <c r="DV5" s="38" t="s">
-        <v>267</v>
-      </c>
-      <c r="DW5" s="39"/>
-      <c r="DX5" s="39"/>
-      <c r="DY5" s="40"/>
-      <c r="DZ5" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="EA5" s="15" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="6" spans="1:131" s="35" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="43" t="s">
-        <v>270</v>
-      </c>
-      <c r="G6" s="43"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46" t="s">
-        <v>272</v>
-      </c>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
-      <c r="U6" s="45"/>
-      <c r="V6" s="45"/>
-      <c r="W6" s="45"/>
-      <c r="X6" s="45"/>
-      <c r="Y6" s="46"/>
-      <c r="Z6" s="46"/>
-      <c r="AA6" s="46" t="s">
-        <v>272</v>
-      </c>
-      <c r="AB6" s="45"/>
-      <c r="AC6" s="45"/>
-      <c r="AD6" s="45"/>
-      <c r="AE6" s="46"/>
-      <c r="AF6" s="46"/>
-      <c r="AG6" s="46"/>
-      <c r="AH6" s="46"/>
-      <c r="AI6" s="46"/>
-      <c r="AJ6" s="46"/>
-      <c r="AK6" s="46"/>
-      <c r="AL6" s="46"/>
-      <c r="AM6" s="46"/>
-      <c r="AN6" s="46"/>
-      <c r="AO6" s="46"/>
-      <c r="AP6" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="AQ6" s="38"/>
-      <c r="AR6" s="39"/>
-      <c r="AS6" s="39"/>
-      <c r="AT6" s="39"/>
-      <c r="AU6" s="39"/>
-      <c r="AV6" s="39"/>
-      <c r="AW6" s="39"/>
-      <c r="AX6" s="39"/>
-      <c r="AY6" s="39"/>
-      <c r="AZ6" s="39"/>
-      <c r="BA6" s="39"/>
-      <c r="BB6" s="39"/>
-      <c r="BC6" s="39"/>
-      <c r="BD6" s="39"/>
-      <c r="BE6" s="39"/>
-      <c r="BF6" s="39"/>
-      <c r="BG6" s="39"/>
-      <c r="BH6" s="39"/>
-      <c r="BI6" s="39"/>
-      <c r="BJ6" s="39"/>
-      <c r="BK6" s="39"/>
-      <c r="BL6" s="39"/>
-      <c r="BM6" s="39"/>
-      <c r="BN6" s="39"/>
-      <c r="BO6" s="39"/>
-      <c r="BP6" s="39"/>
-      <c r="BQ6" s="39"/>
-      <c r="BR6" s="39"/>
-      <c r="BS6" s="39"/>
-      <c r="BT6" s="39"/>
-      <c r="BU6" s="39"/>
-      <c r="BV6" s="39"/>
-      <c r="BW6" s="40"/>
-      <c r="BX6" s="38"/>
-      <c r="BY6" s="39"/>
-      <c r="BZ6" s="39"/>
-      <c r="CA6" s="39"/>
-      <c r="CB6" s="39"/>
-      <c r="CC6" s="39"/>
-      <c r="CD6" s="39"/>
-      <c r="CE6" s="39"/>
-      <c r="CF6" s="39"/>
-      <c r="CG6" s="39"/>
-      <c r="CH6" s="39"/>
-      <c r="CI6" s="39"/>
-      <c r="CJ6" s="39"/>
-      <c r="CK6" s="39"/>
-      <c r="CL6" s="39"/>
-      <c r="CM6" s="39"/>
-      <c r="CN6" s="39"/>
-      <c r="CO6" s="39"/>
-      <c r="CP6" s="39"/>
-      <c r="CQ6" s="39"/>
-      <c r="CR6" s="40"/>
-      <c r="CS6" s="38"/>
-      <c r="CT6" s="39"/>
-      <c r="CU6" s="39"/>
-      <c r="CV6" s="39"/>
-      <c r="CW6" s="39"/>
-      <c r="CX6" s="39"/>
-      <c r="CY6" s="39"/>
-      <c r="CZ6" s="39"/>
-      <c r="DA6" s="39"/>
-      <c r="DB6" s="39"/>
-      <c r="DC6" s="39"/>
-      <c r="DD6" s="39"/>
-      <c r="DE6" s="39"/>
-      <c r="DF6" s="39"/>
-      <c r="DG6" s="39"/>
-      <c r="DH6" s="39"/>
-      <c r="DI6" s="39"/>
-      <c r="DJ6" s="39"/>
-      <c r="DK6" s="39"/>
-      <c r="DL6" s="39"/>
-      <c r="DM6" s="40"/>
-      <c r="DN6" s="38"/>
-      <c r="DO6" s="39"/>
-      <c r="DP6" s="39"/>
-      <c r="DQ6" s="39"/>
-      <c r="DR6" s="40"/>
-      <c r="DS6" s="20" t="s">
-        <v>270</v>
-      </c>
-      <c r="DT6" s="20"/>
-      <c r="DU6" s="20" t="s">
-        <v>270</v>
-      </c>
-      <c r="DV6" s="41"/>
-      <c r="DW6" s="42"/>
-      <c r="DX6" s="42"/>
-      <c r="DY6" s="42"/>
-      <c r="DZ6" s="42"/>
-      <c r="EA6" s="44"/>
-    </row>
-    <row r="7" spans="1:131" s="35" customFormat="1" ht="23" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43" t="s">
-        <v>242</v>
-      </c>
-      <c r="G7" s="43"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="43" t="s">
-        <v>242</v>
-      </c>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="56"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="O7" s="41"/>
-      <c r="P7" s="44"/>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="42"/>
-      <c r="S7" s="42"/>
-      <c r="T7" s="42"/>
-      <c r="U7" s="44"/>
-      <c r="V7" s="43" t="s">
-        <v>242</v>
-      </c>
-      <c r="W7" s="43"/>
-      <c r="X7" s="41"/>
-      <c r="Y7" s="42"/>
-      <c r="Z7" s="42"/>
-      <c r="AA7" s="42"/>
-      <c r="AB7" s="42"/>
-      <c r="AC7" s="42"/>
-      <c r="AD7" s="42"/>
-      <c r="AE7" s="42"/>
-      <c r="AF7" s="42"/>
-      <c r="AG7" s="42"/>
-      <c r="AH7" s="42"/>
-      <c r="AI7" s="42"/>
-      <c r="AJ7" s="44"/>
-      <c r="AK7" s="41"/>
-      <c r="AL7" s="42"/>
-      <c r="AM7" s="42"/>
-      <c r="AN7" s="42"/>
-      <c r="AO7" s="42"/>
-      <c r="AP7" s="44"/>
-      <c r="AQ7" s="41" t="s">
-        <v>242</v>
-      </c>
-      <c r="AR7" s="44"/>
-      <c r="AS7" s="41"/>
-      <c r="AT7" s="44"/>
-      <c r="AU7" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="AV7" s="41"/>
-      <c r="AW7" s="42"/>
-      <c r="AX7" s="42"/>
-      <c r="AY7" s="42"/>
-      <c r="AZ7" s="42"/>
-      <c r="BA7" s="42"/>
-      <c r="BB7" s="42"/>
-      <c r="BC7" s="42"/>
-      <c r="BD7" s="42"/>
-      <c r="BE7" s="42"/>
-      <c r="BF7" s="42"/>
-      <c r="BG7" s="42"/>
-      <c r="BH7" s="42"/>
-      <c r="BI7" s="42"/>
-      <c r="BJ7" s="42"/>
-      <c r="BK7" s="42"/>
-      <c r="BL7" s="42"/>
-      <c r="BM7" s="42"/>
-      <c r="BN7" s="42"/>
-      <c r="BO7" s="42"/>
-      <c r="BP7" s="42"/>
-      <c r="BQ7" s="42"/>
-      <c r="BR7" s="42"/>
-      <c r="BS7" s="42"/>
-      <c r="BT7" s="42"/>
-      <c r="BU7" s="42"/>
-      <c r="BV7" s="42"/>
-      <c r="BW7" s="44"/>
-      <c r="BX7" s="41"/>
-      <c r="BY7" s="42"/>
-      <c r="BZ7" s="42"/>
-      <c r="CA7" s="42"/>
-      <c r="CB7" s="42"/>
-      <c r="CC7" s="42"/>
-      <c r="CD7" s="42"/>
-      <c r="CE7" s="42"/>
-      <c r="CF7" s="42"/>
-      <c r="CG7" s="42"/>
-      <c r="CH7" s="42"/>
-      <c r="CI7" s="42"/>
-      <c r="CJ7" s="42"/>
-      <c r="CK7" s="42"/>
-      <c r="CL7" s="42"/>
-      <c r="CM7" s="42"/>
-      <c r="CN7" s="42"/>
-      <c r="CO7" s="42"/>
-      <c r="CP7" s="42"/>
-      <c r="CQ7" s="42"/>
-      <c r="CR7" s="44"/>
-      <c r="CS7" s="41"/>
-      <c r="CT7" s="42"/>
-      <c r="CU7" s="42"/>
-      <c r="CV7" s="42"/>
-      <c r="CW7" s="42"/>
-      <c r="CX7" s="42"/>
-      <c r="CY7" s="42"/>
-      <c r="CZ7" s="42"/>
-      <c r="DA7" s="42"/>
-      <c r="DB7" s="42"/>
-      <c r="DC7" s="42"/>
-      <c r="DD7" s="42"/>
-      <c r="DE7" s="42"/>
-      <c r="DF7" s="42"/>
-      <c r="DG7" s="42"/>
-      <c r="DH7" s="42"/>
-      <c r="DI7" s="42"/>
-      <c r="DJ7" s="42"/>
-      <c r="DK7" s="42"/>
-      <c r="DL7" s="42"/>
-      <c r="DM7" s="44"/>
-      <c r="DN7" s="41"/>
-      <c r="DO7" s="42"/>
-      <c r="DP7" s="42"/>
-      <c r="DQ7" s="42"/>
-      <c r="DR7" s="42"/>
-      <c r="DS7" s="44"/>
-      <c r="DT7" s="41" t="s">
-        <v>242</v>
-      </c>
-      <c r="DU7" s="42"/>
-      <c r="DV7" s="42"/>
-      <c r="DW7" s="42"/>
-      <c r="DX7" s="42"/>
-      <c r="DY7" s="42"/>
-      <c r="DZ7" s="43"/>
-      <c r="EA7" s="43"/>
-    </row>
-    <row r="8" spans="1:131" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
-        <v>276</v>
-      </c>
-      <c r="B8" s="17">
-        <v>1</v>
-      </c>
-      <c r="C8" s="17">
+      <c r="C8" s="16">
         <v>2</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>3</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="21">
         <v>4</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="16">
         <v>5</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="16">
         <v>6</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="16">
         <v>7</v>
       </c>
-      <c r="I8" s="22">
+      <c r="I8" s="21">
         <v>8</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="16">
         <v>9</v>
       </c>
-      <c r="K8" s="17">
+      <c r="K8" s="16">
         <v>10</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="16">
         <v>11</v>
       </c>
-      <c r="M8" s="22">
+      <c r="M8" s="21">
         <v>12</v>
       </c>
-      <c r="N8" s="17">
+      <c r="N8" s="16">
         <v>13</v>
       </c>
-      <c r="O8" s="17">
+      <c r="O8" s="16">
         <v>14</v>
       </c>
-      <c r="P8" s="17">
+      <c r="P8" s="16">
         <v>15</v>
       </c>
-      <c r="Q8" s="22">
+      <c r="Q8" s="21">
         <v>16</v>
       </c>
-      <c r="R8" s="17">
+      <c r="R8" s="16">
         <v>17</v>
       </c>
-      <c r="S8" s="17">
+      <c r="S8" s="16">
         <v>18</v>
       </c>
-      <c r="T8" s="17">
+      <c r="T8" s="16">
         <v>19</v>
       </c>
-      <c r="U8" s="22">
+      <c r="U8" s="21">
         <v>20</v>
       </c>
-      <c r="V8" s="17">
+      <c r="V8" s="16">
         <v>21</v>
       </c>
-      <c r="W8" s="17">
+      <c r="W8" s="16">
         <v>22</v>
       </c>
-      <c r="X8" s="17">
+      <c r="X8" s="16">
         <v>23</v>
       </c>
-      <c r="Y8" s="22">
+      <c r="Y8" s="21">
         <v>24</v>
       </c>
-      <c r="Z8" s="17">
+      <c r="Z8" s="16">
         <v>25</v>
       </c>
-      <c r="AA8" s="17">
+      <c r="AA8" s="16">
         <v>26</v>
       </c>
-      <c r="AB8" s="17">
+      <c r="AB8" s="16">
         <v>27</v>
       </c>
-      <c r="AC8" s="22">
+      <c r="AC8" s="21">
         <v>28</v>
       </c>
-      <c r="AD8" s="17">
+      <c r="AD8" s="16">
         <v>29</v>
       </c>
-      <c r="AE8" s="17">
+      <c r="AE8" s="16">
         <v>30</v>
       </c>
-      <c r="AF8" s="17">
+      <c r="AF8" s="16">
         <v>31</v>
       </c>
-      <c r="AG8" s="22">
+      <c r="AG8" s="21">
         <v>32</v>
       </c>
-      <c r="AH8" s="17">
+      <c r="AH8" s="16">
         <v>33</v>
       </c>
-      <c r="AI8" s="17">
+      <c r="AI8" s="16">
         <v>34</v>
       </c>
-      <c r="AJ8" s="17">
+      <c r="AJ8" s="16">
         <v>35</v>
       </c>
-      <c r="AK8" s="22">
+      <c r="AK8" s="21">
         <v>36</v>
       </c>
-      <c r="AL8" s="17">
+      <c r="AL8" s="16">
         <v>37</v>
       </c>
-      <c r="AM8" s="17">
+      <c r="AM8" s="16">
         <v>38</v>
       </c>
-      <c r="AN8" s="17">
+      <c r="AN8" s="16">
         <v>39</v>
       </c>
-      <c r="AO8" s="22">
+      <c r="AO8" s="21">
         <v>40</v>
       </c>
-      <c r="AP8" s="17">
+      <c r="AP8" s="16">
         <v>41</v>
       </c>
-      <c r="AQ8" s="17">
+      <c r="AQ8" s="16">
         <v>42</v>
       </c>
-      <c r="AR8" s="17">
+      <c r="AR8" s="16">
         <v>43</v>
       </c>
-      <c r="AS8" s="22">
+      <c r="AS8" s="21">
         <v>44</v>
       </c>
-      <c r="AT8" s="17">
+      <c r="AT8" s="16">
         <v>45</v>
       </c>
-      <c r="AU8" s="17">
+      <c r="AU8" s="16">
         <v>46</v>
       </c>
-      <c r="AV8" s="17">
+      <c r="AV8" s="16">
         <v>47</v>
       </c>
-      <c r="AW8" s="22">
+      <c r="AW8" s="21">
         <v>48</v>
       </c>
-      <c r="AX8" s="17">
+      <c r="AX8" s="16">
         <v>49</v>
       </c>
-      <c r="AY8" s="17">
+      <c r="AY8" s="16">
         <v>50</v>
       </c>
-      <c r="AZ8" s="17">
+      <c r="AZ8" s="16">
         <v>51</v>
       </c>
-      <c r="BA8" s="22">
+      <c r="BA8" s="21">
         <v>52</v>
       </c>
-      <c r="BB8" s="17">
+      <c r="BB8" s="16">
         <v>53</v>
       </c>
-      <c r="BC8" s="17">
+      <c r="BC8" s="16">
         <v>54</v>
       </c>
-      <c r="BD8" s="17">
+      <c r="BD8" s="16">
         <v>55</v>
       </c>
-      <c r="BE8" s="22">
+      <c r="BE8" s="21">
         <v>56</v>
       </c>
-      <c r="BF8" s="17">
+      <c r="BF8" s="16">
         <v>57</v>
       </c>
-      <c r="BG8" s="17">
+      <c r="BG8" s="16">
         <v>58</v>
       </c>
-      <c r="BH8" s="17">
+      <c r="BH8" s="16">
         <v>59</v>
       </c>
-      <c r="BI8" s="22">
+      <c r="BI8" s="21">
         <v>60</v>
       </c>
-      <c r="BJ8" s="17">
+      <c r="BJ8" s="16">
         <v>61</v>
       </c>
-      <c r="BK8" s="17">
+      <c r="BK8" s="16">
         <v>62</v>
       </c>
-      <c r="BL8" s="17">
+      <c r="BL8" s="16">
         <v>63</v>
       </c>
-      <c r="BM8" s="22">
+      <c r="BM8" s="21">
         <v>64</v>
       </c>
-      <c r="BN8" s="17">
+      <c r="BN8" s="16">
         <v>65</v>
       </c>
-      <c r="BO8" s="17">
+      <c r="BO8" s="16">
         <v>66</v>
       </c>
-      <c r="BP8" s="17">
+      <c r="BP8" s="16">
         <v>67</v>
       </c>
-      <c r="BQ8" s="22">
+      <c r="BQ8" s="21">
         <v>68</v>
       </c>
-      <c r="BR8" s="17">
+      <c r="BR8" s="16">
         <v>69</v>
       </c>
-      <c r="BS8" s="17">
+      <c r="BS8" s="16">
         <v>70</v>
       </c>
-      <c r="BT8" s="17">
+      <c r="BT8" s="16">
         <v>71</v>
       </c>
-      <c r="BU8" s="22">
+      <c r="BU8" s="21">
         <v>72</v>
       </c>
-      <c r="BV8" s="17">
+      <c r="BV8" s="16">
         <v>73</v>
       </c>
-      <c r="BW8" s="17">
+      <c r="BW8" s="16">
         <v>74</v>
       </c>
-      <c r="BX8" s="17">
+      <c r="BX8" s="16">
         <v>75</v>
       </c>
-      <c r="BY8" s="22">
+      <c r="BY8" s="21">
         <v>76</v>
       </c>
-      <c r="BZ8" s="17">
+      <c r="BZ8" s="16">
         <v>77</v>
       </c>
-      <c r="CA8" s="17">
+      <c r="CA8" s="16">
         <v>78</v>
       </c>
-      <c r="CB8" s="17">
+      <c r="CB8" s="16">
         <v>79</v>
       </c>
-      <c r="CC8" s="22">
+      <c r="CC8" s="21">
         <v>80</v>
       </c>
-      <c r="CD8" s="17">
+      <c r="CD8" s="16">
         <v>81</v>
       </c>
-      <c r="CE8" s="17">
+      <c r="CE8" s="16">
         <v>82</v>
       </c>
-      <c r="CF8" s="17">
+      <c r="CF8" s="16">
         <v>83</v>
       </c>
-      <c r="CG8" s="22">
+      <c r="CG8" s="21">
         <v>84</v>
       </c>
-      <c r="CH8" s="17">
+      <c r="CH8" s="16">
         <v>85</v>
       </c>
-      <c r="CI8" s="17">
+      <c r="CI8" s="16">
         <v>86</v>
       </c>
-      <c r="CJ8" s="17">
+      <c r="CJ8" s="16">
         <v>87</v>
       </c>
-      <c r="CK8" s="22">
+      <c r="CK8" s="21">
         <v>88</v>
       </c>
-      <c r="CL8" s="17">
+      <c r="CL8" s="16">
         <v>89</v>
       </c>
-      <c r="CM8" s="17">
+      <c r="CM8" s="16">
         <v>90</v>
       </c>
-      <c r="CN8" s="17">
+      <c r="CN8" s="16">
         <v>91</v>
       </c>
-      <c r="CO8" s="22">
+      <c r="CO8" s="21">
         <v>92</v>
       </c>
-      <c r="CP8" s="17">
+      <c r="CP8" s="16">
         <v>93</v>
       </c>
-      <c r="CQ8" s="17">
+      <c r="CQ8" s="16">
         <v>94</v>
       </c>
-      <c r="CR8" s="17">
+      <c r="CR8" s="16">
         <v>95</v>
       </c>
-      <c r="CS8" s="22">
+      <c r="CS8" s="21">
         <v>96</v>
       </c>
-      <c r="CT8" s="17">
+      <c r="CT8" s="16">
         <v>97</v>
       </c>
-      <c r="CU8" s="17">
+      <c r="CU8" s="16">
         <v>98</v>
       </c>
-      <c r="CV8" s="17">
+      <c r="CV8" s="16">
         <v>99</v>
       </c>
-      <c r="CW8" s="22">
+      <c r="CW8" s="21">
         <v>100</v>
       </c>
-      <c r="CX8" s="17">
+      <c r="CX8" s="16">
         <v>101</v>
       </c>
-      <c r="CY8" s="17">
+      <c r="CY8" s="16">
         <v>102</v>
       </c>
-      <c r="CZ8" s="17">
+      <c r="CZ8" s="16">
         <v>103</v>
       </c>
-      <c r="DA8" s="22">
+      <c r="DA8" s="21">
         <v>104</v>
       </c>
-      <c r="DB8" s="17">
+      <c r="DB8" s="16">
         <v>105</v>
       </c>
-      <c r="DC8" s="17">
+      <c r="DC8" s="16">
         <v>106</v>
       </c>
-      <c r="DD8" s="17">
+      <c r="DD8" s="16">
         <v>107</v>
       </c>
-      <c r="DE8" s="22">
+      <c r="DE8" s="21">
         <v>108</v>
       </c>
-      <c r="DF8" s="17">
+      <c r="DF8" s="16">
         <v>109</v>
       </c>
-      <c r="DG8" s="17">
+      <c r="DG8" s="16">
         <v>110</v>
       </c>
-      <c r="DH8" s="17">
+      <c r="DH8" s="16">
         <v>111</v>
       </c>
-      <c r="DI8" s="22">
+      <c r="DI8" s="21">
         <v>112</v>
       </c>
-      <c r="DJ8" s="17">
+      <c r="DJ8" s="16">
         <v>113</v>
       </c>
-      <c r="DK8" s="17">
+      <c r="DK8" s="16">
         <v>114</v>
       </c>
-      <c r="DL8" s="17">
+      <c r="DL8" s="16">
         <v>115</v>
       </c>
-      <c r="DM8" s="22">
+      <c r="DM8" s="21">
         <v>116</v>
       </c>
-      <c r="DN8" s="17">
+      <c r="DN8" s="16">
         <v>117</v>
       </c>
-      <c r="DO8" s="17">
+      <c r="DO8" s="16">
         <v>118</v>
       </c>
-      <c r="DP8" s="17">
+      <c r="DP8" s="16">
         <v>119</v>
       </c>
-      <c r="DQ8" s="22">
+      <c r="DQ8" s="21">
         <v>120</v>
       </c>
-      <c r="DR8" s="17">
+      <c r="DR8" s="16">
         <v>121</v>
       </c>
-      <c r="DS8" s="17">
+      <c r="DS8" s="16">
         <v>122</v>
       </c>
-      <c r="DT8" s="17">
+      <c r="DT8" s="16">
         <v>123</v>
       </c>
-      <c r="DU8" s="22">
+      <c r="DU8" s="21">
         <v>124</v>
       </c>
-      <c r="DV8" s="17">
+      <c r="DV8" s="16">
         <v>125</v>
       </c>
-      <c r="DW8" s="17">
+      <c r="DW8" s="16">
         <v>126</v>
       </c>
-      <c r="DX8" s="17">
+      <c r="DX8" s="16">
         <v>127</v>
       </c>
-      <c r="DY8" s="22">
+      <c r="DY8" s="21">
         <v>128</v>
       </c>
-      <c r="DZ8" s="17">
+      <c r="DZ8" s="16">
         <v>129</v>
       </c>
-      <c r="EA8" s="17">
+      <c r="EA8" s="16">
         <v>130</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="75">
+    <mergeCell ref="DU4:DY4"/>
+    <mergeCell ref="DT7:DY7"/>
+    <mergeCell ref="DZ7:EA7"/>
+    <mergeCell ref="DD4:DH4"/>
+    <mergeCell ref="DI4:DL4"/>
+    <mergeCell ref="DD5:DH5"/>
+    <mergeCell ref="DO5:DP5"/>
+    <mergeCell ref="DI5:DL5"/>
+    <mergeCell ref="CS6:DM6"/>
+    <mergeCell ref="CS7:DM7"/>
+    <mergeCell ref="DN6:DR6"/>
+    <mergeCell ref="DN7:DS7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="CZ5:DA5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="CB5:CE5"/>
+    <mergeCell ref="CF5:CG5"/>
+    <mergeCell ref="CI5:CR5"/>
+    <mergeCell ref="CX5:CY5"/>
+    <mergeCell ref="AQ6:BW6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="AA5:AD5"/>
+    <mergeCell ref="Q6:X6"/>
+    <mergeCell ref="AA6:AD6"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="BZ4:CA4"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="AE6:AO6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="Q1:AJ1"/>
+    <mergeCell ref="AK1:AP1"/>
+    <mergeCell ref="DV6:EA6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="AS7:AT7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="X7:AJ7"/>
+    <mergeCell ref="AK7:AP7"/>
+    <mergeCell ref="AQ7:AR7"/>
+    <mergeCell ref="AV7:BW7"/>
+    <mergeCell ref="BX6:CR6"/>
+    <mergeCell ref="BX7:CR7"/>
     <mergeCell ref="DN1:EA1"/>
     <mergeCell ref="BL5:BO5"/>
     <mergeCell ref="BP5:BS5"/>
@@ -3837,65 +3895,6 @@
     <mergeCell ref="CI4:CR4"/>
     <mergeCell ref="DQ5:DR5"/>
     <mergeCell ref="AQ5:AU5"/>
-    <mergeCell ref="B1:P1"/>
-    <mergeCell ref="Q1:AJ1"/>
-    <mergeCell ref="AK1:AP1"/>
-    <mergeCell ref="DV6:EA6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="AS7:AT7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="X7:AJ7"/>
-    <mergeCell ref="AK7:AP7"/>
-    <mergeCell ref="AQ7:AR7"/>
-    <mergeCell ref="AV7:BW7"/>
-    <mergeCell ref="BX6:CR6"/>
-    <mergeCell ref="BX7:CR7"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="AE6:AO6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AK5:AM5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="BZ4:CA4"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="CZ5:DA5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="CB5:CE5"/>
-    <mergeCell ref="CF5:CG5"/>
-    <mergeCell ref="CI5:CR5"/>
-    <mergeCell ref="CX5:CY5"/>
-    <mergeCell ref="AQ6:BW6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="AA5:AD5"/>
-    <mergeCell ref="Q6:X6"/>
-    <mergeCell ref="AA6:AD6"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="DU4:DY4"/>
-    <mergeCell ref="DT7:DY7"/>
-    <mergeCell ref="DZ7:EA7"/>
-    <mergeCell ref="DD4:DH4"/>
-    <mergeCell ref="DI4:DL4"/>
-    <mergeCell ref="DD5:DH5"/>
-    <mergeCell ref="DO5:DP5"/>
-    <mergeCell ref="DI5:DL5"/>
-    <mergeCell ref="CS6:DM6"/>
-    <mergeCell ref="CS7:DM7"/>
-    <mergeCell ref="DN6:DR6"/>
-    <mergeCell ref="DN7:DS7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="X4" r:id="rId1" xr:uid="{33A4BD0C-7A19-4C88-AF60-902623A24589}"/>
@@ -3910,19 +3909,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ede1785e-3bac-4a90-a48c-62cc0231644e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000BCF930048F2A84190E342D576E507E9" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a5f7dcad46bf03cd06b92fe3a65eb3e5">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ede1785e-3bac-4a90-a48c-62cc0231644e" xmlns:ns3="6c5f9a5a-0dad-4595-a39a-6416e9fb7054" xmlns:ns4="83a87e31-bf32-46ab-8e70-9fa18461fa4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="627fd199b21a7508d85a0883525fd0b8" ns2:_="" ns3:_="" ns4:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000BCF930048F2A84190E342D576E507E9" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="263b522f34af87636eb5a7b2dc30e648">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ede1785e-3bac-4a90-a48c-62cc0231644e" xmlns:ns3="6c5f9a5a-0dad-4595-a39a-6416e9fb7054" xmlns:ns4="83a87e31-bf32-46ab-8e70-9fa18461fa4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a158f55a44c8de9db2cc0af700b09a3c" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
     <xsd:import namespace="6c5f9a5a-0dad-4595-a39a-6416e9fb7054"/>
     <xsd:import namespace="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
@@ -3949,11 +3947,27 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="26" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="27" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="ede1785e-3bac-4a90-a48c-62cc0231644e" elementFormDefault="qualified">
@@ -4181,39 +4195,34 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ede1785e-3bac-4a90-a48c-62cc0231644e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3234EB82-E598-4D46-AACB-BAE493D677A7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D2572BD-7EE7-4817-BEE4-BB014A85EDEE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6c5f9a5a-0dad-4595-a39a-6416e9fb7054"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{844596B9-62AA-44A2-8AEF-70908D01A276}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17AFA51A-13A5-4296-8804-3A0CE81BEA66}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
     <ds:schemaRef ds:uri="6c5f9a5a-0dad-4595-a39a-6416e9fb7054"/>
     <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
@@ -4228,15 +4237,26 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D2572BD-7EE7-4817-BEE4-BB014A85EDEE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3234EB82-E598-4D46-AACB-BAE493D677A7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6c5f9a5a-0dad-4595-a39a-6416e9fb7054"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{fbd41ebe-fca6-4f2c-aecb-bf3a17e72416}" enabled="1" method="Privileged" siteId="{bf346810-9c7d-43de-a872-24a2ef3995a8}" contentBits="3" removed="0"/>
+  <clbl:label id="{fbd41ebe-fca6-4f2c-aecb-bf3a17e72416}" enabled="1" method="Privileged" siteId="{bf346810-9c7d-43de-a872-24a2ef3995a8}" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>

<commit_message>
CLDC-3568: Update collection resources for MHCLG name change (#2536)
</commit_message>
<xml_diff>
--- a/public/files/bulk-upload-lettings-template-2024-25.xlsx
+++ b/public/files/bulk-upload-lettings-template-2024-25.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamuelIvko\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mhclg.sharepoint.com/sites/HousingandplanningandCOREstatistics/Shared Documents/CORE Lettings/01 CORE service/04 Annual log reviews/2024-25/03 Materials for providers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F7A164-145F-401A-B0DA-F89299092402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{296AE3D4-73F7-4BC5-957A-5710BD8CDEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79E053AA-7BEE-4F89-A465-E2DA330BC6D4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="282">
   <si>
     <t>Section</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>What is the property reference?</t>
-  </si>
-  <si>
-    <t>Has the tenant seen or been given access to the DLUHC privacy notice?</t>
   </si>
   <si>
     <t>If known, provide this property’s UPRN</t>
@@ -495,9 +492,6 @@
   </si>
   <si>
     <t>This is how you usually refer to this property on your own systems.</t>
-  </si>
-  <si>
-    <t>Make sure the lead tenant has seen or been given access to the Department for Levelling Up, Housing and Communities (DLUHC) privacy notice before completing this log. This is a legal requirement under data protection legislation.</t>
   </si>
   <si>
     <t>The Unique Property Reference Number (UPRN) is a unique number system created by Ordnance Survey and used by housing providers and various industries across the UK. An example UPRN is 10010457355. 
@@ -809,6 +803,9 @@
     <t>0 - 1</t>
   </si>
   <si>
+    <t>1 - 10</t>
+  </si>
+  <si>
     <t>xxxx.xx</t>
   </si>
   <si>
@@ -895,7 +892,13 @@
     <t>Yes, if household's income is unknown (if field 118 = 2 or 3)</t>
   </si>
   <si>
+    <t xml:space="preserve">Yes, if rent is charged (if field 125 is not empty) </t>
+  </si>
+  <si>
     <t>Yes, if the household does not pay rent (if field 122 = 1) or if the accommodation is not a care home (if field 124 is empty)</t>
+  </si>
+  <si>
+    <t>Yes, if the household doesn't receive housing benefits, or if it is unknown (if field 120 = 3, 9 or 10)</t>
   </si>
   <si>
     <t>Yes, if the household does not need to pay rent or charges after receiving housing benefits (if field 130 is not 1)</t>
@@ -933,16 +936,10 @@
 You can find the location code on the CORE service under 'Schemes', either by searching for the specific location or downloading a csv.</t>
   </si>
   <si>
-    <t>Yes, if rent is charged (if field 125 is not empty), or if there is no charge (if field 122 is 1)</t>
-  </si>
-  <si>
-    <t>Yes, if the household doesn't receive housing benefits, or if it is unknown (if field 120 = 3, 9 or 10), or if there are no charges (if field 122 = 1)</t>
-  </si>
-  <si>
-    <t>Yes, if there are no charges (if field 122 = 1)</t>
-  </si>
-  <si>
-    <t>1 - 11</t>
+    <t>Has the tenant seen or been given access to the MHCLG privacy notice?</t>
+  </si>
+  <si>
+    <t>Make sure the lead tenant has seen or been given access to the Ministry of Housing, Communities and Local Government (MHCLG) privacy notice before completing this log. This is a legal requirement under data protection legislation.</t>
   </si>
 </sst>
 </file>
@@ -1248,9 +1245,6 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1315,9 +1309,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1338,36 +1329,108 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1375,72 +1438,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1661,7 +1658,9 @@
   </sheetPr>
   <dimension ref="A1:EA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="DD1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="DN7" sqref="DN7:DS7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1701,150 +1700,150 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="54" t="s">
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="55" t="s">
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="55"/>
-      <c r="AM1" s="55"/>
-      <c r="AN1" s="55"/>
-      <c r="AO1" s="55"/>
-      <c r="AP1" s="55"/>
-      <c r="AQ1" s="63" t="s">
+      <c r="AL1" s="58"/>
+      <c r="AM1" s="58"/>
+      <c r="AN1" s="58"/>
+      <c r="AO1" s="58"/>
+      <c r="AP1" s="58"/>
+      <c r="AQ1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="AR1" s="64"/>
-      <c r="AS1" s="64"/>
-      <c r="AT1" s="64"/>
-      <c r="AU1" s="64"/>
-      <c r="AV1" s="64"/>
-      <c r="AW1" s="64"/>
-      <c r="AX1" s="64"/>
-      <c r="AY1" s="64"/>
-      <c r="AZ1" s="64"/>
-      <c r="BA1" s="64"/>
-      <c r="BB1" s="64"/>
-      <c r="BC1" s="64"/>
-      <c r="BD1" s="64"/>
-      <c r="BE1" s="64"/>
-      <c r="BF1" s="64"/>
-      <c r="BG1" s="64"/>
-      <c r="BH1" s="64"/>
-      <c r="BI1" s="64"/>
-      <c r="BJ1" s="64"/>
-      <c r="BK1" s="64"/>
-      <c r="BL1" s="64"/>
-      <c r="BM1" s="64"/>
-      <c r="BN1" s="64"/>
-      <c r="BO1" s="64"/>
-      <c r="BP1" s="64"/>
-      <c r="BQ1" s="64"/>
-      <c r="BR1" s="64"/>
-      <c r="BS1" s="64"/>
-      <c r="BT1" s="64"/>
-      <c r="BU1" s="64"/>
-      <c r="BV1" s="64"/>
-      <c r="BW1" s="65"/>
-      <c r="BX1" s="66" t="s">
+      <c r="AR1" s="45"/>
+      <c r="AS1" s="45"/>
+      <c r="AT1" s="45"/>
+      <c r="AU1" s="45"/>
+      <c r="AV1" s="45"/>
+      <c r="AW1" s="45"/>
+      <c r="AX1" s="45"/>
+      <c r="AY1" s="45"/>
+      <c r="AZ1" s="45"/>
+      <c r="BA1" s="45"/>
+      <c r="BB1" s="45"/>
+      <c r="BC1" s="45"/>
+      <c r="BD1" s="45"/>
+      <c r="BE1" s="45"/>
+      <c r="BF1" s="45"/>
+      <c r="BG1" s="45"/>
+      <c r="BH1" s="45"/>
+      <c r="BI1" s="45"/>
+      <c r="BJ1" s="45"/>
+      <c r="BK1" s="45"/>
+      <c r="BL1" s="45"/>
+      <c r="BM1" s="45"/>
+      <c r="BN1" s="45"/>
+      <c r="BO1" s="45"/>
+      <c r="BP1" s="45"/>
+      <c r="BQ1" s="45"/>
+      <c r="BR1" s="45"/>
+      <c r="BS1" s="45"/>
+      <c r="BT1" s="45"/>
+      <c r="BU1" s="45"/>
+      <c r="BV1" s="45"/>
+      <c r="BW1" s="46"/>
+      <c r="BX1" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="BY1" s="67"/>
-      <c r="BZ1" s="67"/>
-      <c r="CA1" s="67"/>
-      <c r="CB1" s="67"/>
-      <c r="CC1" s="67"/>
-      <c r="CD1" s="67"/>
-      <c r="CE1" s="67"/>
-      <c r="CF1" s="67"/>
-      <c r="CG1" s="67"/>
-      <c r="CH1" s="67"/>
-      <c r="CI1" s="67"/>
-      <c r="CJ1" s="67"/>
-      <c r="CK1" s="67"/>
-      <c r="CL1" s="67"/>
-      <c r="CM1" s="67"/>
-      <c r="CN1" s="67"/>
-      <c r="CO1" s="67"/>
-      <c r="CP1" s="67"/>
-      <c r="CQ1" s="67"/>
-      <c r="CR1" s="68"/>
-      <c r="CS1" s="69" t="s">
+      <c r="BY1" s="51"/>
+      <c r="BZ1" s="51"/>
+      <c r="CA1" s="51"/>
+      <c r="CB1" s="51"/>
+      <c r="CC1" s="51"/>
+      <c r="CD1" s="51"/>
+      <c r="CE1" s="51"/>
+      <c r="CF1" s="51"/>
+      <c r="CG1" s="51"/>
+      <c r="CH1" s="51"/>
+      <c r="CI1" s="51"/>
+      <c r="CJ1" s="51"/>
+      <c r="CK1" s="51"/>
+      <c r="CL1" s="51"/>
+      <c r="CM1" s="51"/>
+      <c r="CN1" s="51"/>
+      <c r="CO1" s="51"/>
+      <c r="CP1" s="51"/>
+      <c r="CQ1" s="51"/>
+      <c r="CR1" s="52"/>
+      <c r="CS1" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="CT1" s="70"/>
-      <c r="CU1" s="70"/>
-      <c r="CV1" s="70"/>
-      <c r="CW1" s="70"/>
-      <c r="CX1" s="70"/>
-      <c r="CY1" s="70"/>
-      <c r="CZ1" s="70"/>
-      <c r="DA1" s="70"/>
-      <c r="DB1" s="70"/>
-      <c r="DC1" s="70"/>
-      <c r="DD1" s="70"/>
-      <c r="DE1" s="70"/>
-      <c r="DF1" s="70"/>
-      <c r="DG1" s="70"/>
-      <c r="DH1" s="70"/>
-      <c r="DI1" s="70"/>
-      <c r="DJ1" s="70"/>
-      <c r="DK1" s="70"/>
-      <c r="DL1" s="70"/>
-      <c r="DM1" s="71"/>
-      <c r="DN1" s="57" t="s">
+      <c r="CT1" s="54"/>
+      <c r="CU1" s="54"/>
+      <c r="CV1" s="54"/>
+      <c r="CW1" s="54"/>
+      <c r="CX1" s="54"/>
+      <c r="CY1" s="54"/>
+      <c r="CZ1" s="54"/>
+      <c r="DA1" s="54"/>
+      <c r="DB1" s="54"/>
+      <c r="DC1" s="54"/>
+      <c r="DD1" s="54"/>
+      <c r="DE1" s="54"/>
+      <c r="DF1" s="54"/>
+      <c r="DG1" s="54"/>
+      <c r="DH1" s="54"/>
+      <c r="DI1" s="54"/>
+      <c r="DJ1" s="54"/>
+      <c r="DK1" s="54"/>
+      <c r="DL1" s="54"/>
+      <c r="DM1" s="55"/>
+      <c r="DN1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="DO1" s="58"/>
-      <c r="DP1" s="58"/>
-      <c r="DQ1" s="58"/>
-      <c r="DR1" s="58"/>
-      <c r="DS1" s="58"/>
-      <c r="DT1" s="58"/>
-      <c r="DU1" s="58"/>
-      <c r="DV1" s="58"/>
-      <c r="DW1" s="58"/>
-      <c r="DX1" s="58"/>
-      <c r="DY1" s="58"/>
-      <c r="DZ1" s="58"/>
-      <c r="EA1" s="59"/>
+      <c r="DO1" s="39"/>
+      <c r="DP1" s="39"/>
+      <c r="DQ1" s="39"/>
+      <c r="DR1" s="39"/>
+      <c r="DS1" s="39"/>
+      <c r="DT1" s="39"/>
+      <c r="DU1" s="39"/>
+      <c r="DV1" s="39"/>
+      <c r="DW1" s="39"/>
+      <c r="DX1" s="39"/>
+      <c r="DY1" s="39"/>
+      <c r="DZ1" s="39"/>
+      <c r="EA1" s="40"/>
     </row>
     <row r="2" spans="1:131" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1892,1935 +1891,1994 @@
       <c r="O2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="36" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AF2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AK2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AL2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AM2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AN2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AO2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AP2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AS2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AT2" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="AT2" s="8" t="s">
+      <c r="AU2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AV2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AW2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AX2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AY2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="BA2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BA2" s="4" t="s">
+      <c r="BB2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="BB2" s="4" t="s">
+      <c r="BC2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="BC2" s="4" t="s">
+      <c r="BD2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BD2" s="4" t="s">
+      <c r="BE2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="BE2" s="4" t="s">
+      <c r="BF2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BF2" s="4" t="s">
+      <c r="BG2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BG2" s="4" t="s">
+      <c r="BH2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BH2" s="4" t="s">
+      <c r="BI2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="BI2" s="4" t="s">
+      <c r="BJ2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BJ2" s="4" t="s">
+      <c r="BK2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="BK2" s="4" t="s">
+      <c r="BL2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="BL2" s="4" t="s">
+      <c r="BM2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="BM2" s="4" t="s">
+      <c r="BN2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BN2" s="4" t="s">
+      <c r="BO2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="BO2" s="4" t="s">
+      <c r="BP2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="BP2" s="4" t="s">
+      <c r="BQ2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="BQ2" s="4" t="s">
+      <c r="BR2" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="BR2" s="4" t="s">
+      <c r="BS2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="BS2" s="4" t="s">
+      <c r="BT2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="BT2" s="4" t="s">
+      <c r="BU2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="BU2" s="4" t="s">
+      <c r="BV2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BV2" s="4" t="s">
+      <c r="BW2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BW2" s="4" t="s">
+      <c r="BX2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BX2" s="4" t="s">
+      <c r="BY2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BY2" s="4" t="s">
+      <c r="BZ2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="BZ2" s="4" t="s">
+      <c r="CA2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="CA2" s="4" t="s">
+      <c r="CB2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="CB2" s="4" t="s">
+      <c r="CC2" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="CC2" s="4" t="s">
+      <c r="CD2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="CD2" s="4" t="s">
+      <c r="CE2" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="CE2" s="4" t="s">
+      <c r="CF2" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="CF2" s="4" t="s">
+      <c r="CG2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="CG2" s="4" t="s">
+      <c r="CH2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="CH2" s="4" t="s">
+      <c r="CI2" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="CI2" s="4" t="s">
+      <c r="CJ2" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="CJ2" s="4" t="s">
+      <c r="CK2" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="CK2" s="4" t="s">
+      <c r="CL2" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="CL2" s="4" t="s">
+      <c r="CM2" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="CM2" s="4" t="s">
+      <c r="CN2" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="CN2" s="4" t="s">
+      <c r="CO2" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="CO2" s="4" t="s">
+      <c r="CP2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="CP2" s="4" t="s">
+      <c r="CQ2" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="CQ2" s="4" t="s">
+      <c r="CR2" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="CR2" s="4" t="s">
+      <c r="CS2" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="CS2" s="4" t="s">
+      <c r="CT2" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="CT2" s="4" t="s">
+      <c r="CU2" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="CU2" s="4" t="s">
+      <c r="CV2" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="CV2" s="4" t="s">
+      <c r="CW2" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="CW2" s="4" t="s">
+      <c r="CX2" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="CX2" s="4" t="s">
+      <c r="CY2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="CY2" s="4" t="s">
+      <c r="CZ2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="CZ2" s="4" t="s">
+      <c r="DA2" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="DA2" s="4" t="s">
+      <c r="DB2" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="DB2" s="4" t="s">
+      <c r="DC2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="DC2" s="4" t="s">
+      <c r="DD2" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="DD2" s="4" t="s">
+      <c r="DE2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="DE2" s="4" t="s">
+      <c r="DF2" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="DF2" s="4" t="s">
+      <c r="DG2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="DG2" s="4" t="s">
+      <c r="DH2" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="DH2" s="4" t="s">
+      <c r="DI2" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="DI2" s="4" t="s">
+      <c r="DJ2" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="DJ2" s="4" t="s">
+      <c r="DK2" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="DK2" s="4" t="s">
+      <c r="DL2" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="DL2" s="9" t="s">
+      <c r="DM2" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="DM2" s="4" t="s">
+      <c r="DN2" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="DN2" s="4" t="s">
+      <c r="DO2" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="DP2" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="DO2" s="4" t="s">
+      <c r="DQ2" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="DP2" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="DQ2" s="4" t="s">
+      <c r="DR2" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="DR2" s="4" t="s">
+      <c r="DS2" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="DS2" s="4" t="s">
+      <c r="DT2" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="DT2" s="4" t="s">
+      <c r="DU2" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="DU2" s="10" t="s">
+      <c r="DV2" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="DV2" s="4" t="s">
+      <c r="DW2" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="DW2" s="4" t="s">
+      <c r="DX2" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="DX2" s="4" t="s">
+      <c r="DY2" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="DY2" s="4" t="s">
+      <c r="DZ2" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="DZ2" s="4" t="s">
+      <c r="EA2" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="EA2" s="4" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:131" ht="368" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="D3" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="13" t="s">
+      <c r="M3" s="10"/>
+      <c r="N3" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11" t="s">
+      <c r="O3" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="P3" s="37" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q3" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="P3" s="29" t="s">
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="W3" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="23" t="s">
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="W3" s="23" t="s">
+      <c r="Z3" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11" t="s">
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="Z3" s="11" t="s">
+      <c r="AD3" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="AE3" s="64" t="s">
         <v>153</v>
       </c>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="11"/>
-      <c r="AC3" s="11" t="s">
+      <c r="AF3" s="65"/>
+      <c r="AG3" s="65"/>
+      <c r="AH3" s="64" t="s">
         <v>154</v>
       </c>
-      <c r="AD3" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="AE3" s="50" t="s">
+      <c r="AI3" s="65"/>
+      <c r="AJ3" s="65"/>
+      <c r="AK3" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="AF3" s="51"/>
-      <c r="AG3" s="51"/>
-      <c r="AH3" s="50" t="s">
+      <c r="AL3" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="AI3" s="51"/>
-      <c r="AJ3" s="51"/>
-      <c r="AK3" s="11" t="s">
+      <c r="AM3" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="AL3" s="11" t="s">
+      <c r="AN3" s="10"/>
+      <c r="AO3" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="AM3" s="11" t="s">
+      <c r="AP3" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="AN3" s="11"/>
-      <c r="AO3" s="11" t="s">
+      <c r="AQ3" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="AP3" s="11" t="s">
+      <c r="AR3" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="AQ3" s="11" t="s">
+      <c r="AS3" s="27"/>
+      <c r="AT3" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="AR3" s="27" t="s">
+      <c r="AU3" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="AV3" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="AS3" s="28"/>
-      <c r="AT3" s="27" t="s">
+      <c r="AW3" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="AU3" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="AV3" s="11" t="s">
+      <c r="AX3" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="AY3" s="10"/>
+      <c r="AZ3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="BA3" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="BB3" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="BC3" s="10"/>
+      <c r="BD3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="BE3" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="BF3" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="BG3" s="10"/>
+      <c r="BH3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="BI3" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="BJ3" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="BK3" s="10"/>
+      <c r="BL3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="BM3" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="BN3" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="BO3" s="10"/>
+      <c r="BP3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="BQ3" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="BR3" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="BS3" s="10"/>
+      <c r="BT3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="BU3" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="BV3" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="BW3" s="10"/>
+      <c r="BX3" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="AW3" s="11" t="s">
+      <c r="BY3" s="10"/>
+      <c r="BZ3" s="10"/>
+      <c r="CA3" s="10"/>
+      <c r="CB3" s="10"/>
+      <c r="CC3" s="10"/>
+      <c r="CD3" s="10"/>
+      <c r="CE3" s="10"/>
+      <c r="CF3" s="10"/>
+      <c r="CG3" s="10"/>
+      <c r="CH3" s="10"/>
+      <c r="CI3" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="AX3" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="AY3" s="11"/>
-      <c r="AZ3" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="BA3" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="BB3" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="BC3" s="11"/>
-      <c r="BD3" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="BE3" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="BF3" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="BG3" s="11"/>
-      <c r="BH3" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="BI3" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="BJ3" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="BK3" s="11"/>
-      <c r="BL3" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="BM3" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="BN3" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="BO3" s="11"/>
-      <c r="BP3" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="BQ3" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="BR3" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="BS3" s="11"/>
-      <c r="BT3" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="BU3" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="BV3" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="BW3" s="11"/>
-      <c r="BX3" s="11" t="s">
+      <c r="CJ3" s="10"/>
+      <c r="CK3" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="BY3" s="11"/>
-      <c r="BZ3" s="11"/>
-      <c r="CA3" s="11"/>
-      <c r="CB3" s="11"/>
-      <c r="CC3" s="11"/>
-      <c r="CD3" s="11"/>
-      <c r="CE3" s="11"/>
-      <c r="CF3" s="11"/>
-      <c r="CG3" s="11"/>
-      <c r="CH3" s="11"/>
-      <c r="CI3" s="11" t="s">
+      <c r="CL3" s="10"/>
+      <c r="CM3" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="CJ3" s="11"/>
-      <c r="CK3" s="11" t="s">
+      <c r="CN3" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="CL3" s="11"/>
-      <c r="CM3" s="11" t="s">
+      <c r="CO3" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="CN3" s="11" t="s">
+      <c r="CP3" s="10"/>
+      <c r="CQ3" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="CO3" s="11" t="s">
+      <c r="CR3" s="10"/>
+      <c r="CS3" s="10"/>
+      <c r="CT3" s="10"/>
+      <c r="CU3" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="CP3" s="11"/>
-      <c r="CQ3" s="11" t="s">
+      <c r="CV3" s="10"/>
+      <c r="CW3" s="10"/>
+      <c r="CX3" s="10"/>
+      <c r="CY3" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="CR3" s="11"/>
-      <c r="CS3" s="11"/>
-      <c r="CT3" s="11"/>
-      <c r="CU3" s="11" t="s">
+      <c r="CZ3" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="CV3" s="11"/>
-      <c r="CW3" s="11"/>
-      <c r="CX3" s="11"/>
-      <c r="CY3" s="11" t="s">
+      <c r="DA3" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="CZ3" s="24" t="s">
+      <c r="DB3" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="DC3" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="DA3" s="24" t="s">
+      <c r="DD3" s="10"/>
+      <c r="DE3" s="10"/>
+      <c r="DF3" s="10"/>
+      <c r="DG3" s="10"/>
+      <c r="DH3" s="10"/>
+      <c r="DI3" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="DB3" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="DC3" s="11" t="s">
+      <c r="DJ3" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="DD3" s="11"/>
-      <c r="DE3" s="11"/>
-      <c r="DF3" s="11"/>
-      <c r="DG3" s="11"/>
-      <c r="DH3" s="11"/>
-      <c r="DI3" s="11" t="s">
+      <c r="DK3" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="DJ3" s="11" t="s">
+      <c r="DL3" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="DK3" s="11" t="s">
+      <c r="DM3" s="10"/>
+      <c r="DN3" s="10"/>
+      <c r="DO3" s="10"/>
+      <c r="DP3" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="DL3" s="14" t="s">
+      <c r="DQ3" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="DM3" s="11"/>
-      <c r="DN3" s="11"/>
-      <c r="DO3" s="11"/>
-      <c r="DP3" s="11" t="s">
+      <c r="DR3" s="10"/>
+      <c r="DS3" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="DQ3" s="11" t="s">
+      <c r="DT3" s="10"/>
+      <c r="DU3" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="DR3" s="11"/>
-      <c r="DS3" s="11" t="s">
+      <c r="DV3" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="DT3" s="11"/>
-      <c r="DU3" s="11" t="s">
+      <c r="DW3" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="DV3" s="23" t="s">
+      <c r="DX3" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="DW3" s="23" t="s">
+      <c r="DY3" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="DX3" s="23" t="s">
+      <c r="DZ3" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="DY3" s="23" t="s">
+      <c r="EA3" s="10" t="s">
         <v>190</v>
-      </c>
-      <c r="DZ3" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="EA3" s="11" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:131" ht="115" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="69" t="s">
+        <v>192</v>
+      </c>
+      <c r="C4" s="70"/>
+      <c r="D4" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="E4" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="15" t="s">
+      <c r="F4" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="I4" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="J4" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="K4" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="P4" s="28">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="R4" s="66" t="s">
+        <v>192</v>
+      </c>
+      <c r="S4" s="71"/>
+      <c r="T4" s="66" t="s">
+        <v>199</v>
+      </c>
+      <c r="U4" s="71"/>
+      <c r="V4" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="W4" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="X4" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="Y4" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="Z4" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="AA4" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB4" s="66" t="s">
         <v>194</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="H4" s="16" t="s">
+      <c r="AC4" s="71"/>
+      <c r="AD4" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="AE4" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="AF4" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="I4" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="J4" s="15" t="s">
+      <c r="AG4" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="AH4" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="AI4" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="AJ4" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="AK4" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="AL4" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="AM4" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="AN4" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO4" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="AP4" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="AQ4" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="AR4" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="AS4" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="AT4" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="AU4" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="AV4" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="AW4" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="AX4" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="AY4" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="AZ4" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="BA4" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="BB4" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="BC4" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="BD4" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="BE4" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="BF4" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="BG4" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="BH4" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="BI4" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="BJ4" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="BK4" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="BL4" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="BM4" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="BN4" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="BO4" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="BP4" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="BQ4" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="BR4" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="BS4" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="BT4" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="BU4" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="BV4" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="BW4" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="BX4" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="BY4" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="BZ4" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="CA4" s="49"/>
+      <c r="CB4" s="47" t="s">
+        <v>223</v>
+      </c>
+      <c r="CC4" s="48"/>
+      <c r="CD4" s="48"/>
+      <c r="CE4" s="48"/>
+      <c r="CF4" s="48"/>
+      <c r="CG4" s="49"/>
+      <c r="CH4" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="CI4" s="47" t="s">
+        <v>223</v>
+      </c>
+      <c r="CJ4" s="48"/>
+      <c r="CK4" s="48"/>
+      <c r="CL4" s="48"/>
+      <c r="CM4" s="48"/>
+      <c r="CN4" s="48"/>
+      <c r="CO4" s="48"/>
+      <c r="CP4" s="48"/>
+      <c r="CQ4" s="48"/>
+      <c r="CR4" s="49"/>
+      <c r="CS4" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="CT4" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="CU4" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="CV4" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="L4" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="N4" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="O4" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="P4" s="30">
+      <c r="CW4" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="CX4" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="CY4" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="CZ4" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="DA4" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="DB4" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="DC4" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="DD4" s="47" t="s">
+        <v>223</v>
+      </c>
+      <c r="DE4" s="48"/>
+      <c r="DF4" s="48"/>
+      <c r="DG4" s="48"/>
+      <c r="DH4" s="49"/>
+      <c r="DI4" s="47" t="s">
+        <v>194</v>
+      </c>
+      <c r="DJ4" s="48"/>
+      <c r="DK4" s="48"/>
+      <c r="DL4" s="49"/>
+      <c r="DM4" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="DN4" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="DO4" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="DP4" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="DQ4" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="DR4" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="DS4" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="DT4" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="DU4" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="DV4" s="48"/>
+      <c r="DW4" s="48"/>
+      <c r="DX4" s="48"/>
+      <c r="DY4" s="49"/>
+      <c r="DZ4" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="EA4" s="14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:131" s="32" customFormat="1" ht="137.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="66" t="s">
+        <v>240</v>
+      </c>
+      <c r="C5" s="68"/>
+      <c r="D5" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="H5" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="N5" s="66" t="s">
+        <v>241</v>
+      </c>
+      <c r="O5" s="68"/>
+      <c r="P5" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q5" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="R5" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="S5" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="T5" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="U5" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="V5" s="66" t="s">
+        <v>245</v>
+      </c>
+      <c r="W5" s="68"/>
+      <c r="X5" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="Y5" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="Z5" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA5" s="66" t="s">
+        <v>246</v>
+      </c>
+      <c r="AB5" s="68"/>
+      <c r="AC5" s="68"/>
+      <c r="AD5" s="68"/>
+      <c r="AE5" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="AF5" s="68"/>
+      <c r="AG5" s="68"/>
+      <c r="AH5" s="66" t="s">
+        <v>241</v>
+      </c>
+      <c r="AI5" s="68"/>
+      <c r="AJ5" s="68"/>
+      <c r="AK5" s="66" t="s">
+        <v>240</v>
+      </c>
+      <c r="AL5" s="68"/>
+      <c r="AM5" s="68"/>
+      <c r="AN5" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="AO5" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="AP5" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="AQ5" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="AR5" s="48"/>
+      <c r="AS5" s="48"/>
+      <c r="AT5" s="48"/>
+      <c r="AU5" s="49"/>
+      <c r="AV5" s="41" t="s">
+        <v>251</v>
+      </c>
+      <c r="AW5" s="42"/>
+      <c r="AX5" s="42"/>
+      <c r="AY5" s="43"/>
+      <c r="AZ5" s="41" t="s">
+        <v>276</v>
+      </c>
+      <c r="BA5" s="42"/>
+      <c r="BB5" s="42"/>
+      <c r="BC5" s="43"/>
+      <c r="BD5" s="41" t="s">
+        <v>252</v>
+      </c>
+      <c r="BE5" s="42"/>
+      <c r="BF5" s="42"/>
+      <c r="BG5" s="43"/>
+      <c r="BH5" s="41" t="s">
+        <v>253</v>
+      </c>
+      <c r="BI5" s="42"/>
+      <c r="BJ5" s="42"/>
+      <c r="BK5" s="43"/>
+      <c r="BL5" s="41" t="s">
+        <v>254</v>
+      </c>
+      <c r="BM5" s="42"/>
+      <c r="BN5" s="42"/>
+      <c r="BO5" s="43"/>
+      <c r="BP5" s="41" t="s">
+        <v>255</v>
+      </c>
+      <c r="BQ5" s="42"/>
+      <c r="BR5" s="42"/>
+      <c r="BS5" s="43"/>
+      <c r="BT5" s="41" t="s">
+        <v>256</v>
+      </c>
+      <c r="BU5" s="42"/>
+      <c r="BV5" s="42"/>
+      <c r="BW5" s="43"/>
+      <c r="BX5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="BY5" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="BZ5" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="CA5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="CB5" s="47" t="s">
+        <v>259</v>
+      </c>
+      <c r="CC5" s="48"/>
+      <c r="CD5" s="48"/>
+      <c r="CE5" s="49"/>
+      <c r="CF5" s="47" t="s">
+        <v>260</v>
+      </c>
+      <c r="CG5" s="49"/>
+      <c r="CH5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="CI5" s="47" t="s">
+        <v>261</v>
+      </c>
+      <c r="CJ5" s="48"/>
+      <c r="CK5" s="48"/>
+      <c r="CL5" s="48"/>
+      <c r="CM5" s="48"/>
+      <c r="CN5" s="48"/>
+      <c r="CO5" s="48"/>
+      <c r="CP5" s="48"/>
+      <c r="CQ5" s="48"/>
+      <c r="CR5" s="49"/>
+      <c r="CS5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="CT5" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="CU5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="CV5" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="CW5" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="CX5" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="CY5" s="49"/>
+      <c r="CZ5" s="47" t="s">
+        <v>263</v>
+      </c>
+      <c r="DA5" s="49"/>
+      <c r="DB5" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="DC5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="DD5" s="59" t="s">
+        <v>264</v>
+      </c>
+      <c r="DE5" s="60"/>
+      <c r="DF5" s="60"/>
+      <c r="DG5" s="60"/>
+      <c r="DH5" s="61"/>
+      <c r="DI5" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="DJ5" s="48"/>
+      <c r="DK5" s="48"/>
+      <c r="DL5" s="49"/>
+      <c r="DM5" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="DN5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="DO5" s="47" t="s">
+        <v>265</v>
+      </c>
+      <c r="DP5" s="49"/>
+      <c r="DQ5" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="DR5" s="49"/>
+      <c r="DS5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="DT5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="DU5" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="DV5" s="47" t="s">
+        <v>267</v>
+      </c>
+      <c r="DW5" s="48"/>
+      <c r="DX5" s="48"/>
+      <c r="DY5" s="49"/>
+      <c r="DZ5" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="EA5" s="14" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:131" s="33" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="62" t="s">
+        <v>271</v>
+      </c>
+      <c r="G6" s="62"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="66" t="s">
+        <v>273</v>
+      </c>
+      <c r="R6" s="68"/>
+      <c r="S6" s="68"/>
+      <c r="T6" s="68"/>
+      <c r="U6" s="68"/>
+      <c r="V6" s="68"/>
+      <c r="W6" s="68"/>
+      <c r="X6" s="68"/>
+      <c r="Y6" s="66"/>
+      <c r="Z6" s="66"/>
+      <c r="AA6" s="66" t="s">
+        <v>273</v>
+      </c>
+      <c r="AB6" s="68"/>
+      <c r="AC6" s="68"/>
+      <c r="AD6" s="68"/>
+      <c r="AE6" s="66"/>
+      <c r="AF6" s="66"/>
+      <c r="AG6" s="66"/>
+      <c r="AH6" s="66"/>
+      <c r="AI6" s="66"/>
+      <c r="AJ6" s="66"/>
+      <c r="AK6" s="66"/>
+      <c r="AL6" s="66"/>
+      <c r="AM6" s="66"/>
+      <c r="AN6" s="66"/>
+      <c r="AO6" s="66"/>
+      <c r="AP6" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="AQ6" s="47"/>
+      <c r="AR6" s="48"/>
+      <c r="AS6" s="48"/>
+      <c r="AT6" s="48"/>
+      <c r="AU6" s="48"/>
+      <c r="AV6" s="48"/>
+      <c r="AW6" s="48"/>
+      <c r="AX6" s="48"/>
+      <c r="AY6" s="48"/>
+      <c r="AZ6" s="48"/>
+      <c r="BA6" s="48"/>
+      <c r="BB6" s="48"/>
+      <c r="BC6" s="48"/>
+      <c r="BD6" s="48"/>
+      <c r="BE6" s="48"/>
+      <c r="BF6" s="48"/>
+      <c r="BG6" s="48"/>
+      <c r="BH6" s="48"/>
+      <c r="BI6" s="48"/>
+      <c r="BJ6" s="48"/>
+      <c r="BK6" s="48"/>
+      <c r="BL6" s="48"/>
+      <c r="BM6" s="48"/>
+      <c r="BN6" s="48"/>
+      <c r="BO6" s="48"/>
+      <c r="BP6" s="48"/>
+      <c r="BQ6" s="48"/>
+      <c r="BR6" s="48"/>
+      <c r="BS6" s="48"/>
+      <c r="BT6" s="48"/>
+      <c r="BU6" s="48"/>
+      <c r="BV6" s="48"/>
+      <c r="BW6" s="49"/>
+      <c r="BX6" s="47"/>
+      <c r="BY6" s="48"/>
+      <c r="BZ6" s="48"/>
+      <c r="CA6" s="48"/>
+      <c r="CB6" s="48"/>
+      <c r="CC6" s="48"/>
+      <c r="CD6" s="48"/>
+      <c r="CE6" s="48"/>
+      <c r="CF6" s="48"/>
+      <c r="CG6" s="48"/>
+      <c r="CH6" s="48"/>
+      <c r="CI6" s="48"/>
+      <c r="CJ6" s="48"/>
+      <c r="CK6" s="48"/>
+      <c r="CL6" s="48"/>
+      <c r="CM6" s="48"/>
+      <c r="CN6" s="48"/>
+      <c r="CO6" s="48"/>
+      <c r="CP6" s="48"/>
+      <c r="CQ6" s="48"/>
+      <c r="CR6" s="49"/>
+      <c r="CS6" s="47"/>
+      <c r="CT6" s="48"/>
+      <c r="CU6" s="48"/>
+      <c r="CV6" s="48"/>
+      <c r="CW6" s="48"/>
+      <c r="CX6" s="48"/>
+      <c r="CY6" s="48"/>
+      <c r="CZ6" s="48"/>
+      <c r="DA6" s="48"/>
+      <c r="DB6" s="48"/>
+      <c r="DC6" s="48"/>
+      <c r="DD6" s="48"/>
+      <c r="DE6" s="48"/>
+      <c r="DF6" s="48"/>
+      <c r="DG6" s="48"/>
+      <c r="DH6" s="48"/>
+      <c r="DI6" s="48"/>
+      <c r="DJ6" s="48"/>
+      <c r="DK6" s="48"/>
+      <c r="DL6" s="48"/>
+      <c r="DM6" s="49"/>
+      <c r="DN6" s="47"/>
+      <c r="DO6" s="48"/>
+      <c r="DP6" s="48"/>
+      <c r="DQ6" s="48"/>
+      <c r="DR6" s="49"/>
+      <c r="DS6" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="DT6" s="19"/>
+      <c r="DU6" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="DV6" s="59"/>
+      <c r="DW6" s="60"/>
+      <c r="DX6" s="60"/>
+      <c r="DY6" s="60"/>
+      <c r="DZ6" s="60"/>
+      <c r="EA6" s="61"/>
+    </row>
+    <row r="7" spans="1:131" s="33" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62" t="s">
+        <v>241</v>
+      </c>
+      <c r="G7" s="62"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="62" t="s">
+        <v>241</v>
+      </c>
+      <c r="J7" s="68"/>
+      <c r="K7" s="68"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
+      <c r="N7" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="O7" s="59"/>
+      <c r="P7" s="61"/>
+      <c r="Q7" s="59"/>
+      <c r="R7" s="60"/>
+      <c r="S7" s="60"/>
+      <c r="T7" s="60"/>
+      <c r="U7" s="61"/>
+      <c r="V7" s="62" t="s">
+        <v>241</v>
+      </c>
+      <c r="W7" s="62"/>
+      <c r="X7" s="59"/>
+      <c r="Y7" s="60"/>
+      <c r="Z7" s="60"/>
+      <c r="AA7" s="60"/>
+      <c r="AB7" s="60"/>
+      <c r="AC7" s="60"/>
+      <c r="AD7" s="60"/>
+      <c r="AE7" s="60"/>
+      <c r="AF7" s="60"/>
+      <c r="AG7" s="60"/>
+      <c r="AH7" s="60"/>
+      <c r="AI7" s="60"/>
+      <c r="AJ7" s="61"/>
+      <c r="AK7" s="59"/>
+      <c r="AL7" s="60"/>
+      <c r="AM7" s="60"/>
+      <c r="AN7" s="60"/>
+      <c r="AO7" s="60"/>
+      <c r="AP7" s="61"/>
+      <c r="AQ7" s="59" t="s">
+        <v>241</v>
+      </c>
+      <c r="AR7" s="61"/>
+      <c r="AS7" s="59"/>
+      <c r="AT7" s="61"/>
+      <c r="AU7" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="AV7" s="59"/>
+      <c r="AW7" s="60"/>
+      <c r="AX7" s="60"/>
+      <c r="AY7" s="60"/>
+      <c r="AZ7" s="60"/>
+      <c r="BA7" s="60"/>
+      <c r="BB7" s="60"/>
+      <c r="BC7" s="60"/>
+      <c r="BD7" s="60"/>
+      <c r="BE7" s="60"/>
+      <c r="BF7" s="60"/>
+      <c r="BG7" s="60"/>
+      <c r="BH7" s="60"/>
+      <c r="BI7" s="60"/>
+      <c r="BJ7" s="60"/>
+      <c r="BK7" s="60"/>
+      <c r="BL7" s="60"/>
+      <c r="BM7" s="60"/>
+      <c r="BN7" s="60"/>
+      <c r="BO7" s="60"/>
+      <c r="BP7" s="60"/>
+      <c r="BQ7" s="60"/>
+      <c r="BR7" s="60"/>
+      <c r="BS7" s="60"/>
+      <c r="BT7" s="60"/>
+      <c r="BU7" s="60"/>
+      <c r="BV7" s="60"/>
+      <c r="BW7" s="61"/>
+      <c r="BX7" s="59"/>
+      <c r="BY7" s="60"/>
+      <c r="BZ7" s="60"/>
+      <c r="CA7" s="60"/>
+      <c r="CB7" s="60"/>
+      <c r="CC7" s="60"/>
+      <c r="CD7" s="60"/>
+      <c r="CE7" s="60"/>
+      <c r="CF7" s="60"/>
+      <c r="CG7" s="60"/>
+      <c r="CH7" s="60"/>
+      <c r="CI7" s="60"/>
+      <c r="CJ7" s="60"/>
+      <c r="CK7" s="60"/>
+      <c r="CL7" s="60"/>
+      <c r="CM7" s="60"/>
+      <c r="CN7" s="60"/>
+      <c r="CO7" s="60"/>
+      <c r="CP7" s="60"/>
+      <c r="CQ7" s="60"/>
+      <c r="CR7" s="61"/>
+      <c r="CS7" s="59"/>
+      <c r="CT7" s="60"/>
+      <c r="CU7" s="60"/>
+      <c r="CV7" s="60"/>
+      <c r="CW7" s="60"/>
+      <c r="CX7" s="60"/>
+      <c r="CY7" s="60"/>
+      <c r="CZ7" s="60"/>
+      <c r="DA7" s="60"/>
+      <c r="DB7" s="60"/>
+      <c r="DC7" s="60"/>
+      <c r="DD7" s="60"/>
+      <c r="DE7" s="60"/>
+      <c r="DF7" s="60"/>
+      <c r="DG7" s="60"/>
+      <c r="DH7" s="60"/>
+      <c r="DI7" s="60"/>
+      <c r="DJ7" s="60"/>
+      <c r="DK7" s="60"/>
+      <c r="DL7" s="60"/>
+      <c r="DM7" s="61"/>
+      <c r="DN7" s="59"/>
+      <c r="DO7" s="60"/>
+      <c r="DP7" s="60"/>
+      <c r="DQ7" s="60"/>
+      <c r="DR7" s="60"/>
+      <c r="DS7" s="61"/>
+      <c r="DT7" s="59" t="s">
+        <v>241</v>
+      </c>
+      <c r="DU7" s="60"/>
+      <c r="DV7" s="60"/>
+      <c r="DW7" s="60"/>
+      <c r="DX7" s="60"/>
+      <c r="DY7" s="60"/>
+      <c r="DZ7" s="62"/>
+      <c r="EA7" s="62"/>
+    </row>
+    <row r="8" spans="1:131" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="B8" s="16">
         <v>1</v>
       </c>
-      <c r="Q4" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="R4" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="S4" s="49"/>
-      <c r="T4" s="46" t="s">
-        <v>201</v>
-      </c>
-      <c r="U4" s="49"/>
-      <c r="V4" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="W4" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="X4" s="25" t="s">
-        <v>207</v>
-      </c>
-      <c r="Y4" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="Z4" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="AA4" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="AB4" s="46" t="s">
-        <v>196</v>
-      </c>
-      <c r="AC4" s="49"/>
-      <c r="AD4" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="AE4" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="AF4" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="AG4" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="AH4" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="AI4" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="AJ4" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="AK4" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="AL4" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="AM4" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="AN4" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="AO4" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="AP4" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="AQ4" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="AR4" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="AS4" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="AT4" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="AU4" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="AV4" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="AW4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="AX4" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="AY4" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="AZ4" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="BA4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="BB4" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="BC4" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="BD4" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="BE4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="BF4" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="BG4" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="BH4" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="BI4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="BJ4" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="BK4" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="BL4" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="BM4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="BN4" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="BO4" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="BP4" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="BQ4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="BR4" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="BS4" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="BT4" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="BU4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="BV4" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="BW4" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="BX4" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="BY4" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="BZ4" s="38" t="s">
-        <v>214</v>
-      </c>
-      <c r="CA4" s="40"/>
-      <c r="CB4" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="CC4" s="39"/>
-      <c r="CD4" s="39"/>
-      <c r="CE4" s="39"/>
-      <c r="CF4" s="39"/>
-      <c r="CG4" s="40"/>
-      <c r="CH4" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="CI4" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="CJ4" s="39"/>
-      <c r="CK4" s="39"/>
-      <c r="CL4" s="39"/>
-      <c r="CM4" s="39"/>
-      <c r="CN4" s="39"/>
-      <c r="CO4" s="39"/>
-      <c r="CP4" s="39"/>
-      <c r="CQ4" s="39"/>
-      <c r="CR4" s="40"/>
-      <c r="CS4" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="CT4" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="CU4" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="CV4" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="CW4" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="CX4" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="CY4" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="CZ4" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="DA4" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="DB4" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="DC4" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="DD4" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="DE4" s="39"/>
-      <c r="DF4" s="39"/>
-      <c r="DG4" s="39"/>
-      <c r="DH4" s="40"/>
-      <c r="DI4" s="38" t="s">
-        <v>196</v>
-      </c>
-      <c r="DJ4" s="39"/>
-      <c r="DK4" s="39"/>
-      <c r="DL4" s="40"/>
-      <c r="DM4" s="17" t="s">
-        <v>234</v>
-      </c>
-      <c r="DN4" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="DO4" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="DP4" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="DQ4" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="DR4" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="DS4" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="DT4" s="18" t="s">
-        <v>282</v>
-      </c>
-      <c r="DU4" s="38" t="s">
-        <v>239</v>
-      </c>
-      <c r="DV4" s="39"/>
-      <c r="DW4" s="39"/>
-      <c r="DX4" s="39"/>
-      <c r="DY4" s="40"/>
-      <c r="DZ4" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="EA4" s="15" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="5" spans="1:131" s="34" customFormat="1" ht="137.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="B5" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="H5" s="38" t="s">
-        <v>241</v>
-      </c>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="31" t="s">
-        <v>244</v>
-      </c>
-      <c r="N5" s="46" t="s">
-        <v>242</v>
-      </c>
-      <c r="O5" s="45"/>
-      <c r="P5" s="30" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q5" s="32" t="s">
-        <v>245</v>
-      </c>
-      <c r="R5" s="33" t="s">
-        <v>246</v>
-      </c>
-      <c r="S5" s="32" t="s">
-        <v>242</v>
-      </c>
-      <c r="T5" s="33" t="s">
-        <v>246</v>
-      </c>
-      <c r="U5" s="32" t="s">
-        <v>242</v>
-      </c>
-      <c r="V5" s="46" t="s">
-        <v>246</v>
-      </c>
-      <c r="W5" s="45"/>
-      <c r="X5" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="Y5" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="Z5" s="15" t="s">
-        <v>249</v>
-      </c>
-      <c r="AA5" s="46" t="s">
-        <v>247</v>
-      </c>
-      <c r="AB5" s="45"/>
-      <c r="AC5" s="45"/>
-      <c r="AD5" s="45"/>
-      <c r="AE5" s="46" t="s">
-        <v>248</v>
-      </c>
-      <c r="AF5" s="45"/>
-      <c r="AG5" s="45"/>
-      <c r="AH5" s="46" t="s">
-        <v>242</v>
-      </c>
-      <c r="AI5" s="45"/>
-      <c r="AJ5" s="45"/>
-      <c r="AK5" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="AL5" s="45"/>
-      <c r="AM5" s="45"/>
-      <c r="AN5" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="AO5" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="AP5" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="AQ5" s="38" t="s">
-        <v>241</v>
-      </c>
-      <c r="AR5" s="39"/>
-      <c r="AS5" s="39"/>
-      <c r="AT5" s="39"/>
-      <c r="AU5" s="40"/>
-      <c r="AV5" s="60" t="s">
-        <v>252</v>
-      </c>
-      <c r="AW5" s="61"/>
-      <c r="AX5" s="61"/>
-      <c r="AY5" s="62"/>
-      <c r="AZ5" s="60" t="s">
-        <v>275</v>
-      </c>
-      <c r="BA5" s="61"/>
-      <c r="BB5" s="61"/>
-      <c r="BC5" s="62"/>
-      <c r="BD5" s="60" t="s">
-        <v>253</v>
-      </c>
-      <c r="BE5" s="61"/>
-      <c r="BF5" s="61"/>
-      <c r="BG5" s="62"/>
-      <c r="BH5" s="60" t="s">
-        <v>254</v>
-      </c>
-      <c r="BI5" s="61"/>
-      <c r="BJ5" s="61"/>
-      <c r="BK5" s="62"/>
-      <c r="BL5" s="60" t="s">
-        <v>255</v>
-      </c>
-      <c r="BM5" s="61"/>
-      <c r="BN5" s="61"/>
-      <c r="BO5" s="62"/>
-      <c r="BP5" s="60" t="s">
-        <v>256</v>
-      </c>
-      <c r="BQ5" s="61"/>
-      <c r="BR5" s="61"/>
-      <c r="BS5" s="62"/>
-      <c r="BT5" s="60" t="s">
-        <v>257</v>
-      </c>
-      <c r="BU5" s="61"/>
-      <c r="BV5" s="61"/>
-      <c r="BW5" s="62"/>
-      <c r="BX5" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="BY5" s="15" t="s">
-        <v>258</v>
-      </c>
-      <c r="BZ5" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="CA5" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="CB5" s="38" t="s">
-        <v>260</v>
-      </c>
-      <c r="CC5" s="39"/>
-      <c r="CD5" s="39"/>
-      <c r="CE5" s="40"/>
-      <c r="CF5" s="38" t="s">
-        <v>261</v>
-      </c>
-      <c r="CG5" s="40"/>
-      <c r="CH5" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="CI5" s="38" t="s">
-        <v>262</v>
-      </c>
-      <c r="CJ5" s="39"/>
-      <c r="CK5" s="39"/>
-      <c r="CL5" s="39"/>
-      <c r="CM5" s="39"/>
-      <c r="CN5" s="39"/>
-      <c r="CO5" s="39"/>
-      <c r="CP5" s="39"/>
-      <c r="CQ5" s="39"/>
-      <c r="CR5" s="40"/>
-      <c r="CS5" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="CT5" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="CU5" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="CV5" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="CW5" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="CX5" s="38" t="s">
-        <v>241</v>
-      </c>
-      <c r="CY5" s="40"/>
-      <c r="CZ5" s="38" t="s">
-        <v>264</v>
-      </c>
-      <c r="DA5" s="40"/>
-      <c r="DB5" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="DC5" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="DD5" s="41" t="s">
-        <v>265</v>
-      </c>
-      <c r="DE5" s="42"/>
-      <c r="DF5" s="42"/>
-      <c r="DG5" s="42"/>
-      <c r="DH5" s="44"/>
-      <c r="DI5" s="38" t="s">
-        <v>241</v>
-      </c>
-      <c r="DJ5" s="39"/>
-      <c r="DK5" s="39"/>
-      <c r="DL5" s="40"/>
-      <c r="DM5" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="DN5" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="DO5" s="38" t="s">
-        <v>266</v>
-      </c>
-      <c r="DP5" s="40"/>
-      <c r="DQ5" s="38" t="s">
-        <v>241</v>
-      </c>
-      <c r="DR5" s="40"/>
-      <c r="DS5" s="37" t="s">
-        <v>243</v>
-      </c>
-      <c r="DT5" s="15" t="s">
-        <v>281</v>
-      </c>
-      <c r="DU5" s="15" t="s">
-        <v>279</v>
-      </c>
-      <c r="DV5" s="38" t="s">
-        <v>267</v>
-      </c>
-      <c r="DW5" s="39"/>
-      <c r="DX5" s="39"/>
-      <c r="DY5" s="40"/>
-      <c r="DZ5" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="EA5" s="15" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="6" spans="1:131" s="35" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="43" t="s">
-        <v>270</v>
-      </c>
-      <c r="G6" s="43"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46" t="s">
-        <v>272</v>
-      </c>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
-      <c r="U6" s="45"/>
-      <c r="V6" s="45"/>
-      <c r="W6" s="45"/>
-      <c r="X6" s="45"/>
-      <c r="Y6" s="46"/>
-      <c r="Z6" s="46"/>
-      <c r="AA6" s="46" t="s">
-        <v>272</v>
-      </c>
-      <c r="AB6" s="45"/>
-      <c r="AC6" s="45"/>
-      <c r="AD6" s="45"/>
-      <c r="AE6" s="46"/>
-      <c r="AF6" s="46"/>
-      <c r="AG6" s="46"/>
-      <c r="AH6" s="46"/>
-      <c r="AI6" s="46"/>
-      <c r="AJ6" s="46"/>
-      <c r="AK6" s="46"/>
-      <c r="AL6" s="46"/>
-      <c r="AM6" s="46"/>
-      <c r="AN6" s="46"/>
-      <c r="AO6" s="46"/>
-      <c r="AP6" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="AQ6" s="38"/>
-      <c r="AR6" s="39"/>
-      <c r="AS6" s="39"/>
-      <c r="AT6" s="39"/>
-      <c r="AU6" s="39"/>
-      <c r="AV6" s="39"/>
-      <c r="AW6" s="39"/>
-      <c r="AX6" s="39"/>
-      <c r="AY6" s="39"/>
-      <c r="AZ6" s="39"/>
-      <c r="BA6" s="39"/>
-      <c r="BB6" s="39"/>
-      <c r="BC6" s="39"/>
-      <c r="BD6" s="39"/>
-      <c r="BE6" s="39"/>
-      <c r="BF6" s="39"/>
-      <c r="BG6" s="39"/>
-      <c r="BH6" s="39"/>
-      <c r="BI6" s="39"/>
-      <c r="BJ6" s="39"/>
-      <c r="BK6" s="39"/>
-      <c r="BL6" s="39"/>
-      <c r="BM6" s="39"/>
-      <c r="BN6" s="39"/>
-      <c r="BO6" s="39"/>
-      <c r="BP6" s="39"/>
-      <c r="BQ6" s="39"/>
-      <c r="BR6" s="39"/>
-      <c r="BS6" s="39"/>
-      <c r="BT6" s="39"/>
-      <c r="BU6" s="39"/>
-      <c r="BV6" s="39"/>
-      <c r="BW6" s="40"/>
-      <c r="BX6" s="38"/>
-      <c r="BY6" s="39"/>
-      <c r="BZ6" s="39"/>
-      <c r="CA6" s="39"/>
-      <c r="CB6" s="39"/>
-      <c r="CC6" s="39"/>
-      <c r="CD6" s="39"/>
-      <c r="CE6" s="39"/>
-      <c r="CF6" s="39"/>
-      <c r="CG6" s="39"/>
-      <c r="CH6" s="39"/>
-      <c r="CI6" s="39"/>
-      <c r="CJ6" s="39"/>
-      <c r="CK6" s="39"/>
-      <c r="CL6" s="39"/>
-      <c r="CM6" s="39"/>
-      <c r="CN6" s="39"/>
-      <c r="CO6" s="39"/>
-      <c r="CP6" s="39"/>
-      <c r="CQ6" s="39"/>
-      <c r="CR6" s="40"/>
-      <c r="CS6" s="38"/>
-      <c r="CT6" s="39"/>
-      <c r="CU6" s="39"/>
-      <c r="CV6" s="39"/>
-      <c r="CW6" s="39"/>
-      <c r="CX6" s="39"/>
-      <c r="CY6" s="39"/>
-      <c r="CZ6" s="39"/>
-      <c r="DA6" s="39"/>
-      <c r="DB6" s="39"/>
-      <c r="DC6" s="39"/>
-      <c r="DD6" s="39"/>
-      <c r="DE6" s="39"/>
-      <c r="DF6" s="39"/>
-      <c r="DG6" s="39"/>
-      <c r="DH6" s="39"/>
-      <c r="DI6" s="39"/>
-      <c r="DJ6" s="39"/>
-      <c r="DK6" s="39"/>
-      <c r="DL6" s="39"/>
-      <c r="DM6" s="40"/>
-      <c r="DN6" s="38"/>
-      <c r="DO6" s="39"/>
-      <c r="DP6" s="39"/>
-      <c r="DQ6" s="39"/>
-      <c r="DR6" s="40"/>
-      <c r="DS6" s="20" t="s">
-        <v>270</v>
-      </c>
-      <c r="DT6" s="20"/>
-      <c r="DU6" s="20" t="s">
-        <v>270</v>
-      </c>
-      <c r="DV6" s="41"/>
-      <c r="DW6" s="42"/>
-      <c r="DX6" s="42"/>
-      <c r="DY6" s="42"/>
-      <c r="DZ6" s="42"/>
-      <c r="EA6" s="44"/>
-    </row>
-    <row r="7" spans="1:131" s="35" customFormat="1" ht="23" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43" t="s">
-        <v>242</v>
-      </c>
-      <c r="G7" s="43"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="43" t="s">
-        <v>242</v>
-      </c>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="56"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="O7" s="41"/>
-      <c r="P7" s="44"/>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="42"/>
-      <c r="S7" s="42"/>
-      <c r="T7" s="42"/>
-      <c r="U7" s="44"/>
-      <c r="V7" s="43" t="s">
-        <v>242</v>
-      </c>
-      <c r="W7" s="43"/>
-      <c r="X7" s="41"/>
-      <c r="Y7" s="42"/>
-      <c r="Z7" s="42"/>
-      <c r="AA7" s="42"/>
-      <c r="AB7" s="42"/>
-      <c r="AC7" s="42"/>
-      <c r="AD7" s="42"/>
-      <c r="AE7" s="42"/>
-      <c r="AF7" s="42"/>
-      <c r="AG7" s="42"/>
-      <c r="AH7" s="42"/>
-      <c r="AI7" s="42"/>
-      <c r="AJ7" s="44"/>
-      <c r="AK7" s="41"/>
-      <c r="AL7" s="42"/>
-      <c r="AM7" s="42"/>
-      <c r="AN7" s="42"/>
-      <c r="AO7" s="42"/>
-      <c r="AP7" s="44"/>
-      <c r="AQ7" s="41" t="s">
-        <v>242</v>
-      </c>
-      <c r="AR7" s="44"/>
-      <c r="AS7" s="41"/>
-      <c r="AT7" s="44"/>
-      <c r="AU7" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="AV7" s="41"/>
-      <c r="AW7" s="42"/>
-      <c r="AX7" s="42"/>
-      <c r="AY7" s="42"/>
-      <c r="AZ7" s="42"/>
-      <c r="BA7" s="42"/>
-      <c r="BB7" s="42"/>
-      <c r="BC7" s="42"/>
-      <c r="BD7" s="42"/>
-      <c r="BE7" s="42"/>
-      <c r="BF7" s="42"/>
-      <c r="BG7" s="42"/>
-      <c r="BH7" s="42"/>
-      <c r="BI7" s="42"/>
-      <c r="BJ7" s="42"/>
-      <c r="BK7" s="42"/>
-      <c r="BL7" s="42"/>
-      <c r="BM7" s="42"/>
-      <c r="BN7" s="42"/>
-      <c r="BO7" s="42"/>
-      <c r="BP7" s="42"/>
-      <c r="BQ7" s="42"/>
-      <c r="BR7" s="42"/>
-      <c r="BS7" s="42"/>
-      <c r="BT7" s="42"/>
-      <c r="BU7" s="42"/>
-      <c r="BV7" s="42"/>
-      <c r="BW7" s="44"/>
-      <c r="BX7" s="41"/>
-      <c r="BY7" s="42"/>
-      <c r="BZ7" s="42"/>
-      <c r="CA7" s="42"/>
-      <c r="CB7" s="42"/>
-      <c r="CC7" s="42"/>
-      <c r="CD7" s="42"/>
-      <c r="CE7" s="42"/>
-      <c r="CF7" s="42"/>
-      <c r="CG7" s="42"/>
-      <c r="CH7" s="42"/>
-      <c r="CI7" s="42"/>
-      <c r="CJ7" s="42"/>
-      <c r="CK7" s="42"/>
-      <c r="CL7" s="42"/>
-      <c r="CM7" s="42"/>
-      <c r="CN7" s="42"/>
-      <c r="CO7" s="42"/>
-      <c r="CP7" s="42"/>
-      <c r="CQ7" s="42"/>
-      <c r="CR7" s="44"/>
-      <c r="CS7" s="41"/>
-      <c r="CT7" s="42"/>
-      <c r="CU7" s="42"/>
-      <c r="CV7" s="42"/>
-      <c r="CW7" s="42"/>
-      <c r="CX7" s="42"/>
-      <c r="CY7" s="42"/>
-      <c r="CZ7" s="42"/>
-      <c r="DA7" s="42"/>
-      <c r="DB7" s="42"/>
-      <c r="DC7" s="42"/>
-      <c r="DD7" s="42"/>
-      <c r="DE7" s="42"/>
-      <c r="DF7" s="42"/>
-      <c r="DG7" s="42"/>
-      <c r="DH7" s="42"/>
-      <c r="DI7" s="42"/>
-      <c r="DJ7" s="42"/>
-      <c r="DK7" s="42"/>
-      <c r="DL7" s="42"/>
-      <c r="DM7" s="44"/>
-      <c r="DN7" s="41"/>
-      <c r="DO7" s="42"/>
-      <c r="DP7" s="42"/>
-      <c r="DQ7" s="42"/>
-      <c r="DR7" s="42"/>
-      <c r="DS7" s="44"/>
-      <c r="DT7" s="41" t="s">
-        <v>242</v>
-      </c>
-      <c r="DU7" s="42"/>
-      <c r="DV7" s="42"/>
-      <c r="DW7" s="42"/>
-      <c r="DX7" s="42"/>
-      <c r="DY7" s="42"/>
-      <c r="DZ7" s="43"/>
-      <c r="EA7" s="43"/>
-    </row>
-    <row r="8" spans="1:131" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
-        <v>276</v>
-      </c>
-      <c r="B8" s="17">
-        <v>1</v>
-      </c>
-      <c r="C8" s="17">
+      <c r="C8" s="16">
         <v>2</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>3</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="21">
         <v>4</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="16">
         <v>5</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="16">
         <v>6</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="16">
         <v>7</v>
       </c>
-      <c r="I8" s="22">
+      <c r="I8" s="21">
         <v>8</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="16">
         <v>9</v>
       </c>
-      <c r="K8" s="17">
+      <c r="K8" s="16">
         <v>10</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="16">
         <v>11</v>
       </c>
-      <c r="M8" s="22">
+      <c r="M8" s="21">
         <v>12</v>
       </c>
-      <c r="N8" s="17">
+      <c r="N8" s="16">
         <v>13</v>
       </c>
-      <c r="O8" s="17">
+      <c r="O8" s="16">
         <v>14</v>
       </c>
-      <c r="P8" s="17">
+      <c r="P8" s="16">
         <v>15</v>
       </c>
-      <c r="Q8" s="22">
+      <c r="Q8" s="21">
         <v>16</v>
       </c>
-      <c r="R8" s="17">
+      <c r="R8" s="16">
         <v>17</v>
       </c>
-      <c r="S8" s="17">
+      <c r="S8" s="16">
         <v>18</v>
       </c>
-      <c r="T8" s="17">
+      <c r="T8" s="16">
         <v>19</v>
       </c>
-      <c r="U8" s="22">
+      <c r="U8" s="21">
         <v>20</v>
       </c>
-      <c r="V8" s="17">
+      <c r="V8" s="16">
         <v>21</v>
       </c>
-      <c r="W8" s="17">
+      <c r="W8" s="16">
         <v>22</v>
       </c>
-      <c r="X8" s="17">
+      <c r="X8" s="16">
         <v>23</v>
       </c>
-      <c r="Y8" s="22">
+      <c r="Y8" s="21">
         <v>24</v>
       </c>
-      <c r="Z8" s="17">
+      <c r="Z8" s="16">
         <v>25</v>
       </c>
-      <c r="AA8" s="17">
+      <c r="AA8" s="16">
         <v>26</v>
       </c>
-      <c r="AB8" s="17">
+      <c r="AB8" s="16">
         <v>27</v>
       </c>
-      <c r="AC8" s="22">
+      <c r="AC8" s="21">
         <v>28</v>
       </c>
-      <c r="AD8" s="17">
+      <c r="AD8" s="16">
         <v>29</v>
       </c>
-      <c r="AE8" s="17">
+      <c r="AE8" s="16">
         <v>30</v>
       </c>
-      <c r="AF8" s="17">
+      <c r="AF8" s="16">
         <v>31</v>
       </c>
-      <c r="AG8" s="22">
+      <c r="AG8" s="21">
         <v>32</v>
       </c>
-      <c r="AH8" s="17">
+      <c r="AH8" s="16">
         <v>33</v>
       </c>
-      <c r="AI8" s="17">
+      <c r="AI8" s="16">
         <v>34</v>
       </c>
-      <c r="AJ8" s="17">
+      <c r="AJ8" s="16">
         <v>35</v>
       </c>
-      <c r="AK8" s="22">
+      <c r="AK8" s="21">
         <v>36</v>
       </c>
-      <c r="AL8" s="17">
+      <c r="AL8" s="16">
         <v>37</v>
       </c>
-      <c r="AM8" s="17">
+      <c r="AM8" s="16">
         <v>38</v>
       </c>
-      <c r="AN8" s="17">
+      <c r="AN8" s="16">
         <v>39</v>
       </c>
-      <c r="AO8" s="22">
+      <c r="AO8" s="21">
         <v>40</v>
       </c>
-      <c r="AP8" s="17">
+      <c r="AP8" s="16">
         <v>41</v>
       </c>
-      <c r="AQ8" s="17">
+      <c r="AQ8" s="16">
         <v>42</v>
       </c>
-      <c r="AR8" s="17">
+      <c r="AR8" s="16">
         <v>43</v>
       </c>
-      <c r="AS8" s="22">
+      <c r="AS8" s="21">
         <v>44</v>
       </c>
-      <c r="AT8" s="17">
+      <c r="AT8" s="16">
         <v>45</v>
       </c>
-      <c r="AU8" s="17">
+      <c r="AU8" s="16">
         <v>46</v>
       </c>
-      <c r="AV8" s="17">
+      <c r="AV8" s="16">
         <v>47</v>
       </c>
-      <c r="AW8" s="22">
+      <c r="AW8" s="21">
         <v>48</v>
       </c>
-      <c r="AX8" s="17">
+      <c r="AX8" s="16">
         <v>49</v>
       </c>
-      <c r="AY8" s="17">
+      <c r="AY8" s="16">
         <v>50</v>
       </c>
-      <c r="AZ8" s="17">
+      <c r="AZ8" s="16">
         <v>51</v>
       </c>
-      <c r="BA8" s="22">
+      <c r="BA8" s="21">
         <v>52</v>
       </c>
-      <c r="BB8" s="17">
+      <c r="BB8" s="16">
         <v>53</v>
       </c>
-      <c r="BC8" s="17">
+      <c r="BC8" s="16">
         <v>54</v>
       </c>
-      <c r="BD8" s="17">
+      <c r="BD8" s="16">
         <v>55</v>
       </c>
-      <c r="BE8" s="22">
+      <c r="BE8" s="21">
         <v>56</v>
       </c>
-      <c r="BF8" s="17">
+      <c r="BF8" s="16">
         <v>57</v>
       </c>
-      <c r="BG8" s="17">
+      <c r="BG8" s="16">
         <v>58</v>
       </c>
-      <c r="BH8" s="17">
+      <c r="BH8" s="16">
         <v>59</v>
       </c>
-      <c r="BI8" s="22">
+      <c r="BI8" s="21">
         <v>60</v>
       </c>
-      <c r="BJ8" s="17">
+      <c r="BJ8" s="16">
         <v>61</v>
       </c>
-      <c r="BK8" s="17">
+      <c r="BK8" s="16">
         <v>62</v>
       </c>
-      <c r="BL8" s="17">
+      <c r="BL8" s="16">
         <v>63</v>
       </c>
-      <c r="BM8" s="22">
+      <c r="BM8" s="21">
         <v>64</v>
       </c>
-      <c r="BN8" s="17">
+      <c r="BN8" s="16">
         <v>65</v>
       </c>
-      <c r="BO8" s="17">
+      <c r="BO8" s="16">
         <v>66</v>
       </c>
-      <c r="BP8" s="17">
+      <c r="BP8" s="16">
         <v>67</v>
       </c>
-      <c r="BQ8" s="22">
+      <c r="BQ8" s="21">
         <v>68</v>
       </c>
-      <c r="BR8" s="17">
+      <c r="BR8" s="16">
         <v>69</v>
       </c>
-      <c r="BS8" s="17">
+      <c r="BS8" s="16">
         <v>70</v>
       </c>
-      <c r="BT8" s="17">
+      <c r="BT8" s="16">
         <v>71</v>
       </c>
-      <c r="BU8" s="22">
+      <c r="BU8" s="21">
         <v>72</v>
       </c>
-      <c r="BV8" s="17">
+      <c r="BV8" s="16">
         <v>73</v>
       </c>
-      <c r="BW8" s="17">
+      <c r="BW8" s="16">
         <v>74</v>
       </c>
-      <c r="BX8" s="17">
+      <c r="BX8" s="16">
         <v>75</v>
       </c>
-      <c r="BY8" s="22">
+      <c r="BY8" s="21">
         <v>76</v>
       </c>
-      <c r="BZ8" s="17">
+      <c r="BZ8" s="16">
         <v>77</v>
       </c>
-      <c r="CA8" s="17">
+      <c r="CA8" s="16">
         <v>78</v>
       </c>
-      <c r="CB8" s="17">
+      <c r="CB8" s="16">
         <v>79</v>
       </c>
-      <c r="CC8" s="22">
+      <c r="CC8" s="21">
         <v>80</v>
       </c>
-      <c r="CD8" s="17">
+      <c r="CD8" s="16">
         <v>81</v>
       </c>
-      <c r="CE8" s="17">
+      <c r="CE8" s="16">
         <v>82</v>
       </c>
-      <c r="CF8" s="17">
+      <c r="CF8" s="16">
         <v>83</v>
       </c>
-      <c r="CG8" s="22">
+      <c r="CG8" s="21">
         <v>84</v>
       </c>
-      <c r="CH8" s="17">
+      <c r="CH8" s="16">
         <v>85</v>
       </c>
-      <c r="CI8" s="17">
+      <c r="CI8" s="16">
         <v>86</v>
       </c>
-      <c r="CJ8" s="17">
+      <c r="CJ8" s="16">
         <v>87</v>
       </c>
-      <c r="CK8" s="22">
+      <c r="CK8" s="21">
         <v>88</v>
       </c>
-      <c r="CL8" s="17">
+      <c r="CL8" s="16">
         <v>89</v>
       </c>
-      <c r="CM8" s="17">
+      <c r="CM8" s="16">
         <v>90</v>
       </c>
-      <c r="CN8" s="17">
+      <c r="CN8" s="16">
         <v>91</v>
       </c>
-      <c r="CO8" s="22">
+      <c r="CO8" s="21">
         <v>92</v>
       </c>
-      <c r="CP8" s="17">
+      <c r="CP8" s="16">
         <v>93</v>
       </c>
-      <c r="CQ8" s="17">
+      <c r="CQ8" s="16">
         <v>94</v>
       </c>
-      <c r="CR8" s="17">
+      <c r="CR8" s="16">
         <v>95</v>
       </c>
-      <c r="CS8" s="22">
+      <c r="CS8" s="21">
         <v>96</v>
       </c>
-      <c r="CT8" s="17">
+      <c r="CT8" s="16">
         <v>97</v>
       </c>
-      <c r="CU8" s="17">
+      <c r="CU8" s="16">
         <v>98</v>
       </c>
-      <c r="CV8" s="17">
+      <c r="CV8" s="16">
         <v>99</v>
       </c>
-      <c r="CW8" s="22">
+      <c r="CW8" s="21">
         <v>100</v>
       </c>
-      <c r="CX8" s="17">
+      <c r="CX8" s="16">
         <v>101</v>
       </c>
-      <c r="CY8" s="17">
+      <c r="CY8" s="16">
         <v>102</v>
       </c>
-      <c r="CZ8" s="17">
+      <c r="CZ8" s="16">
         <v>103</v>
       </c>
-      <c r="DA8" s="22">
+      <c r="DA8" s="21">
         <v>104</v>
       </c>
-      <c r="DB8" s="17">
+      <c r="DB8" s="16">
         <v>105</v>
       </c>
-      <c r="DC8" s="17">
+      <c r="DC8" s="16">
         <v>106</v>
       </c>
-      <c r="DD8" s="17">
+      <c r="DD8" s="16">
         <v>107</v>
       </c>
-      <c r="DE8" s="22">
+      <c r="DE8" s="21">
         <v>108</v>
       </c>
-      <c r="DF8" s="17">
+      <c r="DF8" s="16">
         <v>109</v>
       </c>
-      <c r="DG8" s="17">
+      <c r="DG8" s="16">
         <v>110</v>
       </c>
-      <c r="DH8" s="17">
+      <c r="DH8" s="16">
         <v>111</v>
       </c>
-      <c r="DI8" s="22">
+      <c r="DI8" s="21">
         <v>112</v>
       </c>
-      <c r="DJ8" s="17">
+      <c r="DJ8" s="16">
         <v>113</v>
       </c>
-      <c r="DK8" s="17">
+      <c r="DK8" s="16">
         <v>114</v>
       </c>
-      <c r="DL8" s="17">
+      <c r="DL8" s="16">
         <v>115</v>
       </c>
-      <c r="DM8" s="22">
+      <c r="DM8" s="21">
         <v>116</v>
       </c>
-      <c r="DN8" s="17">
+      <c r="DN8" s="16">
         <v>117</v>
       </c>
-      <c r="DO8" s="17">
+      <c r="DO8" s="16">
         <v>118</v>
       </c>
-      <c r="DP8" s="17">
+      <c r="DP8" s="16">
         <v>119</v>
       </c>
-      <c r="DQ8" s="22">
+      <c r="DQ8" s="21">
         <v>120</v>
       </c>
-      <c r="DR8" s="17">
+      <c r="DR8" s="16">
         <v>121</v>
       </c>
-      <c r="DS8" s="17">
+      <c r="DS8" s="16">
         <v>122</v>
       </c>
-      <c r="DT8" s="17">
+      <c r="DT8" s="16">
         <v>123</v>
       </c>
-      <c r="DU8" s="22">
+      <c r="DU8" s="21">
         <v>124</v>
       </c>
-      <c r="DV8" s="17">
+      <c r="DV8" s="16">
         <v>125</v>
       </c>
-      <c r="DW8" s="17">
+      <c r="DW8" s="16">
         <v>126</v>
       </c>
-      <c r="DX8" s="17">
+      <c r="DX8" s="16">
         <v>127</v>
       </c>
-      <c r="DY8" s="22">
+      <c r="DY8" s="21">
         <v>128</v>
       </c>
-      <c r="DZ8" s="17">
+      <c r="DZ8" s="16">
         <v>129</v>
       </c>
-      <c r="EA8" s="17">
+      <c r="EA8" s="16">
         <v>130</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="75">
+    <mergeCell ref="DU4:DY4"/>
+    <mergeCell ref="DT7:DY7"/>
+    <mergeCell ref="DZ7:EA7"/>
+    <mergeCell ref="DD4:DH4"/>
+    <mergeCell ref="DI4:DL4"/>
+    <mergeCell ref="DD5:DH5"/>
+    <mergeCell ref="DO5:DP5"/>
+    <mergeCell ref="DI5:DL5"/>
+    <mergeCell ref="CS6:DM6"/>
+    <mergeCell ref="CS7:DM7"/>
+    <mergeCell ref="DN6:DR6"/>
+    <mergeCell ref="DN7:DS7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="CZ5:DA5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="CB5:CE5"/>
+    <mergeCell ref="CF5:CG5"/>
+    <mergeCell ref="CI5:CR5"/>
+    <mergeCell ref="CX5:CY5"/>
+    <mergeCell ref="AQ6:BW6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="AA5:AD5"/>
+    <mergeCell ref="Q6:X6"/>
+    <mergeCell ref="AA6:AD6"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="BZ4:CA4"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="AE6:AO6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="Q1:AJ1"/>
+    <mergeCell ref="AK1:AP1"/>
+    <mergeCell ref="DV6:EA6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="AS7:AT7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="X7:AJ7"/>
+    <mergeCell ref="AK7:AP7"/>
+    <mergeCell ref="AQ7:AR7"/>
+    <mergeCell ref="AV7:BW7"/>
+    <mergeCell ref="BX6:CR6"/>
+    <mergeCell ref="BX7:CR7"/>
     <mergeCell ref="DN1:EA1"/>
     <mergeCell ref="BL5:BO5"/>
     <mergeCell ref="BP5:BS5"/>
@@ -3837,65 +3895,6 @@
     <mergeCell ref="CI4:CR4"/>
     <mergeCell ref="DQ5:DR5"/>
     <mergeCell ref="AQ5:AU5"/>
-    <mergeCell ref="B1:P1"/>
-    <mergeCell ref="Q1:AJ1"/>
-    <mergeCell ref="AK1:AP1"/>
-    <mergeCell ref="DV6:EA6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="AS7:AT7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="X7:AJ7"/>
-    <mergeCell ref="AK7:AP7"/>
-    <mergeCell ref="AQ7:AR7"/>
-    <mergeCell ref="AV7:BW7"/>
-    <mergeCell ref="BX6:CR6"/>
-    <mergeCell ref="BX7:CR7"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="AE6:AO6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AK5:AM5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="BZ4:CA4"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="CZ5:DA5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="CB5:CE5"/>
-    <mergeCell ref="CF5:CG5"/>
-    <mergeCell ref="CI5:CR5"/>
-    <mergeCell ref="CX5:CY5"/>
-    <mergeCell ref="AQ6:BW6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="AA5:AD5"/>
-    <mergeCell ref="Q6:X6"/>
-    <mergeCell ref="AA6:AD6"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="DU4:DY4"/>
-    <mergeCell ref="DT7:DY7"/>
-    <mergeCell ref="DZ7:EA7"/>
-    <mergeCell ref="DD4:DH4"/>
-    <mergeCell ref="DI4:DL4"/>
-    <mergeCell ref="DD5:DH5"/>
-    <mergeCell ref="DO5:DP5"/>
-    <mergeCell ref="DI5:DL5"/>
-    <mergeCell ref="CS6:DM6"/>
-    <mergeCell ref="CS7:DM7"/>
-    <mergeCell ref="DN6:DR6"/>
-    <mergeCell ref="DN7:DS7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="X4" r:id="rId1" xr:uid="{33A4BD0C-7A19-4C88-AF60-902623A24589}"/>
@@ -3910,19 +3909,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ede1785e-3bac-4a90-a48c-62cc0231644e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000BCF930048F2A84190E342D576E507E9" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a5f7dcad46bf03cd06b92fe3a65eb3e5">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ede1785e-3bac-4a90-a48c-62cc0231644e" xmlns:ns3="6c5f9a5a-0dad-4595-a39a-6416e9fb7054" xmlns:ns4="83a87e31-bf32-46ab-8e70-9fa18461fa4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="627fd199b21a7508d85a0883525fd0b8" ns2:_="" ns3:_="" ns4:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000BCF930048F2A84190E342D576E507E9" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="263b522f34af87636eb5a7b2dc30e648">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ede1785e-3bac-4a90-a48c-62cc0231644e" xmlns:ns3="6c5f9a5a-0dad-4595-a39a-6416e9fb7054" xmlns:ns4="83a87e31-bf32-46ab-8e70-9fa18461fa4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a158f55a44c8de9db2cc0af700b09a3c" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
     <xsd:import namespace="6c5f9a5a-0dad-4595-a39a-6416e9fb7054"/>
     <xsd:import namespace="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
@@ -3949,11 +3947,27 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="26" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="27" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="ede1785e-3bac-4a90-a48c-62cc0231644e" elementFormDefault="qualified">
@@ -4181,39 +4195,34 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ede1785e-3bac-4a90-a48c-62cc0231644e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3234EB82-E598-4D46-AACB-BAE493D677A7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D2572BD-7EE7-4817-BEE4-BB014A85EDEE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6c5f9a5a-0dad-4595-a39a-6416e9fb7054"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{844596B9-62AA-44A2-8AEF-70908D01A276}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17AFA51A-13A5-4296-8804-3A0CE81BEA66}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
     <ds:schemaRef ds:uri="6c5f9a5a-0dad-4595-a39a-6416e9fb7054"/>
     <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
@@ -4228,15 +4237,26 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D2572BD-7EE7-4817-BEE4-BB014A85EDEE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3234EB82-E598-4D46-AACB-BAE493D677A7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6c5f9a5a-0dad-4595-a39a-6416e9fb7054"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{fbd41ebe-fca6-4f2c-aecb-bf3a17e72416}" enabled="1" method="Privileged" siteId="{bf346810-9c7d-43de-a872-24a2ef3995a8}" contentBits="3" removed="0"/>
+  <clbl:label id="{fbd41ebe-fca6-4f2c-aecb-bf3a17e72416}" enabled="1" method="Privileged" siteId="{bf346810-9c7d-43de-a872-24a2ef3995a8}" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>